<commit_message>
iknow_converter agora serve tanto para wpp e rcs; tentativa de aplicar URA, mas o writer está escrevendo abas das outras plataformas
</commit_message>
<xml_diff>
--- a/Saida/N8/finalizado.xlsx
+++ b/Saida/N8/finalizado.xlsx
@@ -10,6 +10,7 @@
     <sheet name="RELATÓRIO" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="RESPOSTAS" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Ativação" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Interação" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -503,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,7 +534,179 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>['85974001107', '85981010387', '85981010504', '85981010801', '85981011300', '85981011982', '85981012709', '85981012859', '85981012916', '85981013105', '85981013139', '85981013252', '85981014486', '85981015083', '85981015199', '85981015345', '85981015408', '85981015858', '85981018191', '85981019737', '85981019859', '85981020615', '85981021220', '85981021847', '85981021858', '85981023473', '85981024243', '85981024932', '85981025159', '85981026077', '85981026188', '85981026342', '85981029941', '85981034608', '85981035347', '85981037998', '85981038369', '85981040609', '85981041303', '85981042289', '85981046232', '85981047325', '85981047447', '85981050094', '85981050305', '85981050670', '85981050778', '85981050921', '85981051007', '85981051157', '85981051236', '85981051357', '85981051407', '85981051960', '85981052023', '85981052147', '85981052388', '85981053361', '85981053645', '85981053870', '85981054245', '85981054310', '85981054721', '85981054784', '85981055402', '85981055606', '85981055887', '85981056204', '85981056432', '85981057133', '85981057473', '85981057594', '85981057657', '85981058510', '85981058575', '85981059167', '85981060358', '85981060840', '85981060881', '85981060903', '85981060912', '85981061514', '85981062036', '85981062783', '85981062811', '85981063144', '85981063180', '85981063445', '85981063577', '85981063706', '85981063708', '85981063769', '85981064311', '85981064501', '85981064633', '85981066228', '85981066596', '85981066800', '85981067063', '85981067120', '85981067303', '85981067738', '85981068259', '85981068383', '85981068838', '85981069073', '85981069268', '85981069285', '85981069288', '85981069331', '85981069531', '85981069805', '85981070139', '85981070716', '85981070933', '85981072516', '85981074292', '85981074824', '85981077799', '85981079793', '85981080110', '85981081102', '85981081645', '85981081717', '85981081963', '85981082567', '85981082798', '85981083944', '85981083955', '85981084430', '85981085176', '85981085425', '85981086055', '85981087566', '85981090951', '85981092003', '85981094270', '85981095658', '85981096027', '85981097092', '85981097525', '85981099771', '85981099834', '85981104139', '85981105541', '85981111379', '85981111687', '85981112198', '85981112368', '85981113354', '85981116111', '85981116475', '85981117229', '85981117240', '85981117970', '85981118916', '85981119356', '85981121743', '85981121756', '85981121918', '85981122659', '85981122830', '85981124417', '85981125198', '85981125364', '85981127000', '85981127863', '85981128332', '85981128640', '85981129033', '85981130954', '85981131390', '85981132338', '85981132657', '85981132861', '85981133001', '85981136515', '85981137269', '85981137935', '85981138484', '85981139818', '85981141110', '85981141235', '85981142047', '85981142397', '85981144074', '85981144194', '85981144290', '85981144476', '85981145210', '85981145431', '85981146150', '85981147761', '85981148652', '85981149605', '85981149798', '85981149833', '85981150270', '85981152513', '85981152668', '85981152923', '85981153276', '85981154070', '85981154704', '85981154767', '85981155516', '85981155609', '85981155832', '85981157497', '85981159783', '85981160701', '85981162279', '85981163532', '85981168773', '85981169336', '85981170375', '85981170419', '85981172174', '85981172237', '85981173080', '85981173491', '85981173596', '85981174595', '85981175102', '85981175961', '85981176245', '85981176511', '85981176843', '85981176855', '85981177377', '85981177436', '85981178111', '85981180220', '85981180748', '85981181223', '85981181460', '85981184568', '85981185113', '85981185397', '85981185432', '85981186162', '85981187777', '85981187790', '85981188522', '85981190449', '85981190603', '85981190941', '85981191324', '85981191501', '85981192668', '85981193462', '85981194504', '85981195274', '85981195777', '85981196765', '85981199009', '85981200624', '85981204580', '85981205000', '85981207224', '85981210397', '85981211722', '85981211785', '85981212297', '85981212335', '85981215121', '85981215323', '85981217007', '85981217070', '85981217271', '85981217334', '85981217865', '85981217880', '85981217928', '85981219726', '85981220015', '85981220097', '85981220132', '85981221107', '85981221148', '85981222412', '85981224119', '85981224486', '85981224995', '85981225097', '85981225167', '85981226403', '85981227172', '85981227283', '85981227812', '85981228111', '85981228405', '85981228468', '85981229862', '85981229918', '85981229981', '85981230013', '85981230104', '85981233010', '85981233031', '85981233110', '85981234275', '85981235443', '85981237281', '85981238571', '85981240151', '85981240906', '85981241794', '85981243937', '85981245200', '85981245595', '85981245660', '85981246453', '85981246810', '85981247191', '85981247682', '85981247801', '85981248056', '85981248614', '85981248938', '85981249006', '85981249077', '85981249520', '85981249804', '85981250065', '85981251340', '85981252190', '85981252202', '85981252814', '85981253454', '85981256347', '85981256415', '85981256918', '85981257594', '85981257644', '85981258954', '85981259116', '85981259996', '85981260093', '85981260293', '85981261976', '85981264023', '85981265628', '85981266155', '85981266554', '85981267575', '85981268163', '85981269254', '85981270887', '85981273817', '85981276088', '85981277050', '85981277171', '85981277778', '85981277862', '85981278172', '85981278481', '85981281110', '85981281122', '85981283976', '85981284254', '85981284771', '85981284904', '85981285694', '85981285757', '85981286755', '85981287954', '85981288208', '85981288338', '85981289201', '85981290315', '85981291170', '85981291852', '85981292335', '85981292898', '85981293237', '85981296943', '85981297006', '85981297774', '85981298411', '85981298474', '85981299369', '85981300207', '85981300265', '85981301018', '85981301029', '85981301090', '85981301430', '85981302820', '85981303653', '85981304383', '85981304684', '85981304736', '85981304842', '85981305581', '85981306366', '85981307620', '85981307802', '85981308045', '85981308259', '85981308292', '85981308328', '85981308337', '85981308391', '85981310114', '85981310742', '85981311091', '85981311398', '85981312075', '85981313089', '85981313134', '85981313616', '85981313627', '85981314051', '85981314422', '85981315654', '85981316754', '85981318080', '85981323921', '85981325550', '85981327070', '85981327436', '85981327760', '85981328852', '85981330136', '85981330758', '85981331850', '85981331913', '85981332190', '85981333065', '85981333339', '85981334650', '85981334713', '85981334761', '85981335534', '85981337373', '85981338263', '85981338307', '85981342092', '85981342565', '85981343138', '85981343533', '85981344833', '85981345060', '85981347012', '85981347371', '85981348351', '85981348558', '85981349404', '85981351875', '85981352588', '85981352826', '85981353374', '85981353997', '85981354648', '85981355846', '85981357814', '85981359310', '85981360852', '85981361507', '85981361779', '85981362003', '85981362066', '85981363777', '85981365886', '85981366880', '85981367170', '85981368633', '85981370043', '85981370894', '85981371153', '85981371868', '85981372645', '85981374219', '85981375527', '85981375801', '85981375825', '85981376079', '85981377391', '85981378159', '85981378792', '85981378905', '85981379505', '85981379662', '85981380597', '85981380924', '85981381707', '85981381999', '85981383237', '85981383353', '85981384426', '85981385151', '85981385624', '85981385673', '85981385841', '85981386704', '85981386821', '85981387227', '85981387362', '85981388619', '85981391330', '85981391423', '85981391880', '85981392100', '85981392565', '85981395635', '85981395687', '85981395818', '85981397246', '85981397372', '85981397409', '85981397411', '85981398764', '85981400369', '85981401399', '85981401626', '85981401752', '85981402041', '85981402081', '85981402748', '85981402997', '85981403093', '85981403964', '85981404116', '85981404174', '85981404374', '85981404793', '85981405917', '85981408267', '85981409242', '85981409843', '85981411024', '85981411624', '85981411687', '85981413039', '85981413532', '85981413653', '85981413838', '85981413892', '85981414546', '85981415469', '85981416386', '85981416409', '85981418850', '85981419344', '85981420019', '85981421525', '85981421738', '85981422245', '85981422308', '85981422576', '85981422856', '85981423490', '85981423505', '85981423933', '85981424271', '85981424607', '85981425703', '85981426537', '85981426942', '85981427253', '85981428860', '85981428912', '85981432332', '85981433880', '85981436330', '85981437233', '85981437797', '85981440921', '85981442203', '85981443375', '85981444452', '85981444515', '85981445843', '85981447674', '85981448037', '85981452309', '85981453385', '85981460147', '85981460175', '85981460392', '85981460457', '85981460646', '85981460699', '85981460861', '85981460924', '85981460996', '85981461065', '85981461106', '85981461610', '85981462406', '85981463746', '85981463860', '85981464262', '85981464411', '85981464530', '85981464545', '85981465735', '85981465772', '85981465798', '85981466545', '85981467570', '85981468790', '85981470659', '85981470831', '85981471492', '85981471759', '85981472233', '85981473750', '85981474263', '85981474389', '85981474696', '85981474697', '85981474756', '85981474760', '85981474778', '85981474912', '85981474923', '85981475220', '85981475230', '85981475761', '85981475972', '85981475980', '85981476043', '85981476212', '85981476638', '85981477326', '85981477413', '85981477799', '85981477812', '85981477813', '85981477916', '85981478494', '85981478784', '85981479493', '85981479515', '85981479752', '85981479774', '85981481053', '85981481331', '85981481726', '85981482109', '85981482140', '85981482476', '85981482990', '85981483810', '85981484967', '85981485284', '85981485480', '85981486380', '85981486397', '85981487878', '85981488161', '85981488741', '85981489506', '85981489546', '85981489609', '85981489986', '85981491380', '85981491428', '85981491439', '85981492666', '85981492729', '85981495205', '85981495268', '85981495465', '85981495615', '85981495911', '85981495935', '85981496025', '85981496943', '85981497099', '85981497122', '85981497496', '85981497614', '85981499186', '85981500414', '85981500847', '85981500940', '85981501090', '85981501968', '85981502098', '85981502241', '85981505500', '85981505522', '85981505531', '85981505586', '85981505887', '85981506224', '85981506332', '85981506467', '85981506955', '85981507053', '85981507770', '85981507930', '85981509140', '85981509349', '85981509981', '85981510677', '85981511295', '85981512929', '85981514081', '85981514747', '85981518467', '85981518484', '85981520304', '85981521334', '85981521816', '85981521879', '85981521962', '85981522121', '85981522321', '85981522480', '85981522523', '85981522914', '85981522917', '85981522933', '85981522980', '85981523042', '85981523247', '85981523548', '85981523703', '85981523830', '85981523864', '85981524209', '85981524336', '85981524345', '85981524388', '85981524433', '85981524474', '85981525329', '85981525392', '85981525946', '85981525956', '85981525970', '85981526066', '85981526142', '85981526377', '85981526414', '85981526660', '85981526890', '85981526953', '85981527026', '85981527241', '85981527738', '85981527876', '85981527926', '85981528100', '85981528344', '85981528523', '85981529250', '85981530016', '85981530202', '85981530228', '85981530264', '85981530358', '85981530695', '85981531466', '85981532323', '85981532367', '85981532706', '85981533140', '85981533536', '85981533817', '85981533861', '85981533924', '85981534836', '85981535019', '85981535381', '85981535444', '85981535702', '85981536001', '85981536037', '85981536784', '85981537054', '85981537071', '85981537451', '85981537531', '85981537646', '85981538008', '85981538403', '85981538473', '85981539100', '85981539364', '85981539374', '85981539613', '85981539674', '85981539710', '85981539904', '85981542565', '85981544220', '85981544377', '85981544415', '85981544420', '85981544535', '85981544744', '85981545730', '85981545967', '85981546135', '85981546201', '85981546486', '85981546524', '85981547100', '85981547151', '85981547181', '85981548573', '85981548663', '85981549807', '85981550607', '85981551701', '85981552786', '85981552815', '85981553207', '85981553257', '85981553774', '85981554041', '85981554682', '85981555448', '85981556360', '85981556386', '85981556391', '85981556708', '85981557599', '85981557763', '85981557766', '85981557996', '85981558443', '85981558444', '85981558593', '85981558734', '85981558921', '85981559352', '85981559880', '85981559990', '85981561122', '85981561397', '85981563114', '85981563918', '85981565385', '85981566296', '85981569388', '85981570332', '85981570553', '85981571936', '85981571948', '85981573149', '85981574029', '85981574749', '85981574828', '85981575288', '85981576121', '85981577685', '85981579715', '85981580747', '85981582223', '85981587265', '85981588881', '85981589028', '85981590283', '85981590581', '85981591212', '85981591394', '85981592814', '85981594445', '85981594455', '85981598314', '85981599091', '85981599720', '85981600032', '85981600288', '85981600746', '85981601467', '85981601515', '85981601621', '85981603545', '85981603701', '85981603764', '85981603922', '85981604044', '85981604097', '85981604901', '85981605888', '85981606241', '85981606453', '85981606516', '85981606875', '85981607061', '85981607171', '85981607847', '85981608039', '85981608131', '85981608656', '85981608885', '85981609224', '85981609765', '85981611504', '85981611687', '85981612354', '85981612497', '85981613707', '85981614805', '85981615721', '85981615726', '85981616672', '85981617048', '85981617443', '85981617809', '85981618157', '85981618463', '85981618696', '85981619089', '85981621012', '85981625207', '85981625719', '85981625789', '85981625797', '85981626292', '85981626455', '85981627178', '85981627515', '85981627750', '85981628353', '85981628962', '85981629450', '85981630101', '85981630164', '85981631945', '85981632116', '85981635515', '85981635650', '85981636098', '85981636649', '85981638200', '85981638739', '85981639201', '85981642110', '85981642480', '85981645543', '85981646909', '85981647853', '85981649485', '85981651235', '85981651813', '85981651856', '85981653359', '85981654096', '85981655420', '85981655504', '85981656015', '85981656761', '85981663973', '85981664051', '85981665088', '85981665658', '85981665867', '85981666220', '85981666585', '85981666685', '85981668986', '85981669316', '85981669696', '85981669892', '85981670050', '85981670209', '85981670557', '85981671233', '85981672007', '85981672198', '85981672687', '85981676600', '85981677013', '85981677923', '85981677986', '85981679022', '85981679393', '85981684827', '85981685253', '85981687262', '85981688088', '85981688530', '85981689614', '85981690885', '85981692225', '85981693076', '85981694698', '85981696440', '85981700371', '85981701616', '85981701789', '85981702211', '85981704587', '85981705823', '85981706117', '85981706812', '85981707565', '85981709424', '85981709639', '85981709959', '85981709997', '85981711415', '85981712700', '85981715589', '85981717124', '85981721330', '85981721470', '85981723162', '85981723682', '85981727178', '85981727333', '85981730276', '85981731368', '85981733009', '85981733173', '85981734225', '85981735351', '85981735457', '85981738337', '85981742689', '85981745007', '85981746191', '85981746231', '85981747230', '85981747684', '85981747880', '85981748018', '85981749098', '85981749311', '85981780097', '85981780698', '85981781860', '85981781956', '85981782615', '85981783993', '85981787014', '85981787375', '85981787694', '85981787878', '85981795562', '85981797415', '85981799011', '85981799243', '85981799393', '85981799969', '85981800644', '85981801187', '85981801628', '85981801718', '85981801761', '85981802537', '85981802631', '85981803848', '85981804731', '85981805074', '85981805578', '85981805682', '85981805712', '85981805995', '85981806062', '85981806192', '85981806838', '85981807096', '85981807746', '85981808109', '85981808226', '85981808940', '85981809310', '85981809579', '85981810401', '85981811681', '85981812231', '85981812420', '85981813215', '85981813326', '85981813696', '85981813745', '85981814222', '85981815518', '85981815719', '85981815951', '85981815995', '85981816185', '85981816597', '85981816953', '85981817644', '85981819191', '85981819878', '85981819898', '85981819971', '85981820302', '85981820909', '85981822288', '85981822627', '85981823737', '85981824050', '85981825667', '85981827171', '85981827298', '85981828133', '85981829674', '85981829888', '85981830615', '85981831333', '85981831807', '85981832616', '85981833911', '85981836027', '85981836192', '85981838197', '85981839905', '85981840699', '85981840997', '85981841498', '85981842018', '85981842026', '85981847568', '85981849140', '85981849448', '85981850329', '85981851336', '85981851657', '85981851806', '85981852483', '85981852871', '85981853361', '85981853473', '85981853498', '85981854188', '85981854400', '85981854701', '85981854966', '85981855387', '85981855943', '85981857602', '85981858378', '85981858585', '85981859714', '85981859843', '85981860190', '85981860939', '85981861386', '85981861390', '85981862200', '85981862732', '85981862812', '85981863520', '85981863917', '85981864665', '85981866872', '85981867198', '85981867874', '85981868706', '85981869078', '85981869877', '85981870279', '85981870625', '85981870769', '85981871433', '85981871482', '85981871725', '85981872527', '85981873853', '85981874873', '85981875089', '85981875839', '85981876038', '85981876387', '85981877277', '85981877340', '85981877666', '85981878608', '85981879558', '85981879727', '85981881447', '85981881564', '85981881903', '85981882019', '85981882233', '85981883888', '85981885848', '85981886408', '85981888076', '85981890073', '85981890692', '85981890804', '85981890897', '85981891321', '85981891476', '85981892737', '85981892922', '85981893512', '85981894559', '85981895421', '85981895778', '85981895877', '85981899243', '85981900080', '85981900730', '85981901391', '85981904698', '85981905011', '85981905074', '85981905075', '85981906452', '85981910262', '85981910771', '85981911604', '85981911984', '85981914747', '85981917082', '85981917653', '85981917936', '85981918090', '85981918203', '85981921936', '85981921999', '85981922555', '85981924869', '85981926087', '85981926161', '85981927362', '85981928269', '85981930502', '85981933090', '85981933446', '85981934488', '85981937771', '85981942675', '85981944086', '85981946447', '85981947455', '85981948504', '85981948560', '85981948709', '85981949370', '85981949405', '85981950680', '85981951197', '85981951207', '85981951277', '85981951294', '85981951433', '85981952223', '85981952606', '85981953266', '85981955156', '85981955666', '85981956683', '85981956798', '85981956914', '85981956977', '85981958219', '85981958833', '85981959454', '85981962203', '85981963748', '85981964770', '85981966391', '85981966744', '85981967093', '85981967347', '85981967672', '85981972215', '85981973787', '85981973850', '85981974619', '85981975003', '85981975335', '85981975643', '85981978964', '85981982384', '85981982415', '85981983536', '85981984160', '85981984196', '85981984205', '85981985320', '85981987749', '85981990206', '85981991814', '85981992200', '85981992221', '85981993841', '85981994171', '85981994544', '85981996677', '85981996968', '85981997233', '85981998183', '85981998880', '85981999101', '85981999393', '85982000080', '85982000103', '85982000124', '85982000407', '85982000597', '85982001158', '85982001480', '85982001603', '85982002244', '85982003360', '85982009691', '85982012352', '85982013350', '85982013725', '85982014410', '85982014728', '85982014859', '85982015963', '85982016650', '85982018181', '85982019178', '85982020684', '85982020732', '85982021675', '85982021901', '85982021970', '85982022116', '85982022707', '85982023008', '85982023198', '85982023449', '85982024092', '85982024412', '85982024556', '85982025193', '85982025465', '85982025505', '85982026115', '85982026559', '85982026582', '85982026618', '85982026681', '85982026958', '85982027257', '85982027456', '85982028016', '85982028614', '85982028717', '85982029544', '85982029630', '85982029656', '85982031994', '85982033246', '85982036215', '85982038136', '85982038199', '85982038964', '85982041982', '85982048028', '85982048400', '85982048768', '85982049005', '85982050430', '85982051850', '85982052170', '85982052833', '85982053074', '85982058486', '85982059867', '85982060243', '85982061188', '85982061715', '85982065404', '85982066323', '85982066720', '85982067095', '85982067924', '85982069921', '85982070325', '85982070442', '85982070505', '85982070537', '85982075392', '85982076079', '85982077220', '85982080055', '85982080963', '85982081863', '85982082408', '85982082685', '85982086204', '85982086988', '85982088181', '85982088401', '85982090444', '85982092229', '85982092410', '85982092535', '85982095933', '85982096408', '85982096638', '85982096702', '85982098898', '85982099596', '85982101224', '85982102764', '85982103459', '85982103837', '85982104191', '85982105219', '85982105253', '85982105588', '85982106049', '85982107612', '85982108435', '85982108824', '85982108871', '85982108995', '85982109939', '85982110388', '85982110918', '85982111162', '85982111405', '85982111461', '85982111682', '85982111714', '85982112134', '85982112150', '85982112252', '85982112330', '85982112561', '85982112835', '85982113153', '85982113424', '85982113947', '85982114041', '85982114590', '85982114798', '85982115352', '85982115530', '85982116277', '85982116934', '85982116997', '85982118281', '85982118296', '85982118359', '85982118717', '85982119038', '85982119077', '85982120196', '85982120770', '85982121018', '85982121624', '85982122300', '85982122468', '85982123793', '85982123880', '85982125254', '85982126275', '85982127512', '85982130408', '85982130446', '85982131720', '85982132411', '85982132443', '85982132450', '85982133520', '85982134594', '85982134658', '85982140032', '85982141654', '85982144572', '85982145647', '85982145648', '85982147385', '85982147517', '85982148150', '85982148935', '85982150345', '85982154109', '85982154431', '85982154497', '85982155595', '85982155633', '85982161243', '85982161749', '85982162384', '85982162735', '85982163153', '85982164038', '85982166162', '85982166295', '85982166369', '85982170184', '85982171502', '85982171541', '85982171985', '85982184521', '85982185872', '85982190343', '85982204545', '85982205828', '85982207580', '85982217764', '85982222262', '85982223649', '85982225298', '85982234415', '85982243000', '85982254767', '85982254833', '85984000187', '85984000206', '85984000276', '85984000283', '85984000366', '85984000374', '85984000408', '85984000419', '85984000570', '85984000752', '85984000901', '85984000924', '85984001030', '85984001034', '85984001146', '85984001200', '85984001263', '85984001399', '85984001670', '85984001714', '85984001904', '85984002329', '85984002699', '85984004021', '85984004143', '85984004381', '85984004513', '85984004885', '85984004934', '85984004937', '85984005030', '85984005089', '85984005191', '85984005207', '85984005486', '85984005676', '85984005684', '85984005854', '85984006088', '85984006430', '85984006519', '85984006807', '85984006822', '85984006945', '85984007418', '85984007839', '85984007934', '85984008090', '85984008165', '85984008494', '85984008541', '85984008711', '85984008837', '85984008876', '85984009118', '85984009152', '85984010102', '85984010119', '85984010346', '85984010352', '85984010376', '85984010523', '85984010651', '85984010721', '85984010796', '85984011030', '85984011127', '85984011205', '85984011272', '85984011345', '85984011423', '85984012202', '85984012591', '85984012893', '85984013559', '85984013847', '85984013900', '85984013932', '85984013963', '85984014210', '85984014231', '85984014288', '85984014376', '85984014432', '85984014547', '85984015074', '85984015099', '85984015349', '85984015384', '85984015385', '85984015469', '85984015572', '85984015631', '85984015661', '85984015695', '85984015758', '85984015793', '85984015918', '85984015943', '85984015948', '85984016599', '85984016848', '85984017946', '85984018354', '85984019606', '85984019846', '85984019986', '85984020049', '85984020051', '85984020177', '85984020235', '85984020417', '85984020826', '85984020911', '85984021324', '85984021461', '85984021871', '85984022102', '85984022241', '85984022389', '85984022437', '85984022645', '85984023016', '85984023231', '85984023332', '85984023361', '85984023534', '85984024023', '85984024057', '85984024750', '85984024773', '85984024790', '85984024966', '85984025156', '85984025366', '85984025761', '85984026229', '85984026355', '85984026707', '85984026882', '85984026909', '85984026937', '85984027014', '85984027778', '85984027803', '85984027980', '85984028311', '85984028478', '85984028528', '85984028635', '85984028807', '85984029384', '85984029403', '85984029645', '85984029647', '85984029806', '85984029997', '85984030002', '85984030015', '85984030126', '85984030128', '85984030255', '85984030534', '85984030799', '85984030914', '85984031018', '85984031134', '85984031235', '85984031240', '85984031369', '85984031377', '85984031387', '85984031438', '85984031757', '85984031799', '85984031859', '85984031951', '85984031983', '85984031996', '85984032024', '85984032030', '85984032046', '85984032152', '85984032209', '85984032278', '85984032838', '85984032911', '85984033253', '85984033308', '85984033709', '85984033733', '85984033741', '85984033796', '85984033825', '85984033893', '85984033983', '85984034114', '85984034385', '85984034577', '85984034588', '85984034633', '85984034782', '85984034964', '85984035081', '85984035134', '85984035188', '85984035416', '85984035423', '85984035459', '85984035494', '85984035559', '85984035765', '85984036032', '85984036315', '85984036485', '85984036570', '85984036614', '85984036676', '85984036734', '85984036808', '85984036872', '85984037291', '85984037296', '85984037302', '85984037313', '85984037354', '85984037682', '85984037921', '85984037935', '85984037947', '85984038033', '85984038229', '85984038524', '85984038538', '85984038620', '85984038850', '85984038856', '85984039320', '85984039429', '85984039451', '85984039728', '85984040449', '85984040502', '85984040554', '85984040731', '85984040757', '85984040783', '85984040792', '85984040899', '85984041029', '85984041044', '85984041297', '85984041417', '85984041458', '85984041670', '85984041713', '85984041805', '85984041914', '85984041986', '85984042380', '85984042425', '85984042497', '85984042509', '85984042623', '85984042895', '85984042963', '85984043070', '85984043137', '85984043296', '85984043323', '85984043326', '85984043413', '85984043751', '85984044012', '85984044067', '85984044191', '85984044248', '85984044283', '85984044300', '85984044346', '85984044633', '85984044683', '85984044763', '85984044963', '85984045050', '85984045056', '85984045115', '85984045640', '85984045722', '85984046240', '85984046424', '85984046625', '85984046753', '85984046806', '85984046807', '85984046867', '85984047111', '85984047230', '85984047233', '85984047367', '85984047472', '85984047476', '85984047517', '85984047596', '85984048175', '85984048182', '85984048183', '85984048283', '85984048339', '85984048508', '85984048524', '85984048559', '85984048759', '85984048849', '85984049026', '85984049029', '85984049263', '85984049442', '85984049451', '85984049504', '85984049679', '85984049735', '85984049763', '85984049858', '85984049949', '85984050227', '85984050228', '85984050250', '85984050371', '85984050677', '85984050801', '85984050882', '85984050887', '85984050928', '85984051292', '85984051333', '85984051412', '85984051489', '85984051523', '85984051742', '85984051769', '85984051840', '85984051889', '85984051935', '85984052109', '85984052112', '85984052208', '85984052217', '85984052263', '85984052298', '85984052611', '85984052730', '85984052764', '85984052843', '85984053038', '85984053174', '85984053179', '85984053330', '85984053556', '85984053869', '85984053880', '85984053887', '85984053943', '85984053956', '85984054025', '85984054056', '85984054133', '85984054160', '85984054172', '85984054228', '85984054266', '85984054556', '85984054674', '85984054734', '85984054739', '85984054879', '85984054912', '85984055156', '85984055310', '85984055345', '85984055442', '85984055473', '85984055502', '85984055688', '85984055714', '85984055899', '85984055933', '85984056265', '85984056517', '85984056826', '85984056911', '85984056971', '85984057268', '85984057361', '85984057589', '85984057713', '85984057802', '85984057880', '85984058809', '85984059297', '85984059565', '85984059708', '85984060013', '85984060654', '85984060832', '85984061103', '85984061137', '85984061447', '85984061486', '85984061543', '85984061639', '85984061962', '85984062029', '85984062279', '85984062320', '85984062358', '85984062494', '85984062505', '85984062530', '85984063166', '85984063203', '85984063719', '85984063744', '85984063839', '85984064263', '85984064393', '85984064541', '85984064961', '85984065160', '85984065816', '85984066050', '85984066966', '85984067046', '85984067756', '85984067873', '85984068456', '85984069092', '85984069667', '85984069722', '85984069938', '85984070019', '85984070211', '85984070265', '85984070421', '85984070652', '85984070895', '85984071052', '85984071611', '85984071870', '85984072029', '85984072045', '85984072051', '85984072058', '85984072071', '85984072145', '85984072225', '85984072316', '85984072445', '85984072480', '85984072653', '85984072933', '85984073162', '85984073973', '85984074264', '85984074313', '85984074778', '85984075096', '85984075666', '85984076005', '85984076212', '85984076393', '85984076578', '85984076839', '85984076847', '85984077031', '85984077361', '85984077370', '85984077740', '85984077801', '85984078005', '85984078034', '85984078218', '85984078233', '85984078314', '85984078445', '85984078614', '85984079116', '85984079245', '85984079370', '85984079725', '85984079880', '85984079915', '85984080469', '85984080471', '85984080593', '85984080601', '85984081278', '85984081475', '85984081680', '85984082025', '85984082125', '85984082555', '85984082670', '85984082940', '85984082979', '85984083419', '85984083846', '85984084306', '85984084464', '85984084549', '85984084550', '85984084823', '85984084857', '85984085018', '85984085176', '85984085262', '85984085880', '85984086976', '85984087409', '85984088006', '85984088529', '85984089052', '85984089070', '85984089220', '85984089798', '85984090380', '85984090552', '85984090594', '85984090882', '85984090929', '85984091124', '85984091289', '85984091406', '85984091518', '85984092054', '85984092195', '85984092230', '85984092539', '85984093168', '85984093610', '85984093759', '85984093855', '85984094073', '85984094849', '85984095284', '85984096033', '85984098963', '85984099235', '85984099245', '85984099377', '85984099885', '85984100300', '85984100698', '85984100822', '85984101624', '85984101697', '85984102042', '85984102155', '85984102262', '85984102480', '85984102514', '85984102560', '85984102571', '85984103927', '85984104957', '85984105301', '85984105524', '85984106425', '85984107192', '85984107381', '85984107762', '85984108029', '85984108520', '85984108531', '85984108645', '85984108950', '85984109045', '85984109435', '85984109534', '85984110121', '85984110186', '85984110449', '85984110493', '85984110570', '85984110730', '85984110811', '85984111215', '85984111369', '85984111609', '85984111626', '85984111796', '85984111877', '85984111930', '85984112126', '85984112139', '85984112386', '85984112657', '85984113012', '85984113687', '85984113734', '85984113870', '85984113916', '85984114001', '85984114121', '85984114826', '85984114827', '85984115475', '85984115569', '85984115651', '85984116121', '85984116540', '85984116596', '85984116734', '85984116933', '85984117008', '85984117204', '85984117429', '85984117798', '85984118037', '85984118042', '85984118203', '85984118581', '85984118664', '85984118708', '85984118774', '85984119107', '85984119481', '85984119572', '85984119808', '85984120393', '85984120682', '85984121272', '85984122145', '85984122414', '85984123034', '85984123448', '85984124093', '85984124208', '85984125015', '85984125036', '85984126078', '85984126186', '85984126390', '85984126584', '85984126778', '85984126955', '85984127219', '85984127242', '85984127734', '85984128627', '85984128634', '85984128869', '85984128924', '85984129311', '85984129612', '85984130038', '85984130659', '85984130724', '85984130979', '85984131046', '85984131139', '85984131313', '85984131574', '85984131761', '85984131881', '85984132127', '85984132128', '85984132149', '85984132782', '85984132844', '85984133084', '85984133130', '85984133206', '85984133331', '85984133448', '85984133534', '85984134089', '85984134736', '85984135015', '85984135302', '85984135420', '85984135573', '85984</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['10', '27', '27', '27', '46', '30', '27', '1', '5', '29', '1', '35', '16', '43', '27', '27', '27', '11', '5', '28', '1', '49', '27', '27', '1', '27', '0', '27', '11', '1', '28', '10', '3', '27', '3', '28', '27', '31', '1', '25', '1', '27', '27', '40', '27', '27', '28', '27', '27', '12', '28', '5', '7', '6', '28', '40', '49', '1', '2', '8', '78', '1', '1', '27', '5', '27', '1', '27', '27', '11', '1', '28', '12', '27', '27', '1', '5', '27', '27', '2', '27', '27', '27', '25', '7', '27', '28', '1', '11', '27', '1', '1', '27', '21', '13', '6', '27', '5', '1', '0', '28', '27', '28', '27', '27', '27', '27', '27', '27', '7', '28', '5', '5', '27', '27', '47', '28', '27', '34', '1', '35', '5', '8', '12', '28', '27', '12', '49', '28', '27', '6', '27', '1', '1', '17', '5', '27', '1', '1', '28', '31', '1', '27', '12', '5', '27', '39', '49', '19', '16', '28', '27', '5', '27', '8', '27', '4', '35', '8', '30', '35', '1', '27', '27', '10', '40', '1', '27', '27', '49', '27', '29', '27', '27', '1', '28', '43', '32', '45', '30', '27', '27', '6', '27', '5', '2', '27', '7', '49', '13', '28', '6', '27', '27', '27', '27', '26', '27', '27', '27', '28', '49', '1', '27', '11', '28', '27', '27', '27', '27', '1', '18', '28', '27', '27', '27', '1', '27', '1', '49', '10', '27', '5', '49', '1', '11', '27', '49', '27', '27', '5', '49', '27', '7', '5', '28', '1', '29', '27', '11', '31', '38', '27', '15', '27', '27', '49', '17', '41', '8', '27', '1', '28', '30', '28', '3', '27', '30', '30', '5', '27', '10', '1', '49', '27', '28', '1', '27', '4', '1', '28', '5', '27', '27', '12', '28', '10', '27', '27', '48', '1', '1', '1', '27', '30', '1', '27', '27', '27', '29', '27', '5', '27', '27', '6', '1', '30', '27', '28', '1', '12', '5', '29', '25', '27', '49', '27', '27', '6', '11', '27', '27', '27', '27', '11', '27', '1', '27', '27', '27', '27', '27', '30', '27', '49', '28', '28', '23', '40', '27', '28', '27', '27', '27', '5', '11', '27', '27', '1', '5', '11', '28', '27', '27', '27', '28', '9', '5', '27', '11', '27', '1', '35', '1', '27', '1', '27', '27', '1', '30', '27', '27', '28', '17', '27', '27', '1', '27', '35', '49', '27', '49', '27', '27', '11', '27', '12', '27', '27', '8', '4', '49', '11', '27', '35', '4', '28', '27', '27', '27', '5', '18', '1', '5', '27', '27', '1', '28', '27', '1', '1', '11', '1', '1', '28', '114', '9', '27', '27', '5', '28', '27', '27', '1', '23', '27', '27', '5', '1', '27', '1', '5', '27', '27', '27', '27', '87', '27', '28', '31', '39', '34', '27', '27', '27', '9', '13', '9', '1', '17', '27', '35', '27', '30', '12', '27', '27', '49', '6', '27', '27', '27', '1', '28', '1', '30', '27', '27', '27', '12', '27', '27', '27', '1', '28', '0', '27', '49', '27', '27', '1', '28', '27', '27', '49', '27', '27', '27', '49', '27', '27', '6', '49', '1', '27', '9', '1', '28', '42', '13', '31', '27', '15', '8', '49', '27', '5', '27', '8', '27', '29', '27', '27', '49', '27', '14', '27', '28', '27', '27', '49', '29', '11', '27', '27', '12', '27', '27', '27', '27', '27', '1', '27', '5', '22', '1', '27', '27', '49', '17', '29', '11', '27', '27', '5', '13', '1', '10', '27', '28', '27', '27', '27', '27', '27', '5', '24', '27', '1', '1', '27', '1', '30', '27', '27', '27', '1', '14', '19', '25', '27', '27', '27', '27', '49', '27', '30', '11', '30', '5', '27', '27', '1', '27', '28', '27', '1', '29', '27', '27', '1', '5', '1', '37', '49', '1', '5', '2', '82', '5', '27', '27', '30', '8', '27', '5', '27', '27', '27', '28', '49', '27', '27', '27', '27', '28', '5', '27', '27', '1', '27', '14', '5', '49', '31', '1', '27', '1', '27', '5', '27', '27', '27', '28', '1', '12', '40', '27', '43', '27', '27', '1', '27', '49', '49', '21', '27', '27', '22', '27', '7', '12', '27', '27', '0', '1', '27', '27', '27', '28', '1', '7', '28', '49', '27', '27', '27', '7', '28', '16', '1', '1', '27', '12', '10', '12', '27', '27', '4', '27', '27', '30', '5', '12', '29', '27', '27', '17', '27', '27', '13', '5', '27', '12', '16', '49', '27', '1', '27', '6', '49', '29', '27', '28', '18', '28', '49', '27', '27', '27', '30', '27', '7', '23', '49', '12', '16', '27', '1', '5', '1', '27', '27', '27', '27', '27', '27', '27', '49', '27', '28', '27', '1', '27', '27', '27', '27', '27', '49', '21', '27', '28', '27', '27', '28', '35', '27', '49', '1', '27', '27', '26', '27', '38', '27', '1', '6', '27', '27', '28', '7', '28', '27', '27', '27', '27', '12', '5', '6', '27', '18', '28', '17', '27', '27', '28', '23', '14', '27', '12', '29', '28', '28', '27', '27', '27', '27', '28', '28', '49', '5', '27', '12', '27', '27', '27', '49', '27', '27', '12', '8', '27', '28', '28', '1', '9', '28', '27', '27', '27', '1', '1', '10', '1', '28', '27', '12', '1', '7', '27', '27', '27', '27', '28', '27', '27', '27', '5', '27', '12', '46', '27', '27', '31', '35', '17', '28', '27', '20', '24', '23', '1', '41', '36', '49', '49', '7', '28', '49', '27', '27', '5', '5', '27', '1', '5', '17', '27', '28', '13', '7', '49', '28', '27', '27', '27', '1', '34', '42', '35', '27', '28', '28', '28', '35', '11', '27', '5', '5', '28', '28', '27', '28', '1', '28', '13', '27', '28', '27', '28', '30', '28', '28', '18', '27', '5', '1', '76', '28', '28', '1', '5', '1', '28', '26', '2', '28', '1', '7', '12', '28', '37', '11', '28', '27', '27', '27', '27', '28', '28', '27', '20', '8', '30', '14', '27', '4', '10', '4', '49', '28', '28', '1', '1', '22', '27', '1', '10', '28', '11', '28', '77', '28', '2', '27', '30', '27', '27', '31', '1', '28', '28', '12', '27', '28', '10', '30', '27', '9', '27', '18', '28', '0', '12', '28', '49', '27', '27', '27', '27', '30', '1', '28', '27', '50', '31', '1', '27', '1', '27', '28', '28', '28', '27', '7', '1', '28', '27', '1', '27', '31', '28', '27', '1', '28', '1', '49', '49', '27', '28', '27', '27', '1', '27', '28', '27', '5', '26', '12', '1', '28', '2', '8', '13', '1', '12', '1', '28', '27', '1', '30', '7', '7', '37', '27', '28', '8', '5', '27', '28', '27', '27', '13', '13', '27', '30', '13', '13', '27', '1', '28', '27', '28', '27', '31', '27', '13', '28', '27', '27', '28', '12', '27', '27', '7', '1', '29', '27', '27', '1', '5', '27', '13', '27', '28', '49', '27', '6', '28', '27', '1', '27', '27', '21', '28', '31', '46', '27', '28', '5', '5', '27', '27', '30', '7', '27', '28', '28', '28', '30', '9', '17', '1', '3', '30', '7', '27', '28', '27', '7', '37', '27', '14', '13', '28', '27', '27', '27', '1', '27', '27', '27', '27', '28', '6', '28', '27', '12', '27', '47', '49', '28', '28', '27', '27', '13', '14', '28', '12', '28', '7', '27', '28', '27', '27', '1', '1', '27', '14', '0', '1', '27', '1', '1', '31', '1', '5', '39', '35', '27', '28', '11', '30', '27', '1', '27', '49', '27', '28', '28', '27', '47', '27', '28', '28', '5', '28', '30', '11', '49', '27', '28', '1', '28', '28', '28', '27', '49', '30', '27', '28', '30', '27', '15', '49', '8', '28', '12', '27', '17', '28', '27', '30', '49', '1', '28', '28', '27', '27', '27', '49', '1', '26', '1', '27', '49', '1', '6', '27', '5', '28', '1', '27', '11', '16', '28', '114', '27', '27', '27', '34', '1', '6', '28', '49', '21', '27', '27', '27', '28', '10', '1', '27', '27', '27', '49', '1', '28', '28', '27', '31', '28', '28', '28', '49', '49', '27', '27', '27', '8', '28', '1', '11', '5', '1', '1', '27', '32', '49', '27', '9', '33', '27', '5', '28', '27', '31', '28', '27', '27', '27', '27', '27', '39', '30', '12', '13', '28', '34', '1', '27', '27', '28', '28', '15', '11', '27', '28', '1', '27', '1', '35', '27', '7', '17', '1', '35', '23', '27', '28', '1', '5', '28', '2', '21', '27', '28', '28', '28', '11', '49', '32', '28', '14', '14', '30', '27', '1', '28', '28', '28', '23', '1', '27', '27', '27', '28', '47', '27', '28', '1', '27', '27', '28', '42', '49', '27', '27', '5', '28', '27', '1', '28', '27', '26', '27', '27', '28', '28', '8', '5', '0', '49', '28', '28', '5', '28', '27', '28', '28', '41', '8', '27', '27', '27', '6', '27', '27', '27', '6', '1', '28', '30', '5', '27', '12', '2', '5', '28', '15', '5', '27', '28', '27', '12', '28', '28', '5', '27', '12', '28', '27', '27', '6', '1', '30', '28', '27', '28', '12', '27', '13', '1', '49', '31', '27', '12', '28', '27', '28', '27', '33', '27', '40', '27', '28', '28', '27', '0', '20', '27', '1', '43', '28', '28', '1', '49', '33', '27', '10', '28', '27', '28', '27', '27', '2', '27', '27', '49', '1', '28', '28', '43', '27', '27', '28', '49', '5', '28', '146', '10', '18', '28', '27', '27', '27', '28', '27', '28', '28', '28', '11', '1', '5', '6', '27', '8', '5', '9', '28', '1', '27', '28', '18', '27', '6', '6', '26', '27', '7', '27', '49', '8', '27', '75', '21', '58', '27', '27', '21', '27', '21', '6', '27', '29', '27', '27', '62', '69', '65', '17', '27', '49', '8', '27', '8', '5', '27', '1', '30', '1', '27', '32', '32', '49', '5', '5', '4', '13', '32', '33', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '32', '5', '4', '5', '32', '4', '3', '4', '4', '4', '5', '35', '33', '4', '5', '5', '5', '4', '30', '32', '5', '4', '5', '19', '5', '5', '4', '5', '5', '5', '5', '5', '4', '4', '5', '5', '5', '32', '32', '39', '4', '4', '4', '34', '5', '33', '34', '49', '4', '5', '4', '5', '3', '77', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '5', '6', '5', '5', '4', '4', '5', '4', '5', '4', '4', '32', '5', '51', '4', '32', '4', '33', '4', '4', '5', '12', '32', '4', '4', '32', '5', '5', '4', '5', '4', '3', '4', '5', '4', '5', '6', '4', '5', '32', '4', '4', '4', '5', '4', '5', '5', '5', '2', '5', '6', '4', '49', '5', '4', '32', '5', '32', '5', '5', '5', '39', '49', '33', '33', '4', '4', '5', '5', '5', '4', '5', '5', '4', '33', '32', '32', '32', '32', '33', '5', '32', '32', '32', '33', '44', '20', '14', '33', '6', '32', '12', '49', '32', '32', '49', '33', '34', '5', '32', '32', '32', '32', '4', '32', '32', '5', '6', '42', '33', '35', '32', '31', '31', '5', '32', '49', '32', '4', '27', '11', '32', '4', '69', '32', '6', '32', '34', '5', '32', '49', '32', '21', '32', '32', '5', '30', '33', '32', '16', '32', '33', '34', '32', '48', '49', '31', '32', '6', '32', '34', '34', '5', '33', '49', '39', '32', '33', '33', '4', '32', '11', '32', '6', '6', '33', '32', '33', '33', '31', '32', '32', '5', '32', '4', '32', '4', '32', '32', '33', '32', '32', '5', '34', '32', '33', '32', '49', '32', '27', '31', '4', '12', '33', '34', '49', '5', '31', '32', '6', '30', '5', '32', '27', '34', '32', '22', '32', '4', '32', '33', '32', '32', '4', '6', '33', '33', '72', '32', '32', '5', '30', '32', '5', '32', '32', '60', '32', '33', '15', '34', '32', '33', '33', '32', '32', '12', '33', '33', '33', '32', '32', '5', '32', '33', '7', '32', '46', '5', '33', '32', '41', '34', '32', '32', '32', '5', '32', '32', '33', '33', '33', '32', '32', '7', '33', '32', '32', '32', '12', '32', '5', '32', '49', '9', '30', '32', '33', '33', '33', '27', '5', '5', '31', '32', '6', '30', '79', '35', '49', '34', '32', '33', '33', '32', '32', '32', '49', '32', '70', '26', '32', '32', '6', '32', '31', '5', '28', '32', '5', '5', '10', '4', '49', '33', '5', '32', '32', '6', '5', '4', '4', '4', '5', '5', '32', '5', '4', '5', '5', '75', '4', '4', '4', '4', '34', '4', '5', '5', '49', '42', '4', '5', '32', '2', '4', '5', '33', '4', '5', '5', '5', '5', '5', '4', '11', '32', '49', '4', '30', '5', '27', '4', '31', '29', '2', '4', '5', '33', '5', '4', '5', '32', '4', '4', '5', '32', '5', '4', '32', '14', '37', '5', '4', '33', '4', '5', '5', '31', '4', '4', '5', '32', '33', '33', '5', '5', '5', '5', '4', '4', '4', '4', '5', '5', '30', '4', '0', '4', '16', '4', '5', '4', '4', '5', '5', '5', '5', '4', '5', '4', '30', '5', '5', '5', '15', '5', '4', '5', '5', '5', '5', '7', '4', '4', '4', '32', '32', '5', '32', '4', '4', '5', '4', '4', '4', '4', '4', '4', '4', '4', '30', '4', '5', '4', '4', '5', '34', '4', '5', '64', '4', '4', '4', '4', '4', '4', '4', '5', '4', '4', '5', '5', '5', '4', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '31', '4', '4', '5', '4', '5', '35', '4', '4', '4', '5', '4', '4', '5', '4', '5', '4', '5', '4', '5', '4', '4', '4', '4', '32', '4', '4', '31', '13', '4', '11', '4', '32', '5', '4', '33', '5', '32', '4', '30', '4', '5', '32', '33', '5', '5', '5', '4', '5', '3', '4', '4', '5', '32', '4', '4', '5', '31', '32', '5', '49', '12', '5', '4', '5', '4', '33', '2', '5', '5', '30', '80', '4', '33', '33', '3', '5', '34', '31', '34', '7', '59', '32', '33', '5', '32', '95', '5', '32', '32', '5', '5', '32', '30', '5', '32', '5', '4', '4', '32', '5', '4', '4', '5', '5', '33', '11', '4', '32', '4', '4', '33', '4', '63', '4', '4', '4', '34', '4', '18', '33', '32', '33', '32', '4', '32', '47', '5', '4', '32', '5', '5', '49', '35', '32', '33', '32', '5', '7', '32', '4', '32', '21', '12', '5', '32', '32', '4', '4', '4', '5', '5', '4', '32', '5', '4', '5', '32', '5', '4', '34', '4', '5', '4', '5', '5', '4', '5', '4', '4', '30', '32', '5', '33', '33', '32', '31', '33', '32', '32', '4', '6', '34', '1', '15', '30', '32', '5', '4', '32', '4', '5', '32', '2', '49', '8', '32', '11', '6', '5', '31', '33', '12', '34', '33', '31', '4', '33', '34', '34', '32', '32', '32', '32', '8', '32', '33', '4', '74', '4', '33', '32', '28', '4', '5', '33', '14', '32', '33', '31', '5', '32', '5', '33', '33', '32', '33', '32', '5', '32', '33', '23', '27', '31', '31', '34', '31', '5', '41', '32', '32', '33', '32', '11', '32', '7', '11', '32', '33', '32', '33', '34', '32', '32', '4', '32', '31', '32', '32', '32', '32', '33', '46', '32', '66', '32', '33', '30', '5', '32', '32', '32', '4', '32', '32', '32', '32', '33', '32', '49', '32', '32', '32', '33', '33', '32', '5', '33', '32', '12', '32', '33', '16', '32', '33', '5', '32', '32', '9', '34', '64', '4', '32', '32', '33', '32', '31', '32', '32', '10', '32', '6', '33', '13', '32', '5', '5', '4', '31', '3', '32', '25', '40', '34', '32', '32', '34', '5', '32', '44', '33', '8', '32', '33', '32', '33', '5', '33', '32', '32', '32', '18', '30', '32', '33', '32', '49', '32', '32', '32', '6', '17', '33', '33', '5', '49', '32', '19', '4', '5', '5', '4', '5', '7', '4', '11', '33', '32', '32', '4', '3', '32', '27', '4', '4', '33', '5', '4', '34', '31', '5', '30', '1', '4', '5', '32', '5', '4', '5', '4', '61', '9', '4', '11', '5', '32', '33', '33', '34', '4', '33', '34', '4', '32', '32', '5', '32', '4', '31', '32', '33', '5', '4', '33', '5', '4', '27', '5', '5', '4', '35', '5', '5', '4', '5', '4', '4', '4', '33', '5', '32', '5', '5', '5', '27', '4', '4', '4', '4', '4', '5', '5', '5', '5', '6', '5', '5', '5', '5', '4', '5', '5', '5', '4', '5', '4', '66', '4', '4', '4', '4', '5', '4', '4', '4', '32', '7', '33', '5', '7', '4', '5', '55', '32', '43', '21', '5', '4', '5', '3', '4', '5', '4', '4', '32', '32', '33', '34', '5', '69', '4', '32', '4', '32', '25', '30', '32', '30', '32', '63', '35', '33', '5', '32', '5', '32', '4', '5', '4', '5', '4', '5', '4', '4', '33', '33', '33', '4', '30', '5', '33', '32', '4', '32', '33', '27', '5', '4', '32', '5', '4', '32', '5', '5', '5', '33', '4', '5', '4', '4', '4', '5', '5', '7', '33', '5', '32', '5', '5', '49', '5', '4', '4', '5', '4', '4', '5', '4', '4', '5', '32', '4', '4', '4', '4', '4', '5', '32', '4', '5', '4', '4', '4', '5', '4', '5', '4', '4', '61', '4', '5', '4', '38', '33', '4', '5', '34', '13', '4', '4', '32', '32', '32', '4', '5', '5', '32', '5', '32', '4', '33', '33', '33', '5', '5', '33', '5', '5', '4', '12', '4', '28', '5', '5', '5', '5', '5', '4', '5', '5', '4', '32', '6', '4', '4', '5', '9', '13', '32', '34', '4', '33', '15', '32', '32', '4', '32', '5', '5', '27', '4', '5', '4', '4', '5', '4', '4', '4', '5', '4', '21', '5', '5', '33', '5', '4', '34', '5', '4', '4', '4', '5', '4', '4', '5', '5', '4', '5', '5', '13', '4', '5', '4', '5', '4', '4', '31', '5', '4', '5', '4', '4', '5', '30', '4', '4', '5', '4', '5', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '5', '5', '5', '46', '4', '4', '4', '4', '5', '4', '5', '22', '5', '5', '4', '49', '5', '5', '32', '5', '4', '5', '5', '5', '4', '4', '32', '4', '30', '32', '4', '4', '4', '4', '5', '5', '12', '5', '4', '5', '4', '33', '4', '4', '4', '32', '4', '4', '4', '4', '5', '4', '4', '32', '4', '35', '5', '4', '4', '5', '4', '5', '32', '0', '67', '4', '31', '4', '5', '30', '4', '17', '3', '5', '4', '4', '4', '5', '22', '5', '4', '4', '4', '4', '5', '5', '5', '5', '4', '5', '5', '2', '4', '4', '5', '32', '5', '5', '5', '4', '4', '4', '50', '4', '5', '4', '4', '5', '5', '5', '32', '5', '30', '32', '4', '5', '32', '4', '4', '4', '4', '4', '5', '5', '4', '5', '68', '5', '29', '4', '5', '5', '4', '5', '5', '6', '6', '6', '6', '6', '6', '5', '6', '6', '32', '35', '6', '33', '6', '24', '5', '34', '33', '32', '30', '31', '32', '33', '13', '32', '32', '93', '8', '33', '32', '32', '5', '33', '31', '32', '32', '33', '13', '32', '9', '32', '30', '3', '4', '9', '33', '3', '32', '33', '19', '32', '32', '33', '32', '33', '30', '30', '32', '5', '33', '32', '81', '7', '7', '32', '79', '33', '15', '32', '32', '32', '32', '5', '30', '32', '7', '32', '33', '5', '32', '33', '33', '35', '33', '32', '33', '33', '33', '31', '33', '32', '34', '32', '32', '32', '34', '33', '7', '33', '13', '32', '32', '32', '49', '32', '33', '33', '32', '32', '4', '32', '32', '33', '33', '4', '32', '33', '33', '12', '49', '33', '32', '80', '32', '33', '32', '25', '32', '34', '33', '4', '32', '32', '33', '32', '33', '33', '32', '33', '32', '4', '21', '32', '5', '32', '49', '71', '33', '33', '16', '13', '4', '32', '32', '5', '27', '18', '34', '33', '32', '65', '32', '32', '22', '27', '49', '34', '33', '33', '5', '4', '5', '5', '44', '32', '30', '12', '32', '32', '11', '33', '33', '33', '33', '32', '4', '11', '32', '32', '11', '8', '32', '4', '5', '5', '5', '33', '4', '4', '4', '70', '12', '27', '32', '32', '5', '17', '33', '32', '32', '8', '34', '32', '59', '32', '32', '33', '31', '31', '32', '49', '5', '15', '13', '33', '34', '32', '4', '33', '32', '4', '8', '32', '33', '22', '34', '49', '11', '33', '32', '32', '5', '28', '32', '31', '32', '32', '12', '32', '32', '32', '28', '49', '30', '33', '33', '32', '3', '18', '30', '33', '4', '32', '4', '31', '1', '12', '28', '5', '49', '33', '23', '32', '32', '33', '33', '33', '8', '33', '4', '29', '4', '32', '13', '32', '33', '33', '34', '32', '31', '33', '32', '4', '5', '32', '32', '5', '33', '15', '11', '33', '9', '50', '59', '13', '32', '32', '34', '33', '34', '33', '33', '33', '32', '20', '20', '33', '33', '34', '33', '32', '31', '12', '32', '33', '33', '5', '32', '32', '31', '33', '5', '32', '33', '7', '33', '32', '26', '13', '34', '12', '4', '5', '12', '49', '32', '33', '33', '32', '32', '32', '33', '33', '32', '17', '13', '32', '33', '10', '32', '32', '30', '32', '32', '32', '8', '5', '32', '32', '32', '32', '32', '12', '30', '12', '34', '33', '32', '45', '32', '34', '28', '32', '4', '4', '17', '32', '33', '49', '33', '26', '33', '49', '33', '31', '32', '32', '14', '5', '32', '32', '32', '32', '27', '32', '5', '33', '32', '32', '32', '32', '32', '32', '13', '15', '32', '30', '32', '32', '32', '32', '26', '32', '18', '33', '32', '32', '32', '49', '32', '33', '31', '32', '4', '5', '34', '32', '33', '33', '34', '32', '32', '6', '33', '5', '31', '32', '33', '32', '31', '29', '12', '32', '32', '5', '33', '30', '33', '32', '32', '31', '32', '39', '7', '61', '25', '34', '33', '32', '32', '7', '32', '31', '31', '33', '10', '34', '32', '31', '22', '32', '20', '9', '32', '32', '33', '30', '12', '33', '33', '33', '27', '5', '32', '5', '27', '24', '12', '32', '32', '62', '32', '22', '32', '5', '32', '33', '24', '49', '32', '32', '32', '4', '6', '33', '4', '33', '32', '32', '32', '32', '1', '11', '32', '26', '24', '5', '5', '32', '7', '5', '31', '33', '5', '54', '32', '33', '32', '32', '32', '32', '30', '32', '32', '12', '31', '32', '33', '33', '32', '33', '49', '33', '22', '32', '12', '32', '27', '55', '32', '34', '60', '32', '4', '5', '4', '4', '4', '4', '4', '4', '4', '5', '6', '4', '4', '34', '33', '4', '4', '33', '5', '35', '33', '33', '4', '5', '5', '33', '32', '32', '32', '5', '4', '4', '5', '5', '5', '32', '32', '4', '49', '5', '15', '33', '32', '32', '32', '34', '32', '60', '32', '32', '32', '27', '33', '30', '15', '5', '5', '72', '4', '4', '33', '33', '11', '32', '32', '32', '44', '63', '6', '7', '32', '32', '32', '5', '4', '19', '32', '14', '1', '33', '32', '71', '4', '48', '4', '31', '34', '5', '35', '5', '32', '32', '33', '32', '32', '26', '13', '32', '28', '32', '6', '21', '31', '64', '11', '33', '32', '32', '34', '5', '32', '26', '32', '5', '14', '32', '5', '5', '32', '4', '39', '13', '4', '35', '0', '32', '33', '33', '32', '32', '32', '49', '15', '33', '32', '32', '27', '32', '32', '5', '46', '11', '24', '33', '11', '4', '32', '12', '5', '5', '5', '32', '33', '32', '1', '32', '7', '13', '32', '32', '32', '13', '5', '30', '5', '4', '32', '30', '33', '33', '4', '7', '5', '33', '33', '33', '32', '14', '29', '6', '13', '32', '10', '33', '33', '5', '30', '12', '21', '33', '32', '33', '31', '30', '32', '18', '34', '32', '32', '34', '30', '12', '32', '32', '30', '32', '33', '34', '30', '32', '5', '33', '32', '12', '33', '33', '32', '32', '32', '11', '32', '32', '33', '32', '33', '32', '30', '32', '5', '32', '32', '25', '32', '33', '31', '32', '14', '33', '57', '30', '32', '49', '27', '5', '32', '12', '33', '33', '32', '32', '33', '21', '33', '33', '32', '10', '33', '33', '33', '32', '4', '4', '32', '32', '31', '33', '33', '33', '32', '24', '5', '35', '32', '32', '5', '3', '34', '32', '32', '5', '32', '33', '57', '33', '4', '34', '52', '33', '32', '33', '32', '33', '33', '1', '33', '33', '33', '22', '27', '33', '32', '32', '34', '33', '7', '12', '1', '4', '33', '32', '33', '33', '32', '32', '31', '32', '32', '29', '33', '31', '49', '5', '11', '34', '32', '32', '25', '35', '32', '25', '32', '33', '33', '5', '32', '27', '32', '31', '30', '30', '34', '32', '31', '5', '13', '30', '32', '4', '33', '32', '32', '32', '34', '4', '33', '30', '31', '32', '32', '33', '34', '49', '32', '5', '31', '33', '32', '32', '49', '8', '33', '32', '5', '32', '32', '33', '5', '32', '4', '36', '5', '32', '4', '32', '32', '18', '33', '33', '34', '34', '32', '8', '41', '32', '33', '49', '32', '32', '32', '5', '30', '49', '27', '32', '55', '49', '49', '26', '5', '33', '33', '33', '32', '32', '34', '32', '32', '12', '32', '11', '31', '33', '34', '32', '21', '28', '57', '32', '30', '4', '32', '4', '32', '17', '31', '33', '32', '32', '32', '32', '5', '30', '32', '32', '32', '32', '34', '32', '32', '32', '32', '32', '32', '33', '33', '13', '32', '34', '32', '32', '32', '32', '32', '5', '33', '32', '32', '33', '32', '5', '12', '33', '32', '5', '32', '32', '32', '5', '32', '5', '16', '34', '33', '33', '4', '30', '11', '34', '32', '35', '94', '10', '4', '14', '32', '28', '4', '32', '32', '17', '15', '4', '27', '4', '32', '32', '5', '34', '32', '32', '7', '33', '18', '31', '58', '20', '32', '11', '67', '36', '4', '27', '12', '32', '33', '26', '33', '5', '32', '32', '32', '32', '33', '77', '4', '33', '35', '32', '31', '31', '24', '32', '32', '33', '32', '24', '29', '33', '32', '32', '32', '24', '32', '5', '32', '16', '33', '33', '32', '32', '32', '11', '32', '5', '32', '32', '32', '32', '45', '32', '32', '31', '32', '32', '15', '32', '30', '31', '32', '5', '33', '5', '32', '32', '32', '32', '52', '26', '32', '32', '5', '33', '2', '34', '36', '33', '49', '33', '32', '5', '32', '6', '14', '32', '33', '32', '31', '31', '32', '33', '32', '33', '32', '32', '5', '32', '28', '32', '33', '32', '33', '8', '32', '5', '33', '12', '48', '32', '32', '32', '32', '32', '33', '4', '32', '13', '8', '32', '32', '33', '38', '33', '34', '33', '6', '33', '32', '32', '32', '13', '5', '4', '32', '16', '34', '7', '11', '12', '5', '11', '9', '33', '11', '33', '4', '34', '32', '32', '6', '49', '31', '32', '32', '5', '32', '4', '32', '32', '15', '6', '49', '32', '5', '32', '32', '32', '32', '6', '32', '32', '33', '32', '5', '11', '7', '5', '32', '31', '45', '33', '31', '32', '30', '6', '33', '33', '31', '34', '70', '1', '32', '31', '5', '32', '19', '5', '32', '32', '32', '32', '32', '31', '4', '32', '4', '32', '32', '11', '33', '32', '49', '33', '32', '33', '5', '32', '32', '33', '12', '49', '33', '32', '32', '11', '32', '32', '32', '33', '26', '33', '32', '32', '26', '0', '32', '31', '10', '32', '4', '31', '27', '5', '32', '33', '51', '12', '49', '6', '33', '33', '34', '32', '32', '32', '33', '32', '33', '5', '33', '32', '4', '49', '34', '32', '32', '5', '25', '31', '32', '33', '2', '5', '32', '14', '32', '32', '78', '32', '32', '32', '9', '20', '33', '33', '34', '32', '15', '33', '31', '32', '31', '32', '7', '11', '33', '32', '22', '49', '32', '32', '31', '33', '33', '32', '24', '32', '34', '33', '32', '34', '33', '14', '32', '33', '33', '19', '32', '32', '32', '14', '32', '8', '33', '33', '33', '32', '1', '33', '32', '32', '33', '27', '33', '11', '32', '33', '5', '32', '32', '12', '5', '11', '32', '33', '32', '32', '33', '32', '32', '45', '9', '32', '33', '32', '32', '32', '32', '32', '13', '32', '32', '5', '32', '32', '8', '7', '32', '33', '13', '49', '38', '6', '32', '33', '33', '19', '32', '32', '4', '4', '32', '32', '32', '33', '5', '33', '32', '12', '31', '32', '32', '33', '32', '38', '49', '33', '11', '32', '14', '6', '32', '33', '5', '5', '31', '32', '32', '32', '49', '32', '30', '70', '5', '33', '4', '16', '32', '32', '4', '32', '63', '6', '33', '49', '49', '5', '33', '32', '33', '33', '32', '5', '22', '5', '32', '11', '33', '32', '32', '11', '30', '33', '30', '34', '24', '21', '5', '32', '32', '32', '9', '13', '32', '48', '18', '5', '8', '7', '33', '32', '32', '32', '32', '19', '8', '32', '30', '33', '5', '32', '33', '32', '32', '32', '35', '11', '4', '32', '31', '32', '32', '32', '33', '33', '32', '10', '32', '32', '32', '1', '30', '7', '24', '33', '33', '32', '4', '33', '32', '5', '10', '27', '32', '33', '34', '32', '33', '33', '32', '32', '32', '32', '32', '32', '5', '33', '4', '32', '5', '32', '32', '7', '32', '33', '33', '32', '30', '16', '32', '5', '5', '5', '5', '5', '31', '33', '33', '4', '33', '32', '32', '5', '32', '33', '24', '31', '33', '8', '33', '32', '32', '32', '5', '32', '32', '5', '12', '41', '8', '33', '32', '32', '17', '5', '32', '32', '49', '32', '32', '4', '32', '9', '32', '33', '31', '33', '33', '31', '5', '32', '32', '4', '32', '32', '27', '32', '32', '32', '33', '32', '12', '49', '13', '32', '32', '30', '32', '5', '11', '32', '32', '3', '4', '33', '32', '58', '33', '30', '33', '49', '32', '33', '32', '16', '4', '33', '16', '33', '32', '5', '15', '33', '33', '32', '32', '35', '32', '33', '32', '34', '32', '32', '33', '10', '32', '31', '34', '33', '12', '32', '33', '27', '5', '4', '32', '32', '32', '31', '32', '33', '33', '31', '32', '33', '33', '32', '32', '6', '32', '49', '32', '6', '5', '4', '33', '15', '32', '32', '32', '5', '32', '33', '49', '32', '32', '32', '32', '33', '17', '32', '32', '4', '32', '31', '32', '37', '35', '1', '32', '12', '30', '33', '5', '32', '20', '5', '5', '32', '32', '49', '31', '32', '32', '6', '4', '32', '26', '31', '5', '5', '32', '32', '32', '33', '32', '32', '33', '30', '33', '32', '31', '32', '5', '32', '32', '32', '4', '49', '31', '32', '32', '33', '31', '32', '32', '11', '32', '49', '31', '4', '36', '5', '3', '9', '31', '12', '32', '32', '30', '4', '4', '4', '33', '49', '32', '32', '30', '4', '49', '31', '31', '33', '33', '32', '34', '32', '49', '32', '32', '5', '4', '8', '32', '32', '33', '12', '5', '32', '32', '32', '32', '32', '32', '8', '32', '32', '32', '32', '33', '2', '33', '32', '30', '33', '31', '32', '23', '30', '25', '5', '66', '36', '5', '32', '33', '31', '32', '32', '10', '33', '33', '14', '33', '33', '32', '13', '9', '18', '32', '34', '2', '32', '32', '4', '49', '5', '19', '4', '32', '33', '33', '35', '31', '22', '32', '32', '5', '30', '28', '32', '32', '32', '34', '32', '4', '6', '31', '32', '4', '32', '4', '33', '32', '33', '31', '6', '4', '32', '29', '13', '34', '32', '11', '34', '32', '8', '32', '33', '32', '49', '4', '32', '36', '33', '33', '7', '32', '32', '85', '32', '32', '33', '32', '9', '5', '4', '32', '12', '32', '32', '4', '30', '16', '32', '32', '1', '32', '33', '5', '32', '49', '33', '72', '31', '11', '5', '33', '49', '4', '31', '6', '33', '17', '33', '32', '5', '32', '32', '32', '14', '5', '26', '5', '17', '31', '4', '33', '30', '4', '32', '27', '23', '12', '32', '32', '32', '32', '32', '25', '32', '30', '32', '31', '33', '32', '32', '4', '5', '4', '33', '32', '33', '32', '32', '32', '32', '49', '31', '25', '32', '6', '33', '32', '5', '65', '8', '7', '32', '32', '32', '49', '32', '32', '6', '32', '15', '32', '11', '32', '32', '31', '32', '34', '6', '33', '32', '33', '32', '31', '15', '33', '32', '33', '32', '34', '25', '32', '32', '32', '33', '32', '50', '33', '32', '32', '49', '32', '6', '32', '5', '32', '32', '49', '32', '32', '5', '32', '4', '49', '32', '32', '33', '9', '32', '16', '33', '32', '33', '31', '4', '8', '5', '35', '5', '49', '6', '49', '32', '32', '32', '34', '32', '1', '9', '49', '32', '33', '4', '30', '49', '30', '4', '33', '32', '5', '30', '33', '11', '32', '32', '49', '4', '5', '33', '31', '5', '5', '25', '58', '32', '32', '13', '5', '31', '30', '32', '40', '12', '32', '12', '34', '33', '5', '35', '22', '25', '33', '28', '30', '5', '32', '27', '33', '33', '32', '5', '33', '5', '33', '30', '32', '9', '5', '30', '33', '48', '32', '12', '32', '32', '25', '32', '4', '32', '32', '16', '4', '5', '32', '45', '32', '5', '33', '32', '54', '14', '7', '5', '32', '4', '47', '33', '49', '5', '30', '7', '30', '5', '6', '30', '32', '5', '7', '5', '33', '32', '33', '5', '49', '30', '30', '35', '4', '8', '33', '32', '30', '8', '32', '5', '5', '32', '15', '30', '5', '32', '5', '72', '13', '10', '31', '4', '28', '20', '71', '32', '5', '19', '33', '32', '32', '7', '10', '94', '32', '32', '33', '28', '8', '34', '15', '4', '32', '1', '32', '15', '8', '32', '8', '5', '33', '34', '6', '32', '32', '12', '11', '79', '32', '32', '32', '33', '33', '18', '5', '49', '5', '33', '32', '6', '32', '13', '4', '33', '32', '4', '33', '4', '5', '73', '33', '31', '12', '13', '33', '32', '32', '33', '23', '33', '33', '33', '32', '32', '32', '33', '57', '4', '35', '6', '31', '33', '5', '30', '30', '32', '33', '6', '32', '32', '5', '8', '82', '33', '32', '34', '11', '5', '15', '33', '32', '6', '32', '5', '33', '32', '32', '32', '33', '33', '11', '28', '28', '32', '5', '35', '33', '32', '33', '32', '33', '32', '5', '32', '32', '33', '19', '32', '49', '33', '33', '32', '3', '32', '32', '34', '32', '5', '32', '32', '33', '13', '29', '35', '32', '32', '5', '29', '33', '5', '33', '32', '33', '33', '7', '32', '33', '32', '7', '32', '14', '5', '32', '32', '32', '5', '5', '5', '4', '5', '5', '5', '14', '8', '32', '33', '32', '30', '32', '33', '24', '11', '32', '4', '32', '32', '27', '32', '32', '51', '31', '33', '49', '6', '33', '12', '33', '5', '33', '8', '5', '33', '32', '30', '9', '31', '33', '32', '14', '5', '32', '32', '32', '32', '32', '49', '32', '32', '32', '21', '33', '33', '32', '32', '32', '33', '32', '33', '32', '19', '23', '33', '33', '32', '32', '32', '33', '33', '30', '32', '33', '5', '32', '4', '32', '32', '7', '33', '5', '5', '5', '30', '5', '32', '30', '12', '7', '53', '6', '32', '6', '5', '5', '48', '33', '34', '4', '33', '32', '32', '33', '8', '32', '32', '33', '32', '32', '32', '12', '32', '5', '33', '32', '33', '15', '32', '16', '32', '33', '32', '32', '32', '32', '27', '33', '32', '32', '34', '33', '32', '34', '7', '32', '33', '32', '32', '33', '48', '12', '33', '32', '33', '33', '32', '33', '4', '5', '32', '33', '32', '32', '61', '13', '32', '32', '35', '32', '35', '32', '32', '33', '85', '32', '5', '30', '32', '33', '32', '5', '33', '4', '4', '32', '5', '4', '32', '25', '34', '32', '11', '32', '33', '32', '5', '4', '32', '32', '33', '47', '33', '12', '12', '32', '32', '33', '7', '32', '32', '32', '30', '32', '32', '32', '32', '4', '32', '33', '5', '31', '8', '11', '76', '32', '6', '32', '11', '49', '5', '25', '49', '32', '11', '4', '32', '32', '32', '33', '32', '32', '71', '32', '4', '32', '32', '33', '32', '12', '32', '29', '13', '12', '5', '31', '32', '32', '34', '33', '31', '8', '33', '32', '32', '33', '33', '32', '32', '9', '12', '32', '33', '32', '46', '32', '32', '34', '32', '33', '11', '5', '32', '32', '33', '30', '32', '21', '32', '33', '33', '33', '32', '33', '14', '33', '32', '32', '33', '33', '7', '33', '32', '45', '42', '32', '51', '1', '33', '8', '32', '33', '33', '5', '33', '32', '32', '10', '33', '32', '32', '32', '32', '32', '33', '31', '5', '6', '5', '10', '32', '30', '33', '5', '32', '27', '38', '12', '5', '32', '33', '32', '32', '12', '32', '67', '34', '33', '32', '32', '32', '33', '8', '33', '33', '60', '7', '33', '32', '8', '5', '61', '32', '32', '5', '7', '32', '19', '32', '6', '32', '33', '4', '49', '34', '33', '32', '32', '31', '49', '30', '10', '11', '33', '33', '33', '32', '30', '32', '32', '11', '33', '33', '32', '49', '15', '32', '64', '12', '33', '5', '6', '5', '30', '33', '32', '33', '11', '32', '26', '34', '31', '33', '33', '49', '13', '</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atend</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>['85974001107', '85981010387', '85981010504', '85981010801', '85981011300', '85981011982', '85981012709', '85981012859', '85981012916', '85981013105', '85981013139', '85981013252', '85981014486', '85981015083', '85981015199', '85981015345', '85981015408', '85981015858', '85981018191', '85981019737', '85981019859', '85981020615', '85981021220', '85981021847', '85981021858', '85981023473', '85981024243', '85981024932', '85981025159', '85981026077', '85981026188', '85981026342', '85981029941', '85981034608', '85981035347', '85981037998', '85981038369', '85981040609', '85981041303', '85981042289', '85981046232', '85981047325', '85981047447', '85981050094', '85981050305', '85981050670', '85981050778', '85981050921', '85981051007', '85981051157', '85981051236', '85981051357', '85981051407', '85981051960', '85981052023', '85981052147', '85981052388', '85981053361', '85981053645', '85981053870', '85981054245', '85981054310', '85981054721', '85981054784', '85981055402', '85981055606', '85981055887', '85981056204', '85981056432', '85981057133', '85981057473', '85981057594', '85981057657', '85981058510', '85981058575', '85981059167', '85981060358', '85981060840', '85981060881', '85981060903', '85981060912', '85981061514', '85981062036', '85981062783', '85981062811', '85981063144', '85981063180', '85981063445', '85981063577', '85981063706', '85981063708', '85981063769', '85981064311', '85981064501', '85981064633', '85981066228', '85981066596', '85981066800', '85981067063', '85981067120', '85981067303', '85981067738', '85981068259', '85981068383', '85981068838', '85981069073', '85981069268', '85981069285', '85981069288', '85981069331', '85981069531', '85981069805', '85981070139', '85981070716', '85981070933', '85981072516', '85981074292', '85981074824', '85981077799', '85981079793', '85981080110', '85981081102', '85981081645', '85981081717', '85981081963', '85981082567', '85981082798', '85981083944', '85981083955', '85981084430', '85981085176', '85981085425', '85981086055', '85981087566', '85981090951', '85981092003', '85981094270', '85981095658', '85981096027', '85981097092', '85981097525', '85981099771', '85981099834', '85981104139', '85981105541', '85981111379', '85981111687', '85981112198', '85981112368', '85981113354', '85981116111', '85981116475', '85981117229', '85981117240', '85981117970', '85981118916', '85981119356', '85981121743', '85981121756', '85981121918', '85981122659', '85981122830', '85981124417', '85981125198', '85981125364', '85981127000', '85981127863', '85981128332', '85981128640', '85981129033', '85981130954', '85981131390', '85981132338', '85981132657', '85981132861', '85981133001', '85981136515', '85981137269', '85981137935', '85981138484', '85981139818', '85981141110', '85981141235', '85981142047', '85981142397', '85981144074', '85981144194', '85981144290', '85981144476', '85981145210', '85981145431', '85981146150', '85981147761', '85981148652', '85981149605', '85981149798', '85981149833', '85981150270', '85981152513', '85981152668', '85981152923', '85981153276', '85981154070', '85981154704', '85981154767', '85981155516', '85981155609', '85981155832', '85981157497', '85981159783', '85981160701', '85981162279', '85981163532', '85981168773', '85981169336', '85981170375', '85981170419', '85981172174', '85981172237', '85981173080', '85981173491', '85981173596', '85981174595', '85981175102', '85981175961', '85981176245', '85981176511', '85981176843', '85981176855', '85981177377', '85981177436', '85981178111', '85981180220', '85981180748', '85981181223', '85981181460', '85981184568', '85981185113', '85981185397', '85981185432', '85981186162', '85981187777', '85981187790', '85981188522', '85981190449', '85981190603', '85981190941', '85981191324', '85981191501', '85981192668', '85981193462', '85981194504', '85981195274', '85981195777', '85981196765', '85981199009', '85981200624', '85981204580', '85981205000', '85981207224', '85981210397', '85981211722', '85981211785', '85981212297', '85981212335', '85981215121', '85981215323', '85981217007', '85981217070', '85981217271', '85981217334', '85981217865', '85981217880', '85981217928', '85981219726', '85981220015', '85981220097', '85981220132', '85981221107', '85981221148', '85981222412', '85981224119', '85981224486', '85981224995', '85981225097', '85981225167', '85981226403', '85981227172', '85981227283', '85981227812', '85981228111', '85981228405', '85981228468', '85981229862', '85981229918', '85981229981', '85981230013', '85981230104', '85981233010', '85981233031', '85981233110', '85981234275', '85981235443', '85981237281', '85981238571', '85981240151', '85981240906', '85981241794', '85981243937', '85981245200', '85981245595', '85981245660', '85981246453', '85981246810', '85981247191', '85981247682', '85981247801', '85981248056', '85981248614', '85981248938', '85981249006', '85981249077', '85981249520', '85981249804', '85981250065', '85981251340', '85981252190', '85981252202', '85981252814', '85981253454', '85981256347', '85981256415', '85981256918', '85981257594', '85981257644', '85981258954', '85981259116', '85981259996', '85981260093', '85981260293', '85981261976', '85981264023', '85981265628', '85981266155', '85981266554', '85981267575', '85981268163', '85981269254', '85981270887', '85981273817', '85981276088', '85981277050', '85981277171', '85981277778', '85981277862', '85981278172', '85981278481', '85981281110', '85981281122', '85981283976', '85981284254', '85981284771', '85981284904', '85981285694', '85981285757', '85981286755', '85981287954', '85981288208', '85981288338', '85981289201', '85981290315', '85981291170', '85981291852', '85981292335', '85981292898', '85981293237', '85981296943', '85981297006', '85981297774', '85981298411', '85981298474', '85981299369', '85981300207', '85981300265', '85981301018', '85981301029', '85981301090', '85981301430', '85981302820', '85981303653', '85981304383', '85981304684', '85981304736', '85981304842', '85981305581', '85981306366', '85981307620', '85981307802', '85981308045', '85981308259', '85981308292', '85981308328', '85981308337', '85981308391', '85981310114', '85981310742', '85981311091', '85981311398', '85981312075', '85981313089', '85981313134', '85981313616', '85981313627', '85981314051', '85981314422', '85981315654', '85981316754', '85981318080', '85981323921', '85981325550', '85981327070', '85981327436', '85981327760', '85981328852', '85981330136', '85981330758', '85981331850', '85981331913', '85981332190', '85981333065', '85981333339', '85981334650', '85981334713', '85981334761', '85981335534', '85981337373', '85981338263', '85981338307', '85981342092', '85981342565', '85981343138', '85981343533', '85981344833', '85981345060', '85981347012', '85981347371', '85981348351', '85981348558', '85981349404', '85981351875', '85981352588', '85981352826', '85981353374', '85981353997', '85981354648', '85981355846', '85981357814', '85981359310', '85981360852', '85981361507', '85981361779', '85981362003', '85981362066', '85981363777', '85981365886', '85981366880', '85981367170', '85981368633', '85981370043', '85981370894', '85981371153', '85981371868', '85981372645', '85981374219', '85981375527', '85981375801', '85981375825', '85981376079', '85981377391', '85981378159', '85981378792', '85981378905', '85981379505', '85981379662', '85981380597', '85981380924', '85981381707', '85981381999', '85981383237', '85981383353', '85981384426', '85981385151', '85981385624', '85981385673', '85981385841', '85981386704', '85981386821', '85981387227', '85981387362', '85981388619', '85981391330', '85981391423', '85981391880', '85981392100', '85981392565', '85981395635', '85981395687', '85981395818', '85981397246', '85981397372', '85981397409', '85981397411', '85981398764', '85981400369', '85981401399', '85981401626', '85981401752', '85981402041', '85981402081', '85981402748', '85981402997', '85981403093', '85981403964', '85981404116', '85981404174', '85981404374', '85981404793', '85981405917', '85981408267', '85981409242', '85981409843', '85981411024', '85981411624', '85981411687', '85981413039', '85981413532', '85981413653', '85981413838', '85981413892', '85981414546', '85981415469', '85981416386', '85981416409', '85981418850', '85981419344', '85981420019', '85981421525', '85981421738', '85981422245', '85981422308', '85981422576', '85981422856', '85981423490', '85981423505', '85981423933', '85981424271', '85981424607', '85981425703', '85981426537', '85981426942', '85981427253', '85981428860', '85981428912', '85981432332', '85981433880', '85981436330', '85981437233', '85981437797', '85981440921', '85981442203', '85981443375', '85981444452', '85981444515', '85981445843', '85981447674', '85981448037', '85981452309', '85981453385', '85981460147', '85981460175', '85981460392', '85981460457', '85981460646', '85981460699', '85981460861', '85981460924', '85981460996', '85981461065', '85981461106', '85981461610', '85981462406', '85981463746', '85981463860', '85981464262', '85981464411', '85981464530', '85981464545', '85981465735', '85981465772', '85981465798', '85981466545', '85981467570', '85981468790', '85981470659', '85981470831', '85981471492', '85981471759', '85981472233', '85981473750', '85981474263', '85981474389', '85981474696', '85981474697', '85981474756', '85981474760', '85981474778', '85981474912', '85981474923', '85981475220', '85981475230', '85981475761', '85981475972', '85981475980', '85981476043', '85981476212', '85981476638', '85981477326', '85981477413', '85981477799', '85981477812', '85981477813', '85981477916', '85981478494', '85981478784', '85981479493', '85981479515', '85981479752', '85981479774', '85981481053', '85981481331', '85981481726', '85981482109', '85981482140', '85981482476', '85981482990', '85981483810', '85981484967', '85981485284', '85981485480', '85981486380', '85981486397', '85981487878', '85981488161', '85981488741', '85981489506', '85981489546', '85981489609', '85981489986', '85981491380', '85981491428', '85981491439', '85981492666', '85981492729', '85981495205', '85981495268', '85981495465', '85981495615', '85981495911', '85981495935', '85981496025', '85981496943', '85981497099', '85981497122', '85981497496', '85981497614', '85981499186', '85981500414', '85981500847', '85981500940', '85981501090', '85981501968', '85981502098', '85981502241', '85981505500', '85981505522', '85981505531', '85981505586', '85981505887', '85981506224', '85981506332', '85981506467', '85981506955', '85981507053', '85981507770', '85981507930', '85981509140', '85981509349', '85981509981', '85981510677', '85981511295', '85981512929', '85981514081', '85981514747', '85981518467', '85981518484', '85981520304', '85981521334', '85981521816', '85981521879', '85981521962', '85981522121', '85981522321', '85981522480', '85981522523', '85981522914', '85981522917', '85981522933', '85981522980', '85981523042', '85981523247', '85981523548', '85981523703', '85981523830', '85981523864', '85981524209', '85981524336', '85981524345', '85981524388', '85981524433', '85981524474', '85981525329', '85981525392', '85981525946', '85981525956', '85981525970', '85981526066', '85981526142', '85981526377', '85981526414', '85981526660', '85981526890', '85981526953', '85981527026', '85981527241', '85981527738', '85981527876', '85981527926', '85981528100', '85981528344', '85981528523', '85981529250', '85981530016', '85981530202', '85981530228', '85981530264', '85981530358', '85981530695', '85981531466', '85981532323', '85981532367', '85981532706', '85981533140', '85981533536', '85981533817', '85981533861', '85981533924', '85981534836', '85981535019', '85981535381', '85981535444', '85981535702', '85981536001', '85981536037', '85981536784', '85981537054', '85981537071', '85981537451', '85981537531', '85981537646', '85981538008', '85981538403', '85981538473', '85981539100', '85981539364', '85981539374', '85981539613', '85981539674', '85981539710', '85981539904', '85981542565', '85981544220', '85981544377', '85981544415', '85981544420', '85981544535', '85981544744', '85981545730', '85981545967', '85981546135', '85981546201', '85981546486', '85981546524', '85981547100', '85981547151', '85981547181', '85981548573', '85981548663', '85981549807', '85981550607', '85981551701', '85981552786', '85981552815', '85981553207', '85981553257', '85981553774', '85981554041', '85981554682', '85981555448', '85981556360', '85981556386', '85981556391', '85981556708', '85981557599', '85981557763', '85981557766', '85981557996', '85981558443', '85981558444', '85981558593', '85981558734', '85981558921', '85981559352', '85981559880', '85981559990', '85981561122', '85981561397', '85981563114', '85981563918', '85981565385', '85981566296', '85981569388', '85981570332', '85981570553', '85981571936', '85981571948', '85981573149', '85981574029', '85981574749', '85981574828', '85981575288', '85981576121', '85981577685', '85981579715', '85981580747', '85981582223', '85981587265', '85981588881', '85981589028', '85981590283', '85981590581', '85981591212', '85981591394', '85981592814', '85981594445', '85981594455', '85981598314', '85981599091', '85981599720', '85981600032', '85981600288', '85981600746', '85981601467', '85981601515', '85981601621', '85981603545', '85981603701', '85981603764', '85981603922', '85981604044', '85981604097', '85981604901', '85981605888', '85981606241', '85981606453', '85981606516', '85981606875', '85981607061', '85981607171', '85981607847', '85981608039', '85981608131', '85981608656', '85981608885', '85981609224', '85981609765', '85981611504', '85981611687', '85981612354', '85981612497', '85981613707', '85981614805', '85981615721', '85981615726', '85981616672', '85981617048', '85981617443', '85981617809', '85981618157', '85981618463', '85981618696', '85981619089', '85981621012', '85981625207', '85981625719', '85981625789', '85981625797', '85981626292', '85981626455', '85981627178', '85981627515', '85981627750', '85981628353', '85981628962', '85981629450', '85981630101', '85981630164', '85981631945', '85981632116', '85981635515', '85981635650', '85981636098', '85981636649', '85981638200', '85981638739', '85981639201', '85981642110', '85981642480', '85981645543', '85981646909', '85981647853', '85981649485', '85981651235', '85981651813', '85981651856', '85981653359', '85981654096', '85981655420', '85981655504', '85981656015', '85981656761', '85981663973', '85981664051', '85981665088', '85981665658', '85981665867', '85981666220', '85981666585', '85981666685', '85981668986', '85981669316', '85981669696', '85981669892', '85981670050', '85981670209', '85981670557', '85981671233', '85981672007', '85981672198', '85981672687', '85981676600', '85981677013', '85981677923', '85981677986', '85981679022', '85981679393', '85981684827', '85981685253', '85981687262', '85981688088', '85981688530', '85981689614', '85981690885', '85981692225', '85981693076', '85981694698', '85981696440', '85981700371', '85981701616', '85981701789', '85981702211', '85981704587', '85981705823', '85981706117', '85981706812', '85981707565', '85981709424', '85981709639', '85981709959', '85981709997', '85981711415', '85981712700', '85981715589', '85981717124', '85981721330', '85981721470', '85981723162', '85981723682', '85981727178', '85981727333', '85981730276', '85981731368', '85981733009', '85981733173', '85981734225', '85981735351', '85981735457', '85981738337', '85981742689', '85981745007', '85981746191', '85981746231', '85981747230', '85981747684', '85981747880', '85981748018', '85981749098', '85981749311', '85981780097', '85981780698', '85981781860', '85981781956', '85981782615', '85981783993', '85981787014', '85981787375', '85981787694', '85981787878', '85981795562', '85981797415', '85981799011', '85981799243', '85981799393', '85981799969', '85981800644', '85981801187', '85981801628', '85981801718', '85981801761', '85981802537', '85981802631', '85981803848', '85981804731', '85981805074', '85981805578', '85981805682', '85981805712', '85981805995', '85981806062', '85981806192', '85981806838', '85981807096', '85981807746', '85981808109', '85981808226', '85981808940', '85981809310', '85981809579', '85981810401', '85981811681', '85981812231', '85981812420', '85981813215', '85981813326', '85981813696', '85981813745', '85981814222', '85981815518', '85981815719', '85981815951', '85981815995', '85981816185', '85981816597', '85981816953', '85981817644', '85981819191', '85981819878', '85981819898', '85981819971', '85981820302', '85981820909', '85981822288', '85981822627', '85981823737', '85981824050', '85981825667', '85981827171', '85981827298', '85981828133', '85981829674', '85981829888', '85981830615', '85981831333', '85981831807', '85981832616', '85981833911', '85981836027', '85981836192', '85981838197', '85981839905', '85981840699', '85981840997', '85981841498', '85981842018', '85981842026', '85981847568', '85981849140', '85981849448', '85981850329', '85981851336', '85981851657', '85981851806', '85981852483', '85981852871', '85981853361', '85981853473', '85981853498', '85981854188', '85981854400', '85981854701', '85981854966', '85981855387', '85981855943', '85981857602', '85981858378', '85981858585', '85981859714', '85981859843', '85981860190', '85981860939', '85981861386', '85981861390', '85981862200', '85981862732', '85981862812', '85981863520', '85981863917', '85981864665', '85981866872', '85981867198', '85981867874', '85981868706', '85981869078', '85981869877', '85981870279', '85981870625', '85981870769', '85981871433', '85981871482', '85981871725', '85981872527', '85981873853', '85981874873', '85981875089', '85981875839', '85981876038', '85981876387', '85981877277', '85981877340', '85981877666', '85981878608', '85981879558', '85981879727', '85981881447', '85981881564', '85981881903', '85981882019', '85981882233', '85981883888', '85981885848', '85981886408', '85981888076', '85981890073', '85981890692', '85981890804', '85981890897', '85981891321', '85981891476', '85981892737', '85981892922', '85981893512', '85981894559', '85981895421', '85981895778', '85981895877', '85981899243', '85981900080', '85981900730', '85981901391', '85981904698', '85981905011', '85981905074', '85981905075', '85981906452', '85981910262', '85981910771', '85981911604', '85981911984', '85981914747', '85981917082', '85981917653', '85981917936', '85981918090', '85981918203', '85981921936', '85981921999', '85981922555', '85981924869', '85981926087', '85981926161', '85981927362', '85981928269', '85981930502', '85981933090', '85981933446', '85981934488', '85981937771', '85981942675', '85981944086', '85981946447', '85981947455', '85981948504', '85981948560', '85981948709', '85981949370', '85981949405', '85981950680', '85981951197', '85981951207', '85981951277', '85981951294', '85981951433', '85981952223', '85981952606', '85981953266', '85981955156', '85981955666', '85981956683', '85981956798', '85981956914', '85981956977', '85981958219', '85981958833', '85981959454', '85981962203', '85981963748', '85981964770', '85981966391', '85981966744', '85981967093', '85981967347', '85981967672', '85981972215', '85981973787', '85981973850', '85981974619', '85981975003', '85981975335', '85981975643', '85981978964', '85981982384', '85981982415', '85981983536', '85981984160', '85981984196', '85981984205', '85981985320', '85981987749', '85981990206', '85981991814', '85981992200', '85981992221', '85981993841', '85981994171', '85981994544', '85981996677', '85981996968', '85981997233', '85981998183', '85981998880', '85981999101', '85981999393', '85982000080', '85982000103', '85982000124', '85982000407', '85982000597', '85982001158', '85982001480', '85982001603', '85982002244', '85982003360', '85982009691', '85982012352', '85982013350', '85982013725', '85982014410', '85982014728', '85982014859', '85982015963', '85982016650', '85982018181', '85982019178', '85982020684', '85982020732', '85982021675', '85982021901', '85982021970', '85982022116', '85982022707', '85982023008', '85982023198', '85982023449', '85982024092', '85982024412', '85982024556', '85982025193', '85982025465', '85982025505', '85982026115', '85982026559', '85982026582', '85982026618', '85982026681', '85982026958', '85982027257', '85982027456', '85982028016', '85982028614', '85982028717', '85982029544', '85982029630', '85982029656', '85982031994', '85982033246', '85982036215', '85982038136', '85982038199', '85982038964', '85982041982', '85982048028', '85982048400', '85982048768', '85982049005', '85982050430', '85982051850', '85982052170', '85982052833', '85982053074', '85982058486', '85982059867', '85982060243', '85982061188', '85982061715', '85982065404', '85982066323', '85982066720', '85982067095', '85982067924', '85982069921', '85982070325', '85982070442', '85982070505', '85982070537', '85982075392', '85982076079', '85982077220', '85982080055', '85982080963', '85982081863', '85982082408', '85982082685', '85982086204', '85982086988', '85982088181', '85982088401', '85982090444', '85982092229', '85982092410', '85982092535', '85982095933', '85982096408', '85982096638', '85982096702', '85982098898', '85982099596', '85982101224', '85982102764', '85982103459', '85982103837', '85982104191', '85982105219', '85982105253', '85982105588', '85982106049', '85982107612', '85982108435', '85982108824', '85982108871', '85982108995', '85982109939', '85982110388', '85982110918', '85982111162', '85982111405', '85982111461', '85982111682', '85982111714', '85982112134', '85982112150', '85982112252', '85982112330', '85982112561', '85982112835', '85982113153', '85982113424', '85982113947', '85982114041', '85982114590', '85982114798', '85982115352', '85982115530', '85982116277', '85982116934', '85982116997', '85982118281', '85982118296', '85982118359', '85982118717', '85982119038', '85982119077', '85982120196', '85982120770', '85982121018', '85982121624', '85982122300', '85982122468', '85982123793', '85982123880', '85982125254', '85982126275', '85982127512', '85982130408', '85982130446', '85982131720', '85982132411', '85982132443', '85982132450', '85982133520', '85982134594', '85982134658', '85982140032', '85982141654', '85982144572', '85982145647', '85982145648', '85982147385', '85982147517', '85982148150', '85982148935', '85982150345', '85982154109', '85982154431', '85982154497', '85982155595', '85982155633', '85982161243', '85982161749', '85982162384', '85982162735', '85982163153', '85982164038', '85982166162', '85982166295', '85982166369', '85982170184', '85982171502', '85982171541', '85982171985', '85982184521', '85982185872', '85982190343', '85982204545', '85982205828', '85982207580', '85982217764', '85982222262', '85982223649', '85982225298', '85982234415', '85982243000', '85982254767', '85982254833', '85984000187', '85984000206', '85984000276', '85984000283', '85984000366', '85984000374', '85984000408', '85984000419', '85984000570', '85984000752', '85984000901', '85984000924', '85984001030', '85984001034', '85984001146', '85984001200', '85984001263', '85984001399', '85984001670', '85984001714', '85984001904', '85984002329', '85984002699', '85984004021', '85984004143', '85984004381', '85984004513', '85984004885', '85984004934', '85984004937', '85984005030', '85984005089', '85984005191', '85984005207', '85984005486', '85984005676', '85984005684', '85984005854', '85984006088', '85984006430', '85984006519', '85984006807', '85984006822', '85984006945', '85984007418', '85984007839', '85984007934', '85984008090', '85984008165', '85984008494', '85984008541', '85984008711', '85984008837', '85984008876', '85984009118', '85984009152', '85984010102', '85984010119', '85984010346', '85984010352', '85984010376', '85984010523', '85984010651', '85984010721', '85984010796', '85984011030', '85984011127', '85984011205', '85984011272', '85984011345', '85984011423', '85984012202', '85984012591', '85984012893', '85984013559', '85984013847', '85984013900', '85984013932', '85984013963', '85984014210', '85984014231', '85984014288', '85984014376', '85984014432', '85984014547', '85984015074', '85984015099', '85984015349', '85984015384', '85984015385', '85984015469', '85984015572', '85984015631', '85984015661', '85984015695', '85984015758', '85984015793', '85984015918', '85984015943', '85984015948', '85984016599', '85984016848', '85984017946', '85984018354', '85984019606', '85984019846', '85984019986', '85984020049', '85984020051', '85984020177', '85984020235', '85984020417', '85984020826', '85984020911', '85984021324', '85984021461', '85984021871', '85984022102', '85984022241', '85984022389', '85984022437', '85984022645', '85984023016', '85984023231', '85984023332', '85984023361', '85984023534', '85984024023', '85984024057', '85984024750', '85984024773', '85984024790', '85984024966', '85984025156', '85984025366', '85984025761', '85984026229', '85984026355', '85984026707', '85984026882', '85984026909', '85984026937', '85984027014', '85984027778', '85984027803', '85984027980', '85984028311', '85984028478', '85984028528', '85984028635', '85984028807', '85984029384', '85984029403', '85984029645', '85984029647', '85984029806', '85984029997', '85984030002', '85984030015', '85984030126', '85984030128', '85984030255', '85984030534', '85984030799', '85984030914', '85984031018', '85984031134', '85984031235', '85984031240', '85984031369', '85984031377', '85984031387', '85984031438', '85984031757', '85984031799', '85984031859', '85984031951', '85984031983', '85984031996', '85984032024', '85984032030', '85984032046', '85984032152', '85984032209', '85984032278', '85984032838', '85984032911', '85984033253', '85984033308', '85984033709', '85984033733', '85984033741', '85984033796', '85984033825', '85984033893', '85984033983', '85984034114', '85984034385', '85984034577', '85984034588', '85984034633', '85984034782', '85984034964', '85984035081', '85984035134', '85984035188', '85984035416', '85984035423', '85984035459', '85984035494', '85984035559', '85984035765', '85984036032', '85984036315', '85984036485', '85984036570', '85984036614', '85984036676', '85984036734', '85984036808', '85984036872', '85984037291', '85984037296', '85984037302', '85984037313', '85984037354', '85984037682', '85984037921', '85984037935', '85984037947', '85984038033', '85984038229', '85984038524', '85984038538', '85984038620', '85984038850', '85984038856', '85984039320', '85984039429', '85984039451', '85984039728', '85984040449', '85984040502', '85984040554', '85984040731', '85984040757', '85984040783', '85984040792', '85984040899', '85984041029', '85984041044', '85984041297', '85984041417', '85984041458', '85984041670', '85984041713', '85984041805', '85984041914', '85984041986', '85984042380', '85984042425', '85984042497', '85984042509', '85984042623', '85984042895', '85984042963', '85984043070', '85984043137', '85984043296', '85984043323', '85984043326', '85984043413', '85984043751', '85984044012', '85984044067', '85984044191', '85984044248', '85984044283', '85984044300', '85984044346', '85984044633', '85984044683', '85984044763', '85984044963', '85984045050', '85984045056', '85984045115', '85984045640', '85984045722', '85984046240', '85984046424', '85984046625', '85984046753', '85984046806', '85984046807', '85984046867', '85984047111', '85984047230', '85984047233', '85984047367', '85984047472', '85984047476', '85984047517', '85984047596', '85984048175', '85984048182', '85984048183', '85984048283', '85984048339', '85984048508', '85984048524', '85984048559', '85984048759', '85984048849', '85984049026', '85984049029', '85984049263', '85984049442', '85984049451', '85984049504', '85984049679', '85984049735', '85984049763', '85984049858', '85984049949', '85984050227', '85984050228', '85984050250', '85984050371', '85984050677', '85984050801', '85984050882', '85984050887', '85984050928', '85984051292', '85984051333', '85984051412', '85984051489', '85984051523', '85984051742', '85984051769', '85984051840', '85984051889', '85984051935', '85984052109', '85984052112', '85984052208', '85984052217', '85984052263', '85984052298', '85984052611', '85984052730', '85984052764', '85984052843', '85984053038', '85984053174', '85984053179', '85984053330', '85984053556', '85984053869', '85984053880', '85984053887', '85984053943', '85984053956', '85984054025', '85984054056', '85984054133', '85984054160', '85984054172', '85984054228', '85984054266', '85984054556', '85984054674', '85984054734', '85984054739', '85984054879', '85984054912', '85984055156', '85984055310', '85984055345', '85984055442', '85984055473', '85984055502', '85984055688', '85984055714', '85984055899', '85984055933', '85984056265', '85984056517', '85984056826', '85984056911', '85984056971', '85984057268', '85984057361', '85984057589', '85984057713', '85984057802', '85984057880', '85984058809', '85984059297', '85984059565', '85984059708', '85984060013', '85984060654', '85984060832', '85984061103', '85984061137', '85984061447', '85984061486', '85984061543', '85984061639', '85984061962', '85984062029', '85984062279', '85984062320', '85984062358', '85984062494', '85984062505', '85984062530', '85984063166', '85984063203', '85984063719', '85984063744', '85984063839', '85984064263', '85984064393', '85984064541', '85984064961', '85984065160', '85984065816', '85984066050', '85984066966', '85984067046', '85984067756', '85984067873', '85984068456', '85984069092', '85984069667', '85984069722', '85984069938', '85984070019', '85984070211', '85984070265', '85984070421', '85984070652', '85984070895', '85984071052', '85984071611', '85984071870', '85984072029', '85984072045', '85984072051', '85984072058', '85984072071', '85984072145', '85984072225', '85984072316', '85984072445', '85984072480', '85984072653', '85984072933', '85984073162', '85984073973', '85984074264', '85984074313', '85984074778', '85984075096', '85984075666', '85984076005', '85984076212', '85984076393', '85984076578', '85984076839', '85984076847', '85984077031', '85984077361', '85984077370', '85984077740', '85984077801', '85984078005', '85984078034', '85984078218', '85984078233', '85984078314', '85984078445', '85984078614', '85984079116', '85984079245', '85984079370', '85984079725', '85984079880', '85984079915', '85984080469', '85984080471', '85984080593', '85984080601', '85984081278', '85984081475', '85984081680', '85984082025', '85984082125', '85984082555', '85984082670', '85984082940', '85984082979', '85984083419', '85984083846', '85984084306', '85984084464', '85984084549', '85984084550', '85984084823', '85984084857', '85984085018', '85984085176', '85984085262', '85984085880', '85984086976', '85984087409', '85984088006', '85984088529', '85984089052', '85984089070', '85984089220', '85984089798', '85984090380', '85984090552', '85984090594', '85984090882', '85984090929', '85984091124', '85984091289', '85984091406', '85984091518', '85984092054', '85984092195', '85984092230', '85984092539', '85984093168', '85984093610', '85984093759', '85984093855', '85984094073', '85984094849', '85984095284', '85984096033', '85984098963', '85984099235', '85984099245', '85984099377', '85984099885', '85984100300', '85984100698', '85984100822', '85984101624', '85984101697', '85984102042', '85984102155', '85984102262', '85984102480', '85984102514', '85984102560', '85984102571', '85984103927', '85984104957', '85984105301', '85984105524', '85984106425', '85984107192', '85984107381', '85984107762', '85984108029', '85984108520', '85984108531', '85984108645', '85984108950', '85984109045', '85984109435', '85984109534', '85984110121', '85984110186', '85984110449', '85984110493', '85984110570', '85984110730', '85984110811', '85984111215', '85984111369', '85984111609', '85984111626', '85984111796', '85984111877', '85984111930', '85984112126', '85984112139', '85984112386', '85984112657', '85984113012', '85984113687', '85984113734', '85984113870', '85984113916', '85984114001', '85984114121', '85984114826', '85984114827', '85984115475', '85984115569', '85984115651', '85984116121', '85984116540', '85984116596', '85984116734', '85984116933', '85984117008', '85984117204', '85984117429', '85984117798', '85984118037', '85984118042', '85984118203', '85984118581', '85984118664', '85984118708', '85984118774', '85984119107', '85984119481', '85984119572', '85984119808', '85984120393', '85984120682', '85984121272', '85984122145', '85984122414', '85984123034', '85984123448', '85984124093', '85984124208', '85984125015', '85984125036', '85984126078', '85984126186', '85984126390', '85984126584', '85984126778', '85984126955', '85984127219', '85984127242', '85984127734', '85984128627', '85984128634', '85984128869', '85984128924', '85984129311', '85984129612', '85984130038', '85984130659', '85984130724', '85984130979', '85984131046', '85984131139', '85984131313', '85984131574', '85984131761', '85984131881', '85984132127', '85984132128', '85984132149', '85984132782', '85984132844', '85984133084', '85984133130', '85984133206', '85984133331', '85984133448', '85984133534', '85984134089', '85984134736', '85984135015', '85984135302', '85984135420', '85984135573', '85984</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['10', '27', '27', '27', '46', '30', '27', '1', '5', '29', '1', '35', '16', '43', '27', '27', '27', '11', '5', '28', '1', '49', '27', '27', '1', '27', '0', '27', '11', '1', '28', '10', '3', '27', '3', '28', '27', '31', '1', '25', '1', '27', '27', '40', '27', '27', '28', '27', '27', '12', '28', '5', '7', '6', '28', '40', '49', '1', '2', '8', '78', '1', '1', '27', '5', '27', '1', '27', '27', '11', '1', '28', '12', '27', '27', '1', '5', '27', '27', '2', '27', '27', '27', '25', '7', '27', '28', '1', '11', '27', '1', '1', '27', '21', '13', '6', '27', '5', '1', '0', '28', '27', '28', '27', '27', '27', '27', '27', '27', '7', '28', '5', '5', '27', '27', '47', '28', '27', '34', '1', '35', '5', '8', '12', '28', '27', '12', '49', '28', '27', '6', '27', '1', '1', '17', '5', '27', '1', '1', '28', '31', '1', '27', '12', '5', '27', '39', '49', '19', '16', '28', '27', '5', '27', '8', '27', '4', '35', '8', '30', '35', '1', '27', '27', '10', '40', '1', '27', '27', '49', '27', '29', '27', '27', '1', '28', '43', '32', '45', '30', '27', '27', '6', '27', '5', '2', '27', '7', '49', '13', '28', '6', '27', '27', '27', '27', '26', '27', '27', '27', '28', '49', '1', '27', '11', '28', '27', '27', '27', '27', '1', '18', '28', '27', '27', '27', '1', '27', '1', '49', '10', '27', '5', '49', '1', '11', '27', '49', '27', '27', '5', '49', '27', '7', '5', '28', '1', '29', '27', '11', '31', '38', '27', '15', '27', '27', '49', '17', '41', '8', '27', '1', '28', '30', '28', '3', '27', '30', '30', '5', '27', '10', '1', '49', '27', '28', '1', '27', '4', '1', '28', '5', '27', '27', '12', '28', '10', '27', '27', '48', '1', '1', '1', '27', '30', '1', '27', '27', '27', '29', '27', '5', '27', '27', '6', '1', '30', '27', '28', '1', '12', '5', '29', '25', '27', '49', '27', '27', '6', '11', '27', '27', '27', '27', '11', '27', '1', '27', '27', '27', '27', '27', '30', '27', '49', '28', '28', '23', '40', '27', '28', '27', '27', '27', '5', '11', '27', '27', '1', '5', '11', '28', '27', '27', '27', '28', '9', '5', '27', '11', '27', '1', '35', '1', '27', '1', '27', '27', '1', '30', '27', '27', '28', '17', '27', '27', '1', '27', '35', '49', '27', '49', '27', '27', '11', '27', '12', '27', '27', '8', '4', '49', '11', '27', '35', '4', '28', '27', '27', '27', '5', '18', '1', '5', '27', '27', '1', '28', '27', '1', '1', '11', '1', '1', '28', '114', '9', '27', '27', '5', '28', '27', '27', '1', '23', '27', '27', '5', '1', '27', '1', '5', '27', '27', '27', '27', '87', '27', '28', '31', '39', '34', '27', '27', '27', '9', '13', '9', '1', '17', '27', '35', '27', '30', '12', '27', '27', '49', '6', '27', '27', '27', '1', '28', '1', '30', '27', '27', '27', '12', '27', '27', '27', '1', '28', '0', '27', '49', '27', '27', '1', '28', '27', '27', '49', '27', '27', '27', '49', '27', '27', '6', '49', '1', '27', '9', '1', '28', '42', '13', '31', '27', '15', '8', '49', '27', '5', '27', '8', '27', '29', '27', '27', '49', '27', '14', '27', '28', '27', '27', '49', '29', '11', '27', '27', '12', '27', '27', '27', '27', '27', '1', '27', '5', '22', '1', '27', '27', '49', '17', '29', '11', '27', '27', '5', '13', '1', '10', '27', '28', '27', '27', '27', '27', '27', '5', '24', '27', '1', '1', '27', '1', '30', '27', '27', '27', '1', '14', '19', '25', '27', '27', '27', '27', '49', '27', '30', '11', '30', '5', '27', '27', '1', '27', '28', '27', '1', '29', '27', '27', '1', '5', '1', '37', '49', '1', '5', '2', '82', '5', '27', '27', '30', '8', '27', '5', '27', '27', '27', '28', '49', '27', '27', '27', '27', '28', '5', '27', '27', '1', '27', '14', '5', '49', '31', '1', '27', '1', '27', '5', '27', '27', '27', '28', '1', '12', '40', '27', '43', '27', '27', '1', '27', '49', '49', '21', '27', '27', '22', '27', '7', '12', '27', '27', '0', '1', '27', '27', '27', '28', '1', '7', '28', '49', '27', '27', '27', '7', '28', '16', '1', '1', '27', '12', '10', '12', '27', '27', '4', '27', '27', '30', '5', '12', '29', '27', '27', '17', '27', '27', '13', '5', '27', '12', '16', '49', '27', '1', '27', '6', '49', '29', '27', '28', '18', '28', '49', '27', '27', '27', '30', '27', '7', '23', '49', '12', '16', '27', '1', '5', '1', '27', '27', '27', '27', '27', '27', '27', '49', '27', '28', '27', '1', '27', '27', '27', '27', '27', '49', '21', '27', '28', '27', '27', '28', '35', '27', '49', '1', '27', '27', '26', '27', '38', '27', '1', '6', '27', '27', '28', '7', '28', '27', '27', '27', '27', '12', '5', '6', '27', '18', '28', '17', '27', '27', '28', '23', '14', '27', '12', '29', '28', '28', '27', '27', '27', '27', '28', '28', '49', '5', '27', '12', '27', '27', '27', '49', '27', '27', '12', '8', '27', '28', '28', '1', '9', '28', '27', '27', '27', '1', '1', '10', '1', '28', '27', '12', '1', '7', '27', '27', '27', '27', '28', '27', '27', '27', '5', '27', '12', '46', '27', '27', '31', '35', '17', '28', '27', '20', '24', '23', '1', '41', '36', '49', '49', '7', '28', '49', '27', '27', '5', '5', '27', '1', '5', '17', '27', '28', '13', '7', '49', '28', '27', '27', '27', '1', '34', '42', '35', '27', '28', '28', '28', '35', '11', '27', '5', '5', '28', '28', '27', '28', '1', '28', '13', '27', '28', '27', '28', '30', '28', '28', '18', '27', '5', '1', '76', '28', '28', '1', '5', '1', '28', '26', '2', '28', '1', '7', '12', '28', '37', '11', '28', '27', '27', '27', '27', '28', '28', '27', '20', '8', '30', '14', '27', '4', '10', '4', '49', '28', '28', '1', '1', '22', '27', '1', '10', '28', '11', '28', '77', '28', '2', '27', '30', '27', '27', '31', '1', '28', '28', '12', '27', '28', '10', '30', '27', '9', '27', '18', '28', '0', '12', '28', '49', '27', '27', '27', '27', '30', '1', '28', '27', '50', '31', '1', '27', '1', '27', '28', '28', '28', '27', '7', '1', '28', '27', '1', '27', '31', '28', '27', '1', '28', '1', '49', '49', '27', '28', '27', '27', '1', '27', '28', '27', '5', '26', '12', '1', '28', '2', '8', '13', '1', '12', '1', '28', '27', '1', '30', '7', '7', '37', '27', '28', '8', '5', '27', '28', '27', '27', '13', '13', '27', '30', '13', '13', '27', '1', '28', '27', '28', '27', '31', '27', '13', '28', '27', '27', '28', '12', '27', '27', '7', '1', '29', '27', '27', '1', '5', '27', '13', '27', '28', '49', '27', '6', '28', '27', '1', '27', '27', '21', '28', '31', '46', '27', '28', '5', '5', '27', '27', '30', '7', '27', '28', '28', '28', '30', '9', '17', '1', '3', '30', '7', '27', '28', '27', '7', '37', '27', '14', '13', '28', '27', '27', '27', '1', '27', '27', '27', '27', '28', '6', '28', '27', '12', '27', '47', '49', '28', '28', '27', '27', '13', '14', '28', '12', '28', '7', '27', '28', '27', '27', '1', '1', '27', '14', '0', '1', '27', '1', '1', '31', '1', '5', '39', '35', '27', '28', '11', '30', '27', '1', '27', '49', '27', '28', '28', '27', '47', '27', '28', '28', '5', '28', '30', '11', '49', '27', '28', '1', '28', '28', '28', '27', '49', '30', '27', '28', '30', '27', '15', '49', '8', '28', '12', '27', '17', '28', '27', '30', '49', '1', '28', '28', '27', '27', '27', '49', '1', '26', '1', '27', '49', '1', '6', '27', '5', '28', '1', '27', '11', '16', '28', '114', '27', '27', '27', '34', '1', '6', '28', '49', '21', '27', '27', '27', '28', '10', '1', '27', '27', '27', '49', '1', '28', '28', '27', '31', '28', '28', '28', '49', '49', '27', '27', '27', '8', '28', '1', '11', '5', '1', '1', '27', '32', '49', '27', '9', '33', '27', '5', '28', '27', '31', '28', '27', '27', '27', '27', '27', '39', '30', '12', '13', '28', '34', '1', '27', '27', '28', '28', '15', '11', '27', '28', '1', '27', '1', '35', '27', '7', '17', '1', '35', '23', '27', '28', '1', '5', '28', '2', '21', '27', '28', '28', '28', '11', '49', '32', '28', '14', '14', '30', '27', '1', '28', '28', '28', '23', '1', '27', '27', '27', '28', '47', '27', '28', '1', '27', '27', '28', '42', '49', '27', '27', '5', '28', '27', '1', '28', '27', '26', '27', '27', '28', '28', '8', '5', '0', '49', '28', '28', '5', '28', '27', '28', '28', '41', '8', '27', '27', '27', '6', '27', '27', '27', '6', '1', '28', '30', '5', '27', '12', '2', '5', '28', '15', '5', '27', '28', '27', '12', '28', '28', '5', '27', '12', '28', '27', '27', '6', '1', '30', '28', '27', '28', '12', '27', '13', '1', '49', '31', '27', '12', '28', '27', '28', '27', '33', '27', '40', '27', '28', '28', '27', '0', '20', '27', '1', '43', '28', '28', '1', '49', '33', '27', '10', '28', '27', '28', '27', '27', '2', '27', '27', '49', '1', '28', '28', '43', '27', '27', '28', '49', '5', '28', '146', '10', '18', '28', '27', '27', '27', '28', '27', '28', '28', '28', '11', '1', '5', '6', '27', '8', '5', '9', '28', '1', '27', '28', '18', '27', '6', '6', '26', '27', '7', '27', '49', '8', '27', '75', '21', '58', '27', '27', '21', '27', '21', '6', '27', '29', '27', '27', '62', '69', '65', '17', '27', '49', '8', '27', '8', '5', '27', '1', '30', '1', '27', '32', '32', '49', '5', '5', '4', '13', '32', '33', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '32', '5', '4', '5', '32', '4', '3', '4', '4', '4', '5', '35', '33', '4', '5', '5', '5', '4', '30', '32', '5', '4', '5', '19', '5', '5', '4', '5', '5', '5', '5', '5', '4', '4', '5', '5', '5', '32', '32', '39', '4', '4', '4', '34', '5', '33', '34', '49', '4', '5', '4', '5', '3', '77', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '5', '6', '5', '5', '4', '4', '5', '4', '5', '4', '4', '32', '5', '51', '4', '32', '4', '33', '4', '4', '5', '12', '32', '4', '4', '32', '5', '5', '4', '5', '4', '3', '4', '5', '4', '5', '6', '4', '5', '32', '4', '4', '4', '5', '4', '5', '5', '5', '2', '5', '6', '4', '49', '5', '4', '32', '5', '32', '5', '5', '5', '39', '49', '33', '33', '4', '4', '5', '5', '5', '4', '5', '5', '4', '33', '32', '32', '32', '32', '33', '5', '32', '32', '32', '33', '44', '20', '14', '33', '6', '32', '12', '49', '32', '32', '49', '33', '34', '5', '32', '32', '32', '32', '4', '32', '32', '5', '6', '42', '33', '35', '32', '31', '31', '5', '32', '49', '32', '4', '27', '11', '32', '4', '69', '32', '6', '32', '34', '5', '32', '49', '32', '21', '32', '32', '5', '30', '33', '32', '16', '32', '33', '34', '32', '48', '49', '31', '32', '6', '32', '34', '34', '5', '33', '49', '39', '32', '33', '33', '4', '32', '11', '32', '6', '6', '33', '32', '33', '33', '31', '32', '32', '5', '32', '4', '32', '4', '32', '32', '33', '32', '32', '5', '34', '32', '33', '32', '49', '32', '27', '31', '4', '12', '33', '34', '49', '5', '31', '32', '6', '30', '5', '32', '27', '34', '32', '22', '32', '4', '32', '33', '32', '32', '4', '6', '33', '33', '72', '32', '32', '5', '30', '32', '5', '32', '32', '60', '32', '33', '15', '34', '32', '33', '33', '32', '32', '12', '33', '33', '33', '32', '32', '5', '32', '33', '7', '32', '46', '5', '33', '32', '41', '34', '32', '32', '32', '5', '32', '32', '33', '33', '33', '32', '32', '7', '33', '32', '32', '32', '12', '32', '5', '32', '49', '9', '30', '32', '33', '33', '33', '27', '5', '5', '31', '32', '6', '30', '79', '35', '49', '34', '32', '33', '33', '32', '32', '32', '49', '32', '70', '26', '32', '32', '6', '32', '31', '5', '28', '32', '5', '5', '10', '4', '49', '33', '5', '32', '32', '6', '5', '4', '4', '4', '5', '5', '32', '5', '4', '5', '5', '75', '4', '4', '4', '4', '34', '4', '5', '5', '49', '42', '4', '5', '32', '2', '4', '5', '33', '4', '5', '5', '5', '5', '5', '4', '11', '32', '49', '4', '30', '5', '27', '4', '31', '29', '2', '4', '5', '33', '5', '4', '5', '32', '4', '4', '5', '32', '5', '4', '32', '14', '37', '5', '4', '33', '4', '5', '5', '31', '4', '4', '5', '32', '33', '33', '5', '5', '5', '5', '4', '4', '4', '4', '5', '5', '30', '4', '0', '4', '16', '4', '5', '4', '4', '5', '5', '5', '5', '4', '5', '4', '30', '5', '5', '5', '15', '5', '4', '5', '5', '5', '5', '7', '4', '4', '4', '32', '32', '5', '32', '4', '4', '5', '4', '4', '4', '4', '4', '4', '4', '4', '30', '4', '5', '4', '4', '5', '34', '4', '5', '64', '4', '4', '4', '4', '4', '4', '4', '5', '4', '4', '5', '5', '5', '4', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '31', '4', '4', '5', '4', '5', '35', '4', '4', '4', '5', '4', '4', '5', '4', '5', '4', '5', '4', '5', '4', '4', '4', '4', '32', '4', '4', '31', '13', '4', '11', '4', '32', '5', '4', '33', '5', '32', '4', '30', '4', '5', '32', '33', '5', '5', '5', '4', '5', '3', '4', '4', '5', '32', '4', '4', '5', '31', '32', '5', '49', '12', '5', '4', '5', '4', '33', '2', '5', '5', '30', '80', '4', '33', '33', '3', '5', '34', '31', '34', '7', '59', '32', '33', '5', '32', '95', '5', '32', '32', '5', '5', '32', '30', '5', '32', '5', '4', '4', '32', '5', '4', '4', '5', '5', '33', '11', '4', '32', '4', '4', '33', '4', '63', '4', '4', '4', '34', '4', '18', '33', '32', '33', '32', '4', '32', '47', '5', '4', '32', '5', '5', '49', '35', '32', '33', '32', '5', '7', '32', '4', '32', '21', '12', '5', '32', '32', '4', '4', '4', '5', '5', '4', '32', '5', '4', '5', '32', '5', '4', '34', '4', '5', '4', '5', '5', '4', '5', '4', '4', '30', '32', '5', '33', '33', '32', '31', '33', '32', '32', '4', '6', '34', '1', '15', '30', '32', '5', '4', '32', '4', '5', '32', '2', '49', '8', '32', '11', '6', '5', '31', '33', '12', '34', '33', '31', '4', '33', '34', '34', '32', '32', '32', '32', '8', '32', '33', '4', '74', '4', '33', '32', '28', '4', '5', '33', '14', '32', '33', '31', '5', '32', '5', '33', '33', '32', '33', '32', '5', '32', '33', '23', '27', '31', '31', '34', '31', '5', '41', '32', '32', '33', '32', '11', '32', '7', '11', '32', '33', '32', '33', '34', '32', '32', '4', '32', '31', '32', '32', '32', '32', '33', '46', '32', '66', '32', '33', '30', '5', '32', '32', '32', '4', '32', '32', '32', '32', '33', '32', '49', '32', '32', '32', '33', '33', '32', '5', '33', '32', '12', '32', '33', '16', '32', '33', '5', '32', '32', '9', '34', '64', '4', '32', '32', '33', '32', '31', '32', '32', '10', '32', '6', '33', '13', '32', '5', '5', '4', '31', '3', '32', '25', '40', '34', '32', '32', '34', '5', '32', '44', '33', '8', '32', '33', '32', '33', '5', '33', '32', '32', '32', '18', '30', '32', '33', '32', '49', '32', '32', '32', '6', '17', '33', '33', '5', '49', '32', '19', '4', '5', '5', '4', '5', '7', '4', '11', '33', '32', '32', '4', '3', '32', '27', '4', '4', '33', '5', '4', '34', '31', '5', '30', '1', '4', '5', '32', '5', '4', '5', '4', '61', '9', '4', '11', '5', '32', '33', '33', '34', '4', '33', '34', '4', '32', '32', '5', '32', '4', '31', '32', '33', '5', '4', '33', '5', '4', '27', '5', '5', '4', '35', '5', '5', '4', '5', '4', '4', '4', '33', '5', '32', '5', '5', '5', '27', '4', '4', '4', '4', '4', '5', '5', '5', '5', '6', '5', '5', '5', '5', '4', '5', '5', '5', '4', '5', '4', '66', '4', '4', '4', '4', '5', '4', '4', '4', '32', '7', '33', '5', '7', '4', '5', '55', '32', '43', '21', '5', '4', '5', '3', '4', '5', '4', '4', '32', '32', '33', '34', '5', '69', '4', '32', '4', '32', '25', '30', '32', '30', '32', '63', '35', '33', '5', '32', '5', '32', '4', '5', '4', '5', '4', '5', '4', '4', '33', '33', '33', '4', '30', '5', '33', '32', '4', '32', '33', '27', '5', '4', '32', '5', '4', '32', '5', '5', '5', '33', '4', '5', '4', '4', '4', '5', '5', '7', '33', '5', '32', '5', '5', '49', '5', '4', '4', '5', '4', '4', '5', '4', '4', '5', '32', '4', '4', '4', '4', '4', '5', '32', '4', '5', '4', '4', '4', '5', '4', '5', '4', '4', '61', '4', '5', '4', '38', '33', '4', '5', '34', '13', '4', '4', '32', '32', '32', '4', '5', '5', '32', '5', '32', '4', '33', '33', '33', '5', '5', '33', '5', '5', '4', '12', '4', '28', '5', '5', '5', '5', '5', '4', '5', '5', '4', '32', '6', '4', '4', '5', '9', '13', '32', '34', '4', '33', '15', '32', '32', '4', '32', '5', '5', '27', '4', '5', '4', '4', '5', '4', '4', '4', '5', '4', '21', '5', '5', '33', '5', '4', '34', '5', '4', '4', '4', '5', '4', '4', '5', '5', '4', '5', '5', '13', '4', '5', '4', '5', '4', '4', '31', '5', '4', '5', '4', '4', '5', '30', '4', '4', '5', '4', '5', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '5', '5', '5', '46', '4', '4', '4', '4', '5', '4', '5', '22', '5', '5', '4', '49', '5', '5', '32', '5', '4', '5', '5', '5', '4', '4', '32', '4', '30', '32', '4', '4', '4', '4', '5', '5', '12', '5', '4', '5', '4', '33', '4', '4', '4', '32', '4', '4', '4', '4', '5', '4', '4', '32', '4', '35', '5', '4', '4', '5', '4', '5', '32', '0', '67', '4', '31', '4', '5', '30', '4', '17', '3', '5', '4', '4', '4', '5', '22', '5', '4', '4', '4', '4', '5', '5', '5', '5', '4', '5', '5', '2', '4', '4', '5', '32', '5', '5', '5', '4', '4', '4', '50', '4', '5', '4', '4', '5', '5', '5', '32', '5', '30', '32', '4', '5', '32', '4', '4', '4', '4', '4', '5', '5', '4', '5', '68', '5', '29', '4', '5', '5', '4', '5', '5', '6', '6', '6', '6', '6', '6', '5', '6', '6', '32', '35', '6', '33', '6', '24', '5', '34', '33', '32', '30', '31', '32', '33', '13', '32', '32', '93', '8', '33', '32', '32', '5', '33', '31', '32', '32', '33', '13', '32', '9', '32', '30', '3', '4', '9', '33', '3', '32', '33', '19', '32', '32', '33', '32', '33', '30', '30', '32', '5', '33', '32', '81', '7', '7', '32', '79', '33', '15', '32', '32', '32', '32', '5', '30', '32', '7', '32', '33', '5', '32', '33', '33', '35', '33', '32', '33', '33', '33', '31', '33', '32', '34', '32', '32', '32', '34', '33', '7', '33', '13', '32', '32', '32', '49', '32', '33', '33', '32', '32', '4', '32', '32', '33', '33', '4', '32', '33', '33', '12', '49', '33', '32', '80', '32', '33', '32', '25', '32', '34', '33', '4', '32', '32', '33', '32', '33', '33', '32', '33', '32', '4', '21', '32', '5', '32', '49', '71', '33', '33', '16', '13', '4', '32', '32', '5', '27', '18', '34', '33', '32', '65', '32', '32', '22', '27', '49', '34', '33', '33', '5', '4', '5', '5', '44', '32', '30', '12', '32', '32', '11', '33', '33', '33', '33', '32', '4', '11', '32', '32', '11', '8', '32', '4', '5', '5', '5', '33', '4', '4', '4', '70', '12', '27', '32', '32', '5', '17', '33', '32', '32', '8', '34', '32', '59', '32', '32', '33', '31', '31', '32', '49', '5', '15', '13', '33', '34', '32', '4', '33', '32', '4', '8', '32', '33', '22', '34', '49', '11', '33', '32', '32', '5', '28', '32', '31', '32', '32', '12', '32', '32', '32', '28', '49', '30', '33', '33', '32', '3', '18', '30', '33', '4', '32', '4', '31', '1', '12', '28', '5', '49', '33', '23', '32', '32', '33', '33', '33', '8', '33', '4', '29', '4', '32', '13', '32', '33', '33', '34', '32', '31', '33', '32', '4', '5', '32', '32', '5', '33', '15', '11', '33', '9', '50', '59', '13', '32', '32', '34', '33', '34', '33', '33', '33', '32', '20', '20', '33', '33', '34', '33', '32', '31', '12', '32', '33', '33', '5', '32', '32', '31', '33', '5', '32', '33', '7', '33', '32', '26', '13', '34', '12', '4', '5', '12', '49', '32', '33', '33', '32', '32', '32', '33', '33', '32', '17', '13', '32', '33', '10', '32', '32', '30', '32', '32', '32', '8', '5', '32', '32', '32', '32', '32', '12', '30', '12', '34', '33', '32', '45', '32', '34', '28', '32', '4', '4', '17', '32', '33', '49', '33', '26', '33', '49', '33', '31', '32', '32', '14', '5', '32', '32', '32', '32', '27', '32', '5', '33', '32', '32', '32', '32', '32', '32', '13', '15', '32', '30', '32', '32', '32', '32', '26', '32', '18', '33', '32', '32', '32', '49', '32', '33', '31', '32', '4', '5', '34', '32', '33', '33', '34', '32', '32', '6', '33', '5', '31', '32', '33', '32', '31', '29', '12', '32', '32', '5', '33', '30', '33', '32', '32', '31', '32', '39', '7', '61', '25', '34', '33', '32', '32', '7', '32', '31', '31', '33', '10', '34', '32', '31', '22', '32', '20', '9', '32', '32', '33', '30', '12', '33', '33', '33', '27', '5', '32', '5', '27', '24', '12', '32', '32', '62', '32', '22', '32', '5', '32', '33', '24', '49', '32', '32', '32', '4', '6', '33', '4', '33', '32', '32', '32', '32', '1', '11', '32', '26', '24', '5', '5', '32', '7', '5', '31', '33', '5', '54', '32', '33', '32', '32', '32', '32', '30', '32', '32', '12', '31', '32', '33', '33', '32', '33', '49', '33', '22', '32', '12', '32', '27', '55', '32', '34', '60', '32', '4', '5', '4', '4', '4', '4', '4', '4', '4', '5', '6', '4', '4', '34', '33', '4', '4', '33', '5', '35', '33', '33', '4', '5', '5', '33', '32', '32', '32', '5', '4', '4', '5', '5', '5', '32', '32', '4', '49', '5', '15', '33', '32', '32', '32', '34', '32', '60', '32', '32', '32', '27', '33', '30', '15', '5', '5', '72', '4', '4', '33', '33', '11', '32', '32', '32', '44', '63', '6', '7', '32', '32', '32', '5', '4', '19', '32', '14', '1', '33', '32', '71', '4', '48', '4', '31', '34', '5', '35', '5', '32', '32', '33', '32', '32', '26', '13', '32', '28', '32', '6', '21', '31', '64', '11', '33', '32', '32', '34', '5', '32', '26', '32', '5', '14', '32', '5', '5', '32', '4', '39', '13', '4', '35', '0', '32', '33', '33', '32', '32', '32', '49', '15', '33', '32', '32', '27', '32', '32', '5', '46', '11', '24', '33', '11', '4', '32', '12', '5', '5', '5', '32', '33', '32', '1', '32', '7', '13', '32', '32', '32', '13', '5', '30', '5', '4', '32', '30', '33', '33', '4', '7', '5', '33', '33', '33', '32', '14', '29', '6', '13', '32', '10', '33', '33', '5', '30', '12', '21', '33', '32', '33', '31', '30', '32', '18', '34', '32', '32', '34', '30', '12', '32', '32', '30', '32', '33', '34', '30', '32', '5', '33', '32', '12', '33', '33', '32', '32', '32', '11', '32', '32', '33', '32', '33', '32', '30', '32', '5', '32', '32', '25', '32', '33', '31', '32', '14', '33', '57', '30', '32', '49', '27', '5', '32', '12', '33', '33', '32', '32', '33', '21', '33', '33', '32', '10', '33', '33', '33', '32', '4', '4', '32', '32', '31', '33', '33', '33', '32', '24', '5', '35', '32', '32', '5', '3', '34', '32', '32', '5', '32', '33', '57', '33', '4', '34', '52', '33', '32', '33', '32', '33', '33', '1', '33', '33', '33', '22', '27', '33', '32', '32', '34', '33', '7', '12', '1', '4', '33', '32', '33', '33', '32', '32', '31', '32', '32', '29', '33', '31', '49', '5', '11', '34', '32', '32', '25', '35', '32', '25', '32', '33', '33', '5', '32', '27', '32', '31', '30', '30', '34', '32', '31', '5', '13', '30', '32', '4', '33', '32', '32', '32', '34', '4', '33', '30', '31', '32', '32', '33', '34', '49', '32', '5', '31', '33', '32', '32', '49', '8', '33', '32', '5', '32', '32', '33', '5', '32', '4', '36', '5', '32', '4', '32', '32', '18', '33', '33', '34', '34', '32', '8', '41', '32', '33', '49', '32', '32', '32', '5', '30', '49', '27', '32', '55', '49', '49', '26', '5', '33', '33', '33', '32', '32', '34', '32', '32', '12', '32', '11', '31', '33', '34', '32', '21', '28', '57', '32', '30', '4', '32', '4', '32', '17', '31', '33', '32', '32', '32', '32', '5', '30', '32', '32', '32', '32', '34', '32', '32', '32', '32', '32', '32', '33', '33', '13', '32', '34', '32', '32', '32', '32', '32', '5', '33', '32', '32', '33', '32', '5', '12', '33', '32', '5', '32', '32', '32', '5', '32', '5', '16', '34', '33', '33', '4', '30', '11', '34', '32', '35', '94', '10', '4', '14', '32', '28', '4', '32', '32', '17', '15', '4', '27', '4', '32', '32', '5', '34', '32', '32', '7', '33', '18', '31', '58', '20', '32', '11', '67', '36', '4', '27', '12', '32', '33', '26', '33', '5', '32', '32', '32', '32', '33', '77', '4', '33', '35', '32', '31', '31', '24', '32', '32', '33', '32', '24', '29', '33', '32', '32', '32', '24', '32', '5', '32', '16', '33', '33', '32', '32', '32', '11', '32', '5', '32', '32', '32', '32', '45', '32', '32', '31', '32', '32', '15', '32', '30', '31', '32', '5', '33', '5', '32', '32', '32', '32', '52', '26', '32', '32', '5', '33', '2', '34', '36', '33', '49', '33', '32', '5', '32', '6', '14', '32', '33', '32', '31', '31', '32', '33', '32', '33', '32', '32', '5', '32', '28', '32', '33', '32', '33', '8', '32', '5', '33', '12', '48', '32', '32', '32', '32', '32', '33', '4', '32', '13', '8', '32', '32', '33', '38', '33', '34', '33', '6', '33', '32', '32', '32', '13', '5', '4', '32', '16', '34', '7', '11', '12', '5', '11', '9', '33', '11', '33', '4', '34', '32', '32', '6', '49', '31', '32', '32', '5', '32', '4', '32', '32', '15', '6', '49', '32', '5', '32', '32', '32', '32', '6', '32', '32', '33', '32', '5', '11', '7', '5', '32', '31', '45', '33', '31', '32', '30', '6', '33', '33', '31', '34', '70', '1', '32', '31', '5', '32', '19', '5', '32', '32', '32', '32', '32', '31', '4', '32', '4', '32', '32', '11', '33', '32', '49', '33', '32', '33', '5', '32', '32', '33', '12', '49', '33', '32', '32', '11', '32', '32', '32', '33', '26', '33', '32', '32', '26', '0', '32', '31', '10', '32', '4', '31', '27', '5', '32', '33', '51', '12', '49', '6', '33', '33', '34', '32', '32', '32', '33', '32', '33', '5', '33', '32', '4', '49', '34', '32', '32', '5', '25', '31', '32', '33', '2', '5', '32', '14', '32', '32', '78', '32', '32', '32', '9', '20', '33', '33', '34', '32', '15', '33', '31', '32', '31', '32', '7', '11', '33', '32', '22', '49', '32', '32', '31', '33', '33', '32', '24', '32', '34', '33', '32', '34', '33', '14', '32', '33', '33', '19', '32', '32', '32', '14', '32', '8', '33', '33', '33', '32', '1', '33', '32', '32', '33', '27', '33', '11', '32', '33', '5', '32', '32', '12', '5', '11', '32', '33', '32', '32', '33', '32', '32', '45', '9', '32', '33', '32', '32', '32', '32', '32', '13', '32', '32', '5', '32', '32', '8', '7', '32', '33', '13', '49', '38', '6', '32', '33', '33', '19', '32', '32', '4', '4', '32', '32', '32', '33', '5', '33', '32', '12', '31', '32', '32', '33', '32', '38', '49', '33', '11', '32', '14', '6', '32', '33', '5', '5', '31', '32', '32', '32', '49', '32', '30', '70', '5', '33', '4', '16', '32', '32', '4', '32', '63', '6', '33', '49', '49', '5', '33', '32', '33', '33', '32', '5', '22', '5', '32', '11', '33', '32', '32', '11', '30', '33', '30', '34', '24', '21', '5', '32', '32', '32', '9', '13', '32', '48', '18', '5', '8', '7', '33', '32', '32', '32', '32', '19', '8', '32', '30', '33', '5', '32', '33', '32', '32', '32', '35', '11', '4', '32', '31', '32', '32', '32', '33', '33', '32', '10', '32', '32', '32', '1', '30', '7', '24', '33', '33', '32', '4', '33', '32', '5', '10', '27', '32', '33', '34', '32', '33', '33', '32', '32', '32', '32', '32', '32', '5', '33', '4', '32', '5', '32', '32', '7', '32', '33', '33', '32', '30', '16', '32', '5', '5', '5', '5', '5', '31', '33', '33', '4', '33', '32', '32', '5', '32', '33', '24', '31', '33', '8', '33', '32', '32', '32', '5', '32', '32', '5', '12', '41', '8', '33', '32', '32', '17', '5', '32', '32', '49', '32', '32', '4', '32', '9', '32', '33', '31', '33', '33', '31', '5', '32', '32', '4', '32', '32', '27', '32', '32', '32', '33', '32', '12', '49', '13', '32', '32', '30', '32', '5', '11', '32', '32', '3', '4', '33', '32', '58', '33', '30', '33', '49', '32', '33', '32', '16', '4', '33', '16', '33', '32', '5', '15', '33', '33', '32', '32', '35', '32', '33', '32', '34', '32', '32', '33', '10', '32', '31', '34', '33', '12', '32', '33', '27', '5', '4', '32', '32', '32', '31', '32', '33', '33', '31', '32', '33', '33', '32', '32', '6', '32', '49', '32', '6', '5', '4', '33', '15', '32', '32', '32', '5', '32', '33', '49', '32', '32', '32', '32', '33', '17', '32', '32', '4', '32', '31', '32', '37', '35', '1', '32', '12', '30', '33', '5', '32', '20', '5', '5', '32', '32', '49', '31', '32', '32', '6', '4', '32', '26', '31', '5', '5', '32', '32', '32', '33', '32', '32', '33', '30', '33', '32', '31', '32', '5', '32', '32', '32', '4', '49', '31', '32', '32', '33', '31', '32', '32', '11', '32', '49', '31', '4', '36', '5', '3', '9', '31', '12', '32', '32', '30', '4', '4', '4', '33', '49', '32', '32', '30', '4', '49', '31', '31', '33', '33', '32', '34', '32', '49', '32', '32', '5', '4', '8', '32', '32', '33', '12', '5', '32', '32', '32', '32', '32', '32', '8', '32', '32', '32', '32', '33', '2', '33', '32', '30', '33', '31', '32', '23', '30', '25', '5', '66', '36', '5', '32', '33', '31', '32', '32', '10', '33', '33', '14', '33', '33', '32', '13', '9', '18', '32', '34', '2', '32', '32', '4', '49', '5', '19', '4', '32', '33', '33', '35', '31', '22', '32', '32', '5', '30', '28', '32', '32', '32', '34', '32', '4', '6', '31', '32', '4', '32', '4', '33', '32', '33', '31', '6', '4', '32', '29', '13', '34', '32', '11', '34', '32', '8', '32', '33', '32', '49', '4', '32', '36', '33', '33', '7', '32', '32', '85', '32', '32', '33', '32', '9', '5', '4', '32', '12', '32', '32', '4', '30', '16', '32', '32', '1', '32', '33', '5', '32', '49', '33', '72', '31', '11', '5', '33', '49', '4', '31', '6', '33', '17', '33', '32', '5', '32', '32', '32', '14', '5', '26', '5', '17', '31', '4', '33', '30', '4', '32', '27', '23', '12', '32', '32', '32', '32', '32', '25', '32', '30', '32', '31', '33', '32', '32', '4', '5', '4', '33', '32', '33', '32', '32', '32', '32', '49', '31', '25', '32', '6', '33', '32', '5', '65', '8', '7', '32', '32', '32', '49', '32', '32', '6', '32', '15', '32', '11', '32', '32', '31', '32', '34', '6', '33', '32', '33', '32', '31', '15', '33', '32', '33', '32', '34', '25', '32', '32', '32', '33', '32', '50', '33', '32', '32', '49', '32', '6', '32', '5', '32', '32', '49', '32', '32', '5', '32', '4', '49', '32', '32', '33', '9', '32', '16', '33', '32', '33', '31', '4', '8', '5', '35', '5', '49', '6', '49', '32', '32', '32', '34', '32', '1', '9', '49', '32', '33', '4', '30', '49', '30', '4', '33', '32', '5', '30', '33', '11', '32', '32', '49', '4', '5', '33', '31', '5', '5', '25', '58', '32', '32', '13', '5', '31', '30', '32', '40', '12', '32', '12', '34', '33', '5', '35', '22', '25', '33', '28', '30', '5', '32', '27', '33', '33', '32', '5', '33', '5', '33', '30', '32', '9', '5', '30', '33', '48', '32', '12', '32', '32', '25', '32', '4', '32', '32', '16', '4', '5', '32', '45', '32', '5', '33', '32', '54', '14', '7', '5', '32', '4', '47', '33', '49', '5', '30', '7', '30', '5', '6', '30', '32', '5', '7', '5', '33', '32', '33', '5', '49', '30', '30', '35', '4', '8', '33', '32', '30', '8', '32', '5', '5', '32', '15', '30', '5', '32', '5', '72', '13', '10', '31', '4', '28', '20', '71', '32', '5', '19', '33', '32', '32', '7', '10', '94', '32', '32', '33', '28', '8', '34', '15', '4', '32', '1', '32', '15', '8', '32', '8', '5', '33', '34', '6', '32', '32', '12', '11', '79', '32', '32', '32', '33', '33', '18', '5', '49', '5', '33', '32', '6', '32', '13', '4', '33', '32', '4', '33', '4', '5', '73', '33', '31', '12', '13', '33', '32', '32', '33', '23', '33', '33', '33', '32', '32', '32', '33', '57', '4', '35', '6', '31', '33', '5', '30', '30', '32', '33', '6', '32', '32', '5', '8', '82', '33', '32', '34', '11', '5', '15', '33', '32', '6', '32', '5', '33', '32', '32', '32', '33', '33', '11', '28', '28', '32', '5', '35', '33', '32', '33', '32', '33', '32', '5', '32', '32', '33', '19', '32', '49', '33', '33', '32', '3', '32', '32', '34', '32', '5', '32', '32', '33', '13', '29', '35', '32', '32', '5', '29', '33', '5', '33', '32', '33', '33', '7', '32', '33', '32', '7', '32', '14', '5', '32', '32', '32', '5', '5', '5', '4', '5', '5', '5', '14', '8', '32', '33', '32', '30', '32', '33', '24', '11', '32', '4', '32', '32', '27', '32', '32', '51', '31', '33', '49', '6', '33', '12', '33', '5', '33', '8', '5', '33', '32', '30', '9', '31', '33', '32', '14', '5', '32', '32', '32', '32', '32', '49', '32', '32', '32', '21', '33', '33', '32', '32', '32', '33', '32', '33', '32', '19', '23', '33', '33', '32', '32', '32', '33', '33', '30', '32', '33', '5', '32', '4', '32', '32', '7', '33', '5', '5', '5', '30', '5', '32', '30', '12', '7', '53', '6', '32', '6', '5', '5', '48', '33', '34', '4', '33', '32', '32', '33', '8', '32', '32', '33', '32', '32', '32', '12', '32', '5', '33', '32', '33', '15', '32', '16', '32', '33', '32', '32', '32', '32', '27', '33', '32', '32', '34', '33', '32', '34', '7', '32', '33', '32', '32', '33', '48', '12', '33', '32', '33', '33', '32', '33', '4', '5', '32', '33', '32', '32', '61', '13', '32', '32', '35', '32', '35', '32', '32', '33', '85', '32', '5', '30', '32', '33', '32', '5', '33', '4', '4', '32', '5', '4', '32', '25', '34', '32', '11', '32', '33', '32', '5', '4', '32', '32', '33', '47', '33', '12', '12', '32', '32', '33', '7', '32', '32', '32', '30', '32', '32', '32', '32', '4', '32', '33', '5', '31', '8', '11', '76', '32', '6', '32', '11', '49', '5', '25', '49', '32', '11', '4', '32', '32', '32', '33', '32', '32', '71', '32', '4', '32', '32', '33', '32', '12', '32', '29', '13', '12', '5', '31', '32', '32', '34', '33', '31', '8', '33', '32', '32', '33', '33', '32', '32', '9', '12', '32', '33', '32', '46', '32', '32', '34', '32', '33', '11', '5', '32', '32', '33', '30', '32', '21', '32', '33', '33', '33', '32', '33', '14', '33', '32', '32', '33', '33', '7', '33', '32', '45', '42', '32', '51', '1', '33', '8', '32', '33', '33', '5', '33', '32', '32', '10', '33', '32', '32', '32', '32', '32', '33', '31', '5', '6', '5', '10', '32', '30', '33', '5', '32', '27', '38', '12', '5', '32', '33', '32', '32', '12', '32', '67', '34', '33', '32', '32', '32', '33', '8', '33', '33', '60', '7', '33', '32', '8', '5', '61', '32', '32', '5', '7', '32', '19', '32', '6', '32', '33', '4', '49', '34', '33', '32', '32', '31', '49', '30', '10', '11', '33', '33', '33', '32', '30', '32', '32', '11', '33', '33', '32', '49', '15', '32', '64', '12', '33', '5', '6', '5', '30', '33', '32', '33', '11', '32', '26', '34', '31', '33', '33', '49', '13', '</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atend</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>['85974001107', '85981010387', '85981010504', '85981010801', '85981011300', '85981011982', '85981012709', '85981012859', '85981012916', '85981013105', '85981013139', '85981013252', '85981014486', '85981015083', '85981015199', '85981015345', '85981015408', '85981015858', '85981018191', '85981019737', '85981019859', '85981020615', '85981021220', '85981021847', '85981021858', '85981023473', '85981024243', '85981024932', '85981025159', '85981026077', '85981026188', '85981026342', '85981029941', '85981034608', '85981035347', '85981037998', '85981038369', '85981040609', '85981041303', '85981042289', '85981046232', '85981047325', '85981047447', '85981050094', '85981050305', '85981050670', '85981050778', '85981050921', '85981051007', '85981051157', '85981051236', '85981051357', '85981051407', '85981051960', '85981052023', '85981052147', '85981052388', '85981053361', '85981053645', '85981053870', '85981054245', '85981054310', '85981054721', '85981054784', '85981055402', '85981055606', '85981055887', '85981056204', '85981056432', '85981057133', '85981057473', '85981057594', '85981057657', '85981058510', '85981058575', '85981059167', '85981060358', '85981060840', '85981060881', '85981060903', '85981060912', '85981061514', '85981062036', '85981062783', '85981062811', '85981063144', '85981063180', '85981063445', '85981063577', '85981063706', '85981063708', '85981063769', '85981064311', '85981064501', '85981064633', '85981066228', '85981066596', '85981066800', '85981067063', '85981067120', '85981067303', '85981067738', '85981068259', '85981068383', '85981068838', '85981069073', '85981069268', '85981069285', '85981069288', '85981069331', '85981069531', '85981069805', '85981070139', '85981070716', '85981070933', '85981072516', '85981074292', '85981074824', '85981077799', '85981079793', '85981080110', '85981081102', '85981081645', '85981081717', '85981081963', '85981082567', '85981082798', '85981083944', '85981083955', '85981084430', '85981085176', '85981085425', '85981086055', '85981087566', '85981090951', '85981092003', '85981094270', '85981095658', '85981096027', '85981097092', '85981097525', '85981099771', '85981099834', '85981104139', '85981105541', '85981111379', '85981111687', '85981112198', '85981112368', '85981113354', '85981116111', '85981116475', '85981117229', '85981117240', '85981117970', '85981118916', '85981119356', '85981121743', '85981121756', '85981121918', '85981122659', '85981122830', '85981124417', '85981125198', '85981125364', '85981127000', '85981127863', '85981128332', '85981128640', '85981129033', '85981130954', '85981131390', '85981132338', '85981132657', '85981132861', '85981133001', '85981136515', '85981137269', '85981137935', '85981138484', '85981139818', '85981141110', '85981141235', '85981142047', '85981142397', '85981144074', '85981144194', '85981144290', '85981144476', '85981145210', '85981145431', '85981146150', '85981147761', '85981148652', '85981149605', '85981149798', '85981149833', '85981150270', '85981152513', '85981152668', '85981152923', '85981153276', '85981154070', '85981154704', '85981154767', '85981155516', '85981155609', '85981155832', '85981157497', '85981159783', '85981160701', '85981162279', '85981163532', '85981168773', '85981169336', '85981170375', '85981170419', '85981172174', '85981172237', '85981173080', '85981173491', '85981173596', '85981174595', '85981175102', '85981175961', '85981176245', '85981176511', '85981176843', '85981176855', '85981177377', '85981177436', '85981178111', '85981180220', '85981180748', '85981181223', '85981181460', '85981184568', '85981185113', '85981185397', '85981185432', '85981186162', '85981187777', '85981187790', '85981188522', '85981190449', '85981190603', '85981190941', '85981191324', '85981191501', '85981192668', '85981193462', '85981194504', '85981195274', '85981195777', '85981196765', '85981199009', '85981200624', '85981204580', '85981205000', '85981207224', '85981210397', '85981211722', '85981211785', '85981212297', '85981212335', '85981215121', '85981215323', '85981217007', '85981217070', '85981217271', '85981217334', '85981217865', '85981217880', '85981217928', '85981219726', '85981220015', '85981220097', '85981220132', '85981221107', '85981221148', '85981222412', '85981224119', '85981224486', '85981224995', '85981225097', '85981225167', '85981226403', '85981227172', '85981227283', '85981227812', '85981228111', '85981228405', '85981228468', '85981229862', '85981229918', '85981229981', '85981230013', '85981230104', '85981233010', '85981233031', '85981233110', '85981234275', '85981235443', '85981237281', '85981238571', '85981240151', '85981240906', '85981241794', '85981243937', '85981245200', '85981245595', '85981245660', '85981246453', '85981246810', '85981247191', '85981247682', '85981247801', '85981248056', '85981248614', '85981248938', '85981249006', '85981249077', '85981249520', '85981249804', '85981250065', '85981251340', '85981252190', '85981252202', '85981252814', '85981253454', '85981256347', '85981256415', '85981256918', '85981257594', '85981257644', '85981258954', '85981259116', '85981259996', '85981260093', '85981260293', '85981261976', '85981264023', '85981265628', '85981266155', '85981266554', '85981267575', '85981268163', '85981269254', '85981270887', '85981273817', '85981276088', '85981277050', '85981277171', '85981277778', '85981277862', '85981278172', '85981278481', '85981281110', '85981281122', '85981283976', '85981284254', '85981284771', '85981284904', '85981285694', '85981285757', '85981286755', '85981287954', '85981288208', '85981288338', '85981289201', '85981290315', '85981291170', '85981291852', '85981292335', '85981292898', '85981293237', '85981296943', '85981297006', '85981297774', '85981298411', '85981298474', '85981299369', '85981300207', '85981300265', '85981301018', '85981301029', '85981301090', '85981301430', '85981302820', '85981303653', '85981304383', '85981304684', '85981304736', '85981304842', '85981305581', '85981306366', '85981307620', '85981307802', '85981308045', '85981308259', '85981308292', '85981308328', '85981308337', '85981308391', '85981310114', '85981310742', '85981311091', '85981311398', '85981312075', '85981313089', '85981313134', '85981313616', '85981313627', '85981314051', '85981314422', '85981315654', '85981316754', '85981318080', '85981323921', '85981325550', '85981327070', '85981327436', '85981327760', '85981328852', '85981330136', '85981330758', '85981331850', '85981331913', '85981332190', '85981333065', '85981333339', '85981334650', '85981334713', '85981334761', '85981335534', '85981337373', '85981338263', '85981338307', '85981342092', '85981342565', '85981343138', '85981343533', '85981344833', '85981345060', '85981347012', '85981347371', '85981348351', '85981348558', '85981349404', '85981351875', '85981352588', '85981352826', '85981353374', '85981353997', '85981354648', '85981355846', '85981357814', '85981359310', '85981360852', '85981361507', '85981361779', '85981362003', '85981362066', '85981363777', '85981365886', '85981366880', '85981367170', '85981368633', '85981370043', '85981370894', '85981371153', '85981371868', '85981372645', '85981374219', '85981375527', '85981375801', '85981375825', '85981376079', '85981377391', '85981378159', '85981378792', '85981378905', '85981379505', '85981379662', '85981380597', '85981380924', '85981381707', '85981381999', '85981383237', '85981383353', '85981384426', '85981385151', '85981385624', '85981385673', '85981385841', '85981386704', '85981386821', '85981387227', '85981387362', '85981388619', '85981391330', '85981391423', '85981391880', '85981392100', '85981392565', '85981395635', '85981395687', '85981395818', '85981397246', '85981397372', '85981397409', '85981397411', '85981398764', '85981400369', '85981401399', '85981401626', '85981401752', '85981402041', '85981402081', '85981402748', '85981402997', '85981403093', '85981403964', '85981404116', '85981404174', '85981404374', '85981404793', '85981405917', '85981408267', '85981409242', '85981409843', '85981411024', '85981411624', '85981411687', '85981413039', '85981413532', '85981413653', '85981413838', '85981413892', '85981414546', '85981415469', '85981416386', '85981416409', '85981418850', '85981419344', '85981420019', '85981421525', '85981421738', '85981422245', '85981422308', '85981422576', '85981422856', '85981423490', '85981423505', '85981423933', '85981424271', '85981424607', '85981425703', '85981426537', '85981426942', '85981427253', '85981428860', '85981428912', '85981432332', '85981433880', '85981436330', '85981437233', '85981437797', '85981440921', '85981442203', '85981443375', '85981444452', '85981444515', '85981445843', '85981447674', '85981448037', '85981452309', '85981453385', '85981460147', '85981460175', '85981460392', '85981460457', '85981460646', '85981460699', '85981460861', '85981460924', '85981460996', '85981461065', '85981461106', '85981461610', '85981462406', '85981463746', '85981463860', '85981464262', '85981464411', '85981464530', '85981464545', '85981465735', '85981465772', '85981465798', '85981466545', '85981467570', '85981468790', '85981470659', '85981470831', '85981471492', '85981471759', '85981472233', '85981473750', '85981474263', '85981474389', '85981474696', '85981474697', '85981474756', '85981474760', '85981474778', '85981474912', '85981474923', '85981475220', '85981475230', '85981475761', '85981475972', '85981475980', '85981476043', '85981476212', '85981476638', '85981477326', '85981477413', '85981477799', '85981477812', '85981477813', '85981477916', '85981478494', '85981478784', '85981479493', '85981479515', '85981479752', '85981479774', '85981481053', '85981481331', '85981481726', '85981482109', '85981482140', '85981482476', '85981482990', '85981483810', '85981484967', '85981485284', '85981485480', '85981486380', '85981486397', '85981487878', '85981488161', '85981488741', '85981489506', '85981489546', '85981489609', '85981489986', '85981491380', '85981491428', '85981491439', '85981492666', '85981492729', '85981495205', '85981495268', '85981495465', '85981495615', '85981495911', '85981495935', '85981496025', '85981496943', '85981497099', '85981497122', '85981497496', '85981497614', '85981499186', '85981500414', '85981500847', '85981500940', '85981501090', '85981501968', '85981502098', '85981502241', '85981505500', '85981505522', '85981505531', '85981505586', '85981505887', '85981506224', '85981506332', '85981506467', '85981506955', '85981507053', '85981507770', '85981507930', '85981509140', '85981509349', '85981509981', '85981510677', '85981511295', '85981512929', '85981514081', '85981514747', '85981518467', '85981518484', '85981520304', '85981521334', '85981521816', '85981521879', '85981521962', '85981522121', '85981522321', '85981522480', '85981522523', '85981522914', '85981522917', '85981522933', '85981522980', '85981523042', '85981523247', '85981523548', '85981523703', '85981523830', '85981523864', '85981524209', '85981524336', '85981524345', '85981524388', '85981524433', '85981524474', '85981525329', '85981525392', '85981525946', '85981525956', '85981525970', '85981526066', '85981526142', '85981526377', '85981526414', '85981526660', '85981526890', '85981526953', '85981527026', '85981527241', '85981527738', '85981527876', '85981527926', '85981528100', '85981528344', '85981528523', '85981529250', '85981530016', '85981530202', '85981530228', '85981530264', '85981530358', '85981530695', '85981531466', '85981532323', '85981532367', '85981532706', '85981533140', '85981533536', '85981533817', '85981533861', '85981533924', '85981534836', '85981535019', '85981535381', '85981535444', '85981535702', '85981536001', '85981536037', '85981536784', '85981537054', '85981537071', '85981537451', '85981537531', '85981537646', '85981538008', '85981538403', '85981538473', '85981539100', '85981539364', '85981539374', '85981539613', '85981539674', '85981539710', '85981539904', '85981542565', '85981544220', '85981544377', '85981544415', '85981544420', '85981544535', '85981544744', '85981545730', '85981545967', '85981546135', '85981546201', '85981546486', '85981546524', '85981547100', '85981547151', '85981547181', '85981548573', '85981548663', '85981549807', '85981550607', '85981551701', '85981552786', '85981552815', '85981553207', '85981553257', '85981553774', '85981554041', '85981554682', '85981555448', '85981556360', '85981556386', '85981556391', '85981556708', '85981557599', '85981557763', '85981557766', '85981557996', '85981558443', '85981558444', '85981558593', '85981558734', '85981558921', '85981559352', '85981559880', '85981559990', '85981561122', '85981561397', '85981563114', '85981563918', '85981565385', '85981566296', '85981569388', '85981570332', '85981570553', '85981571936', '85981571948', '85981573149', '85981574029', '85981574749', '85981574828', '85981575288', '85981576121', '85981577685', '85981579715', '85981580747', '85981582223', '85981587265', '85981588881', '85981589028', '85981590283', '85981590581', '85981591212', '85981591394', '85981592814', '85981594445', '85981594455', '85981598314', '85981599091', '85981599720', '85981600032', '85981600288', '85981600746', '85981601467', '85981601515', '85981601621', '85981603545', '85981603701', '85981603764', '85981603922', '85981604044', '85981604097', '85981604901', '85981605888', '85981606241', '85981606453', '85981606516', '85981606875', '85981607061', '85981607171', '85981607847', '85981608039', '85981608131', '85981608656', '85981608885', '85981609224', '85981609765', '85981611504', '85981611687', '85981612354', '85981612497', '85981613707', '85981614805', '85981615721', '85981615726', '85981616672', '85981617048', '85981617443', '85981617809', '85981618157', '85981618463', '85981618696', '85981619089', '85981621012', '85981625207', '85981625719', '85981625789', '85981625797', '85981626292', '85981626455', '85981627178', '85981627515', '85981627750', '85981628353', '85981628962', '85981629450', '85981630101', '85981630164', '85981631945', '85981632116', '85981635515', '85981635650', '85981636098', '85981636649', '85981638200', '85981638739', '85981639201', '85981642110', '85981642480', '85981645543', '85981646909', '85981647853', '85981649485', '85981651235', '85981651813', '85981651856', '85981653359', '85981654096', '85981655420', '85981655504', '85981656015', '85981656761', '85981663973', '85981664051', '85981665088', '85981665658', '85981665867', '85981666220', '85981666585', '85981666685', '85981668986', '85981669316', '85981669696', '85981669892', '85981670050', '85981670209', '85981670557', '85981671233', '85981672007', '85981672198', '85981672687', '85981676600', '85981677013', '85981677923', '85981677986', '85981679022', '85981679393', '85981684827', '85981685253', '85981687262', '85981688088', '85981688530', '85981689614', '85981690885', '85981692225', '85981693076', '85981694698', '85981696440', '85981700371', '85981701616', '85981701789', '85981702211', '85981704587', '85981705823', '85981706117', '85981706812', '85981707565', '85981709424', '85981709639', '85981709959', '85981709997', '85981711415', '85981712700', '85981715589', '85981717124', '85981721330', '85981721470', '85981723162', '85981723682', '85981727178', '85981727333', '85981730276', '85981731368', '85981733009', '85981733173', '85981734225', '85981735351', '85981735457', '85981738337', '85981742689', '85981745007', '85981746191', '85981746231', '85981747230', '85981747684', '85981747880', '85981748018', '85981749098', '85981749311', '85981780097', '85981780698', '85981781860', '85981781956', '85981782615', '85981783993', '85981787014', '85981787375', '85981787694', '85981787878', '85981795562', '85981797415', '85981799011', '85981799243', '85981799393', '85981799969', '85981800644', '85981801187', '85981801628', '85981801718', '85981801761', '85981802537', '85981802631', '85981803848', '85981804731', '85981805074', '85981805578', '85981805682', '85981805712', '85981805995', '85981806062', '85981806192', '85981806838', '85981807096', '85981807746', '85981808109', '85981808226', '85981808940', '85981809310', '85981809579', '85981810401', '85981811681', '85981812231', '85981812420', '85981813215', '85981813326', '85981813696', '85981813745', '85981814222', '85981815518', '85981815719', '85981815951', '85981815995', '85981816185', '85981816597', '85981816953', '85981817644', '85981819191', '85981819878', '85981819898', '85981819971', '85981820302', '85981820909', '85981822288', '85981822627', '85981823737', '85981824050', '85981825667', '85981827171', '85981827298', '85981828133', '85981829674', '85981829888', '85981830615', '85981831333', '85981831807', '85981832616', '85981833911', '85981836027', '85981836192', '85981838197', '85981839905', '85981840699', '85981840997', '85981841498', '85981842018', '85981842026', '85981847568', '85981849140', '85981849448', '85981850329', '85981851336', '85981851657', '85981851806', '85981852483', '85981852871', '85981853361', '85981853473', '85981853498', '85981854188', '85981854400', '85981854701', '85981854966', '85981855387', '85981855943', '85981857602', '85981858378', '85981858585', '85981859714', '85981859843', '85981860190', '85981860939', '85981861386', '85981861390', '85981862200', '85981862732', '85981862812', '85981863520', '85981863917', '85981864665', '85981866872', '85981867198', '85981867874', '85981868706', '85981869078', '85981869877', '85981870279', '85981870625', '85981870769', '85981871433', '85981871482', '85981871725', '85981872527', '85981873853', '85981874873', '85981875089', '85981875839', '85981876038', '85981876387', '85981877277', '85981877340', '85981877666', '85981878608', '85981879558', '85981879727', '85981881447', '85981881564', '85981881903', '85981882019', '85981882233', '85981883888', '85981885848', '85981886408', '85981888076', '85981890073', '85981890692', '85981890804', '85981890897', '85981891321', '85981891476', '85981892737', '85981892922', '85981893512', '85981894559', '85981895421', '85981895778', '85981895877', '85981899243', '85981900080', '85981900730', '85981901391', '85981904698', '85981905011', '85981905074', '85981905075', '85981906452', '85981910262', '85981910771', '85981911604', '85981911984', '85981914747', '85981917082', '85981917653', '85981917936', '85981918090', '85981918203', '85981921936', '85981921999', '85981922555', '85981924869', '85981926087', '85981926161', '85981927362', '85981928269', '85981930502', '85981933090', '85981933446', '85981934488', '85981937771', '85981942675', '85981944086', '85981946447', '85981947455', '85981948504', '85981948560', '85981948709', '85981949370', '85981949405', '85981950680', '85981951197', '85981951207', '85981951277', '85981951294', '85981951433', '85981952223', '85981952606', '85981953266', '85981955156', '85981955666', '85981956683', '85981956798', '85981956914', '85981956977', '85981958219', '85981958833', '85981959454', '85981962203', '85981963748', '85981964770', '85981966391', '85981966744', '85981967093', '85981967347', '85981967672', '85981972215', '85981973787', '85981973850', '85981974619', '85981975003', '85981975335', '85981975643', '85981978964', '85981982384', '85981982415', '85981983536', '85981984160', '85981984196', '85981984205', '85981985320', '85981987749', '85981990206', '85981991814', '85981992200', '85981992221', '85981993841', '85981994171', '85981994544', '85981996677', '85981996968', '85981997233', '85981998183', '85981998880', '85981999101', '85981999393', '85982000080', '85982000103', '85982000124', '85982000407', '85982000597', '85982001158', '85982001480', '85982001603', '85982002244', '85982003360', '85982009691', '85982012352', '85982013350', '85982013725', '85982014410', '85982014728', '85982014859', '85982015963', '85982016650', '85982018181', '85982019178', '85982020684', '85982020732', '85982021675', '85982021901', '85982021970', '85982022116', '85982022707', '85982023008', '85982023198', '85982023449', '85982024092', '85982024412', '85982024556', '85982025193', '85982025465', '85982025505', '85982026115', '85982026559', '85982026582', '85982026618', '85982026681', '85982026958', '85982027257', '85982027456', '85982028016', '85982028614', '85982028717', '85982029544', '85982029630', '85982029656', '85982031994', '85982033246', '85982036215', '85982038136', '85982038199', '85982038964', '85982041982', '85982048028', '85982048400', '85982048768', '85982049005', '85982050430', '85982051850', '85982052170', '85982052833', '85982053074', '85982058486', '85982059867', '85982060243', '85982061188', '85982061715', '85982065404', '85982066323', '85982066720', '85982067095', '85982067924', '85982069921', '85982070325', '85982070442', '85982070505', '85982070537', '85982075392', '85982076079', '85982077220', '85982080055', '85982080963', '85982081863', '85982082408', '85982082685', '85982086204', '85982086988', '85982088181', '85982088401', '85982090444', '85982092229', '85982092410', '85982092535', '85982095933', '85982096408', '85982096638', '85982096702', '85982098898', '85982099596', '85982101224', '85982102764', '85982103459', '85982103837', '85982104191', '85982105219', '85982105253', '85982105588', '85982106049', '85982107612', '85982108435', '85982108824', '85982108871', '85982108995', '85982109939', '85982110388', '85982110918', '85982111162', '85982111405', '85982111461', '85982111682', '85982111714', '85982112134', '85982112150', '85982112252', '85982112330', '85982112561', '85982112835', '85982113153', '85982113424', '85982113947', '85982114041', '85982114590', '85982114798', '85982115352', '85982115530', '85982116277', '85982116934', '85982116997', '85982118281', '85982118296', '85982118359', '85982118717', '85982119038', '85982119077', '85982120196', '85982120770', '85982121018', '85982121624', '85982122300', '85982122468', '85982123793', '85982123880', '85982125254', '85982126275', '85982127512', '85982130408', '85982130446', '85982131720', '85982132411', '85982132443', '85982132450', '85982133520', '85982134594', '85982134658', '85982140032', '85982141654', '85982144572', '85982145647', '85982145648', '85982147385', '85982147517', '85982148150', '85982148935', '85982150345', '85982154109', '85982154431', '85982154497', '85982155595', '85982155633', '85982161243', '85982161749', '85982162384', '85982162735', '85982163153', '85982164038', '85982166162', '85982166295', '85982166369', '85982170184', '85982171502', '85982171541', '85982171985', '85982184521', '85982185872', '85982190343', '85982204545', '85982205828', '85982207580', '85982217764', '85982222262', '85982223649', '85982225298', '85982234415', '85982243000', '85982254767', '85982254833', '85984000187', '85984000206', '85984000276', '85984000283', '85984000366', '85984000374', '85984000408', '85984000419', '85984000570', '85984000752', '85984000901', '85984000924', '85984001030', '85984001034', '85984001146', '85984001200', '85984001263', '85984001399', '85984001670', '85984001714', '85984001904', '85984002329', '85984002699', '85984004021', '85984004143', '85984004381', '85984004513', '85984004885', '85984004934', '85984004937', '85984005030', '85984005089', '85984005191', '85984005207', '85984005486', '85984005676', '85984005684', '85984005854', '85984006088', '85984006430', '85984006519', '85984006807', '85984006822', '85984006945', '85984007418', '85984007839', '85984007934', '85984008090', '85984008165', '85984008494', '85984008541', '85984008711', '85984008837', '85984008876', '85984009118', '85984009152', '85984010102', '85984010119', '85984010346', '85984010352', '85984010376', '85984010523', '85984010651', '85984010721', '85984010796', '85984011030', '85984011127', '85984011205', '85984011272', '85984011345', '85984011423', '85984012202', '85984012591', '85984012893', '85984013559', '85984013847', '85984013900', '85984013932', '85984013963', '85984014210', '85984014231', '85984014288', '85984014376', '85984014432', '85984014547', '85984015074', '85984015099', '85984015349', '85984015384', '85984015385', '85984015469', '85984015572', '85984015631', '85984015661', '85984015695', '85984015758', '85984015793', '85984015918', '85984015943', '85984015948', '85984016599', '85984016848', '85984017946', '85984018354', '85984019606', '85984019846', '85984019986', '85984020049', '85984020051', '85984020177', '85984020235', '85984020417', '85984020826', '85984020911', '85984021324', '85984021461', '85984021871', '85984022102', '85984022241', '85984022389', '85984022437', '85984022645', '85984023016', '85984023231', '85984023332', '85984023361', '85984023534', '85984024023', '85984024057', '85984024750', '85984024773', '85984024790', '85984024966', '85984025156', '85984025366', '85984025761', '85984026229', '85984026355', '85984026707', '85984026882', '85984026909', '85984026937', '85984027014', '85984027778', '85984027803', '85984027980', '85984028311', '85984028478', '85984028528', '85984028635', '85984028807', '85984029384', '85984029403', '85984029645', '85984029647', '85984029806', '85984029997', '85984030002', '85984030015', '85984030126', '85984030128', '85984030255', '85984030534', '85984030799', '85984030914', '85984031018', '85984031134', '85984031235', '85984031240', '85984031369', '85984031377', '85984031387', '85984031438', '85984031757', '85984031799', '85984031859', '85984031951', '85984031983', '85984031996', '85984032024', '85984032030', '85984032046', '85984032152', '85984032209', '85984032278', '85984032838', '85984032911', '85984033253', '85984033308', '85984033709', '85984033733', '85984033741', '85984033796', '85984033825', '85984033893', '85984033983', '85984034114', '85984034385', '85984034577', '85984034588', '85984034633', '85984034782', '85984034964', '85984035081', '85984035134', '85984035188', '85984035416', '85984035423', '85984035459', '85984035494', '85984035559', '85984035765', '85984036032', '85984036315', '85984036485', '85984036570', '85984036614', '85984036676', '85984036734', '85984036808', '85984036872', '85984037291', '85984037296', '85984037302', '85984037313', '85984037354', '85984037682', '85984037921', '85984037935', '85984037947', '85984038033', '85984038229', '85984038524', '85984038538', '85984038620', '85984038850', '85984038856', '85984039320', '85984039429', '85984039451', '85984039728', '85984040449', '85984040502', '85984040554', '85984040731', '85984040757', '85984040783', '85984040792', '85984040899', '85984041029', '85984041044', '85984041297', '85984041417', '85984041458', '85984041670', '85984041713', '85984041805', '85984041914', '85984041986', '85984042380', '85984042425', '85984042497', '85984042509', '85984042623', '85984042895', '85984042963', '85984043070', '85984043137', '85984043296', '85984043323', '85984043326', '85984043413', '85984043751', '85984044012', '85984044067', '85984044191', '85984044248', '85984044283', '85984044300', '85984044346', '85984044633', '85984044683', '85984044763', '85984044963', '85984045050', '85984045056', '85984045115', '85984045640', '85984045722', '85984046240', '85984046424', '85984046625', '85984046753', '85984046806', '85984046807', '85984046867', '85984047111', '85984047230', '85984047233', '85984047367', '85984047472', '85984047476', '85984047517', '85984047596', '85984048175', '85984048182', '85984048183', '85984048283', '85984048339', '85984048508', '85984048524', '85984048559', '85984048759', '85984048849', '85984049026', '85984049029', '85984049263', '85984049442', '85984049451', '85984049504', '85984049679', '85984049735', '85984049763', '85984049858', '85984049949', '85984050227', '85984050228', '85984050250', '85984050371', '85984050677', '85984050801', '85984050882', '85984050887', '85984050928', '85984051292', '85984051333', '85984051412', '85984051489', '85984051523', '85984051742', '85984051769', '85984051840', '85984051889', '85984051935', '85984052109', '85984052112', '85984052208', '85984052217', '85984052263', '85984052298', '85984052611', '85984052730', '85984052764', '85984052843', '85984053038', '85984053174', '85984053179', '85984053330', '85984053556', '85984053869', '85984053880', '85984053887', '85984053943', '85984053956', '85984054025', '85984054056', '85984054133', '85984054160', '85984054172', '85984054228', '85984054266', '85984054556', '85984054674', '85984054734', '85984054739', '85984054879', '85984054912', '85984055156', '85984055310', '85984055345', '85984055442', '85984055473', '85984055502', '85984055688', '85984055714', '85984055899', '85984055933', '85984056265', '85984056517', '85984056826', '85984056911', '85984056971', '85984057268', '85984057361', '85984057589', '85984057713', '85984057802', '85984057880', '85984058809', '85984059297', '85984059565', '85984059708', '85984060013', '85984060654', '85984060832', '85984061103', '85984061137', '85984061447', '85984061486', '85984061543', '85984061639', '85984061962', '85984062029', '85984062279', '85984062320', '85984062358', '85984062494', '85984062505', '85984062530', '85984063166', '85984063203', '85984063719', '85984063744', '85984063839', '85984064263', '85984064393', '85984064541', '85984064961', '85984065160', '85984065816', '85984066050', '85984066966', '85984067046', '85984067756', '85984067873', '85984068456', '85984069092', '85984069667', '85984069722', '85984069938', '85984070019', '85984070211', '85984070265', '85984070421', '85984070652', '85984070895', '85984071052', '85984071611', '85984071870', '85984072029', '85984072045', '85984072051', '85984072058', '85984072071', '85984072145', '85984072225', '85984072316', '85984072445', '85984072480', '85984072653', '85984072933', '85984073162', '85984073973', '85984074264', '85984074313', '85984074778', '85984075096', '85984075666', '85984076005', '85984076212', '85984076393', '85984076578', '85984076839', '85984076847', '85984077031', '85984077361', '85984077370', '85984077740', '85984077801', '85984078005', '85984078034', '85984078218', '85984078233', '85984078314', '85984078445', '85984078614', '85984079116', '85984079245', '85984079370', '85984079725', '85984079880', '85984079915', '85984080469', '85984080471', '85984080593', '85984080601', '85984081278', '85984081475', '85984081680', '85984082025', '85984082125', '85984082555', '85984082670', '85984082940', '85984082979', '85984083419', '85984083846', '85984084306', '85984084464', '85984084549', '85984084550', '85984084823', '85984084857', '85984085018', '85984085176', '85984085262', '85984085880', '85984086976', '85984087409', '85984088006', '85984088529', '85984089052', '85984089070', '85984089220', '85984089798', '85984090380', '85984090552', '85984090594', '85984090882', '85984090929', '85984091124', '85984091289', '85984091406', '85984091518', '85984092054', '85984092195', '85984092230', '85984092539', '85984093168', '85984093610', '85984093759', '85984093855', '85984094073', '85984094849', '85984095284', '85984096033', '85984098963', '85984099235', '85984099245', '85984099377', '85984099885', '85984100300', '85984100698', '85984100822', '85984101624', '85984101697', '85984102042', '85984102155', '85984102262', '85984102480', '85984102514', '85984102560', '85984102571', '85984103927', '85984104957', '85984105301', '85984105524', '85984106425', '85984107192', '85984107381', '85984107762', '85984108029', '85984108520', '85984108531', '85984108645', '85984108950', '85984109045', '85984109435', '85984109534', '85984110121', '85984110186', '85984110449', '85984110493', '85984110570', '85984110730', '85984110811', '85984111215', '85984111369', '85984111609', '85984111626', '85984111796', '85984111877', '85984111930', '85984112126', '85984112139', '85984112386', '85984112657', '85984113012', '85984113687', '85984113734', '85984113870', '85984113916', '85984114001', '85984114121', '85984114826', '85984114827', '85984115475', '85984115569', '85984115651', '85984116121', '85984116540', '85984116596', '85984116734', '85984116933', '85984117008', '85984117204', '85984117429', '85984117798', '85984118037', '85984118042', '85984118203', '85984118581', '85984118664', '85984118708', '85984118774', '85984119107', '85984119481', '85984119572', '85984119808', '85984120393', '85984120682', '85984121272', '85984122145', '85984122414', '85984123034', '85984123448', '85984124093', '85984124208', '85984125015', '85984125036', '85984126078', '85984126186', '85984126390', '85984126584', '85984126778', '85984126955', '85984127219', '85984127242', '85984127734', '85984128627', '85984128634', '85984128869', '85984128924', '85984129311', '85984129612', '85984130038', '85984130659', '85984130724', '85984130979', '85984131046', '85984131139', '85984131313', '85984131574', '85984131761', '85984131881', '85984132127', '85984132128', '85984132149', '85984132782', '85984132844', '85984133084', '85984133130', '85984133206', '85984133331', '85984133448', '85984133534', '85984134089', '85984134736', '85984135015', '85984135302', '85984135420', '85984135573', '85984</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['10', '27', '27', '27', '46', '30', '27', '1', '5', '29', '1', '35', '16', '43', '27', '27', '27', '11', '5', '28', '1', '49', '27', '27', '1', '27', '0', '27', '11', '1', '28', '10', '3', '27', '3', '28', '27', '31', '1', '25', '1', '27', '27', '40', '27', '27', '28', '27', '27', '12', '28', '5', '7', '6', '28', '40', '49', '1', '2', '8', '78', '1', '1', '27', '5', '27', '1', '27', '27', '11', '1', '28', '12', '27', '27', '1', '5', '27', '27', '2', '27', '27', '27', '25', '7', '27', '28', '1', '11', '27', '1', '1', '27', '21', '13', '6', '27', '5', '1', '0', '28', '27', '28', '27', '27', '27', '27', '27', '27', '7', '28', '5', '5', '27', '27', '47', '28', '27', '34', '1', '35', '5', '8', '12', '28', '27', '12', '49', '28', '27', '6', '27', '1', '1', '17', '5', '27', '1', '1', '28', '31', '1', '27', '12', '5', '27', '39', '49', '19', '16', '28', '27', '5', '27', '8', '27', '4', '35', '8', '30', '35', '1', '27', '27', '10', '40', '1', '27', '27', '49', '27', '29', '27', '27', '1', '28', '43', '32', '45', '30', '27', '27', '6', '27', '5', '2', '27', '7', '49', '13', '28', '6', '27', '27', '27', '27', '26', '27', '27', '27', '28', '49', '1', '27', '11', '28', '27', '27', '27', '27', '1', '18', '28', '27', '27', '27', '1', '27', '1', '49', '10', '27', '5', '49', '1', '11', '27', '49', '27', '27', '5', '49', '27', '7', '5', '28', '1', '29', '27', '11', '31', '38', '27', '15', '27', '27', '49', '17', '41', '8', '27', '1', '28', '30', '28', '3', '27', '30', '30', '5', '27', '10', '1', '49', '27', '28', '1', '27', '4', '1', '28', '5', '27', '27', '12', '28', '10', '27', '27', '48', '1', '1', '1', '27', '30', '1', '27', '27', '27', '29', '27', '5', '27', '27', '6', '1', '30', '27', '28', '1', '12', '5', '29', '25', '27', '49', '27', '27', '6', '11', '27', '27', '27', '27', '11', '27', '1', '27', '27', '27', '27', '27', '30', '27', '49', '28', '28', '23', '40', '27', '28', '27', '27', '27', '5', '11', '27', '27', '1', '5', '11', '28', '27', '27', '27', '28', '9', '5', '27', '11', '27', '1', '35', '1', '27', '1', '27', '27', '1', '30', '27', '27', '28', '17', '27', '27', '1', '27', '35', '49', '27', '49', '27', '27', '11', '27', '12', '27', '27', '8', '4', '49', '11', '27', '35', '4', '28', '27', '27', '27', '5', '18', '1', '5', '27', '27', '1', '28', '27', '1', '1', '11', '1', '1', '28', '114', '9', '27', '27', '5', '28', '27', '27', '1', '23', '27', '27', '5', '1', '27', '1', '5', '27', '27', '27', '27', '87', '27', '28', '31', '39', '34', '27', '27', '27', '9', '13', '9', '1', '17', '27', '35', '27', '30', '12', '27', '27', '49', '6', '27', '27', '27', '1', '28', '1', '30', '27', '27', '27', '12', '27', '27', '27', '1', '28', '0', '27', '49', '27', '27', '1', '28', '27', '27', '49', '27', '27', '27', '49', '27', '27', '6', '49', '1', '27', '9', '1', '28', '42', '13', '31', '27', '15', '8', '49', '27', '5', '27', '8', '27', '29', '27', '27', '49', '27', '14', '27', '28', '27', '27', '49', '29', '11', '27', '27', '12', '27', '27', '27', '27', '27', '1', '27', '5', '22', '1', '27', '27', '49', '17', '29', '11', '27', '27', '5', '13', '1', '10', '27', '28', '27', '27', '27', '27', '27', '5', '24', '27', '1', '1', '27', '1', '30', '27', '27', '27', '1', '14', '19', '25', '27', '27', '27', '27', '49', '27', '30', '11', '30', '5', '27', '27', '1', '27', '28', '27', '1', '29', '27', '27', '1', '5', '1', '37', '49', '1', '5', '2', '82', '5', '27', '27', '30', '8', '27', '5', '27', '27', '27', '28', '49', '27', '27', '27', '27', '28', '5', '27', '27', '1', '27', '14', '5', '49', '31', '1', '27', '1', '27', '5', '27', '27', '27', '28', '1', '12', '40', '27', '43', '27', '27', '1', '27', '49', '49', '21', '27', '27', '22', '27', '7', '12', '27', '27', '0', '1', '27', '27', '27', '28', '1', '7', '28', '49', '27', '27', '27', '7', '28', '16', '1', '1', '27', '12', '10', '12', '27', '27', '4', '27', '27', '30', '5', '12', '29', '27', '27', '17', '27', '27', '13', '5', '27', '12', '16', '49', '27', '1', '27', '6', '49', '29', '27', '28', '18', '28', '49', '27', '27', '27', '30', '27', '7', '23', '49', '12', '16', '27', '1', '5', '1', '27', '27', '27', '27', '27', '27', '27', '49', '27', '28', '27', '1', '27', '27', '27', '27', '27', '49', '21', '27', '28', '27', '27', '28', '35', '27', '49', '1', '27', '27', '26', '27', '38', '27', '1', '6', '27', '27', '28', '7', '28', '27', '27', '27', '27', '12', '5', '6', '27', '18', '28', '17', '27', '27', '28', '23', '14', '27', '12', '29', '28', '28', '27', '27', '27', '27', '28', '28', '49', '5', '27', '12', '27', '27', '27', '49', '27', '27', '12', '8', '27', '28', '28', '1', '9', '28', '27', '27', '27', '1', '1', '10', '1', '28', '27', '12', '1', '7', '27', '27', '27', '27', '28', '27', '27', '27', '5', '27', '12', '46', '27', '27', '31', '35', '17', '28', '27', '20', '24', '23', '1', '41', '36', '49', '49', '7', '28', '49', '27', '27', '5', '5', '27', '1', '5', '17', '27', '28', '13', '7', '49', '28', '27', '27', '27', '1', '34', '42', '35', '27', '28', '28', '28', '35', '11', '27', '5', '5', '28', '28', '27', '28', '1', '28', '13', '27', '28', '27', '28', '30', '28', '28', '18', '27', '5', '1', '76', '28', '28', '1', '5', '1', '28', '26', '2', '28', '1', '7', '12', '28', '37', '11', '28', '27', '27', '27', '27', '28', '28', '27', '20', '8', '30', '14', '27', '4', '10', '4', '49', '28', '28', '1', '1', '22', '27', '1', '10', '28', '11', '28', '77', '28', '2', '27', '30', '27', '27', '31', '1', '28', '28', '12', '27', '28', '10', '30', '27', '9', '27', '18', '28', '0', '12', '28', '49', '27', '27', '27', '27', '30', '1', '28', '27', '50', '31', '1', '27', '1', '27', '28', '28', '28', '27', '7', '1', '28', '27', '1', '27', '31', '28', '27', '1', '28', '1', '49', '49', '27', '28', '27', '27', '1', '27', '28', '27', '5', '26', '12', '1', '28', '2', '8', '13', '1', '12', '1', '28', '27', '1', '30', '7', '7', '37', '27', '28', '8', '5', '27', '28', '27', '27', '13', '13', '27', '30', '13', '13', '27', '1', '28', '27', '28', '27', '31', '27', '13', '28', '27', '27', '28', '12', '27', '27', '7', '1', '29', '27', '27', '1', '5', '27', '13', '27', '28', '49', '27', '6', '28', '27', '1', '27', '27', '21', '28', '31', '46', '27', '28', '5', '5', '27', '27', '30', '7', '27', '28', '28', '28', '30', '9', '17', '1', '3', '30', '7', '27', '28', '27', '7', '37', '27', '14', '13', '28', '27', '27', '27', '1', '27', '27', '27', '27', '28', '6', '28', '27', '12', '27', '47', '49', '28', '28', '27', '27', '13', '14', '28', '12', '28', '7', '27', '28', '27', '27', '1', '1', '27', '14', '0', '1', '27', '1', '1', '31', '1', '5', '39', '35', '27', '28', '11', '30', '27', '1', '27', '49', '27', '28', '28', '27', '47', '27', '28', '28', '5', '28', '30', '11', '49', '27', '28', '1', '28', '28', '28', '27', '49', '30', '27', '28', '30', '27', '15', '49', '8', '28', '12', '27', '17', '28', '27', '30', '49', '1', '28', '28', '27', '27', '27', '49', '1', '26', '1', '27', '49', '1', '6', '27', '5', '28', '1', '27', '11', '16', '28', '114', '27', '27', '27', '34', '1', '6', '28', '49', '21', '27', '27', '27', '28', '10', '1', '27', '27', '27', '49', '1', '28', '28', '27', '31', '28', '28', '28', '49', '49', '27', '27', '27', '8', '28', '1', '11', '5', '1', '1', '27', '32', '49', '27', '9', '33', '27', '5', '28', '27', '31', '28', '27', '27', '27', '27', '27', '39', '30', '12', '13', '28', '34', '1', '27', '27', '28', '28', '15', '11', '27', '28', '1', '27', '1', '35', '27', '7', '17', '1', '35', '23', '27', '28', '1', '5', '28', '2', '21', '27', '28', '28', '28', '11', '49', '32', '28', '14', '14', '30', '27', '1', '28', '28', '28', '23', '1', '27', '27', '27', '28', '47', '27', '28', '1', '27', '27', '28', '42', '49', '27', '27', '5', '28', '27', '1', '28', '27', '26', '27', '27', '28', '28', '8', '5', '0', '49', '28', '28', '5', '28', '27', '28', '28', '41', '8', '27', '27', '27', '6', '27', '27', '27', '6', '1', '28', '30', '5', '27', '12', '2', '5', '28', '15', '5', '27', '28', '27', '12', '28', '28', '5', '27', '12', '28', '27', '27', '6', '1', '30', '28', '27', '28', '12', '27', '13', '1', '49', '31', '27', '12', '28', '27', '28', '27', '33', '27', '40', '27', '28', '28', '27', '0', '20', '27', '1', '43', '28', '28', '1', '49', '33', '27', '10', '28', '27', '28', '27', '27', '2', '27', '27', '49', '1', '28', '28', '43', '27', '27', '28', '49', '5', '28', '146', '10', '18', '28', '27', '27', '27', '28', '27', '28', '28', '28', '11', '1', '5', '6', '27', '8', '5', '9', '28', '1', '27', '28', '18', '27', '6', '6', '26', '27', '7', '27', '49', '8', '27', '75', '21', '58', '27', '27', '21', '27', '21', '6', '27', '29', '27', '27', '62', '69', '65', '17', '27', '49', '8', '27', '8', '5', '27', '1', '30', '1', '27', '32', '32', '49', '5', '5', '4', '13', '32', '33', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '32', '5', '4', '5', '32', '4', '3', '4', '4', '4', '5', '35', '33', '4', '5', '5', '5', '4', '30', '32', '5', '4', '5', '19', '5', '5', '4', '5', '5', '5', '5', '5', '4', '4', '5', '5', '5', '32', '32', '39', '4', '4', '4', '34', '5', '33', '34', '49', '4', '5', '4', '5', '3', '77', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '5', '6', '5', '5', '4', '4', '5', '4', '5', '4', '4', '32', '5', '51', '4', '32', '4', '33', '4', '4', '5', '12', '32', '4', '4', '32', '5', '5', '4', '5', '4', '3', '4', '5', '4', '5', '6', '4', '5', '32', '4', '4', '4', '5', '4', '5', '5', '5', '2', '5', '6', '4', '49', '5', '4', '32', '5', '32', '5', '5', '5', '39', '49', '33', '33', '4', '4', '5', '5', '5', '4', '5', '5', '4', '33', '32', '32', '32', '32', '33', '5', '32', '32', '32', '33', '44', '20', '14', '33', '6', '32', '12', '49', '32', '32', '49', '33', '34', '5', '32', '32', '32', '32', '4', '32', '32', '5', '6', '42', '33', '35', '32', '31', '31', '5', '32', '49', '32', '4', '27', '11', '32', '4', '69', '32', '6', '32', '34', '5', '32', '49', '32', '21', '32', '32', '5', '30', '33', '32', '16', '32', '33', '34', '32', '48', '49', '31', '32', '6', '32', '34', '34', '5', '33', '49', '39', '32', '33', '33', '4', '32', '11', '32', '6', '6', '33', '32', '33', '33', '31', '32', '32', '5', '32', '4', '32', '4', '32', '32', '33', '32', '32', '5', '34', '32', '33', '32', '49', '32', '27', '31', '4', '12', '33', '34', '49', '5', '31', '32', '6', '30', '5', '32', '27', '34', '32', '22', '32', '4', '32', '33', '32', '32', '4', '6', '33', '33', '72', '32', '32', '5', '30', '32', '5', '32', '32', '60', '32', '33', '15', '34', '32', '33', '33', '32', '32', '12', '33', '33', '33', '32', '32', '5', '32', '33', '7', '32', '46', '5', '33', '32', '41', '34', '32', '32', '32', '5', '32', '32', '33', '33', '33', '32', '32', '7', '33', '32', '32', '32', '12', '32', '5', '32', '49', '9', '30', '32', '33', '33', '33', '27', '5', '5', '31', '32', '6', '30', '79', '35', '49', '34', '32', '33', '33', '32', '32', '32', '49', '32', '70', '26', '32', '32', '6', '32', '31', '5', '28', '32', '5', '5', '10', '4', '49', '33', '5', '32', '32', '6', '5', '4', '4', '4', '5', '5', '32', '5', '4', '5', '5', '75', '4', '4', '4', '4', '34', '4', '5', '5', '49', '42', '4', '5', '32', '2', '4', '5', '33', '4', '5', '5', '5', '5', '5', '4', '11', '32', '49', '4', '30', '5', '27', '4', '31', '29', '2', '4', '5', '33', '5', '4', '5', '32', '4', '4', '5', '32', '5', '4', '32', '14', '37', '5', '4', '33', '4', '5', '5', '31', '4', '4', '5', '32', '33', '33', '5', '5', '5', '5', '4', '4', '4', '4', '5', '5', '30', '4', '0', '4', '16', '4', '5', '4', '4', '5', '5', '5', '5', '4', '5', '4', '30', '5', '5', '5', '15', '5', '4', '5', '5', '5', '5', '7', '4', '4', '4', '32', '32', '5', '32', '4', '4', '5', '4', '4', '4', '4', '4', '4', '4', '4', '30', '4', '5', '4', '4', '5', '34', '4', '5', '64', '4', '4', '4', '4', '4', '4', '4', '5', '4', '4', '5', '5', '5', '4', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '31', '4', '4', '5', '4', '5', '35', '4', '4', '4', '5', '4', '4', '5', '4', '5', '4', '5', '4', '5', '4', '4', '4', '4', '32', '4', '4', '31', '13', '4', '11', '4', '32', '5', '4', '33', '5', '32', '4', '30', '4', '5', '32', '33', '5', '5', '5', '4', '5', '3', '4', '4', '5', '32', '4', '4', '5', '31', '32', '5', '49', '12', '5', '4', '5', '4', '33', '2', '5', '5', '30', '80', '4', '33', '33', '3', '5', '34', '31', '34', '7', '59', '32', '33', '5', '32', '95', '5', '32', '32', '5', '5', '32', '30', '5', '32', '5', '4', '4', '32', '5', '4', '4', '5', '5', '33', '11', '4', '32', '4', '4', '33', '4', '63', '4', '4', '4', '34', '4', '18', '33', '32', '33', '32', '4', '32', '47', '5', '4', '32', '5', '5', '49', '35', '32', '33', '32', '5', '7', '32', '4', '32', '21', '12', '5', '32', '32', '4', '4', '4', '5', '5', '4', '32', '5', '4', '5', '32', '5', '4', '34', '4', '5', '4', '5', '5', '4', '5', '4', '4', '30', '32', '5', '33', '33', '32', '31', '33', '32', '32', '4', '6', '34', '1', '15', '30', '32', '5', '4', '32', '4', '5', '32', '2', '49', '8', '32', '11', '6', '5', '31', '33', '12', '34', '33', '31', '4', '33', '34', '34', '32', '32', '32', '32', '8', '32', '33', '4', '74', '4', '33', '32', '28', '4', '5', '33', '14', '32', '33', '31', '5', '32', '5', '33', '33', '32', '33', '32', '5', '32', '33', '23', '27', '31', '31', '34', '31', '5', '41', '32', '32', '33', '32', '11', '32', '7', '11', '32', '33', '32', '33', '34', '32', '32', '4', '32', '31', '32', '32', '32', '32', '33', '46', '32', '66', '32', '33', '30', '5', '32', '32', '32', '4', '32', '32', '32', '32', '33', '32', '49', '32', '32', '32', '33', '33', '32', '5', '33', '32', '12', '32', '33', '16', '32', '33', '5', '32', '32', '9', '34', '64', '4', '32', '32', '33', '32', '31', '32', '32', '10', '32', '6', '33', '13', '32', '5', '5', '4', '31', '3', '32', '25', '40', '34', '32', '32', '34', '5', '32', '44', '33', '8', '32', '33', '32', '33', '5', '33', '32', '32', '32', '18', '30', '32', '33', '32', '49', '32', '32', '32', '6', '17', '33', '33', '5', '49', '32', '19', '4', '5', '5', '4', '5', '7', '4', '11', '33', '32', '32', '4', '3', '32', '27', '4', '4', '33', '5', '4', '34', '31', '5', '30', '1', '4', '5', '32', '5', '4', '5', '4', '61', '9', '4', '11', '5', '32', '33', '33', '34', '4', '33', '34', '4', '32', '32', '5', '32', '4', '31', '32', '33', '5', '4', '33', '5', '4', '27', '5', '5', '4', '35', '5', '5', '4', '5', '4', '4', '4', '33', '5', '32', '5', '5', '5', '27', '4', '4', '4', '4', '4', '5', '5', '5', '5', '6', '5', '5', '5', '5', '4', '5', '5', '5', '4', '5', '4', '66', '4', '4', '4', '4', '5', '4', '4', '4', '32', '7', '33', '5', '7', '4', '5', '55', '32', '43', '21', '5', '4', '5', '3', '4', '5', '4', '4', '32', '32', '33', '34', '5', '69', '4', '32', '4', '32', '25', '30', '32', '30', '32', '63', '35', '33', '5', '32', '5', '32', '4', '5', '4', '5', '4', '5', '4', '4', '33', '33', '33', '4', '30', '5', '33', '32', '4', '32', '33', '27', '5', '4', '32', '5', '4', '32', '5', '5', '5', '33', '4', '5', '4', '4', '4', '5', '5', '7', '33', '5', '32', '5', '5', '49', '5', '4', '4', '5', '4', '4', '5', '4', '4', '5', '32', '4', '4', '4', '4', '4', '5', '32', '4', '5', '4', '4', '4', '5', '4', '5', '4', '4', '61', '4', '5', '4', '38', '33', '4', '5', '34', '13', '4', '4', '32', '32', '32', '4', '5', '5', '32', '5', '32', '4', '33', '33', '33', '5', '5', '33', '5', '5', '4', '12', '4', '28', '5', '5', '5', '5', '5', '4', '5', '5', '4', '32', '6', '4', '4', '5', '9', '13', '32', '34', '4', '33', '15', '32', '32', '4', '32', '5', '5', '27', '4', '5', '4', '4', '5', '4', '4', '4', '5', '4', '21', '5', '5', '33', '5', '4', '34', '5', '4', '4', '4', '5', '4', '4', '5', '5', '4', '5', '5', '13', '4', '5', '4', '5', '4', '4', '31', '5', '4', '5', '4', '4', '5', '30', '4', '4', '5', '4', '5', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '5', '5', '5', '46', '4', '4', '4', '4', '5', '4', '5', '22', '5', '5', '4', '49', '5', '5', '32', '5', '4', '5', '5', '5', '4', '4', '32', '4', '30', '32', '4', '4', '4', '4', '5', '5', '12', '5', '4', '5', '4', '33', '4', '4', '4', '32', '4', '4', '4', '4', '5', '4', '4', '32', '4', '35', '5', '4', '4', '5', '4', '5', '32', '0', '67', '4', '31', '4', '5', '30', '4', '17', '3', '5', '4', '4', '4', '5', '22', '5', '4', '4', '4', '4', '5', '5', '5', '5', '4', '5', '5', '2', '4', '4', '5', '32', '5', '5', '5', '4', '4', '4', '50', '4', '5', '4', '4', '5', '5', '5', '32', '5', '30', '32', '4', '5', '32', '4', '4', '4', '4', '4', '5', '5', '4', '5', '68', '5', '29', '4', '5', '5', '4', '5', '5', '6', '6', '6', '6', '6', '6', '5', '6', '6', '32', '35', '6', '33', '6', '24', '5', '34', '33', '32', '30', '31', '32', '33', '13', '32', '32', '93', '8', '33', '32', '32', '5', '33', '31', '32', '32', '33', '13', '32', '9', '32', '30', '3', '4', '9', '33', '3', '32', '33', '19', '32', '32', '33', '32', '33', '30', '30', '32', '5', '33', '32', '81', '7', '7', '32', '79', '33', '15', '32', '32', '32', '32', '5', '30', '32', '7', '32', '33', '5', '32', '33', '33', '35', '33', '32', '33', '33', '33', '31', '33', '32', '34', '32', '32', '32', '34', '33', '7', '33', '13', '32', '32', '32', '49', '32', '33', '33', '32', '32', '4', '32', '32', '33', '33', '4', '32', '33', '33', '12', '49', '33', '32', '80', '32', '33', '32', '25', '32', '34', '33', '4', '32', '32', '33', '32', '33', '33', '32', '33', '32', '4', '21', '32', '5', '32', '49', '71', '33', '33', '16', '13', '4', '32', '32', '5', '27', '18', '34', '33', '32', '65', '32', '32', '22', '27', '49', '34', '33', '33', '5', '4', '5', '5', '44', '32', '30', '12', '32', '32', '11', '33', '33', '33', '33', '32', '4', '11', '32', '32', '11', '8', '32', '4', '5', '5', '5', '33', '4', '4', '4', '70', '12', '27', '32', '32', '5', '17', '33', '32', '32', '8', '34', '32', '59', '32', '32', '33', '31', '31', '32', '49', '5', '15', '13', '33', '34', '32', '4', '33', '32', '4', '8', '32', '33', '22', '34', '49', '11', '33', '32', '32', '5', '28', '32', '31', '32', '32', '12', '32', '32', '32', '28', '49', '30', '33', '33', '32', '3', '18', '30', '33', '4', '32', '4', '31', '1', '12', '28', '5', '49', '33', '23', '32', '32', '33', '33', '33', '8', '33', '4', '29', '4', '32', '13', '32', '33', '33', '34', '32', '31', '33', '32', '4', '5', '32', '32', '5', '33', '15', '11', '33', '9', '50', '59', '13', '32', '32', '34', '33', '34', '33', '33', '33', '32', '20', '20', '33', '33', '34', '33', '32', '31', '12', '32', '33', '33', '5', '32', '32', '31', '33', '5', '32', '33', '7', '33', '32', '26', '13', '34', '12', '4', '5', '12', '49', '32', '33', '33', '32', '32', '32', '33', '33', '32', '17', '13', '32', '33', '10', '32', '32', '30', '32', '32', '32', '8', '5', '32', '32', '32', '32', '32', '12', '30', '12', '34', '33', '32', '45', '32', '34', '28', '32', '4', '4', '17', '32', '33', '49', '33', '26', '33', '49', '33', '31', '32', '32', '14', '5', '32', '32', '32', '32', '27', '32', '5', '33', '32', '32', '32', '32', '32', '32', '13', '15', '32', '30', '32', '32', '32', '32', '26', '32', '18', '33', '32', '32', '32', '49', '32', '33', '31', '32', '4', '5', '34', '32', '33', '33', '34', '32', '32', '6', '33', '5', '31', '32', '33', '32', '31', '29', '12', '32', '32', '5', '33', '30', '33', '32', '32', '31', '32', '39', '7', '61', '25', '34', '33', '32', '32', '7', '32', '31', '31', '33', '10', '34', '32', '31', '22', '32', '20', '9', '32', '32', '33', '30', '12', '33', '33', '33', '27', '5', '32', '5', '27', '24', '12', '32', '32', '62', '32', '22', '32', '5', '32', '33', '24', '49', '32', '32', '32', '4', '6', '33', '4', '33', '32', '32', '32', '32', '1', '11', '32', '26', '24', '5', '5', '32', '7', '5', '31', '33', '5', '54', '32', '33', '32', '32', '32', '32', '30', '32', '32', '12', '31', '32', '33', '33', '32', '33', '49', '33', '22', '32', '12', '32', '27', '55', '32', '34', '60', '32', '4', '5', '4', '4', '4', '4', '4', '4', '4', '5', '6', '4', '4', '34', '33', '4', '4', '33', '5', '35', '33', '33', '4', '5', '5', '33', '32', '32', '32', '5', '4', '4', '5', '5', '5', '32', '32', '4', '49', '5', '15', '33', '32', '32', '32', '34', '32', '60', '32', '32', '32', '27', '33', '30', '15', '5', '5', '72', '4', '4', '33', '33', '11', '32', '32', '32', '44', '63', '6', '7', '32', '32', '32', '5', '4', '19', '32', '14', '1', '33', '32', '71', '4', '48', '4', '31', '34', '5', '35', '5', '32', '32', '33', '32', '32', '26', '13', '32', '28', '32', '6', '21', '31', '64', '11', '33', '32', '32', '34', '5', '32', '26', '32', '5', '14', '32', '5', '5', '32', '4', '39', '13', '4', '35', '0', '32', '33', '33', '32', '32', '32', '49', '15', '33', '32', '32', '27', '32', '32', '5', '46', '11', '24', '33', '11', '4', '32', '12', '5', '5', '5', '32', '33', '32', '1', '32', '7', '13', '32', '32', '32', '13', '5', '30', '5', '4', '32', '30', '33', '33', '4', '7', '5', '33', '33', '33', '32', '14', '29', '6', '13', '32', '10', '33', '33', '5', '30', '12', '21', '33', '32', '33', '31', '30', '32', '18', '34', '32', '32', '34', '30', '12', '32', '32', '30', '32', '33', '34', '30', '32', '5', '33', '32', '12', '33', '33', '32', '32', '32', '11', '32', '32', '33', '32', '33', '32', '30', '32', '5', '32', '32', '25', '32', '33', '31', '32', '14', '33', '57', '30', '32', '49', '27', '5', '32', '12', '33', '33', '32', '32', '33', '21', '33', '33', '32', '10', '33', '33', '33', '32', '4', '4', '32', '32', '31', '33', '33', '33', '32', '24', '5', '35', '32', '32', '5', '3', '34', '32', '32', '5', '32', '33', '57', '33', '4', '34', '52', '33', '32', '33', '32', '33', '33', '1', '33', '33', '33', '22', '27', '33', '32', '32', '34', '33', '7', '12', '1', '4', '33', '32', '33', '33', '32', '32', '31', '32', '32', '29', '33', '31', '49', '5', '11', '34', '32', '32', '25', '35', '32', '25', '32', '33', '33', '5', '32', '27', '32', '31', '30', '30', '34', '32', '31', '5', '13', '30', '32', '4', '33', '32', '32', '32', '34', '4', '33', '30', '31', '32', '32', '33', '34', '49', '32', '5', '31', '33', '32', '32', '49', '8', '33', '32', '5', '32', '32', '33', '5', '32', '4', '36', '5', '32', '4', '32', '32', '18', '33', '33', '34', '34', '32', '8', '41', '32', '33', '49', '32', '32', '32', '5', '30', '49', '27', '32', '55', '49', '49', '26', '5', '33', '33', '33', '32', '32', '34', '32', '32', '12', '32', '11', '31', '33', '34', '32', '21', '28', '57', '32', '30', '4', '32', '4', '32', '17', '31', '33', '32', '32', '32', '32', '5', '30', '32', '32', '32', '32', '34', '32', '32', '32', '32', '32', '32', '33', '33', '13', '32', '34', '32', '32', '32', '32', '32', '5', '33', '32', '32', '33', '32', '5', '12', '33', '32', '5', '32', '32', '32', '5', '32', '5', '16', '34', '33', '33', '4', '30', '11', '34', '32', '35', '94', '10', '4', '14', '32', '28', '4', '32', '32', '17', '15', '4', '27', '4', '32', '32', '5', '34', '32', '32', '7', '33', '18', '31', '58', '20', '32', '11', '67', '36', '4', '27', '12', '32', '33', '26', '33', '5', '32', '32', '32', '32', '33', '77', '4', '33', '35', '32', '31', '31', '24', '32', '32', '33', '32', '24', '29', '33', '32', '32', '32', '24', '32', '5', '32', '16', '33', '33', '32', '32', '32', '11', '32', '5', '32', '32', '32', '32', '45', '32', '32', '31', '32', '32', '15', '32', '30', '31', '32', '5', '33', '5', '32', '32', '32', '32', '52', '26', '32', '32', '5', '33', '2', '34', '36', '33', '49', '33', '32', '5', '32', '6', '14', '32', '33', '32', '31', '31', '32', '33', '32', '33', '32', '32', '5', '32', '28', '32', '33', '32', '33', '8', '32', '5', '33', '12', '48', '32', '32', '32', '32', '32', '33', '4', '32', '13', '8', '32', '32', '33', '38', '33', '34', '33', '6', '33', '32', '32', '32', '13', '5', '4', '32', '16', '34', '7', '11', '12', '5', '11', '9', '33', '11', '33', '4', '34', '32', '32', '6', '49', '31', '32', '32', '5', '32', '4', '32', '32', '15', '6', '49', '32', '5', '32', '32', '32', '32', '6', '32', '32', '33', '32', '5', '11', '7', '5', '32', '31', '45', '33', '31', '32', '30', '6', '33', '33', '31', '34', '70', '1', '32', '31', '5', '32', '19', '5', '32', '32', '32', '32', '32', '31', '4', '32', '4', '32', '32', '11', '33', '32', '49', '33', '32', '33', '5', '32', '32', '33', '12', '49', '33', '32', '32', '11', '32', '32', '32', '33', '26', '33', '32', '32', '26', '0', '32', '31', '10', '32', '4', '31', '27', '5', '32', '33', '51', '12', '49', '6', '33', '33', '34', '32', '32', '32', '33', '32', '33', '5', '33', '32', '4', '49', '34', '32', '32', '5', '25', '31', '32', '33', '2', '5', '32', '14', '32', '32', '78', '32', '32', '32', '9', '20', '33', '33', '34', '32', '15', '33', '31', '32', '31', '32', '7', '11', '33', '32', '22', '49', '32', '32', '31', '33', '33', '32', '24', '32', '34', '33', '32', '34', '33', '14', '32', '33', '33', '19', '32', '32', '32', '14', '32', '8', '33', '33', '33', '32', '1', '33', '32', '32', '33', '27', '33', '11', '32', '33', '5', '32', '32', '12', '5', '11', '32', '33', '32', '32', '33', '32', '32', '45', '9', '32', '33', '32', '32', '32', '32', '32', '13', '32', '32', '5', '32', '32', '8', '7', '32', '33', '13', '49', '38', '6', '32', '33', '33', '19', '32', '32', '4', '4', '32', '32', '32', '33', '5', '33', '32', '12', '31', '32', '32', '33', '32', '38', '49', '33', '11', '32', '14', '6', '32', '33', '5', '5', '31', '32', '32', '32', '49', '32', '30', '70', '5', '33', '4', '16', '32', '32', '4', '32', '63', '6', '33', '49', '49', '5', '33', '32', '33', '33', '32', '5', '22', '5', '32', '11', '33', '32', '32', '11', '30', '33', '30', '34', '24', '21', '5', '32', '32', '32', '9', '13', '32', '48', '18', '5', '8', '7', '33', '32', '32', '32', '32', '19', '8', '32', '30', '33', '5', '32', '33', '32', '32', '32', '35', '11', '4', '32', '31', '32', '32', '32', '33', '33', '32', '10', '32', '32', '32', '1', '30', '7', '24', '33', '33', '32', '4', '33', '32', '5', '10', '27', '32', '33', '34', '32', '33', '33', '32', '32', '32', '32', '32', '32', '5', '33', '4', '32', '5', '32', '32', '7', '32', '33', '33', '32', '30', '16', '32', '5', '5', '5', '5', '5', '31', '33', '33', '4', '33', '32', '32', '5', '32', '33', '24', '31', '33', '8', '33', '32', '32', '32', '5', '32', '32', '5', '12', '41', '8', '33', '32', '32', '17', '5', '32', '32', '49', '32', '32', '4', '32', '9', '32', '33', '31', '33', '33', '31', '5', '32', '32', '4', '32', '32', '27', '32', '32', '32', '33', '32', '12', '49', '13', '32', '32', '30', '32', '5', '11', '32', '32', '3', '4', '33', '32', '58', '33', '30', '33', '49', '32', '33', '32', '16', '4', '33', '16', '33', '32', '5', '15', '33', '33', '32', '32', '35', '32', '33', '32', '34', '32', '32', '33', '10', '32', '31', '34', '33', '12', '32', '33', '27', '5', '4', '32', '32', '32', '31', '32', '33', '33', '31', '32', '33', '33', '32', '32', '6', '32', '49', '32', '6', '5', '4', '33', '15', '32', '32', '32', '5', '32', '33', '49', '32', '32', '32', '32', '33', '17', '32', '32', '4', '32', '31', '32', '37', '35', '1', '32', '12', '30', '33', '5', '32', '20', '5', '5', '32', '32', '49', '31', '32', '32', '6', '4', '32', '26', '31', '5', '5', '32', '32', '32', '33', '32', '32', '33', '30', '33', '32', '31', '32', '5', '32', '32', '32', '4', '49', '31', '32', '32', '33', '31', '32', '32', '11', '32', '49', '31', '4', '36', '5', '3', '9', '31', '12', '32', '32', '30', '4', '4', '4', '33', '49', '32', '32', '30', '4', '49', '31', '31', '33', '33', '32', '34', '32', '49', '32', '32', '5', '4', '8', '32', '32', '33', '12', '5', '32', '32', '32', '32', '32', '32', '8', '32', '32', '32', '32', '33', '2', '33', '32', '30', '33', '31', '32', '23', '30', '25', '5', '66', '36', '5', '32', '33', '31', '32', '32', '10', '33', '33', '14', '33', '33', '32', '13', '9', '18', '32', '34', '2', '32', '32', '4', '49', '5', '19', '4', '32', '33', '33', '35', '31', '22', '32', '32', '5', '30', '28', '32', '32', '32', '34', '32', '4', '6', '31', '32', '4', '32', '4', '33', '32', '33', '31', '6', '4', '32', '29', '13', '34', '32', '11', '34', '32', '8', '32', '33', '32', '49', '4', '32', '36', '33', '33', '7', '32', '32', '85', '32', '32', '33', '32', '9', '5', '4', '32', '12', '32', '32', '4', '30', '16', '32', '32', '1', '32', '33', '5', '32', '49', '33', '72', '31', '11', '5', '33', '49', '4', '31', '6', '33', '17', '33', '32', '5', '32', '32', '32', '14', '5', '26', '5', '17', '31', '4', '33', '30', '4', '32', '27', '23', '12', '32', '32', '32', '32', '32', '25', '32', '30', '32', '31', '33', '32', '32', '4', '5', '4', '33', '32', '33', '32', '32', '32', '32', '49', '31', '25', '32', '6', '33', '32', '5', '65', '8', '7', '32', '32', '32', '49', '32', '32', '6', '32', '15', '32', '11', '32', '32', '31', '32', '34', '6', '33', '32', '33', '32', '31', '15', '33', '32', '33', '32', '34', '25', '32', '32', '32', '33', '32', '50', '33', '32', '32', '49', '32', '6', '32', '5', '32', '32', '49', '32', '32', '5', '32', '4', '49', '32', '32', '33', '9', '32', '16', '33', '32', '33', '31', '4', '8', '5', '35', '5', '49', '6', '49', '32', '32', '32', '34', '32', '1', '9', '49', '32', '33', '4', '30', '49', '30', '4', '33', '32', '5', '30', '33', '11', '32', '32', '49', '4', '5', '33', '31', '5', '5', '25', '58', '32', '32', '13', '5', '31', '30', '32', '40', '12', '32', '12', '34', '33', '5', '35', '22', '25', '33', '28', '30', '5', '32', '27', '33', '33', '32', '5', '33', '5', '33', '30', '32', '9', '5', '30', '33', '48', '32', '12', '32', '32', '25', '32', '4', '32', '32', '16', '4', '5', '32', '45', '32', '5', '33', '32', '54', '14', '7', '5', '32', '4', '47', '33', '49', '5', '30', '7', '30', '5', '6', '30', '32', '5', '7', '5', '33', '32', '33', '5', '49', '30', '30', '35', '4', '8', '33', '32', '30', '8', '32', '5', '5', '32', '15', '30', '5', '32', '5', '72', '13', '10', '31', '4', '28', '20', '71', '32', '5', '19', '33', '32', '32', '7', '10', '94', '32', '32', '33', '28', '8', '34', '15', '4', '32', '1', '32', '15', '8', '32', '8', '5', '33', '34', '6', '32', '32', '12', '11', '79', '32', '32', '32', '33', '33', '18', '5', '49', '5', '33', '32', '6', '32', '13', '4', '33', '32', '4', '33', '4', '5', '73', '33', '31', '12', '13', '33', '32', '32', '33', '23', '33', '33', '33', '32', '32', '32', '33', '57', '4', '35', '6', '31', '33', '5', '30', '30', '32', '33', '6', '32', '32', '5', '8', '82', '33', '32', '34', '11', '5', '15', '33', '32', '6', '32', '5', '33', '32', '32', '32', '33', '33', '11', '28', '28', '32', '5', '35', '33', '32', '33', '32', '33', '32', '5', '32', '32', '33', '19', '32', '49', '33', '33', '32', '3', '32', '32', '34', '32', '5', '32', '32', '33', '13', '29', '35', '32', '32', '5', '29', '33', '5', '33', '32', '33', '33', '7', '32', '33', '32', '7', '32', '14', '5', '32', '32', '32', '5', '5', '5', '4', '5', '5', '5', '14', '8', '32', '33', '32', '30', '32', '33', '24', '11', '32', '4', '32', '32', '27', '32', '32', '51', '31', '33', '49', '6', '33', '12', '33', '5', '33', '8', '5', '33', '32', '30', '9', '31', '33', '32', '14', '5', '32', '32', '32', '32', '32', '49', '32', '32', '32', '21', '33', '33', '32', '32', '32', '33', '32', '33', '32', '19', '23', '33', '33', '32', '32', '32', '33', '33', '30', '32', '33', '5', '32', '4', '32', '32', '7', '33', '5', '5', '5', '30', '5', '32', '30', '12', '7', '53', '6', '32', '6', '5', '5', '48', '33', '34', '4', '33', '32', '32', '33', '8', '32', '32', '33', '32', '32', '32', '12', '32', '5', '33', '32', '33', '15', '32', '16', '32', '33', '32', '32', '32', '32', '27', '33', '32', '32', '34', '33', '32', '34', '7', '32', '33', '32', '32', '33', '48', '12', '33', '32', '33', '33', '32', '33', '4', '5', '32', '33', '32', '32', '61', '13', '32', '32', '35', '32', '35', '32', '32', '33', '85', '32', '5', '30', '32', '33', '32', '5', '33', '4', '4', '32', '5', '4', '32', '25', '34', '32', '11', '32', '33', '32', '5', '4', '32', '32', '33', '47', '33', '12', '12', '32', '32', '33', '7', '32', '32', '32', '30', '32', '32', '32', '32', '4', '32', '33', '5', '31', '8', '11', '76', '32', '6', '32', '11', '49', '5', '25', '49', '32', '11', '4', '32', '32', '32', '33', '32', '32', '71', '32', '4', '32', '32', '33', '32', '12', '32', '29', '13', '12', '5', '31', '32', '32', '34', '33', '31', '8', '33', '32', '32', '33', '33', '32', '32', '9', '12', '32', '33', '32', '46', '32', '32', '34', '32', '33', '11', '5', '32', '32', '33', '30', '32', '21', '32', '33', '33', '33', '32', '33', '14', '33', '32', '32', '33', '33', '7', '33', '32', '45', '42', '32', '51', '1', '33', '8', '32', '33', '33', '5', '33', '32', '32', '10', '33', '32', '32', '32', '32', '32', '33', '31', '5', '6', '5', '10', '32', '30', '33', '5', '32', '27', '38', '12', '5', '32', '33', '32', '32', '12', '32', '67', '34', '33', '32', '32', '32', '33', '8', '33', '33', '60', '7', '33', '32', '8', '5', '61', '32', '32', '5', '7', '32', '19', '32', '6', '32', '33', '4', '49', '34', '33', '32', '32', '31', '49', '30', '10', '11', '33', '33', '33', '32', '30', '32', '32', '11', '33', '33', '32', '49', '15', '32', '64', '12', '33', '5', '6', '5', '30', '33', '32', '33', '11', '32', '26', '34', '31', '33', '33', '49', '13', '</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atend</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>['85974001107', '85981010387', '85981010504', '85981010801', '85981011300', '85981011982', '85981012709', '85981012859', '85981012916', '85981013105', '85981013139', '85981013252', '85981014486', '85981015083', '85981015199', '85981015345', '85981015408', '85981015858', '85981018191', '85981019737', '85981019859', '85981020615', '85981021220', '85981021847', '85981021858', '85981023473', '85981024243', '85981024932', '85981025159', '85981026077', '85981026188', '85981026342', '85981029941', '85981034608', '85981035347', '85981037998', '85981038369', '85981040609', '85981041303', '85981042289', '85981046232', '85981047325', '85981047447', '85981050094', '85981050305', '85981050670', '85981050778', '85981050921', '85981051007', '85981051157', '85981051236', '85981051357', '85981051407', '85981051960', '85981052023', '85981052147', '85981052388', '85981053361', '85981053645', '85981053870', '85981054245', '85981054310', '85981054721', '85981054784', '85981055402', '85981055606', '85981055887', '85981056204', '85981056432', '85981057133', '85981057473', '85981057594', '85981057657', '85981058510', '85981058575', '85981059167', '85981060358', '85981060840', '85981060881', '85981060903', '85981060912', '85981061514', '85981062036', '85981062783', '85981062811', '85981063144', '85981063180', '85981063445', '85981063577', '85981063706', '85981063708', '85981063769', '85981064311', '85981064501', '85981064633', '85981066228', '85981066596', '85981066800', '85981067063', '85981067120', '85981067303', '85981067738', '85981068259', '85981068383', '85981068838', '85981069073', '85981069268', '85981069285', '85981069288', '85981069331', '85981069531', '85981069805', '85981070139', '85981070716', '85981070933', '85981072516', '85981074292', '85981074824', '85981077799', '85981079793', '85981080110', '85981081102', '85981081645', '85981081717', '85981081963', '85981082567', '85981082798', '85981083944', '85981083955', '85981084430', '85981085176', '85981085425', '85981086055', '85981087566', '85981090951', '85981092003', '85981094270', '85981095658', '85981096027', '85981097092', '85981097525', '85981099771', '85981099834', '85981104139', '85981105541', '85981111379', '85981111687', '85981112198', '85981112368', '85981113354', '85981116111', '85981116475', '85981117229', '85981117240', '85981117970', '85981118916', '85981119356', '85981121743', '85981121756', '85981121918', '85981122659', '85981122830', '85981124417', '85981125198', '85981125364', '85981127000', '85981127863', '85981128332', '85981128640', '85981129033', '85981130954', '85981131390', '85981132338', '85981132657', '85981132861', '85981133001', '85981136515', '85981137269', '85981137935', '85981138484', '85981139818', '85981141110', '85981141235', '85981142047', '85981142397', '85981144074', '85981144194', '85981144290', '85981144476', '85981145210', '85981145431', '85981146150', '85981147761', '85981148652', '85981149605', '85981149798', '85981149833', '85981150270', '85981152513', '85981152668', '85981152923', '85981153276', '85981154070', '85981154704', '85981154767', '85981155516', '85981155609', '85981155832', '85981157497', '85981159783', '85981160701', '85981162279', '85981163532', '85981168773', '85981169336', '85981170375', '85981170419', '85981172174', '85981172237', '85981173080', '85981173491', '85981173596', '85981174595', '85981175102', '85981175961', '85981176245', '85981176511', '85981176843', '85981176855', '85981177377', '85981177436', '85981178111', '85981180220', '85981180748', '85981181223', '85981181460', '85981184568', '85981185113', '85981185397', '85981185432', '85981186162', '85981187777', '85981187790', '85981188522', '85981190449', '85981190603', '85981190941', '85981191324', '85981191501', '85981192668', '85981193462', '85981194504', '85981195274', '85981195777', '85981196765', '85981199009', '85981200624', '85981204580', '85981205000', '85981207224', '85981210397', '85981211722', '85981211785', '85981212297', '85981212335', '85981215121', '85981215323', '85981217007', '85981217070', '85981217271', '85981217334', '85981217865', '85981217880', '85981217928', '85981219726', '85981220015', '85981220097', '85981220132', '85981221107', '85981221148', '85981222412', '85981224119', '85981224486', '85981224995', '85981225097', '85981225167', '85981226403', '85981227172', '85981227283', '85981227812', '85981228111', '85981228405', '85981228468', '85981229862', '85981229918', '85981229981', '85981230013', '85981230104', '85981233010', '85981233031', '85981233110', '85981234275', '85981235443', '85981237281', '85981238571', '85981240151', '85981240906', '85981241794', '85981243937', '85981245200', '85981245595', '85981245660', '85981246453', '85981246810', '85981247191', '85981247682', '85981247801', '85981248056', '85981248614', '85981248938', '85981249006', '85981249077', '85981249520', '85981249804', '85981250065', '85981251340', '85981252190', '85981252202', '85981252814', '85981253454', '85981256347', '85981256415', '85981256918', '85981257594', '85981257644', '85981258954', '85981259116', '85981259996', '85981260093', '85981260293', '85981261976', '85981264023', '85981265628', '85981266155', '85981266554', '85981267575', '85981268163', '85981269254', '85981270887', '85981273817', '85981276088', '85981277050', '85981277171', '85981277778', '85981277862', '85981278172', '85981278481', '85981281110', '85981281122', '85981283976', '85981284254', '85981284771', '85981284904', '85981285694', '85981285757', '85981286755', '85981287954', '85981288208', '85981288338', '85981289201', '85981290315', '85981291170', '85981291852', '85981292335', '85981292898', '85981293237', '85981296943', '85981297006', '85981297774', '85981298411', '85981298474', '85981299369', '85981300207', '85981300265', '85981301018', '85981301029', '85981301090', '85981301430', '85981302820', '85981303653', '85981304383', '85981304684', '85981304736', '85981304842', '85981305581', '85981306366', '85981307620', '85981307802', '85981308045', '85981308259', '85981308292', '85981308328', '85981308337', '85981308391', '85981310114', '85981310742', '85981311091', '85981311398', '85981312075', '85981313089', '85981313134', '85981313616', '85981313627', '85981314051', '85981314422', '85981315654', '85981316754', '85981318080', '85981323921', '85981325550', '85981327070', '85981327436', '85981327760', '85981328852', '85981330136', '85981330758', '85981331850', '85981331913', '85981332190', '85981333065', '85981333339', '85981334650', '85981334713', '85981334761', '85981335534', '85981337373', '85981338263', '85981338307', '85981342092', '85981342565', '85981343138', '85981343533', '85981344833', '85981345060', '85981347012', '85981347371', '85981348351', '85981348558', '85981349404', '85981351875', '85981352588', '85981352826', '85981353374', '85981353997', '85981354648', '85981355846', '85981357814', '85981359310', '85981360852', '85981361507', '85981361779', '85981362003', '85981362066', '85981363777', '85981365886', '85981366880', '85981367170', '85981368633', '85981370043', '85981370894', '85981371153', '85981371868', '85981372645', '85981374219', '85981375527', '85981375801', '85981375825', '85981376079', '85981377391', '85981378159', '85981378792', '85981378905', '85981379505', '85981379662', '85981380597', '85981380924', '85981381707', '85981381999', '85981383237', '85981383353', '85981384426', '85981385151', '85981385624', '85981385673', '85981385841', '85981386704', '85981386821', '85981387227', '85981387362', '85981388619', '85981391330', '85981391423', '85981391880', '85981392100', '85981392565', '85981395635', '85981395687', '85981395818', '85981397246', '85981397372', '85981397409', '85981397411', '85981398764', '85981400369', '85981401399', '85981401626', '85981401752', '85981402041', '85981402081', '85981402748', '85981402997', '85981403093', '85981403964', '85981404116', '85981404174', '85981404374', '85981404793', '85981405917', '85981408267', '85981409242', '85981409843', '85981411024', '85981411624', '85981411687', '85981413039', '85981413532', '85981413653', '85981413838', '85981413892', '85981414546', '85981415469', '85981416386', '85981416409', '85981418850', '85981419344', '85981420019', '85981421525', '85981421738', '85981422245', '85981422308', '85981422576', '85981422856', '85981423490', '85981423505', '85981423933', '85981424271', '85981424607', '85981425703', '85981426537', '85981426942', '85981427253', '85981428860', '85981428912', '85981432332', '85981433880', '85981436330', '85981437233', '85981437797', '85981440921', '85981442203', '85981443375', '85981444452', '85981444515', '85981445843', '85981447674', '85981448037', '85981452309', '85981453385', '85981460147', '85981460175', '85981460392', '85981460457', '85981460646', '85981460699', '85981460861', '85981460924', '85981460996', '85981461065', '85981461106', '85981461610', '85981462406', '85981463746', '85981463860', '85981464262', '85981464411', '85981464530', '85981464545', '85981465735', '85981465772', '85981465798', '85981466545', '85981467570', '85981468790', '85981470659', '85981470831', '85981471492', '85981471759', '85981472233', '85981473750', '85981474263', '85981474389', '85981474696', '85981474697', '85981474756', '85981474760', '85981474778', '85981474912', '85981474923', '85981475220', '85981475230', '85981475761', '85981475972', '85981475980', '85981476043', '85981476212', '85981476638', '85981477326', '85981477413', '85981477799', '85981477812', '85981477813', '85981477916', '85981478494', '85981478784', '85981479493', '85981479515', '85981479752', '85981479774', '85981481053', '85981481331', '85981481726', '85981482109', '85981482140', '85981482476', '85981482990', '85981483810', '85981484967', '85981485284', '85981485480', '85981486380', '85981486397', '85981487878', '85981488161', '85981488741', '85981489506', '85981489546', '85981489609', '85981489986', '85981491380', '85981491428', '85981491439', '85981492666', '85981492729', '85981495205', '85981495268', '85981495465', '85981495615', '85981495911', '85981495935', '85981496025', '85981496943', '85981497099', '85981497122', '85981497496', '85981497614', '85981499186', '85981500414', '85981500847', '85981500940', '85981501090', '85981501968', '85981502098', '85981502241', '85981505500', '85981505522', '85981505531', '85981505586', '85981505887', '85981506224', '85981506332', '85981506467', '85981506955', '85981507053', '85981507770', '85981507930', '85981509140', '85981509349', '85981509981', '85981510677', '85981511295', '85981512929', '85981514081', '85981514747', '85981518467', '85981518484', '85981520304', '85981521334', '85981521816', '85981521879', '85981521962', '85981522121', '85981522321', '85981522480', '85981522523', '85981522914', '85981522917', '85981522933', '85981522980', '85981523042', '85981523247', '85981523548', '85981523703', '85981523830', '85981523864', '85981524209', '85981524336', '85981524345', '85981524388', '85981524433', '85981524474', '85981525329', '85981525392', '85981525946', '85981525956', '85981525970', '85981526066', '85981526142', '85981526377', '85981526414', '85981526660', '85981526890', '85981526953', '85981527026', '85981527241', '85981527738', '85981527876', '85981527926', '85981528100', '85981528344', '85981528523', '85981529250', '85981530016', '85981530202', '85981530228', '85981530264', '85981530358', '85981530695', '85981531466', '85981532323', '85981532367', '85981532706', '85981533140', '85981533536', '85981533817', '85981533861', '85981533924', '85981534836', '85981535019', '85981535381', '85981535444', '85981535702', '85981536001', '85981536037', '85981536784', '85981537054', '85981537071', '85981537451', '85981537531', '85981537646', '85981538008', '85981538403', '85981538473', '85981539100', '85981539364', '85981539374', '85981539613', '85981539674', '85981539710', '85981539904', '85981542565', '85981544220', '85981544377', '85981544415', '85981544420', '85981544535', '85981544744', '85981545730', '85981545967', '85981546135', '85981546201', '85981546486', '85981546524', '85981547100', '85981547151', '85981547181', '85981548573', '85981548663', '85981549807', '85981550607', '85981551701', '85981552786', '85981552815', '85981553207', '85981553257', '85981553774', '85981554041', '85981554682', '85981555448', '85981556360', '85981556386', '85981556391', '85981556708', '85981557599', '85981557763', '85981557766', '85981557996', '85981558443', '85981558444', '85981558593', '85981558734', '85981558921', '85981559352', '85981559880', '85981559990', '85981561122', '85981561397', '85981563114', '85981563918', '85981565385', '85981566296', '85981569388', '85981570332', '85981570553', '85981571936', '85981571948', '85981573149', '85981574029', '85981574749', '85981574828', '85981575288', '85981576121', '85981577685', '85981579715', '85981580747', '85981582223', '85981587265', '85981588881', '85981589028', '85981590283', '85981590581', '85981591212', '85981591394', '85981592814', '85981594445', '85981594455', '85981598314', '85981599091', '85981599720', '85981600032', '85981600288', '85981600746', '85981601467', '85981601515', '85981601621', '85981603545', '85981603701', '85981603764', '85981603922', '85981604044', '85981604097', '85981604901', '85981605888', '85981606241', '85981606453', '85981606516', '85981606875', '85981607061', '85981607171', '85981607847', '85981608039', '85981608131', '85981608656', '85981608885', '85981609224', '85981609765', '85981611504', '85981611687', '85981612354', '85981612497', '85981613707', '85981614805', '85981615721', '85981615726', '85981616672', '85981617048', '85981617443', '85981617809', '85981618157', '85981618463', '85981618696', '85981619089', '85981621012', '85981625207', '85981625719', '85981625789', '85981625797', '85981626292', '85981626455', '85981627178', '85981627515', '85981627750', '85981628353', '85981628962', '85981629450', '85981630101', '85981630164', '85981631945', '85981632116', '85981635515', '85981635650', '85981636098', '85981636649', '85981638200', '85981638739', '85981639201', '85981642110', '85981642480', '85981645543', '85981646909', '85981647853', '85981649485', '85981651235', '85981651813', '85981651856', '85981653359', '85981654096', '85981655420', '85981655504', '85981656015', '85981656761', '85981663973', '85981664051', '85981665088', '85981665658', '85981665867', '85981666220', '85981666585', '85981666685', '85981668986', '85981669316', '85981669696', '85981669892', '85981670050', '85981670209', '85981670557', '85981671233', '85981672007', '85981672198', '85981672687', '85981676600', '85981677013', '85981677923', '85981677986', '85981679022', '85981679393', '85981684827', '85981685253', '85981687262', '85981688088', '85981688530', '85981689614', '85981690885', '85981692225', '85981693076', '85981694698', '85981696440', '85981700371', '85981701616', '85981701789', '85981702211', '85981704587', '85981705823', '85981706117', '85981706812', '85981707565', '85981709424', '85981709639', '85981709959', '85981709997', '85981711415', '85981712700', '85981715589', '85981717124', '85981721330', '85981721470', '85981723162', '85981723682', '85981727178', '85981727333', '85981730276', '85981731368', '85981733009', '85981733173', '85981734225', '85981735351', '85981735457', '85981738337', '85981742689', '85981745007', '85981746191', '85981746231', '85981747230', '85981747684', '85981747880', '85981748018', '85981749098', '85981749311', '85981780097', '85981780698', '85981781860', '85981781956', '85981782615', '85981783993', '85981787014', '85981787375', '85981787694', '85981787878', '85981795562', '85981797415', '85981799011', '85981799243', '85981799393', '85981799969', '85981800644', '85981801187', '85981801628', '85981801718', '85981801761', '85981802537', '85981802631', '85981803848', '85981804731', '85981805074', '85981805578', '85981805682', '85981805712', '85981805995', '85981806062', '85981806192', '85981806838', '85981807096', '85981807746', '85981808109', '85981808226', '85981808940', '85981809310', '85981809579', '85981810401', '85981811681', '85981812231', '85981812420', '85981813215', '85981813326', '85981813696', '85981813745', '85981814222', '85981815518', '85981815719', '85981815951', '85981815995', '85981816185', '85981816597', '85981816953', '85981817644', '85981819191', '85981819878', '85981819898', '85981819971', '85981820302', '85981820909', '85981822288', '85981822627', '85981823737', '85981824050', '85981825667', '85981827171', '85981827298', '85981828133', '85981829674', '85981829888', '85981830615', '85981831333', '85981831807', '85981832616', '85981833911', '85981836027', '85981836192', '85981838197', '85981839905', '85981840699', '85981840997', '85981841498', '85981842018', '85981842026', '85981847568', '85981849140', '85981849448', '85981850329', '85981851336', '85981851657', '85981851806', '85981852483', '85981852871', '85981853361', '85981853473', '85981853498', '85981854188', '85981854400', '85981854701', '85981854966', '85981855387', '85981855943', '85981857602', '85981858378', '85981858585', '85981859714', '85981859843', '85981860190', '85981860939', '85981861386', '85981861390', '85981862200', '85981862732', '85981862812', '85981863520', '85981863917', '85981864665', '85981866872', '85981867198', '85981867874', '85981868706', '85981869078', '85981869877', '85981870279', '85981870625', '85981870769', '85981871433', '85981871482', '85981871725', '85981872527', '85981873853', '85981874873', '85981875089', '85981875839', '85981876038', '85981876387', '85981877277', '85981877340', '85981877666', '85981878608', '85981879558', '85981879727', '85981881447', '85981881564', '85981881903', '85981882019', '85981882233', '85981883888', '85981885848', '85981886408', '85981888076', '85981890073', '85981890692', '85981890804', '85981890897', '85981891321', '85981891476', '85981892737', '85981892922', '85981893512', '85981894559', '85981895421', '85981895778', '85981895877', '85981899243', '85981900080', '85981900730', '85981901391', '85981904698', '85981905011', '85981905074', '85981905075', '85981906452', '85981910262', '85981910771', '85981911604', '85981911984', '85981914747', '85981917082', '85981917653', '85981917936', '85981918090', '85981918203', '85981921936', '85981921999', '85981922555', '85981924869', '85981926087', '85981926161', '85981927362', '85981928269', '85981930502', '85981933090', '85981933446', '85981934488', '85981937771', '85981942675', '85981944086', '85981946447', '85981947455', '85981948504', '85981948560', '85981948709', '85981949370', '85981949405', '85981950680', '85981951197', '85981951207', '85981951277', '85981951294', '85981951433', '85981952223', '85981952606', '85981953266', '85981955156', '85981955666', '85981956683', '85981956798', '85981956914', '85981956977', '85981958219', '85981958833', '85981959454', '85981962203', '85981963748', '85981964770', '85981966391', '85981966744', '85981967093', '85981967347', '85981967672', '85981972215', '85981973787', '85981973850', '85981974619', '85981975003', '85981975335', '85981975643', '85981978964', '85981982384', '85981982415', '85981983536', '85981984160', '85981984196', '85981984205', '85981985320', '85981987749', '85981990206', '85981991814', '85981992200', '85981992221', '85981993841', '85981994171', '85981994544', '85981996677', '85981996968', '85981997233', '85981998183', '85981998880', '85981999101', '85981999393', '85982000080', '85982000103', '85982000124', '85982000407', '85982000597', '85982001158', '85982001480', '85982001603', '85982002244', '85982003360', '85982009691', '85982012352', '85982013350', '85982013725', '85982014410', '85982014728', '85982014859', '85982015963', '85982016650', '85982018181', '85982019178', '85982020684', '85982020732', '85982021675', '85982021901', '85982021970', '85982022116', '85982022707', '85982023008', '85982023198', '85982023449', '85982024092', '85982024412', '85982024556', '85982025193', '85982025465', '85982025505', '85982026115', '85982026559', '85982026582', '85982026618', '85982026681', '85982026958', '85982027257', '85982027456', '85982028016', '85982028614', '85982028717', '85982029544', '85982029630', '85982029656', '85982031994', '85982033246', '85982036215', '85982038136', '85982038199', '85982038964', '85982041982', '85982048028', '85982048400', '85982048768', '85982049005', '85982050430', '85982051850', '85982052170', '85982052833', '85982053074', '85982058486', '85982059867', '85982060243', '85982061188', '85982061715', '85982065404', '85982066323', '85982066720', '85982067095', '85982067924', '85982069921', '85982070325', '85982070442', '85982070505', '85982070537', '85982075392', '85982076079', '85982077220', '85982080055', '85982080963', '85982081863', '85982082408', '85982082685', '85982086204', '85982086988', '85982088181', '85982088401', '85982090444', '85982092229', '85982092410', '85982092535', '85982095933', '85982096408', '85982096638', '85982096702', '85982098898', '85982099596', '85982101224', '85982102764', '85982103459', '85982103837', '85982104191', '85982105219', '85982105253', '85982105588', '85982106049', '85982107612', '85982108435', '85982108824', '85982108871', '85982108995', '85982109939', '85982110388', '85982110918', '85982111162', '85982111405', '85982111461', '85982111682', '85982111714', '85982112134', '85982112150', '85982112252', '85982112330', '85982112561', '85982112835', '85982113153', '85982113424', '85982113947', '85982114041', '85982114590', '85982114798', '85982115352', '85982115530', '85982116277', '85982116934', '85982116997', '85982118281', '85982118296', '85982118359', '85982118717', '85982119038', '85982119077', '85982120196', '85982120770', '85982121018', '85982121624', '85982122300', '85982122468', '85982123793', '85982123880', '85982125254', '85982126275', '85982127512', '85982130408', '85982130446', '85982131720', '85982132411', '85982132443', '85982132450', '85982133520', '85982134594', '85982134658', '85982140032', '85982141654', '85982144572', '85982145647', '85982145648', '85982147385', '85982147517', '85982148150', '85982148935', '85982150345', '85982154109', '85982154431', '85982154497', '85982155595', '85982155633', '85982161243', '85982161749', '85982162384', '85982162735', '85982163153', '85982164038', '85982166162', '85982166295', '85982166369', '85982170184', '85982171502', '85982171541', '85982171985', '85982184521', '85982185872', '85982190343', '85982204545', '85982205828', '85982207580', '85982217764', '85982222262', '85982223649', '85982225298', '85982234415', '85982243000', '85982254767', '85982254833', '85984000187', '85984000206', '85984000276', '85984000283', '85984000366', '85984000374', '85984000408', '85984000419', '85984000570', '85984000752', '85984000901', '85984000924', '85984001030', '85984001034', '85984001146', '85984001200', '85984001263', '85984001399', '85984001670', '85984001714', '85984001904', '85984002329', '85984002699', '85984004021', '85984004143', '85984004381', '85984004513', '85984004885', '85984004934', '85984004937', '85984005030', '85984005089', '85984005191', '85984005207', '85984005486', '85984005676', '85984005684', '85984005854', '85984006088', '85984006430', '85984006519', '85984006807', '85984006822', '85984006945', '85984007418', '85984007839', '85984007934', '85984008090', '85984008165', '85984008494', '85984008541', '85984008711', '85984008837', '85984008876', '85984009118', '85984009152', '85984010102', '85984010119', '85984010346', '85984010352', '85984010376', '85984010523', '85984010651', '85984010721', '85984010796', '85984011030', '85984011127', '85984011205', '85984011272', '85984011345', '85984011423', '85984012202', '85984012591', '85984012893', '85984013559', '85984013847', '85984013900', '85984013932', '85984013963', '85984014210', '85984014231', '85984014288', '85984014376', '85984014432', '85984014547', '85984015074', '85984015099', '85984015349', '85984015384', '85984015385', '85984015469', '85984015572', '85984015631', '85984015661', '85984015695', '85984015758', '85984015793', '85984015918', '85984015943', '85984015948', '85984016599', '85984016848', '85984017946', '85984018354', '85984019606', '85984019846', '85984019986', '85984020049', '85984020051', '85984020177', '85984020235', '85984020417', '85984020826', '85984020911', '85984021324', '85984021461', '85984021871', '85984022102', '85984022241', '85984022389', '85984022437', '85984022645', '85984023016', '85984023231', '85984023332', '85984023361', '85984023534', '85984024023', '85984024057', '85984024750', '85984024773', '85984024790', '85984024966', '85984025156', '85984025366', '85984025761', '85984026229', '85984026355', '85984026707', '85984026882', '85984026909', '85984026937', '85984027014', '85984027778', '85984027803', '85984027980', '85984028311', '85984028478', '85984028528', '85984028635', '85984028807', '85984029384', '85984029403', '85984029645', '85984029647', '85984029806', '85984029997', '85984030002', '85984030015', '85984030126', '85984030128', '85984030255', '85984030534', '85984030799', '85984030914', '85984031018', '85984031134', '85984031235', '85984031240', '85984031369', '85984031377', '85984031387', '85984031438', '85984031757', '85984031799', '85984031859', '85984031951', '85984031983', '85984031996', '85984032024', '85984032030', '85984032046', '85984032152', '85984032209', '85984032278', '85984032838', '85984032911', '85984033253', '85984033308', '85984033709', '85984033733', '85984033741', '85984033796', '85984033825', '85984033893', '85984033983', '85984034114', '85984034385', '85984034577', '85984034588', '85984034633', '85984034782', '85984034964', '85984035081', '85984035134', '85984035188', '85984035416', '85984035423', '85984035459', '85984035494', '85984035559', '85984035765', '85984036032', '85984036315', '85984036485', '85984036570', '85984036614', '85984036676', '85984036734', '85984036808', '85984036872', '85984037291', '85984037296', '85984037302', '85984037313', '85984037354', '85984037682', '85984037921', '85984037935', '85984037947', '85984038033', '85984038229', '85984038524', '85984038538', '85984038620', '85984038850', '85984038856', '85984039320', '85984039429', '85984039451', '85984039728', '85984040449', '85984040502', '85984040554', '85984040731', '85984040757', '85984040783', '85984040792', '85984040899', '85984041029', '85984041044', '85984041297', '85984041417', '85984041458', '85984041670', '85984041713', '85984041805', '85984041914', '85984041986', '85984042380', '85984042425', '85984042497', '85984042509', '85984042623', '85984042895', '85984042963', '85984043070', '85984043137', '85984043296', '85984043323', '85984043326', '85984043413', '85984043751', '85984044012', '85984044067', '85984044191', '85984044248', '85984044283', '85984044300', '85984044346', '85984044633', '85984044683', '85984044763', '85984044963', '85984045050', '85984045056', '85984045115', '85984045640', '85984045722', '85984046240', '85984046424', '85984046625', '85984046753', '85984046806', '85984046807', '85984046867', '85984047111', '85984047230', '85984047233', '85984047367', '85984047472', '85984047476', '85984047517', '85984047596', '85984048175', '85984048182', '85984048183', '85984048283', '85984048339', '85984048508', '85984048524', '85984048559', '85984048759', '85984048849', '85984049026', '85984049029', '85984049263', '85984049442', '85984049451', '85984049504', '85984049679', '85984049735', '85984049763', '85984049858', '85984049949', '85984050227', '85984050228', '85984050250', '85984050371', '85984050677', '85984050801', '85984050882', '85984050887', '85984050928', '85984051292', '85984051333', '85984051412', '85984051489', '85984051523', '85984051742', '85984051769', '85984051840', '85984051889', '85984051935', '85984052109', '85984052112', '85984052208', '85984052217', '85984052263', '85984052298', '85984052611', '85984052730', '85984052764', '85984052843', '85984053038', '85984053174', '85984053179', '85984053330', '85984053556', '85984053869', '85984053880', '85984053887', '85984053943', '85984053956', '85984054025', '85984054056', '85984054133', '85984054160', '85984054172', '85984054228', '85984054266', '85984054556', '85984054674', '85984054734', '85984054739', '85984054879', '85984054912', '85984055156', '85984055310', '85984055345', '85984055442', '85984055473', '85984055502', '85984055688', '85984055714', '85984055899', '85984055933', '85984056265', '85984056517', '85984056826', '85984056911', '85984056971', '85984057268', '85984057361', '85984057589', '85984057713', '85984057802', '85984057880', '85984058809', '85984059297', '85984059565', '85984059708', '85984060013', '85984060654', '85984060832', '85984061103', '85984061137', '85984061447', '85984061486', '85984061543', '85984061639', '85984061962', '85984062029', '85984062279', '85984062320', '85984062358', '85984062494', '85984062505', '85984062530', '85984063166', '85984063203', '85984063719', '85984063744', '85984063839', '85984064263', '85984064393', '85984064541', '85984064961', '85984065160', '85984065816', '85984066050', '85984066966', '85984067046', '85984067756', '85984067873', '85984068456', '85984069092', '85984069667', '85984069722', '85984069938', '85984070019', '85984070211', '85984070265', '85984070421', '85984070652', '85984070895', '85984071052', '85984071611', '85984071870', '85984072029', '85984072045', '85984072051', '85984072058', '85984072071', '85984072145', '85984072225', '85984072316', '85984072445', '85984072480', '85984072653', '85984072933', '85984073162', '85984073973', '85984074264', '85984074313', '85984074778', '85984075096', '85984075666', '85984076005', '85984076212', '85984076393', '85984076578', '85984076839', '85984076847', '85984077031', '85984077361', '85984077370', '85984077740', '85984077801', '85984078005', '85984078034', '85984078218', '85984078233', '85984078314', '85984078445', '85984078614', '85984079116', '85984079245', '85984079370', '85984079725', '85984079880', '85984079915', '85984080469', '85984080471', '85984080593', '85984080601', '85984081278', '85984081475', '85984081680', '85984082025', '85984082125', '85984082555', '85984082670', '85984082940', '85984082979', '85984083419', '85984083846', '85984084306', '85984084464', '85984084549', '85984084550', '85984084823', '85984084857', '85984085018', '85984085176', '85984085262', '85984085880', '85984086976', '85984087409', '85984088006', '85984088529', '85984089052', '85984089070', '85984089220', '85984089798', '85984090380', '85984090552', '85984090594', '85984090882', '85984090929', '85984091124', '85984091289', '85984091406', '85984091518', '85984092054', '85984092195', '85984092230', '85984092539', '85984093168', '85984093610', '85984093759', '85984093855', '85984094073', '85984094849', '85984095284', '85984096033', '85984098963', '85984099235', '85984099245', '85984099377', '85984099885', '85984100300', '85984100698', '85984100822', '85984101624', '85984101697', '85984102042', '85984102155', '85984102262', '85984102480', '85984102514', '85984102560', '85984102571', '85984103927', '85984104957', '85984105301', '85984105524', '85984106425', '85984107192', '85984107381', '85984107762', '85984108029', '85984108520', '85984108531', '85984108645', '85984108950', '85984109045', '85984109435', '85984109534', '85984110121', '85984110186', '85984110449', '85984110493', '85984110570', '85984110730', '85984110811', '85984111215', '85984111369', '85984111609', '85984111626', '85984111796', '85984111877', '85984111930', '85984112126', '85984112139', '85984112386', '85984112657', '85984113012', '85984113687', '85984113734', '85984113870', '85984113916', '85984114001', '85984114121', '85984114826', '85984114827', '85984115475', '85984115569', '85984115651', '85984116121', '85984116540', '85984116596', '85984116734', '85984116933', '85984117008', '85984117204', '85984117429', '85984117798', '85984118037', '85984118042', '85984118203', '85984118581', '85984118664', '85984118708', '85984118774', '85984119107', '85984119481', '85984119572', '85984119808', '85984120393', '85984120682', '85984121272', '85984122145', '85984122414', '85984123034', '85984123448', '85984124093', '85984124208', '85984125015', '85984125036', '85984126078', '85984126186', '85984126390', '85984126584', '85984126778', '85984126955', '85984127219', '85984127242', '85984127734', '85984128627', '85984128634', '85984128869', '85984128924', '85984129311', '85984129612', '85984130038', '85984130659', '85984130724', '85984130979', '85984131046', '85984131139', '85984131313', '85984131574', '85984131761', '85984131881', '85984132127', '85984132128', '85984132149', '85984132782', '85984132844', '85984133084', '85984133130', '85984133206', '85984133331', '85984133448', '85984133534', '85984134089', '85984134736', '85984135015', '85984135302', '85984135420', '85984135573', '85984</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['10', '27', '27', '27', '46', '30', '27', '1', '5', '29', '1', '35', '16', '43', '27', '27', '27', '11', '5', '28', '1', '49', '27', '27', '1', '27', '0', '27', '11', '1', '28', '10', '3', '27', '3', '28', '27', '31', '1', '25', '1', '27', '27', '40', '27', '27', '28', '27', '27', '12', '28', '5', '7', '6', '28', '40', '49', '1', '2', '8', '78', '1', '1', '27', '5', '27', '1', '27', '27', '11', '1', '28', '12', '27', '27', '1', '5', '27', '27', '2', '27', '27', '27', '25', '7', '27', '28', '1', '11', '27', '1', '1', '27', '21', '13', '6', '27', '5', '1', '0', '28', '27', '28', '27', '27', '27', '27', '27', '27', '7', '28', '5', '5', '27', '27', '47', '28', '27', '34', '1', '35', '5', '8', '12', '28', '27', '12', '49', '28', '27', '6', '27', '1', '1', '17', '5', '27', '1', '1', '28', '31', '1', '27', '12', '5', '27', '39', '49', '19', '16', '28', '27', '5', '27', '8', '27', '4', '35', '8', '30', '35', '1', '27', '27', '10', '40', '1', '27', '27', '49', '27', '29', '27', '27', '1', '28', '43', '32', '45', '30', '27', '27', '6', '27', '5', '2', '27', '7', '49', '13', '28', '6', '27', '27', '27', '27', '26', '27', '27', '27', '28', '49', '1', '27', '11', '28', '27', '27', '27', '27', '1', '18', '28', '27', '27', '27', '1', '27', '1', '49', '10', '27', '5', '49', '1', '11', '27', '49', '27', '27', '5', '49', '27', '7', '5', '28', '1', '29', '27', '11', '31', '38', '27', '15', '27', '27', '49', '17', '41', '8', '27', '1', '28', '30', '28', '3', '27', '30', '30', '5', '27', '10', '1', '49', '27', '28', '1', '27', '4', '1', '28', '5', '27', '27', '12', '28', '10', '27', '27', '48', '1', '1', '1', '27', '30', '1', '27', '27', '27', '29', '27', '5', '27', '27', '6', '1', '30', '27', '28', '1', '12', '5', '29', '25', '27', '49', '27', '27', '6', '11', '27', '27', '27', '27', '11', '27', '1', '27', '27', '27', '27', '27', '30', '27', '49', '28', '28', '23', '40', '27', '28', '27', '27', '27', '5', '11', '27', '27', '1', '5', '11', '28', '27', '27', '27', '28', '9', '5', '27', '11', '27', '1', '35', '1', '27', '1', '27', '27', '1', '30', '27', '27', '28', '17', '27', '27', '1', '27', '35', '49', '27', '49', '27', '27', '11', '27', '12', '27', '27', '8', '4', '49', '11', '27', '35', '4', '28', '27', '27', '27', '5', '18', '1', '5', '27', '27', '1', '28', '27', '1', '1', '11', '1', '1', '28', '114', '9', '27', '27', '5', '28', '27', '27', '1', '23', '27', '27', '5', '1', '27', '1', '5', '27', '27', '27', '27', '87', '27', '28', '31', '39', '34', '27', '27', '27', '9', '13', '9', '1', '17', '27', '35', '27', '30', '12', '27', '27', '49', '6', '27', '27', '27', '1', '28', '1', '30', '27', '27', '27', '12', '27', '27', '27', '1', '28', '0', '27', '49', '27', '27', '1', '28', '27', '27', '49', '27', '27', '27', '49', '27', '27', '6', '49', '1', '27', '9', '1', '28', '42', '13', '31', '27', '15', '8', '49', '27', '5', '27', '8', '27', '29', '27', '27', '49', '27', '14', '27', '28', '27', '27', '49', '29', '11', '27', '27', '12', '27', '27', '27', '27', '27', '1', '27', '5', '22', '1', '27', '27', '49', '17', '29', '11', '27', '27', '5', '13', '1', '10', '27', '28', '27', '27', '27', '27', '27', '5', '24', '27', '1', '1', '27', '1', '30', '27', '27', '27', '1', '14', '19', '25', '27', '27', '27', '27', '49', '27', '30', '11', '30', '5', '27', '27', '1', '27', '28', '27', '1', '29', '27', '27', '1', '5', '1', '37', '49', '1', '5', '2', '82', '5', '27', '27', '30', '8', '27', '5', '27', '27', '27', '28', '49', '27', '27', '27', '27', '28', '5', '27', '27', '1', '27', '14', '5', '49', '31', '1', '27', '1', '27', '5', '27', '27', '27', '28', '1', '12', '40', '27', '43', '27', '27', '1', '27', '49', '49', '21', '27', '27', '22', '27', '7', '12', '27', '27', '0', '1', '27', '27', '27', '28', '1', '7', '28', '49', '27', '27', '27', '7', '28', '16', '1', '1', '27', '12', '10', '12', '27', '27', '4', '27', '27', '30', '5', '12', '29', '27', '27', '17', '27', '27', '13', '5', '27', '12', '16', '49', '27', '1', '27', '6', '49', '29', '27', '28', '18', '28', '49', '27', '27', '27', '30', '27', '7', '23', '49', '12', '16', '27', '1', '5', '1', '27', '27', '27', '27', '27', '27', '27', '49', '27', '28', '27', '1', '27', '27', '27', '27', '27', '49', '21', '27', '28', '27', '27', '28', '35', '27', '49', '1', '27', '27', '26', '27', '38', '27', '1', '6', '27', '27', '28', '7', '28', '27', '27', '27', '27', '12', '5', '6', '27', '18', '28', '17', '27', '27', '28', '23', '14', '27', '12', '29', '28', '28', '27', '27', '27', '27', '28', '28', '49', '5', '27', '12', '27', '27', '27', '49', '27', '27', '12', '8', '27', '28', '28', '1', '9', '28', '27', '27', '27', '1', '1', '10', '1', '28', '27', '12', '1', '7', '27', '27', '27', '27', '28', '27', '27', '27', '5', '27', '12', '46', '27', '27', '31', '35', '17', '28', '27', '20', '24', '23', '1', '41', '36', '49', '49', '7', '28', '49', '27', '27', '5', '5', '27', '1', '5', '17', '27', '28', '13', '7', '49', '28', '27', '27', '27', '1', '34', '42', '35', '27', '28', '28', '28', '35', '11', '27', '5', '5', '28', '28', '27', '28', '1', '28', '13', '27', '28', '27', '28', '30', '28', '28', '18', '27', '5', '1', '76', '28', '28', '1', '5', '1', '28', '26', '2', '28', '1', '7', '12', '28', '37', '11', '28', '27', '27', '27', '27', '28', '28', '27', '20', '8', '30', '14', '27', '4', '10', '4', '49', '28', '28', '1', '1', '22', '27', '1', '10', '28', '11', '28', '77', '28', '2', '27', '30', '27', '27', '31', '1', '28', '28', '12', '27', '28', '10', '30', '27', '9', '27', '18', '28', '0', '12', '28', '49', '27', '27', '27', '27', '30', '1', '28', '27', '50', '31', '1', '27', '1', '27', '28', '28', '28', '27', '7', '1', '28', '27', '1', '27', '31', '28', '27', '1', '28', '1', '49', '49', '27', '28', '27', '27', '1', '27', '28', '27', '5', '26', '12', '1', '28', '2', '8', '13', '1', '12', '1', '28', '27', '1', '30', '7', '7', '37', '27', '28', '8', '5', '27', '28', '27', '27', '13', '13', '27', '30', '13', '13', '27', '1', '28', '27', '28', '27', '31', '27', '13', '28', '27', '27', '28', '12', '27', '27', '7', '1', '29', '27', '27', '1', '5', '27', '13', '27', '28', '49', '27', '6', '28', '27', '1', '27', '27', '21', '28', '31', '46', '27', '28', '5', '5', '27', '27', '30', '7', '27', '28', '28', '28', '30', '9', '17', '1', '3', '30', '7', '27', '28', '27', '7', '37', '27', '14', '13', '28', '27', '27', '27', '1', '27', '27', '27', '27', '28', '6', '28', '27', '12', '27', '47', '49', '28', '28', '27', '27', '13', '14', '28', '12', '28', '7', '27', '28', '27', '27', '1', '1', '27', '14', '0', '1', '27', '1', '1', '31', '1', '5', '39', '35', '27', '28', '11', '30', '27', '1', '27', '49', '27', '28', '28', '27', '47', '27', '28', '28', '5', '28', '30', '11', '49', '27', '28', '1', '28', '28', '28', '27', '49', '30', '27', '28', '30', '27', '15', '49', '8', '28', '12', '27', '17', '28', '27', '30', '49', '1', '28', '28', '27', '27', '27', '49', '1', '26', '1', '27', '49', '1', '6', '27', '5', '28', '1', '27', '11', '16', '28', '114', '27', '27', '27', '34', '1', '6', '28', '49', '21', '27', '27', '27', '28', '10', '1', '27', '27', '27', '49', '1', '28', '28', '27', '31', '28', '28', '28', '49', '49', '27', '27', '27', '8', '28', '1', '11', '5', '1', '1', '27', '32', '49', '27', '9', '33', '27', '5', '28', '27', '31', '28', '27', '27', '27', '27', '27', '39', '30', '12', '13', '28', '34', '1', '27', '27', '28', '28', '15', '11', '27', '28', '1', '27', '1', '35', '27', '7', '17', '1', '35', '23', '27', '28', '1', '5', '28', '2', '21', '27', '28', '28', '28', '11', '49', '32', '28', '14', '14', '30', '27', '1', '28', '28', '28', '23', '1', '27', '27', '27', '28', '47', '27', '28', '1', '27', '27', '28', '42', '49', '27', '27', '5', '28', '27', '1', '28', '27', '26', '27', '27', '28', '28', '8', '5', '0', '49', '28', '28', '5', '28', '27', '28', '28', '41', '8', '27', '27', '27', '6', '27', '27', '27', '6', '1', '28', '30', '5', '27', '12', '2', '5', '28', '15', '5', '27', '28', '27', '12', '28', '28', '5', '27', '12', '28', '27', '27', '6', '1', '30', '28', '27', '28', '12', '27', '13', '1', '49', '31', '27', '12', '28', '27', '28', '27', '33', '27', '40', '27', '28', '28', '27', '0', '20', '27', '1', '43', '28', '28', '1', '49', '33', '27', '10', '28', '27', '28', '27', '27', '2', '27', '27', '49', '1', '28', '28', '43', '27', '27', '28', '49', '5', '28', '146', '10', '18', '28', '27', '27', '27', '28', '27', '28', '28', '28', '11', '1', '5', '6', '27', '8', '5', '9', '28', '1', '27', '28', '18', '27', '6', '6', '26', '27', '7', '27', '49', '8', '27', '75', '21', '58', '27', '27', '21', '27', '21', '6', '27', '29', '27', '27', '62', '69', '65', '17', '27', '49', '8', '27', '8', '5', '27', '1', '30', '1', '27', '32', '32', '49', '5', '5', '4', '13', '32', '33', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '32', '5', '4', '5', '32', '4', '3', '4', '4', '4', '5', '35', '33', '4', '5', '5', '5', '4', '30', '32', '5', '4', '5', '19', '5', '5', '4', '5', '5', '5', '5', '5', '4', '4', '5', '5', '5', '32', '32', '39', '4', '4', '4', '34', '5', '33', '34', '49', '4', '5', '4', '5', '3', '77', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '5', '6', '5', '5', '4', '4', '5', '4', '5', '4', '4', '32', '5', '51', '4', '32', '4', '33', '4', '4', '5', '12', '32', '4', '4', '32', '5', '5', '4', '5', '4', '3', '4', '5', '4', '5', '6', '4', '5', '32', '4', '4', '4', '5', '4', '5', '5', '5', '2', '5', '6', '4', '49', '5', '4', '32', '5', '32', '5', '5', '5', '39', '49', '33', '33', '4', '4', '5', '5', '5', '4', '5', '5', '4', '33', '32', '32', '32', '32', '33', '5', '32', '32', '32', '33', '44', '20', '14', '33', '6', '32', '12', '49', '32', '32', '49', '33', '34', '5', '32', '32', '32', '32', '4', '32', '32', '5', '6', '42', '33', '35', '32', '31', '31', '5', '32', '49', '32', '4', '27', '11', '32', '4', '69', '32', '6', '32', '34', '5', '32', '49', '32', '21', '32', '32', '5', '30', '33', '32', '16', '32', '33', '34', '32', '48', '49', '31', '32', '6', '32', '34', '34', '5', '33', '49', '39', '32', '33', '33', '4', '32', '11', '32', '6', '6', '33', '32', '33', '33', '31', '32', '32', '5', '32', '4', '32', '4', '32', '32', '33', '32', '32', '5', '34', '32', '33', '32', '49', '32', '27', '31', '4', '12', '33', '34', '49', '5', '31', '32', '6', '30', '5', '32', '27', '34', '32', '22', '32', '4', '32', '33', '32', '32', '4', '6', '33', '33', '72', '32', '32', '5', '30', '32', '5', '32', '32', '60', '32', '33', '15', '34', '32', '33', '33', '32', '32', '12', '33', '33', '33', '32', '32', '5', '32', '33', '7', '32', '46', '5', '33', '32', '41', '34', '32', '32', '32', '5', '32', '32', '33', '33', '33', '32', '32', '7', '33', '32', '32', '32', '12', '32', '5', '32', '49', '9', '30', '32', '33', '33', '33', '27', '5', '5', '31', '32', '6', '30', '79', '35', '49', '34', '32', '33', '33', '32', '32', '32', '49', '32', '70', '26', '32', '32', '6', '32', '31', '5', '28', '32', '5', '5', '10', '4', '49', '33', '5', '32', '32', '6', '5', '4', '4', '4', '5', '5', '32', '5', '4', '5', '5', '75', '4', '4', '4', '4', '34', '4', '5', '5', '49', '42', '4', '5', '32', '2', '4', '5', '33', '4', '5', '5', '5', '5', '5', '4', '11', '32', '49', '4', '30', '5', '27', '4', '31', '29', '2', '4', '5', '33', '5', '4', '5', '32', '4', '4', '5', '32', '5', '4', '32', '14', '37', '5', '4', '33', '4', '5', '5', '31', '4', '4', '5', '32', '33', '33', '5', '5', '5', '5', '4', '4', '4', '4', '5', '5', '30', '4', '0', '4', '16', '4', '5', '4', '4', '5', '5', '5', '5', '4', '5', '4', '30', '5', '5', '5', '15', '5', '4', '5', '5', '5', '5', '7', '4', '4', '4', '32', '32', '5', '32', '4', '4', '5', '4', '4', '4', '4', '4', '4', '4', '4', '30', '4', '5', '4', '4', '5', '34', '4', '5', '64', '4', '4', '4', '4', '4', '4', '4', '5', '4', '4', '5', '5', '5', '4', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '31', '4', '4', '5', '4', '5', '35', '4', '4', '4', '5', '4', '4', '5', '4', '5', '4', '5', '4', '5', '4', '4', '4', '4', '32', '4', '4', '31', '13', '4', '11', '4', '32', '5', '4', '33', '5', '32', '4', '30', '4', '5', '32', '33', '5', '5', '5', '4', '5', '3', '4', '4', '5', '32', '4', '4', '5', '31', '32', '5', '49', '12', '5', '4', '5', '4', '33', '2', '5', '5', '30', '80', '4', '33', '33', '3', '5', '34', '31', '34', '7', '59', '32', '33', '5', '32', '95', '5', '32', '32', '5', '5', '32', '30', '5', '32', '5', '4', '4', '32', '5', '4', '4', '5', '5', '33', '11', '4', '32', '4', '4', '33', '4', '63', '4', '4', '4', '34', '4', '18', '33', '32', '33', '32', '4', '32', '47', '5', '4', '32', '5', '5', '49', '35', '32', '33', '32', '5', '7', '32', '4', '32', '21', '12', '5', '32', '32', '4', '4', '4', '5', '5', '4', '32', '5', '4', '5', '32', '5', '4', '34', '4', '5', '4', '5', '5', '4', '5', '4', '4', '30', '32', '5', '33', '33', '32', '31', '33', '32', '32', '4', '6', '34', '1', '15', '30', '32', '5', '4', '32', '4', '5', '32', '2', '49', '8', '32', '11', '6', '5', '31', '33', '12', '34', '33', '31', '4', '33', '34', '34', '32', '32', '32', '32', '8', '32', '33', '4', '74', '4', '33', '32', '28', '4', '5', '33', '14', '32', '33', '31', '5', '32', '5', '33', '33', '32', '33', '32', '5', '32', '33', '23', '27', '31', '31', '34', '31', '5', '41', '32', '32', '33', '32', '11', '32', '7', '11', '32', '33', '32', '33', '34', '32', '32', '4', '32', '31', '32', '32', '32', '32', '33', '46', '32', '66', '32', '33', '30', '5', '32', '32', '32', '4', '32', '32', '32', '32', '33', '32', '49', '32', '32', '32', '33', '33', '32', '5', '33', '32', '12', '32', '33', '16', '32', '33', '5', '32', '32', '9', '34', '64', '4', '32', '32', '33', '32', '31', '32', '32', '10', '32', '6', '33', '13', '32', '5', '5', '4', '31', '3', '32', '25', '40', '34', '32', '32', '34', '5', '32', '44', '33', '8', '32', '33', '32', '33', '5', '33', '32', '32', '32', '18', '30', '32', '33', '32', '49', '32', '32', '32', '6', '17', '33', '33', '5', '49', '32', '19', '4', '5', '5', '4', '5', '7', '4', '11', '33', '32', '32', '4', '3', '32', '27', '4', '4', '33', '5', '4', '34', '31', '5', '30', '1', '4', '5', '32', '5', '4', '5', '4', '61', '9', '4', '11', '5', '32', '33', '33', '34', '4', '33', '34', '4', '32', '32', '5', '32', '4', '31', '32', '33', '5', '4', '33', '5', '4', '27', '5', '5', '4', '35', '5', '5', '4', '5', '4', '4', '4', '33', '5', '32', '5', '5', '5', '27', '4', '4', '4', '4', '4', '5', '5', '5', '5', '6', '5', '5', '5', '5', '4', '5', '5', '5', '4', '5', '4', '66', '4', '4', '4', '4', '5', '4', '4', '4', '32', '7', '33', '5', '7', '4', '5', '55', '32', '43', '21', '5', '4', '5', '3', '4', '5', '4', '4', '32', '32', '33', '34', '5', '69', '4', '32', '4', '32', '25', '30', '32', '30', '32', '63', '35', '33', '5', '32', '5', '32', '4', '5', '4', '5', '4', '5', '4', '4', '33', '33', '33', '4', '30', '5', '33', '32', '4', '32', '33', '27', '5', '4', '32', '5', '4', '32', '5', '5', '5', '33', '4', '5', '4', '4', '4', '5', '5', '7', '33', '5', '32', '5', '5', '49', '5', '4', '4', '5', '4', '4', '5', '4', '4', '5', '32', '4', '4', '4', '4', '4', '5', '32', '4', '5', '4', '4', '4', '5', '4', '5', '4', '4', '61', '4', '5', '4', '38', '33', '4', '5', '34', '13', '4', '4', '32', '32', '32', '4', '5', '5', '32', '5', '32', '4', '33', '33', '33', '5', '5', '33', '5', '5', '4', '12', '4', '28', '5', '5', '5', '5', '5', '4', '5', '5', '4', '32', '6', '4', '4', '5', '9', '13', '32', '34', '4', '33', '15', '32', '32', '4', '32', '5', '5', '27', '4', '5', '4', '4', '5', '4', '4', '4', '5', '4', '21', '5', '5', '33', '5', '4', '34', '5', '4', '4', '4', '5', '4', '4', '5', '5', '4', '5', '5', '13', '4', '5', '4', '5', '4', '4', '31', '5', '4', '5', '4', '4', '5', '30', '4', '4', '5', '4', '5', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '5', '5', '5', '46', '4', '4', '4', '4', '5', '4', '5', '22', '5', '5', '4', '49', '5', '5', '32', '5', '4', '5', '5', '5', '4', '4', '32', '4', '30', '32', '4', '4', '4', '4', '5', '5', '12', '5', '4', '5', '4', '33', '4', '4', '4', '32', '4', '4', '4', '4', '5', '4', '4', '32', '4', '35', '5', '4', '4', '5', '4', '5', '32', '0', '67', '4', '31', '4', '5', '30', '4', '17', '3', '5', '4', '4', '4', '5', '22', '5', '4', '4', '4', '4', '5', '5', '5', '5', '4', '5', '5', '2', '4', '4', '5', '32', '5', '5', '5', '4', '4', '4', '50', '4', '5', '4', '4', '5', '5', '5', '32', '5', '30', '32', '4', '5', '32', '4', '4', '4', '4', '4', '5', '5', '4', '5', '68', '5', '29', '4', '5', '5', '4', '5', '5', '6', '6', '6', '6', '6', '6', '5', '6', '6', '32', '35', '6', '33', '6', '24', '5', '34', '33', '32', '30', '31', '32', '33', '13', '32', '32', '93', '8', '33', '32', '32', '5', '33', '31', '32', '32', '33', '13', '32', '9', '32', '30', '3', '4', '9', '33', '3', '32', '33', '19', '32', '32', '33', '32', '33', '30', '30', '32', '5', '33', '32', '81', '7', '7', '32', '79', '33', '15', '32', '32', '32', '32', '5', '30', '32', '7', '32', '33', '5', '32', '33', '33', '35', '33', '32', '33', '33', '33', '31', '33', '32', '34', '32', '32', '32', '34', '33', '7', '33', '13', '32', '32', '32', '49', '32', '33', '33', '32', '32', '4', '32', '32', '33', '33', '4', '32', '33', '33', '12', '49', '33', '32', '80', '32', '33', '32', '25', '32', '34', '33', '4', '32', '32', '33', '32', '33', '33', '32', '33', '32', '4', '21', '32', '5', '32', '49', '71', '33', '33', '16', '13', '4', '32', '32', '5', '27', '18', '34', '33', '32', '65', '32', '32', '22', '27', '49', '34', '33', '33', '5', '4', '5', '5', '44', '32', '30', '12', '32', '32', '11', '33', '33', '33', '33', '32', '4', '11', '32', '32', '11', '8', '32', '4', '5', '5', '5', '33', '4', '4', '4', '70', '12', '27', '32', '32', '5', '17', '33', '32', '32', '8', '34', '32', '59', '32', '32', '33', '31', '31', '32', '49', '5', '15', '13', '33', '34', '32', '4', '33', '32', '4', '8', '32', '33', '22', '34', '49', '11', '33', '32', '32', '5', '28', '32', '31', '32', '32', '12', '32', '32', '32', '28', '49', '30', '33', '33', '32', '3', '18', '30', '33', '4', '32', '4', '31', '1', '12', '28', '5', '49', '33', '23', '32', '32', '33', '33', '33', '8', '33', '4', '29', '4', '32', '13', '32', '33', '33', '34', '32', '31', '33', '32', '4', '5', '32', '32', '5', '33', '15', '11', '33', '9', '50', '59', '13', '32', '32', '34', '33', '34', '33', '33', '33', '32', '20', '20', '33', '33', '34', '33', '32', '31', '12', '32', '33', '33', '5', '32', '32', '31', '33', '5', '32', '33', '7', '33', '32', '26', '13', '34', '12', '4', '5', '12', '49', '32', '33', '33', '32', '32', '32', '33', '33', '32', '17', '13', '32', '33', '10', '32', '32', '30', '32', '32', '32', '8', '5', '32', '32', '32', '32', '32', '12', '30', '12', '34', '33', '32', '45', '32', '34', '28', '32', '4', '4', '17', '32', '33', '49', '33', '26', '33', '49', '33', '31', '32', '32', '14', '5', '32', '32', '32', '32', '27', '32', '5', '33', '32', '32', '32', '32', '32', '32', '13', '15', '32', '30', '32', '32', '32', '32', '26', '32', '18', '33', '32', '32', '32', '49', '32', '33', '31', '32', '4', '5', '34', '32', '33', '33', '34', '32', '32', '6', '33', '5', '31', '32', '33', '32', '31', '29', '12', '32', '32', '5', '33', '30', '33', '32', '32', '31', '32', '39', '7', '61', '25', '34', '33', '32', '32', '7', '32', '31', '31', '33', '10', '34', '32', '31', '22', '32', '20', '9', '32', '32', '33', '30', '12', '33', '33', '33', '27', '5', '32', '5', '27', '24', '12', '32', '32', '62', '32', '22', '32', '5', '32', '33', '24', '49', '32', '32', '32', '4', '6', '33', '4', '33', '32', '32', '32', '32', '1', '11', '32', '26', '24', '5', '5', '32', '7', '5', '31', '33', '5', '54', '32', '33', '32', '32', '32', '32', '30', '32', '32', '12', '31', '32', '33', '33', '32', '33', '49', '33', '22', '32', '12', '32', '27', '55', '32', '34', '60', '32', '4', '5', '4', '4', '4', '4', '4', '4', '4', '5', '6', '4', '4', '34', '33', '4', '4', '33', '5', '35', '33', '33', '4', '5', '5', '33', '32', '32', '32', '5', '4', '4', '5', '5', '5', '32', '32', '4', '49', '5', '15', '33', '32', '32', '32', '34', '32', '60', '32', '32', '32', '27', '33', '30', '15', '5', '5', '72', '4', '4', '33', '33', '11', '32', '32', '32', '44', '63', '6', '7', '32', '32', '32', '5', '4', '19', '32', '14', '1', '33', '32', '71', '4', '48', '4', '31', '34', '5', '35', '5', '32', '32', '33', '32', '32', '26', '13', '32', '28', '32', '6', '21', '31', '64', '11', '33', '32', '32', '34', '5', '32', '26', '32', '5', '14', '32', '5', '5', '32', '4', '39', '13', '4', '35', '0', '32', '33', '33', '32', '32', '32', '49', '15', '33', '32', '32', '27', '32', '32', '5', '46', '11', '24', '33', '11', '4', '32', '12', '5', '5', '5', '32', '33', '32', '1', '32', '7', '13', '32', '32', '32', '13', '5', '30', '5', '4', '32', '30', '33', '33', '4', '7', '5', '33', '33', '33', '32', '14', '29', '6', '13', '32', '10', '33', '33', '5', '30', '12', '21', '33', '32', '33', '31', '30', '32', '18', '34', '32', '32', '34', '30', '12', '32', '32', '30', '32', '33', '34', '30', '32', '5', '33', '32', '12', '33', '33', '32', '32', '32', '11', '32', '32', '33', '32', '33', '32', '30', '32', '5', '32', '32', '25', '32', '33', '31', '32', '14', '33', '57', '30', '32', '49', '27', '5', '32', '12', '33', '33', '32', '32', '33', '21', '33', '33', '32', '10', '33', '33', '33', '32', '4', '4', '32', '32', '31', '33', '33', '33', '32', '24', '5', '35', '32', '32', '5', '3', '34', '32', '32', '5', '32', '33', '57', '33', '4', '34', '52', '33', '32', '33', '32', '33', '33', '1', '33', '33', '33', '22', '27', '33', '32', '32', '34', '33', '7', '12', '1', '4', '33', '32', '33', '33', '32', '32', '31', '32', '32', '29', '33', '31', '49', '5', '11', '34', '32', '32', '25', '35', '32', '25', '32', '33', '33', '5', '32', '27', '32', '31', '30', '30', '34', '32', '31', '5', '13', '30', '32', '4', '33', '32', '32', '32', '34', '4', '33', '30', '31', '32', '32', '33', '34', '49', '32', '5', '31', '33', '32', '32', '49', '8', '33', '32', '5', '32', '32', '33', '5', '32', '4', '36', '5', '32', '4', '32', '32', '18', '33', '33', '34', '34', '32', '8', '41', '32', '33', '49', '32', '32', '32', '5', '30', '49', '27', '32', '55', '49', '49', '26', '5', '33', '33', '33', '32', '32', '34', '32', '32', '12', '32', '11', '31', '33', '34', '32', '21', '28', '57', '32', '30', '4', '32', '4', '32', '17', '31', '33', '32', '32', '32', '32', '5', '30', '32', '32', '32', '32', '34', '32', '32', '32', '32', '32', '32', '33', '33', '13', '32', '34', '32', '32', '32', '32', '32', '5', '33', '32', '32', '33', '32', '5', '12', '33', '32', '5', '32', '32', '32', '5', '32', '5', '16', '34', '33', '33', '4', '30', '11', '34', '32', '35', '94', '10', '4', '14', '32', '28', '4', '32', '32', '17', '15', '4', '27', '4', '32', '32', '5', '34', '32', '32', '7', '33', '18', '31', '58', '20', '32', '11', '67', '36', '4', '27', '12', '32', '33', '26', '33', '5', '32', '32', '32', '32', '33', '77', '4', '33', '35', '32', '31', '31', '24', '32', '32', '33', '32', '24', '29', '33', '32', '32', '32', '24', '32', '5', '32', '16', '33', '33', '32', '32', '32', '11', '32', '5', '32', '32', '32', '32', '45', '32', '32', '31', '32', '32', '15', '32', '30', '31', '32', '5', '33', '5', '32', '32', '32', '32', '52', '26', '32', '32', '5', '33', '2', '34', '36', '33', '49', '33', '32', '5', '32', '6', '14', '32', '33', '32', '31', '31', '32', '33', '32', '33', '32', '32', '5', '32', '28', '32', '33', '32', '33', '8', '32', '5', '33', '12', '48', '32', '32', '32', '32', '32', '33', '4', '32', '13', '8', '32', '32', '33', '38', '33', '34', '33', '6', '33', '32', '32', '32', '13', '5', '4', '32', '16', '34', '7', '11', '12', '5', '11', '9', '33', '11', '33', '4', '34', '32', '32', '6', '49', '31', '32', '32', '5', '32', '4', '32', '32', '15', '6', '49', '32', '5', '32', '32', '32', '32', '6', '32', '32', '33', '32', '5', '11', '7', '5', '32', '31', '45', '33', '31', '32', '30', '6', '33', '33', '31', '34', '70', '1', '32', '31', '5', '32', '19', '5', '32', '32', '32', '32', '32', '31', '4', '32', '4', '32', '32', '11', '33', '32', '49', '33', '32', '33', '5', '32', '32', '33', '12', '49', '33', '32', '32', '11', '32', '32', '32', '33', '26', '33', '32', '32', '26', '0', '32', '31', '10', '32', '4', '31', '27', '5', '32', '33', '51', '12', '49', '6', '33', '33', '34', '32', '32', '32', '33', '32', '33', '5', '33', '32', '4', '49', '34', '32', '32', '5', '25', '31', '32', '33', '2', '5', '32', '14', '32', '32', '78', '32', '32', '32', '9', '20', '33', '33', '34', '32', '15', '33', '31', '32', '31', '32', '7', '11', '33', '32', '22', '49', '32', '32', '31', '33', '33', '32', '24', '32', '34', '33', '32', '34', '33', '14', '32', '33', '33', '19', '32', '32', '32', '14', '32', '8', '33', '33', '33', '32', '1', '33', '32', '32', '33', '27', '33', '11', '32', '33', '5', '32', '32', '12', '5', '11', '32', '33', '32', '32', '33', '32', '32', '45', '9', '32', '33', '32', '32', '32', '32', '32', '13', '32', '32', '5', '32', '32', '8', '7', '32', '33', '13', '49', '38', '6', '32', '33', '33', '19', '32', '32', '4', '4', '32', '32', '32', '33', '5', '33', '32', '12', '31', '32', '32', '33', '32', '38', '49', '33', '11', '32', '14', '6', '32', '33', '5', '5', '31', '32', '32', '32', '49', '32', '30', '70', '5', '33', '4', '16', '32', '32', '4', '32', '63', '6', '33', '49', '49', '5', '33', '32', '33', '33', '32', '5', '22', '5', '32', '11', '33', '32', '32', '11', '30', '33', '30', '34', '24', '21', '5', '32', '32', '32', '9', '13', '32', '48', '18', '5', '8', '7', '33', '32', '32', '32', '32', '19', '8', '32', '30', '33', '5', '32', '33', '32', '32', '32', '35', '11', '4', '32', '31', '32', '32', '32', '33', '33', '32', '10', '32', '32', '32', '1', '30', '7', '24', '33', '33', '32', '4', '33', '32', '5', '10', '27', '32', '33', '34', '32', '33', '33', '32', '32', '32', '32', '32', '32', '5', '33', '4', '32', '5', '32', '32', '7', '32', '33', '33', '32', '30', '16', '32', '5', '5', '5', '5', '5', '31', '33', '33', '4', '33', '32', '32', '5', '32', '33', '24', '31', '33', '8', '33', '32', '32', '32', '5', '32', '32', '5', '12', '41', '8', '33', '32', '32', '17', '5', '32', '32', '49', '32', '32', '4', '32', '9', '32', '33', '31', '33', '33', '31', '5', '32', '32', '4', '32', '32', '27', '32', '32', '32', '33', '32', '12', '49', '13', '32', '32', '30', '32', '5', '11', '32', '32', '3', '4', '33', '32', '58', '33', '30', '33', '49', '32', '33', '32', '16', '4', '33', '16', '33', '32', '5', '15', '33', '33', '32', '32', '35', '32', '33', '32', '34', '32', '32', '33', '10', '32', '31', '34', '33', '12', '32', '33', '27', '5', '4', '32', '32', '32', '31', '32', '33', '33', '31', '32', '33', '33', '32', '32', '6', '32', '49', '32', '6', '5', '4', '33', '15', '32', '32', '32', '5', '32', '33', '49', '32', '32', '32', '32', '33', '17', '32', '32', '4', '32', '31', '32', '37', '35', '1', '32', '12', '30', '33', '5', '32', '20', '5', '5', '32', '32', '49', '31', '32', '32', '6', '4', '32', '26', '31', '5', '5', '32', '32', '32', '33', '32', '32', '33', '30', '33', '32', '31', '32', '5', '32', '32', '32', '4', '49', '31', '32', '32', '33', '31', '32', '32', '11', '32', '49', '31', '4', '36', '5', '3', '9', '31', '12', '32', '32', '30', '4', '4', '4', '33', '49', '32', '32', '30', '4', '49', '31', '31', '33', '33', '32', '34', '32', '49', '32', '32', '5', '4', '8', '32', '32', '33', '12', '5', '32', '32', '32', '32', '32', '32', '8', '32', '32', '32', '32', '33', '2', '33', '32', '30', '33', '31', '32', '23', '30', '25', '5', '66', '36', '5', '32', '33', '31', '32', '32', '10', '33', '33', '14', '33', '33', '32', '13', '9', '18', '32', '34', '2', '32', '32', '4', '49', '5', '19', '4', '32', '33', '33', '35', '31', '22', '32', '32', '5', '30', '28', '32', '32', '32', '34', '32', '4', '6', '31', '32', '4', '32', '4', '33', '32', '33', '31', '6', '4', '32', '29', '13', '34', '32', '11', '34', '32', '8', '32', '33', '32', '49', '4', '32', '36', '33', '33', '7', '32', '32', '85', '32', '32', '33', '32', '9', '5', '4', '32', '12', '32', '32', '4', '30', '16', '32', '32', '1', '32', '33', '5', '32', '49', '33', '72', '31', '11', '5', '33', '49', '4', '31', '6', '33', '17', '33', '32', '5', '32', '32', '32', '14', '5', '26', '5', '17', '31', '4', '33', '30', '4', '32', '27', '23', '12', '32', '32', '32', '32', '32', '25', '32', '30', '32', '31', '33', '32', '32', '4', '5', '4', '33', '32', '33', '32', '32', '32', '32', '49', '31', '25', '32', '6', '33', '32', '5', '65', '8', '7', '32', '32', '32', '49', '32', '32', '6', '32', '15', '32', '11', '32', '32', '31', '32', '34', '6', '33', '32', '33', '32', '31', '15', '33', '32', '33', '32', '34', '25', '32', '32', '32', '33', '32', '50', '33', '32', '32', '49', '32', '6', '32', '5', '32', '32', '49', '32', '32', '5', '32', '4', '49', '32', '32', '33', '9', '32', '16', '33', '32', '33', '31', '4', '8', '5', '35', '5', '49', '6', '49', '32', '32', '32', '34', '32', '1', '9', '49', '32', '33', '4', '30', '49', '30', '4', '33', '32', '5', '30', '33', '11', '32', '32', '49', '4', '5', '33', '31', '5', '5', '25', '58', '32', '32', '13', '5', '31', '30', '32', '40', '12', '32', '12', '34', '33', '5', '35', '22', '25', '33', '28', '30', '5', '32', '27', '33', '33', '32', '5', '33', '5', '33', '30', '32', '9', '5', '30', '33', '48', '32', '12', '32', '32', '25', '32', '4', '32', '32', '16', '4', '5', '32', '45', '32', '5', '33', '32', '54', '14', '7', '5', '32', '4', '47', '33', '49', '5', '30', '7', '30', '5', '6', '30', '32', '5', '7', '5', '33', '32', '33', '5', '49', '30', '30', '35', '4', '8', '33', '32', '30', '8', '32', '5', '5', '32', '15', '30', '5', '32', '5', '72', '13', '10', '31', '4', '28', '20', '71', '32', '5', '19', '33', '32', '32', '7', '10', '94', '32', '32', '33', '28', '8', '34', '15', '4', '32', '1', '32', '15', '8', '32', '8', '5', '33', '34', '6', '32', '32', '12', '11', '79', '32', '32', '32', '33', '33', '18', '5', '49', '5', '33', '32', '6', '32', '13', '4', '33', '32', '4', '33', '4', '5', '73', '33', '31', '12', '13', '33', '32', '32', '33', '23', '33', '33', '33', '32', '32', '32', '33', '57', '4', '35', '6', '31', '33', '5', '30', '30', '32', '33', '6', '32', '32', '5', '8', '82', '33', '32', '34', '11', '5', '15', '33', '32', '6', '32', '5', '33', '32', '32', '32', '33', '33', '11', '28', '28', '32', '5', '35', '33', '32', '33', '32', '33', '32', '5', '32', '32', '33', '19', '32', '49', '33', '33', '32', '3', '32', '32', '34', '32', '5', '32', '32', '33', '13', '29', '35', '32', '32', '5', '29', '33', '5', '33', '32', '33', '33', '7', '32', '33', '32', '7', '32', '14', '5', '32', '32', '32', '5', '5', '5', '4', '5', '5', '5', '14', '8', '32', '33', '32', '30', '32', '33', '24', '11', '32', '4', '32', '32', '27', '32', '32', '51', '31', '33', '49', '6', '33', '12', '33', '5', '33', '8', '5', '33', '32', '30', '9', '31', '33', '32', '14', '5', '32', '32', '32', '32', '32', '49', '32', '32', '32', '21', '33', '33', '32', '32', '32', '33', '32', '33', '32', '19', '23', '33', '33', '32', '32', '32', '33', '33', '30', '32', '33', '5', '32', '4', '32', '32', '7', '33', '5', '5', '5', '30', '5', '32', '30', '12', '7', '53', '6', '32', '6', '5', '5', '48', '33', '34', '4', '33', '32', '32', '33', '8', '32', '32', '33', '32', '32', '32', '12', '32', '5', '33', '32', '33', '15', '32', '16', '32', '33', '32', '32', '32', '32', '27', '33', '32', '32', '34', '33', '32', '34', '7', '32', '33', '32', '32', '33', '48', '12', '33', '32', '33', '33', '32', '33', '4', '5', '32', '33', '32', '32', '61', '13', '32', '32', '35', '32', '35', '32', '32', '33', '85', '32', '5', '30', '32', '33', '32', '5', '33', '4', '4', '32', '5', '4', '32', '25', '34', '32', '11', '32', '33', '32', '5', '4', '32', '32', '33', '47', '33', '12', '12', '32', '32', '33', '7', '32', '32', '32', '30', '32', '32', '32', '32', '4', '32', '33', '5', '31', '8', '11', '76', '32', '6', '32', '11', '49', '5', '25', '49', '32', '11', '4', '32', '32', '32', '33', '32', '32', '71', '32', '4', '32', '32', '33', '32', '12', '32', '29', '13', '12', '5', '31', '32', '32', '34', '33', '31', '8', '33', '32', '32', '33', '33', '32', '32', '9', '12', '32', '33', '32', '46', '32', '32', '34', '32', '33', '11', '5', '32', '32', '33', '30', '32', '21', '32', '33', '33', '33', '32', '33', '14', '33', '32', '32', '33', '33', '7', '33', '32', '45', '42', '32', '51', '1', '33', '8', '32', '33', '33', '5', '33', '32', '32', '10', '33', '32', '32', '32', '32', '32', '33', '31', '5', '6', '5', '10', '32', '30', '33', '5', '32', '27', '38', '12', '5', '32', '33', '32', '32', '12', '32', '67', '34', '33', '32', '32', '32', '33', '8', '33', '33', '60', '7', '33', '32', '8', '5', '61', '32', '32', '5', '7', '32', '19', '32', '6', '32', '33', '4', '49', '34', '33', '32', '32', '31', '49', '30', '10', '11', '33', '33', '33', '32', '30', '32', '32', '11', '33', '33', '32', '49', '15', '32', '64', '12', '33', '5', '6', '5', '30', '33', '32', '33', '11', '32', '26', '34', '31', '33', '33', '49', '13', '</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atend</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>['85974001107', '85981010387', '85981010504', '85981010801', '85981011300', '85981011982', '85981012709', '85981012859', '85981012916', '85981013105', '85981013139', '85981013252', '85981014486', '85981015083', '85981015199', '85981015345', '85981015408', '85981015858', '85981018191', '85981019737', '85981019859', '85981020615', '85981021220', '85981021847', '85981021858', '85981023473', '85981024243', '85981024932', '85981025159', '85981026077', '85981026188', '85981026342', '85981029941', '85981034608', '85981035347', '85981037998', '85981038369', '85981040609', '85981041303', '85981042289', '85981046232', '85981047325', '85981047447', '85981050094', '85981050305', '85981050670', '85981050778', '85981050921', '85981051007', '85981051157', '85981051236', '85981051357', '85981051407', '85981051960', '85981052023', '85981052147', '85981052388', '85981053361', '85981053645', '85981053870', '85981054245', '85981054310', '85981054721', '85981054784', '85981055402', '85981055606', '85981055887', '85981056204', '85981056432', '85981057133', '85981057473', '85981057594', '85981057657', '85981058510', '85981058575', '85981059167', '85981060358', '85981060840', '85981060881', '85981060903', '85981060912', '85981061514', '85981062036', '85981062783', '85981062811', '85981063144', '85981063180', '85981063445', '85981063577', '85981063706', '85981063708', '85981063769', '85981064311', '85981064501', '85981064633', '85981066228', '85981066596', '85981066800', '85981067063', '85981067120', '85981067303', '85981067738', '85981068259', '85981068383', '85981068838', '85981069073', '85981069268', '85981069285', '85981069288', '85981069331', '85981069531', '85981069805', '85981070139', '85981070716', '85981070933', '85981072516', '85981074292', '85981074824', '85981077799', '85981079793', '85981080110', '85981081102', '85981081645', '85981081717', '85981081963', '85981082567', '85981082798', '85981083944', '85981083955', '85981084430', '85981085176', '85981085425', '85981086055', '85981087566', '85981090951', '85981092003', '85981094270', '85981095658', '85981096027', '85981097092', '85981097525', '85981099771', '85981099834', '85981104139', '85981105541', '85981111379', '85981111687', '85981112198', '85981112368', '85981113354', '85981116111', '85981116475', '85981117229', '85981117240', '85981117970', '85981118916', '85981119356', '85981121743', '85981121756', '85981121918', '85981122659', '85981122830', '85981124417', '85981125198', '85981125364', '85981127000', '85981127863', '85981128332', '85981128640', '85981129033', '85981130954', '85981131390', '85981132338', '85981132657', '85981132861', '85981133001', '85981136515', '85981137269', '85981137935', '85981138484', '85981139818', '85981141110', '85981141235', '85981142047', '85981142397', '85981144074', '85981144194', '85981144290', '85981144476', '85981145210', '85981145431', '85981146150', '85981147761', '85981148652', '85981149605', '85981149798', '85981149833', '85981150270', '85981152513', '85981152668', '85981152923', '85981153276', '85981154070', '85981154704', '85981154767', '85981155516', '85981155609', '85981155832', '85981157497', '85981159783', '85981160701', '85981162279', '85981163532', '85981168773', '85981169336', '85981170375', '85981170419', '85981172174', '85981172237', '85981173080', '85981173491', '85981173596', '85981174595', '85981175102', '85981175961', '85981176245', '85981176511', '85981176843', '85981176855', '85981177377', '85981177436', '85981178111', '85981180220', '85981180748', '85981181223', '85981181460', '85981184568', '85981185113', '85981185397', '85981185432', '85981186162', '85981187777', '85981187790', '85981188522', '85981190449', '85981190603', '85981190941', '85981191324', '85981191501', '85981192668', '85981193462', '85981194504', '85981195274', '85981195777', '85981196765', '85981199009', '85981200624', '85981204580', '85981205000', '85981207224', '85981210397', '85981211722', '85981211785', '85981212297', '85981212335', '85981215121', '85981215323', '85981217007', '85981217070', '85981217271', '85981217334', '85981217865', '85981217880', '85981217928', '85981219726', '85981220015', '85981220097', '85981220132', '85981221107', '85981221148', '85981222412', '85981224119', '85981224486', '85981224995', '85981225097', '85981225167', '85981226403', '85981227172', '85981227283', '85981227812', '85981228111', '85981228405', '85981228468', '85981229862', '85981229918', '85981229981', '85981230013', '85981230104', '85981233010', '85981233031', '85981233110', '85981234275', '85981235443', '85981237281', '85981238571', '85981240151', '85981240906', '85981241794', '85981243937', '85981245200', '85981245595', '85981245660', '85981246453', '85981246810', '85981247191', '85981247682', '85981247801', '85981248056', '85981248614', '85981248938', '85981249006', '85981249077', '85981249520', '85981249804', '85981250065', '85981251340', '85981252190', '85981252202', '85981252814', '85981253454', '85981256347', '85981256415', '85981256918', '85981257594', '85981257644', '85981258954', '85981259116', '85981259996', '85981260093', '85981260293', '85981261976', '85981264023', '85981265628', '85981266155', '85981266554', '85981267575', '85981268163', '85981269254', '85981270887', '85981273817', '85981276088', '85981277050', '85981277171', '85981277778', '85981277862', '85981278172', '85981278481', '85981281110', '85981281122', '85981283976', '85981284254', '85981284771', '85981284904', '85981285694', '85981285757', '85981286755', '85981287954', '85981288208', '85981288338', '85981289201', '85981290315', '85981291170', '85981291852', '85981292335', '85981292898', '85981293237', '85981296943', '85981297006', '85981297774', '85981298411', '85981298474', '85981299369', '85981300207', '85981300265', '85981301018', '85981301029', '85981301090', '85981301430', '85981302820', '85981303653', '85981304383', '85981304684', '85981304736', '85981304842', '85981305581', '85981306366', '85981307620', '85981307802', '85981308045', '85981308259', '85981308292', '85981308328', '85981308337', '85981308391', '85981310114', '85981310742', '85981311091', '85981311398', '85981312075', '85981313089', '85981313134', '85981313616', '85981313627', '85981314051', '85981314422', '85981315654', '85981316754', '85981318080', '85981323921', '85981325550', '85981327070', '85981327436', '85981327760', '85981328852', '85981330136', '85981330758', '85981331850', '85981331913', '85981332190', '85981333065', '85981333339', '85981334650', '85981334713', '85981334761', '85981335534', '85981337373', '85981338263', '85981338307', '85981342092', '85981342565', '85981343138', '85981343533', '85981344833', '85981345060', '85981347012', '85981347371', '85981348351', '85981348558', '85981349404', '85981351875', '85981352588', '85981352826', '85981353374', '85981353997', '85981354648', '85981355846', '85981357814', '85981359310', '85981360852', '85981361507', '85981361779', '85981362003', '85981362066', '85981363777', '85981365886', '85981366880', '85981367170', '85981368633', '85981370043', '85981370894', '85981371153', '85981371868', '85981372645', '85981374219', '85981375527', '85981375801', '85981375825', '85981376079', '85981377391', '85981378159', '85981378792', '85981378905', '85981379505', '85981379662', '85981380597', '85981380924', '85981381707', '85981381999', '85981383237', '85981383353', '85981384426', '85981385151', '85981385624', '85981385673', '85981385841', '85981386704', '85981386821', '85981387227', '85981387362', '85981388619', '85981391330', '85981391423', '85981391880', '85981392100', '85981392565', '85981395635', '85981395687', '85981395818', '85981397246', '85981397372', '85981397409', '85981397411', '85981398764', '85981400369', '85981401399', '85981401626', '85981401752', '85981402041', '85981402081', '85981402748', '85981402997', '85981403093', '85981403964', '85981404116', '85981404174', '85981404374', '85981404793', '85981405917', '85981408267', '85981409242', '85981409843', '85981411024', '85981411624', '85981411687', '85981413039', '85981413532', '85981413653', '85981413838', '85981413892', '85981414546', '85981415469', '85981416386', '85981416409', '85981418850', '85981419344', '85981420019', '85981421525', '85981421738', '85981422245', '85981422308', '85981422576', '85981422856', '85981423490', '85981423505', '85981423933', '85981424271', '85981424607', '85981425703', '85981426537', '85981426942', '85981427253', '85981428860', '85981428912', '85981432332', '85981433880', '85981436330', '85981437233', '85981437797', '85981440921', '85981442203', '85981443375', '85981444452', '85981444515', '85981445843', '85981447674', '85981448037', '85981452309', '85981453385', '85981460147', '85981460175', '85981460392', '85981460457', '85981460646', '85981460699', '85981460861', '85981460924', '85981460996', '85981461065', '85981461106', '85981461610', '85981462406', '85981463746', '85981463860', '85981464262', '85981464411', '85981464530', '85981464545', '85981465735', '85981465772', '85981465798', '85981466545', '85981467570', '85981468790', '85981470659', '85981470831', '85981471492', '85981471759', '85981472233', '85981473750', '85981474263', '85981474389', '85981474696', '85981474697', '85981474756', '85981474760', '85981474778', '85981474912', '85981474923', '85981475220', '85981475230', '85981475761', '85981475972', '85981475980', '85981476043', '85981476212', '85981476638', '85981477326', '85981477413', '85981477799', '85981477812', '85981477813', '85981477916', '85981478494', '85981478784', '85981479493', '85981479515', '85981479752', '85981479774', '85981481053', '85981481331', '85981481726', '85981482109', '85981482140', '85981482476', '85981482990', '85981483810', '85981484967', '85981485284', '85981485480', '85981486380', '85981486397', '85981487878', '85981488161', '85981488741', '85981489506', '85981489546', '85981489609', '85981489986', '85981491380', '85981491428', '85981491439', '85981492666', '85981492729', '85981495205', '85981495268', '85981495465', '85981495615', '85981495911', '85981495935', '85981496025', '85981496943', '85981497099', '85981497122', '85981497496', '85981497614', '85981499186', '85981500414', '85981500847', '85981500940', '85981501090', '85981501968', '85981502098', '85981502241', '85981505500', '85981505522', '85981505531', '85981505586', '85981505887', '85981506224', '85981506332', '85981506467', '85981506955', '85981507053', '85981507770', '85981507930', '85981509140', '85981509349', '85981509981', '85981510677', '85981511295', '85981512929', '85981514081', '85981514747', '85981518467', '85981518484', '85981520304', '85981521334', '85981521816', '85981521879', '85981521962', '85981522121', '85981522321', '85981522480', '85981522523', '85981522914', '85981522917', '85981522933', '85981522980', '85981523042', '85981523247', '85981523548', '85981523703', '85981523830', '85981523864', '85981524209', '85981524336', '85981524345', '85981524388', '85981524433', '85981524474', '85981525329', '85981525392', '85981525946', '85981525956', '85981525970', '85981526066', '85981526142', '85981526377', '85981526414', '85981526660', '85981526890', '85981526953', '85981527026', '85981527241', '85981527738', '85981527876', '85981527926', '85981528100', '85981528344', '85981528523', '85981529250', '85981530016', '85981530202', '85981530228', '85981530264', '85981530358', '85981530695', '85981531466', '85981532323', '85981532367', '85981532706', '85981533140', '85981533536', '85981533817', '85981533861', '85981533924', '85981534836', '85981535019', '85981535381', '85981535444', '85981535702', '85981536001', '85981536037', '85981536784', '85981537054', '85981537071', '85981537451', '85981537531', '85981537646', '85981538008', '85981538403', '85981538473', '85981539100', '85981539364', '85981539374', '85981539613', '85981539674', '85981539710', '85981539904', '85981542565', '85981544220', '85981544377', '85981544415', '85981544420', '85981544535', '85981544744', '85981545730', '85981545967', '85981546135', '85981546201', '85981546486', '85981546524', '85981547100', '85981547151', '85981547181', '85981548573', '85981548663', '85981549807', '85981550607', '85981551701', '85981552786', '85981552815', '85981553207', '85981553257', '85981553774', '85981554041', '85981554682', '85981555448', '85981556360', '85981556386', '85981556391', '85981556708', '85981557599', '85981557763', '85981557766', '85981557996', '85981558443', '85981558444', '85981558593', '85981558734', '85981558921', '85981559352', '85981559880', '85981559990', '85981561122', '85981561397', '85981563114', '85981563918', '85981565385', '85981566296', '85981569388', '85981570332', '85981570553', '85981571936', '85981571948', '85981573149', '85981574029', '85981574749', '85981574828', '85981575288', '85981576121', '85981577685', '85981579715', '85981580747', '85981582223', '85981587265', '85981588881', '85981589028', '85981590283', '85981590581', '85981591212', '85981591394', '85981592814', '85981594445', '85981594455', '85981598314', '85981599091', '85981599720', '85981600032', '85981600288', '85981600746', '85981601467', '85981601515', '85981601621', '85981603545', '85981603701', '85981603764', '85981603922', '85981604044', '85981604097', '85981604901', '85981605888', '85981606241', '85981606453', '85981606516', '85981606875', '85981607061', '85981607171', '85981607847', '85981608039', '85981608131', '85981608656', '85981608885', '85981609224', '85981609765', '85981611504', '85981611687', '85981612354', '85981612497', '85981613707', '85981614805', '85981615721', '85981615726', '85981616672', '85981617048', '85981617443', '85981617809', '85981618157', '85981618463', '85981618696', '85981619089', '85981621012', '85981625207', '85981625719', '85981625789', '85981625797', '85981626292', '85981626455', '85981627178', '85981627515', '85981627750', '85981628353', '85981628962', '85981629450', '85981630101', '85981630164', '85981631945', '85981632116', '85981635515', '85981635650', '85981636098', '85981636649', '85981638200', '85981638739', '85981639201', '85981642110', '85981642480', '85981645543', '85981646909', '85981647853', '85981649485', '85981651235', '85981651813', '85981651856', '85981653359', '85981654096', '85981655420', '85981655504', '85981656015', '85981656761', '85981663973', '85981664051', '85981665088', '85981665658', '85981665867', '85981666220', '85981666585', '85981666685', '85981668986', '85981669316', '85981669696', '85981669892', '85981670050', '85981670209', '85981670557', '85981671233', '85981672007', '85981672198', '85981672687', '85981676600', '85981677013', '85981677923', '85981677986', '85981679022', '85981679393', '85981684827', '85981685253', '85981687262', '85981688088', '85981688530', '85981689614', '85981690885', '85981692225', '85981693076', '85981694698', '85981696440', '85981700371', '85981701616', '85981701789', '85981702211', '85981704587', '85981705823', '85981706117', '85981706812', '85981707565', '85981709424', '85981709639', '85981709959', '85981709997', '85981711415', '85981712700', '85981715589', '85981717124', '85981721330', '85981721470', '85981723162', '85981723682', '85981727178', '85981727333', '85981730276', '85981731368', '85981733009', '85981733173', '85981734225', '85981735351', '85981735457', '85981738337', '85981742689', '85981745007', '85981746191', '85981746231', '85981747230', '85981747684', '85981747880', '85981748018', '85981749098', '85981749311', '85981780097', '85981780698', '85981781860', '85981781956', '85981782615', '85981783993', '85981787014', '85981787375', '85981787694', '85981787878', '85981795562', '85981797415', '85981799011', '85981799243', '85981799393', '85981799969', '85981800644', '85981801187', '85981801628', '85981801718', '85981801761', '85981802537', '85981802631', '85981803848', '85981804731', '85981805074', '85981805578', '85981805682', '85981805712', '85981805995', '85981806062', '85981806192', '85981806838', '85981807096', '85981807746', '85981808109', '85981808226', '85981808940', '85981809310', '85981809579', '85981810401', '85981811681', '85981812231', '85981812420', '85981813215', '85981813326', '85981813696', '85981813745', '85981814222', '85981815518', '85981815719', '85981815951', '85981815995', '85981816185', '85981816597', '85981816953', '85981817644', '85981819191', '85981819878', '85981819898', '85981819971', '85981820302', '85981820909', '85981822288', '85981822627', '85981823737', '85981824050', '85981825667', '85981827171', '85981827298', '85981828133', '85981829674', '85981829888', '85981830615', '85981831333', '85981831807', '85981832616', '85981833911', '85981836027', '85981836192', '85981838197', '85981839905', '85981840699', '85981840997', '85981841498', '85981842018', '85981842026', '85981847568', '85981849140', '85981849448', '85981850329', '85981851336', '85981851657', '85981851806', '85981852483', '85981852871', '85981853361', '85981853473', '85981853498', '85981854188', '85981854400', '85981854701', '85981854966', '85981855387', '85981855943', '85981857602', '85981858378', '85981858585', '85981859714', '85981859843', '85981860190', '85981860939', '85981861386', '85981861390', '85981862200', '85981862732', '85981862812', '85981863520', '85981863917', '85981864665', '85981866872', '85981867198', '85981867874', '85981868706', '85981869078', '85981869877', '85981870279', '85981870625', '85981870769', '85981871433', '85981871482', '85981871725', '85981872527', '85981873853', '85981874873', '85981875089', '85981875839', '85981876038', '85981876387', '85981877277', '85981877340', '85981877666', '85981878608', '85981879558', '85981879727', '85981881447', '85981881564', '85981881903', '85981882019', '85981882233', '85981883888', '85981885848', '85981886408', '85981888076', '85981890073', '85981890692', '85981890804', '85981890897', '85981891321', '85981891476', '85981892737', '85981892922', '85981893512', '85981894559', '85981895421', '85981895778', '85981895877', '85981899243', '85981900080', '85981900730', '85981901391', '85981904698', '85981905011', '85981905074', '85981905075', '85981906452', '85981910262', '85981910771', '85981911604', '85981911984', '85981914747', '85981917082', '85981917653', '85981917936', '85981918090', '85981918203', '85981921936', '85981921999', '85981922555', '85981924869', '85981926087', '85981926161', '85981927362', '85981928269', '85981930502', '85981933090', '85981933446', '85981934488', '85981937771', '85981942675', '85981944086', '85981946447', '85981947455', '85981948504', '85981948560', '85981948709', '85981949370', '85981949405', '85981950680', '85981951197', '85981951207', '85981951277', '85981951294', '85981951433', '85981952223', '85981952606', '85981953266', '85981955156', '85981955666', '85981956683', '85981956798', '85981956914', '85981956977', '85981958219', '85981958833', '85981959454', '85981962203', '85981963748', '85981964770', '85981966391', '85981966744', '85981967093', '85981967347', '85981967672', '85981972215', '85981973787', '85981973850', '85981974619', '85981975003', '85981975335', '85981975643', '85981978964', '85981982384', '85981982415', '85981983536', '85981984160', '85981984196', '85981984205', '85981985320', '85981987749', '85981990206', '85981991814', '85981992200', '85981992221', '85981993841', '85981994171', '85981994544', '85981996677', '85981996968', '85981997233', '85981998183', '85981998880', '85981999101', '85981999393', '85982000080', '85982000103', '85982000124', '85982000407', '85982000597', '85982001158', '85982001480', '85982001603', '85982002244', '85982003360', '85982009691', '85982012352', '85982013350', '85982013725', '85982014410', '85982014728', '85982014859', '85982015963', '85982016650', '85982018181', '85982019178', '85982020684', '85982020732', '85982021675', '85982021901', '85982021970', '85982022116', '85982022707', '85982023008', '85982023198', '85982023449', '85982024092', '85982024412', '85982024556', '85982025193', '85982025465', '85982025505', '85982026115', '85982026559', '85982026582', '85982026618', '85982026681', '85982026958', '85982027257', '85982027456', '85982028016', '85982028614', '85982028717', '85982029544', '85982029630', '85982029656', '85982031994', '85982033246', '85982036215', '85982038136', '85982038199', '85982038964', '85982041982', '85982048028', '85982048400', '85982048768', '85982049005', '85982050430', '85982051850', '85982052170', '85982052833', '85982053074', '85982058486', '85982059867', '85982060243', '85982061188', '85982061715', '85982065404', '85982066323', '85982066720', '85982067095', '85982067924', '85982069921', '85982070325', '85982070442', '85982070505', '85982070537', '85982075392', '85982076079', '85982077220', '85982080055', '85982080963', '85982081863', '85982082408', '85982082685', '85982086204', '85982086988', '85982088181', '85982088401', '85982090444', '85982092229', '85982092410', '85982092535', '85982095933', '85982096408', '85982096638', '85982096702', '85982098898', '85982099596', '85982101224', '85982102764', '85982103459', '85982103837', '85982104191', '85982105219', '85982105253', '85982105588', '85982106049', '85982107612', '85982108435', '85982108824', '85982108871', '85982108995', '85982109939', '85982110388', '85982110918', '85982111162', '85982111405', '85982111461', '85982111682', '85982111714', '85982112134', '85982112150', '85982112252', '85982112330', '85982112561', '85982112835', '85982113153', '85982113424', '85982113947', '85982114041', '85982114590', '85982114798', '85982115352', '85982115530', '85982116277', '85982116934', '85982116997', '85982118281', '85982118296', '85982118359', '85982118717', '85982119038', '85982119077', '85982120196', '85982120770', '85982121018', '85982121624', '85982122300', '85982122468', '85982123793', '85982123880', '85982125254', '85982126275', '85982127512', '85982130408', '85982130446', '85982131720', '85982132411', '85982132443', '85982132450', '85982133520', '85982134594', '85982134658', '85982140032', '85982141654', '85982144572', '85982145647', '85982145648', '85982147385', '85982147517', '85982148150', '85982148935', '85982150345', '85982154109', '85982154431', '85982154497', '85982155595', '85982155633', '85982161243', '85982161749', '85982162384', '85982162735', '85982163153', '85982164038', '85982166162', '85982166295', '85982166369', '85982170184', '85982171502', '85982171541', '85982171985', '85982184521', '85982185872', '85982190343', '85982204545', '85982205828', '85982207580', '85982217764', '85982222262', '85982223649', '85982225298', '85982234415', '85982243000', '85982254767', '85982254833', '85984000187', '85984000206', '85984000276', '85984000283', '85984000366', '85984000374', '85984000408', '85984000419', '85984000570', '85984000752', '85984000901', '85984000924', '85984001030', '85984001034', '85984001146', '85984001200', '85984001263', '85984001399', '85984001670', '85984001714', '85984001904', '85984002329', '85984002699', '85984004021', '85984004143', '85984004381', '85984004513', '85984004885', '85984004934', '85984004937', '85984005030', '85984005089', '85984005191', '85984005207', '85984005486', '85984005676', '85984005684', '85984005854', '85984006088', '85984006430', '85984006519', '85984006807', '85984006822', '85984006945', '85984007418', '85984007839', '85984007934', '85984008090', '85984008165', '85984008494', '85984008541', '85984008711', '85984008837', '85984008876', '85984009118', '85984009152', '85984010102', '85984010119', '85984010346', '85984010352', '85984010376', '85984010523', '85984010651', '85984010721', '85984010796', '85984011030', '85984011127', '85984011205', '85984011272', '85984011345', '85984011423', '85984012202', '85984012591', '85984012893', '85984013559', '85984013847', '85984013900', '85984013932', '85984013963', '85984014210', '85984014231', '85984014288', '85984014376', '85984014432', '85984014547', '85984015074', '85984015099', '85984015349', '85984015384', '85984015385', '85984015469', '85984015572', '85984015631', '85984015661', '85984015695', '85984015758', '85984015793', '85984015918', '85984015943', '85984015948', '85984016599', '85984016848', '85984017946', '85984018354', '85984019606', '85984019846', '85984019986', '85984020049', '85984020051', '85984020177', '85984020235', '85984020417', '85984020826', '85984020911', '85984021324', '85984021461', '85984021871', '85984022102', '85984022241', '85984022389', '85984022437', '85984022645', '85984023016', '85984023231', '85984023332', '85984023361', '85984023534', '85984024023', '85984024057', '85984024750', '85984024773', '85984024790', '85984024966', '85984025156', '85984025366', '85984025761', '85984026229', '85984026355', '85984026707', '85984026882', '85984026909', '85984026937', '85984027014', '85984027778', '85984027803', '85984027980', '85984028311', '85984028478', '85984028528', '85984028635', '85984028807', '85984029384', '85984029403', '85984029645', '85984029647', '85984029806', '85984029997', '85984030002', '85984030015', '85984030126', '85984030128', '85984030255', '85984030534', '85984030799', '85984030914', '85984031018', '85984031134', '85984031235', '85984031240', '85984031369', '85984031377', '85984031387', '85984031438', '85984031757', '85984031799', '85984031859', '85984031951', '85984031983', '85984031996', '85984032024', '85984032030', '85984032046', '85984032152', '85984032209', '85984032278', '85984032838', '85984032911', '85984033253', '85984033308', '85984033709', '85984033733', '85984033741', '85984033796', '85984033825', '85984033893', '85984033983', '85984034114', '85984034385', '85984034577', '85984034588', '85984034633', '85984034782', '85984034964', '85984035081', '85984035134', '85984035188', '85984035416', '85984035423', '85984035459', '85984035494', '85984035559', '85984035765', '85984036032', '85984036315', '85984036485', '85984036570', '85984036614', '85984036676', '85984036734', '85984036808', '85984036872', '85984037291', '85984037296', '85984037302', '85984037313', '85984037354', '85984037682', '85984037921', '85984037935', '85984037947', '85984038033', '85984038229', '85984038524', '85984038538', '85984038620', '85984038850', '85984038856', '85984039320', '85984039429', '85984039451', '85984039728', '85984040449', '85984040502', '85984040554', '85984040731', '85984040757', '85984040783', '85984040792', '85984040899', '85984041029', '85984041044', '85984041297', '85984041417', '85984041458', '85984041670', '85984041713', '85984041805', '85984041914', '85984041986', '85984042380', '85984042425', '85984042497', '85984042509', '85984042623', '85984042895', '85984042963', '85984043070', '85984043137', '85984043296', '85984043323', '85984043326', '85984043413', '85984043751', '85984044012', '85984044067', '85984044191', '85984044248', '85984044283', '85984044300', '85984044346', '85984044633', '85984044683', '85984044763', '85984044963', '85984045050', '85984045056', '85984045115', '85984045640', '85984045722', '85984046240', '85984046424', '85984046625', '85984046753', '85984046806', '85984046807', '85984046867', '85984047111', '85984047230', '85984047233', '85984047367', '85984047472', '85984047476', '85984047517', '85984047596', '85984048175', '85984048182', '85984048183', '85984048283', '85984048339', '85984048508', '85984048524', '85984048559', '85984048759', '85984048849', '85984049026', '85984049029', '85984049263', '85984049442', '85984049451', '85984049504', '85984049679', '85984049735', '85984049763', '85984049858', '85984049949', '85984050227', '85984050228', '85984050250', '85984050371', '85984050677', '85984050801', '85984050882', '85984050887', '85984050928', '85984051292', '85984051333', '85984051412', '85984051489', '85984051523', '85984051742', '85984051769', '85984051840', '85984051889', '85984051935', '85984052109', '85984052112', '85984052208', '85984052217', '85984052263', '85984052298', '85984052611', '85984052730', '85984052764', '85984052843', '85984053038', '85984053174', '85984053179', '85984053330', '85984053556', '85984053869', '85984053880', '85984053887', '85984053943', '85984053956', '85984054025', '85984054056', '85984054133', '85984054160', '85984054172', '85984054228', '85984054266', '85984054556', '85984054674', '85984054734', '85984054739', '85984054879', '85984054912', '85984055156', '85984055310', '85984055345', '85984055442', '85984055473', '85984055502', '85984055688', '85984055714', '85984055899', '85984055933', '85984056265', '85984056517', '85984056826', '85984056911', '85984056971', '85984057268', '85984057361', '85984057589', '85984057713', '85984057802', '85984057880', '85984058809', '85984059297', '85984059565', '85984059708', '85984060013', '85984060654', '85984060832', '85984061103', '85984061137', '85984061447', '85984061486', '85984061543', '85984061639', '85984061962', '85984062029', '85984062279', '85984062320', '85984062358', '85984062494', '85984062505', '85984062530', '85984063166', '85984063203', '85984063719', '85984063744', '85984063839', '85984064263', '85984064393', '85984064541', '85984064961', '85984065160', '85984065816', '85984066050', '85984066966', '85984067046', '85984067756', '85984067873', '85984068456', '85984069092', '85984069667', '85984069722', '85984069938', '85984070019', '85984070211', '85984070265', '85984070421', '85984070652', '85984070895', '85984071052', '85984071611', '85984071870', '85984072029', '85984072045', '85984072051', '85984072058', '85984072071', '85984072145', '85984072225', '85984072316', '85984072445', '85984072480', '85984072653', '85984072933', '85984073162', '85984073973', '85984074264', '85984074313', '85984074778', '85984075096', '85984075666', '85984076005', '85984076212', '85984076393', '85984076578', '85984076839', '85984076847', '85984077031', '85984077361', '85984077370', '85984077740', '85984077801', '85984078005', '85984078034', '85984078218', '85984078233', '85984078314', '85984078445', '85984078614', '85984079116', '85984079245', '85984079370', '85984079725', '85984079880', '85984079915', '85984080469', '85984080471', '85984080593', '85984080601', '85984081278', '85984081475', '85984081680', '85984082025', '85984082125', '85984082555', '85984082670', '85984082940', '85984082979', '85984083419', '85984083846', '85984084306', '85984084464', '85984084549', '85984084550', '85984084823', '85984084857', '85984085018', '85984085176', '85984085262', '85984085880', '85984086976', '85984087409', '85984088006', '85984088529', '85984089052', '85984089070', '85984089220', '85984089798', '85984090380', '85984090552', '85984090594', '85984090882', '85984090929', '85984091124', '85984091289', '85984091406', '85984091518', '85984092054', '85984092195', '85984092230', '85984092539', '85984093168', '85984093610', '85984093759', '85984093855', '85984094073', '85984094849', '85984095284', '85984096033', '85984098963', '85984099235', '85984099245', '85984099377', '85984099885', '85984100300', '85984100698', '85984100822', '85984101624', '85984101697', '85984102042', '85984102155', '85984102262', '85984102480', '85984102514', '85984102560', '85984102571', '85984103927', '85984104957', '85984105301', '85984105524', '85984106425', '85984107192', '85984107381', '85984107762', '85984108029', '85984108520', '85984108531', '85984108645', '85984108950', '85984109045', '85984109435', '85984109534', '85984110121', '85984110186', '85984110449', '85984110493', '85984110570', '85984110730', '85984110811', '85984111215', '85984111369', '85984111609', '85984111626', '85984111796', '85984111877', '85984111930', '85984112126', '85984112139', '85984112386', '85984112657', '85984113012', '85984113687', '85984113734', '85984113870', '85984113916', '85984114001', '85984114121', '85984114826', '85984114827', '85984115475', '85984115569', '85984115651', '85984116121', '85984116540', '85984116596', '85984116734', '85984116933', '85984117008', '85984117204', '85984117429', '85984117798', '85984118037', '85984118042', '85984118203', '85984118581', '85984118664', '85984118708', '85984118774', '85984119107', '85984119481', '85984119572', '85984119808', '85984120393', '85984120682', '85984121272', '85984122145', '85984122414', '85984123034', '85984123448', '85984124093', '85984124208', '85984125015', '85984125036', '85984126078', '85984126186', '85984126390', '85984126584', '85984126778', '85984126955', '85984127219', '85984127242', '85984127734', '85984128627', '85984128634', '85984128869', '85984128924', '85984129311', '85984129612', '85984130038', '85984130659', '85984130724', '85984130979', '85984131046', '85984131139', '85984131313', '85984131574', '85984131761', '85984131881', '85984132127', '85984132128', '85984132149', '85984132782', '85984132844', '85984133084', '85984133130', '85984133206', '85984133331', '85984133448', '85984133534', '85984134089', '85984134736', '85984135015', '85984135302', '85984135420', '85984135573', '85984</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['10', '27', '27', '27', '46', '30', '27', '1', '5', '29', '1', '35', '16', '43', '27', '27', '27', '11', '5', '28', '1', '49', '27', '27', '1', '27', '0', '27', '11', '1', '28', '10', '3', '27', '3', '28', '27', '31', '1', '25', '1', '27', '27', '40', '27', '27', '28', '27', '27', '12', '28', '5', '7', '6', '28', '40', '49', '1', '2', '8', '78', '1', '1', '27', '5', '27', '1', '27', '27', '11', '1', '28', '12', '27', '27', '1', '5', '27', '27', '2', '27', '27', '27', '25', '7', '27', '28', '1', '11', '27', '1', '1', '27', '21', '13', '6', '27', '5', '1', '0', '28', '27', '28', '27', '27', '27', '27', '27', '27', '7', '28', '5', '5', '27', '27', '47', '28', '27', '34', '1', '35', '5', '8', '12', '28', '27', '12', '49', '28', '27', '6', '27', '1', '1', '17', '5', '27', '1', '1', '28', '31', '1', '27', '12', '5', '27', '39', '49', '19', '16', '28', '27', '5', '27', '8', '27', '4', '35', '8', '30', '35', '1', '27', '27', '10', '40', '1', '27', '27', '49', '27', '29', '27', '27', '1', '28', '43', '32', '45', '30', '27', '27', '6', '27', '5', '2', '27', '7', '49', '13', '28', '6', '27', '27', '27', '27', '26', '27', '27', '27', '28', '49', '1', '27', '11', '28', '27', '27', '27', '27', '1', '18', '28', '27', '27', '27', '1', '27', '1', '49', '10', '27', '5', '49', '1', '11', '27', '49', '27', '27', '5', '49', '27', '7', '5', '28', '1', '29', '27', '11', '31', '38', '27', '15', '27', '27', '49', '17', '41', '8', '27', '1', '28', '30', '28', '3', '27', '30', '30', '5', '27', '10', '1', '49', '27', '28', '1', '27', '4', '1', '28', '5', '27', '27', '12', '28', '10', '27', '27', '48', '1', '1', '1', '27', '30', '1', '27', '27', '27', '29', '27', '5', '27', '27', '6', '1', '30', '27', '28', '1', '12', '5', '29', '25', '27', '49', '27', '27', '6', '11', '27', '27', '27', '27', '11', '27', '1', '27', '27', '27', '27', '27', '30', '27', '49', '28', '28', '23', '40', '27', '28', '27', '27', '27', '5', '11', '27', '27', '1', '5', '11', '28', '27', '27', '27', '28', '9', '5', '27', '11', '27', '1', '35', '1', '27', '1', '27', '27', '1', '30', '27', '27', '28', '17', '27', '27', '1', '27', '35', '49', '27', '49', '27', '27', '11', '27', '12', '27', '27', '8', '4', '49', '11', '27', '35', '4', '28', '27', '27', '27', '5', '18', '1', '5', '27', '27', '1', '28', '27', '1', '1', '11', '1', '1', '28', '114', '9', '27', '27', '5', '28', '27', '27', '1', '23', '27', '27', '5', '1', '27', '1', '5', '27', '27', '27', '27', '87', '27', '28', '31', '39', '34', '27', '27', '27', '9', '13', '9', '1', '17', '27', '35', '27', '30', '12', '27', '27', '49', '6', '27', '27', '27', '1', '28', '1', '30', '27', '27', '27', '12', '27', '27', '27', '1', '28', '0', '27', '49', '27', '27', '1', '28', '27', '27', '49', '27', '27', '27', '49', '27', '27', '6', '49', '1', '27', '9', '1', '28', '42', '13', '31', '27', '15', '8', '49', '27', '5', '27', '8', '27', '29', '27', '27', '49', '27', '14', '27', '28', '27', '27', '49', '29', '11', '27', '27', '12', '27', '27', '27', '27', '27', '1', '27', '5', '22', '1', '27', '27', '49', '17', '29', '11', '27', '27', '5', '13', '1', '10', '27', '28', '27', '27', '27', '27', '27', '5', '24', '27', '1', '1', '27', '1', '30', '27', '27', '27', '1', '14', '19', '25', '27', '27', '27', '27', '49', '27', '30', '11', '30', '5', '27', '27', '1', '27', '28', '27', '1', '29', '27', '27', '1', '5', '1', '37', '49', '1', '5', '2', '82', '5', '27', '27', '30', '8', '27', '5', '27', '27', '27', '28', '49', '27', '27', '27', '27', '28', '5', '27', '27', '1', '27', '14', '5', '49', '31', '1', '27', '1', '27', '5', '27', '27', '27', '28', '1', '12', '40', '27', '43', '27', '27', '1', '27', '49', '49', '21', '27', '27', '22', '27', '7', '12', '27', '27', '0', '1', '27', '27', '27', '28', '1', '7', '28', '49', '27', '27', '27', '7', '28', '16', '1', '1', '27', '12', '10', '12', '27', '27', '4', '27', '27', '30', '5', '12', '29', '27', '27', '17', '27', '27', '13', '5', '27', '12', '16', '49', '27', '1', '27', '6', '49', '29', '27', '28', '18', '28', '49', '27', '27', '27', '30', '27', '7', '23', '49', '12', '16', '27', '1', '5', '1', '27', '27', '27', '27', '27', '27', '27', '49', '27', '28', '27', '1', '27', '27', '27', '27', '27', '49', '21', '27', '28', '27', '27', '28', '35', '27', '49', '1', '27', '27', '26', '27', '38', '27', '1', '6', '27', '27', '28', '7', '28', '27', '27', '27', '27', '12', '5', '6', '27', '18', '28', '17', '27', '27', '28', '23', '14', '27', '12', '29', '28', '28', '27', '27', '27', '27', '28', '28', '49', '5', '27', '12', '27', '27', '27', '49', '27', '27', '12', '8', '27', '28', '28', '1', '9', '28', '27', '27', '27', '1', '1', '10', '1', '28', '27', '12', '1', '7', '27', '27', '27', '27', '28', '27', '27', '27', '5', '27', '12', '46', '27', '27', '31', '35', '17', '28', '27', '20', '24', '23', '1', '41', '36', '49', '49', '7', '28', '49', '27', '27', '5', '5', '27', '1', '5', '17', '27', '28', '13', '7', '49', '28', '27', '27', '27', '1', '34', '42', '35', '27', '28', '28', '28', '35', '11', '27', '5', '5', '28', '28', '27', '28', '1', '28', '13', '27', '28', '27', '28', '30', '28', '28', '18', '27', '5', '1', '76', '28', '28', '1', '5', '1', '28', '26', '2', '28', '1', '7', '12', '28', '37', '11', '28', '27', '27', '27', '27', '28', '28', '27', '20', '8', '30', '14', '27', '4', '10', '4', '49', '28', '28', '1', '1', '22', '27', '1', '10', '28', '11', '28', '77', '28', '2', '27', '30', '27', '27', '31', '1', '28', '28', '12', '27', '28', '10', '30', '27', '9', '27', '18', '28', '0', '12', '28', '49', '27', '27', '27', '27', '30', '1', '28', '27', '50', '31', '1', '27', '1', '27', '28', '28', '28', '27', '7', '1', '28', '27', '1', '27', '31', '28', '27', '1', '28', '1', '49', '49', '27', '28', '27', '27', '1', '27', '28', '27', '5', '26', '12', '1', '28', '2', '8', '13', '1', '12', '1', '28', '27', '1', '30', '7', '7', '37', '27', '28', '8', '5', '27', '28', '27', '27', '13', '13', '27', '30', '13', '13', '27', '1', '28', '27', '28', '27', '31', '27', '13', '28', '27', '27', '28', '12', '27', '27', '7', '1', '29', '27', '27', '1', '5', '27', '13', '27', '28', '49', '27', '6', '28', '27', '1', '27', '27', '21', '28', '31', '46', '27', '28', '5', '5', '27', '27', '30', '7', '27', '28', '28', '28', '30', '9', '17', '1', '3', '30', '7', '27', '28', '27', '7', '37', '27', '14', '13', '28', '27', '27', '27', '1', '27', '27', '27', '27', '28', '6', '28', '27', '12', '27', '47', '49', '28', '28', '27', '27', '13', '14', '28', '12', '28', '7', '27', '28', '27', '27', '1', '1', '27', '14', '0', '1', '27', '1', '1', '31', '1', '5', '39', '35', '27', '28', '11', '30', '27', '1', '27', '49', '27', '28', '28', '27', '47', '27', '28', '28', '5', '28', '30', '11', '49', '27', '28', '1', '28', '28', '28', '27', '49', '30', '27', '28', '30', '27', '15', '49', '8', '28', '12', '27', '17', '28', '27', '30', '49', '1', '28', '28', '27', '27', '27', '49', '1', '26', '1', '27', '49', '1', '6', '27', '5', '28', '1', '27', '11', '16', '28', '114', '27', '27', '27', '34', '1', '6', '28', '49', '21', '27', '27', '27', '28', '10', '1', '27', '27', '27', '49', '1', '28', '28', '27', '31', '28', '28', '28', '49', '49', '27', '27', '27', '8', '28', '1', '11', '5', '1', '1', '27', '32', '49', '27', '9', '33', '27', '5', '28', '27', '31', '28', '27', '27', '27', '27', '27', '39', '30', '12', '13', '28', '34', '1', '27', '27', '28', '28', '15', '11', '27', '28', '1', '27', '1', '35', '27', '7', '17', '1', '35', '23', '27', '28', '1', '5', '28', '2', '21', '27', '28', '28', '28', '11', '49', '32', '28', '14', '14', '30', '27', '1', '28', '28', '28', '23', '1', '27', '27', '27', '28', '47', '27', '28', '1', '27', '27', '28', '42', '49', '27', '27', '5', '28', '27', '1', '28', '27', '26', '27', '27', '28', '28', '8', '5', '0', '49', '28', '28', '5', '28', '27', '28', '28', '41', '8', '27', '27', '27', '6', '27', '27', '27', '6', '1', '28', '30', '5', '27', '12', '2', '5', '28', '15', '5', '27', '28', '27', '12', '28', '28', '5', '27', '12', '28', '27', '27', '6', '1', '30', '28', '27', '28', '12', '27', '13', '1', '49', '31', '27', '12', '28', '27', '28', '27', '33', '27', '40', '27', '28', '28', '27', '0', '20', '27', '1', '43', '28', '28', '1', '49', '33', '27', '10', '28', '27', '28', '27', '27', '2', '27', '27', '49', '1', '28', '28', '43', '27', '27', '28', '49', '5', '28', '146', '10', '18', '28', '27', '27', '27', '28', '27', '28', '28', '28', '11', '1', '5', '6', '27', '8', '5', '9', '28', '1', '27', '28', '18', '27', '6', '6', '26', '27', '7', '27', '49', '8', '27', '75', '21', '58', '27', '27', '21', '27', '21', '6', '27', '29', '27', '27', '62', '69', '65', '17', '27', '49', '8', '27', '8', '5', '27', '1', '30', '1', '27', '32', '32', '49', '5', '5', '4', '13', '32', '33', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '32', '5', '4', '5', '32', '4', '3', '4', '4', '4', '5', '35', '33', '4', '5', '5', '5', '4', '30', '32', '5', '4', '5', '19', '5', '5', '4', '5', '5', '5', '5', '5', '4', '4', '5', '5', '5', '32', '32', '39', '4', '4', '4', '34', '5', '33', '34', '49', '4', '5', '4', '5', '3', '77', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '5', '6', '5', '5', '4', '4', '5', '4', '5', '4', '4', '32', '5', '51', '4', '32', '4', '33', '4', '4', '5', '12', '32', '4', '4', '32', '5', '5', '4', '5', '4', '3', '4', '5', '4', '5', '6', '4', '5', '32', '4', '4', '4', '5', '4', '5', '5', '5', '2', '5', '6', '4', '49', '5', '4', '32', '5', '32', '5', '5', '5', '39', '49', '33', '33', '4', '4', '5', '5', '5', '4', '5', '5', '4', '33', '32', '32', '32', '32', '33', '5', '32', '32', '32', '33', '44', '20', '14', '33', '6', '32', '12', '49', '32', '32', '49', '33', '34', '5', '32', '32', '32', '32', '4', '32', '32', '5', '6', '42', '33', '35', '32', '31', '31', '5', '32', '49', '32', '4', '27', '11', '32', '4', '69', '32', '6', '32', '34', '5', '32', '49', '32', '21', '32', '32', '5', '30', '33', '32', '16', '32', '33', '34', '32', '48', '49', '31', '32', '6', '32', '34', '34', '5', '33', '49', '39', '32', '33', '33', '4', '32', '11', '32', '6', '6', '33', '32', '33', '33', '31', '32', '32', '5', '32', '4', '32', '4', '32', '32', '33', '32', '32', '5', '34', '32', '33', '32', '49', '32', '27', '31', '4', '12', '33', '34', '49', '5', '31', '32', '6', '30', '5', '32', '27', '34', '32', '22', '32', '4', '32', '33', '32', '32', '4', '6', '33', '33', '72', '32', '32', '5', '30', '32', '5', '32', '32', '60', '32', '33', '15', '34', '32', '33', '33', '32', '32', '12', '33', '33', '33', '32', '32', '5', '32', '33', '7', '32', '46', '5', '33', '32', '41', '34', '32', '32', '32', '5', '32', '32', '33', '33', '33', '32', '32', '7', '33', '32', '32', '32', '12', '32', '5', '32', '49', '9', '30', '32', '33', '33', '33', '27', '5', '5', '31', '32', '6', '30', '79', '35', '49', '34', '32', '33', '33', '32', '32', '32', '49', '32', '70', '26', '32', '32', '6', '32', '31', '5', '28', '32', '5', '5', '10', '4', '49', '33', '5', '32', '32', '6', '5', '4', '4', '4', '5', '5', '32', '5', '4', '5', '5', '75', '4', '4', '4', '4', '34', '4', '5', '5', '49', '42', '4', '5', '32', '2', '4', '5', '33', '4', '5', '5', '5', '5', '5', '4', '11', '32', '49', '4', '30', '5', '27', '4', '31', '29', '2', '4', '5', '33', '5', '4', '5', '32', '4', '4', '5', '32', '5', '4', '32', '14', '37', '5', '4', '33', '4', '5', '5', '31', '4', '4', '5', '32', '33', '33', '5', '5', '5', '5', '4', '4', '4', '4', '5', '5', '30', '4', '0', '4', '16', '4', '5', '4', '4', '5', '5', '5', '5', '4', '5', '4', '30', '5', '5', '5', '15', '5', '4', '5', '5', '5', '5', '7', '4', '4', '4', '32', '32', '5', '32', '4', '4', '5', '4', '4', '4', '4', '4', '4', '4', '4', '30', '4', '5', '4', '4', '5', '34', '4', '5', '64', '4', '4', '4', '4', '4', '4', '4', '5', '4', '4', '5', '5', '5', '4', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '31', '4', '4', '5', '4', '5', '35', '4', '4', '4', '5', '4', '4', '5', '4', '5', '4', '5', '4', '5', '4', '4', '4', '4', '32', '4', '4', '31', '13', '4', '11', '4', '32', '5', '4', '33', '5', '32', '4', '30', '4', '5', '32', '33', '5', '5', '5', '4', '5', '3', '4', '4', '5', '32', '4', '4', '5', '31', '32', '5', '49', '12', '5', '4', '5', '4', '33', '2', '5', '5', '30', '80', '4', '33', '33', '3', '5', '34', '31', '34', '7', '59', '32', '33', '5', '32', '95', '5', '32', '32', '5', '5', '32', '30', '5', '32', '5', '4', '4', '32', '5', '4', '4', '5', '5', '33', '11', '4', '32', '4', '4', '33', '4', '63', '4', '4', '4', '34', '4', '18', '33', '32', '33', '32', '4', '32', '47', '5', '4', '32', '5', '5', '49', '35', '32', '33', '32', '5', '7', '32', '4', '32', '21', '12', '5', '32', '32', '4', '4', '4', '5', '5', '4', '32', '5', '4', '5', '32', '5', '4', '34', '4', '5', '4', '5', '5', '4', '5', '4', '4', '30', '32', '5', '33', '33', '32', '31', '33', '32', '32', '4', '6', '34', '1', '15', '30', '32', '5', '4', '32', '4', '5', '32', '2', '49', '8', '32', '11', '6', '5', '31', '33', '12', '34', '33', '31', '4', '33', '34', '34', '32', '32', '32', '32', '8', '32', '33', '4', '74', '4', '33', '32', '28', '4', '5', '33', '14', '32', '33', '31', '5', '32', '5', '33', '33', '32', '33', '32', '5', '32', '33', '23', '27', '31', '31', '34', '31', '5', '41', '32', '32', '33', '32', '11', '32', '7', '11', '32', '33', '32', '33', '34', '32', '32', '4', '32', '31', '32', '32', '32', '32', '33', '46', '32', '66', '32', '33', '30', '5', '32', '32', '32', '4', '32', '32', '32', '32', '33', '32', '49', '32', '32', '32', '33', '33', '32', '5', '33', '32', '12', '32', '33', '16', '32', '33', '5', '32', '32', '9', '34', '64', '4', '32', '32', '33', '32', '31', '32', '32', '10', '32', '6', '33', '13', '32', '5', '5', '4', '31', '3', '32', '25', '40', '34', '32', '32', '34', '5', '32', '44', '33', '8', '32', '33', '32', '33', '5', '33', '32', '32', '32', '18', '30', '32', '33', '32', '49', '32', '32', '32', '6', '17', '33', '33', '5', '49', '32', '19', '4', '5', '5', '4', '5', '7', '4', '11', '33', '32', '32', '4', '3', '32', '27', '4', '4', '33', '5', '4', '34', '31', '5', '30', '1', '4', '5', '32', '5', '4', '5', '4', '61', '9', '4', '11', '5', '32', '33', '33', '34', '4', '33', '34', '4', '32', '32', '5', '32', '4', '31', '32', '33', '5', '4', '33', '5', '4', '27', '5', '5', '4', '35', '5', '5', '4', '5', '4', '4', '4', '33', '5', '32', '5', '5', '5', '27', '4', '4', '4', '4', '4', '5', '5', '5', '5', '6', '5', '5', '5', '5', '4', '5', '5', '5', '4', '5', '4', '66', '4', '4', '4', '4', '5', '4', '4', '4', '32', '7', '33', '5', '7', '4', '5', '55', '32', '43', '21', '5', '4', '5', '3', '4', '5', '4', '4', '32', '32', '33', '34', '5', '69', '4', '32', '4', '32', '25', '30', '32', '30', '32', '63', '35', '33', '5', '32', '5', '32', '4', '5', '4', '5', '4', '5', '4', '4', '33', '33', '33', '4', '30', '5', '33', '32', '4', '32', '33', '27', '5', '4', '32', '5', '4', '32', '5', '5', '5', '33', '4', '5', '4', '4', '4', '5', '5', '7', '33', '5', '32', '5', '5', '49', '5', '4', '4', '5', '4', '4', '5', '4', '4', '5', '32', '4', '4', '4', '4', '4', '5', '32', '4', '5', '4', '4', '4', '5', '4', '5', '4', '4', '61', '4', '5', '4', '38', '33', '4', '5', '34', '13', '4', '4', '32', '32', '32', '4', '5', '5', '32', '5', '32', '4', '33', '33', '33', '5', '5', '33', '5', '5', '4', '12', '4', '28', '5', '5', '5', '5', '5', '4', '5', '5', '4', '32', '6', '4', '4', '5', '9', '13', '32', '34', '4', '33', '15', '32', '32', '4', '32', '5', '5', '27', '4', '5', '4', '4', '5', '4', '4', '4', '5', '4', '21', '5', '5', '33', '5', '4', '34', '5', '4', '4', '4', '5', '4', '4', '5', '5', '4', '5', '5', '13', '4', '5', '4', '5', '4', '4', '31', '5', '4', '5', '4', '4', '5', '30', '4', '4', '5', '4', '5', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '5', '5', '5', '46', '4', '4', '4', '4', '5', '4', '5', '22', '5', '5', '4', '49', '5', '5', '32', '5', '4', '5', '5', '5', '4', '4', '32', '4', '30', '32', '4', '4', '4', '4', '5', '5', '12', '5', '4', '5', '4', '33', '4', '4', '4', '32', '4', '4', '4', '4', '5', '4', '4', '32', '4', '35', '5', '4', '4', '5', '4', '5', '32', '0', '67', '4', '31', '4', '5', '30', '4', '17', '3', '5', '4', '4', '4', '5', '22', '5', '4', '4', '4', '4', '5', '5', '5', '5', '4', '5', '5', '2', '4', '4', '5', '32', '5', '5', '5', '4', '4', '4', '50', '4', '5', '4', '4', '5', '5', '5', '32', '5', '30', '32', '4', '5', '32', '4', '4', '4', '4', '4', '5', '5', '4', '5', '68', '5', '29', '4', '5', '5', '4', '5', '5', '6', '6', '6', '6', '6', '6', '5', '6', '6', '32', '35', '6', '33', '6', '24', '5', '34', '33', '32', '30', '31', '32', '33', '13', '32', '32', '93', '8', '33', '32', '32', '5', '33', '31', '32', '32', '33', '13', '32', '9', '32', '30', '3', '4', '9', '33', '3', '32', '33', '19', '32', '32', '33', '32', '33', '30', '30', '32', '5', '33', '32', '81', '7', '7', '32', '79', '33', '15', '32', '32', '32', '32', '5', '30', '32', '7', '32', '33', '5', '32', '33', '33', '35', '33', '32', '33', '33', '33', '31', '33', '32', '34', '32', '32', '32', '34', '33', '7', '33', '13', '32', '32', '32', '49', '32', '33', '33', '32', '32', '4', '32', '32', '33', '33', '4', '32', '33', '33', '12', '49', '33', '32', '80', '32', '33', '32', '25', '32', '34', '33', '4', '32', '32', '33', '32', '33', '33', '32', '33', '32', '4', '21', '32', '5', '32', '49', '71', '33', '33', '16', '13', '4', '32', '32', '5', '27', '18', '34', '33', '32', '65', '32', '32', '22', '27', '49', '34', '33', '33', '5', '4', '5', '5', '44', '32', '30', '12', '32', '32', '11', '33', '33', '33', '33', '32', '4', '11', '32', '32', '11', '8', '32', '4', '5', '5', '5', '33', '4', '4', '4', '70', '12', '27', '32', '32', '5', '17', '33', '32', '32', '8', '34', '32', '59', '32', '32', '33', '31', '31', '32', '49', '5', '15', '13', '33', '34', '32', '4', '33', '32', '4', '8', '32', '33', '22', '34', '49', '11', '33', '32', '32', '5', '28', '32', '31', '32', '32', '12', '32', '32', '32', '28', '49', '30', '33', '33', '32', '3', '18', '30', '33', '4', '32', '4', '31', '1', '12', '28', '5', '49', '33', '23', '32', '32', '33', '33', '33', '8', '33', '4', '29', '4', '32', '13', '32', '33', '33', '34', '32', '31', '33', '32', '4', '5', '32', '32', '5', '33', '15', '11', '33', '9', '50', '59', '13', '32', '32', '34', '33', '34', '33', '33', '33', '32', '20', '20', '33', '33', '34', '33', '32', '31', '12', '32', '33', '33', '5', '32', '32', '31', '33', '5', '32', '33', '7', '33', '32', '26', '13', '34', '12', '4', '5', '12', '49', '32', '33', '33', '32', '32', '32', '33', '33', '32', '17', '13', '32', '33', '10', '32', '32', '30', '32', '32', '32', '8', '5', '32', '32', '32', '32', '32', '12', '30', '12', '34', '33', '32', '45', '32', '34', '28', '32', '4', '4', '17', '32', '33', '49', '33', '26', '33', '49', '33', '31', '32', '32', '14', '5', '32', '32', '32', '32', '27', '32', '5', '33', '32', '32', '32', '32', '32', '32', '13', '15', '32', '30', '32', '32', '32', '32', '26', '32', '18', '33', '32', '32', '32', '49', '32', '33', '31', '32', '4', '5', '34', '32', '33', '33', '34', '32', '32', '6', '33', '5', '31', '32', '33', '32', '31', '29', '12', '32', '32', '5', '33', '30', '33', '32', '32', '31', '32', '39', '7', '61', '25', '34', '33', '32', '32', '7', '32', '31', '31', '33', '10', '34', '32', '31', '22', '32', '20', '9', '32', '32', '33', '30', '12', '33', '33', '33', '27', '5', '32', '5', '27', '24', '12', '32', '32', '62', '32', '22', '32', '5', '32', '33', '24', '49', '32', '32', '32', '4', '6', '33', '4', '33', '32', '32', '32', '32', '1', '11', '32', '26', '24', '5', '5', '32', '7', '5', '31', '33', '5', '54', '32', '33', '32', '32', '32', '32', '30', '32', '32', '12', '31', '32', '33', '33', '32', '33', '49', '33', '22', '32', '12', '32', '27', '55', '32', '34', '60', '32', '4', '5', '4', '4', '4', '4', '4', '4', '4', '5', '6', '4', '4', '34', '33', '4', '4', '33', '5', '35', '33', '33', '4', '5', '5', '33', '32', '32', '32', '5', '4', '4', '5', '5', '5', '32', '32', '4', '49', '5', '15', '33', '32', '32', '32', '34', '32', '60', '32', '32', '32', '27', '33', '30', '15', '5', '5', '72', '4', '4', '33', '33', '11', '32', '32', '32', '44', '63', '6', '7', '32', '32', '32', '5', '4', '19', '32', '14', '1', '33', '32', '71', '4', '48', '4', '31', '34', '5', '35', '5', '32', '32', '33', '32', '32', '26', '13', '32', '28', '32', '6', '21', '31', '64', '11', '33', '32', '32', '34', '5', '32', '26', '32', '5', '14', '32', '5', '5', '32', '4', '39', '13', '4', '35', '0', '32', '33', '33', '32', '32', '32', '49', '15', '33', '32', '32', '27', '32', '32', '5', '46', '11', '24', '33', '11', '4', '32', '12', '5', '5', '5', '32', '33', '32', '1', '32', '7', '13', '32', '32', '32', '13', '5', '30', '5', '4', '32', '30', '33', '33', '4', '7', '5', '33', '33', '33', '32', '14', '29', '6', '13', '32', '10', '33', '33', '5', '30', '12', '21', '33', '32', '33', '31', '30', '32', '18', '34', '32', '32', '34', '30', '12', '32', '32', '30', '32', '33', '34', '30', '32', '5', '33', '32', '12', '33', '33', '32', '32', '32', '11', '32', '32', '33', '32', '33', '32', '30', '32', '5', '32', '32', '25', '32', '33', '31', '32', '14', '33', '57', '30', '32', '49', '27', '5', '32', '12', '33', '33', '32', '32', '33', '21', '33', '33', '32', '10', '33', '33', '33', '32', '4', '4', '32', '32', '31', '33', '33', '33', '32', '24', '5', '35', '32', '32', '5', '3', '34', '32', '32', '5', '32', '33', '57', '33', '4', '34', '52', '33', '32', '33', '32', '33', '33', '1', '33', '33', '33', '22', '27', '33', '32', '32', '34', '33', '7', '12', '1', '4', '33', '32', '33', '33', '32', '32', '31', '32', '32', '29', '33', '31', '49', '5', '11', '34', '32', '32', '25', '35', '32', '25', '32', '33', '33', '5', '32', '27', '32', '31', '30', '30', '34', '32', '31', '5', '13', '30', '32', '4', '33', '32', '32', '32', '34', '4', '33', '30', '31', '32', '32', '33', '34', '49', '32', '5', '31', '33', '32', '32', '49', '8', '33', '32', '5', '32', '32', '33', '5', '32', '4', '36', '5', '32', '4', '32', '32', '18', '33', '33', '34', '34', '32', '8', '41', '32', '33', '49', '32', '32', '32', '5', '30', '49', '27', '32', '55', '49', '49', '26', '5', '33', '33', '33', '32', '32', '34', '32', '32', '12', '32', '11', '31', '33', '34', '32', '21', '28', '57', '32', '30', '4', '32', '4', '32', '17', '31', '33', '32', '32', '32', '32', '5', '30', '32', '32', '32', '32', '34', '32', '32', '32', '32', '32', '32', '33', '33', '13', '32', '34', '32', '32', '32', '32', '32', '5', '33', '32', '32', '33', '32', '5', '12', '33', '32', '5', '32', '32', '32', '5', '32', '5', '16', '34', '33', '33', '4', '30', '11', '34', '32', '35', '94', '10', '4', '14', '32', '28', '4', '32', '32', '17', '15', '4', '27', '4', '32', '32', '5', '34', '32', '32', '7', '33', '18', '31', '58', '20', '32', '11', '67', '36', '4', '27', '12', '32', '33', '26', '33', '5', '32', '32', '32', '32', '33', '77', '4', '33', '35', '32', '31', '31', '24', '32', '32', '33', '32', '24', '29', '33', '32', '32', '32', '24', '32', '5', '32', '16', '33', '33', '32', '32', '32', '11', '32', '5', '32', '32', '32', '32', '45', '32', '32', '31', '32', '32', '15', '32', '30', '31', '32', '5', '33', '5', '32', '32', '32', '32', '52', '26', '32', '32', '5', '33', '2', '34', '36', '33', '49', '33', '32', '5', '32', '6', '14', '32', '33', '32', '31', '31', '32', '33', '32', '33', '32', '32', '5', '32', '28', '32', '33', '32', '33', '8', '32', '5', '33', '12', '48', '32', '32', '32', '32', '32', '33', '4', '32', '13', '8', '32', '32', '33', '38', '33', '34', '33', '6', '33', '32', '32', '32', '13', '5', '4', '32', '16', '34', '7', '11', '12', '5', '11', '9', '33', '11', '33', '4', '34', '32', '32', '6', '49', '31', '32', '32', '5', '32', '4', '32', '32', '15', '6', '49', '32', '5', '32', '32', '32', '32', '6', '32', '32', '33', '32', '5', '11', '7', '5', '32', '31', '45', '33', '31', '32', '30', '6', '33', '33', '31', '34', '70', '1', '32', '31', '5', '32', '19', '5', '32', '32', '32', '32', '32', '31', '4', '32', '4', '32', '32', '11', '33', '32', '49', '33', '32', '33', '5', '32', '32', '33', '12', '49', '33', '32', '32', '11', '32', '32', '32', '33', '26', '33', '32', '32', '26', '0', '32', '31', '10', '32', '4', '31', '27', '5', '32', '33', '51', '12', '49', '6', '33', '33', '34', '32', '32', '32', '33', '32', '33', '5', '33', '32', '4', '49', '34', '32', '32', '5', '25', '31', '32', '33', '2', '5', '32', '14', '32', '32', '78', '32', '32', '32', '9', '20', '33', '33', '34', '32', '15', '33', '31', '32', '31', '32', '7', '11', '33', '32', '22', '49', '32', '32', '31', '33', '33', '32', '24', '32', '34', '33', '32', '34', '33', '14', '32', '33', '33', '19', '32', '32', '32', '14', '32', '8', '33', '33', '33', '32', '1', '33', '32', '32', '33', '27', '33', '11', '32', '33', '5', '32', '32', '12', '5', '11', '32', '33', '32', '32', '33', '32', '32', '45', '9', '32', '33', '32', '32', '32', '32', '32', '13', '32', '32', '5', '32', '32', '8', '7', '32', '33', '13', '49', '38', '6', '32', '33', '33', '19', '32', '32', '4', '4', '32', '32', '32', '33', '5', '33', '32', '12', '31', '32', '32', '33', '32', '38', '49', '33', '11', '32', '14', '6', '32', '33', '5', '5', '31', '32', '32', '32', '49', '32', '30', '70', '5', '33', '4', '16', '32', '32', '4', '32', '63', '6', '33', '49', '49', '5', '33', '32', '33', '33', '32', '5', '22', '5', '32', '11', '33', '32', '32', '11', '30', '33', '30', '34', '24', '21', '5', '32', '32', '32', '9', '13', '32', '48', '18', '5', '8', '7', '33', '32', '32', '32', '32', '19', '8', '32', '30', '33', '5', '32', '33', '32', '32', '32', '35', '11', '4', '32', '31', '32', '32', '32', '33', '33', '32', '10', '32', '32', '32', '1', '30', '7', '24', '33', '33', '32', '4', '33', '32', '5', '10', '27', '32', '33', '34', '32', '33', '33', '32', '32', '32', '32', '32', '32', '5', '33', '4', '32', '5', '32', '32', '7', '32', '33', '33', '32', '30', '16', '32', '5', '5', '5', '5', '5', '31', '33', '33', '4', '33', '32', '32', '5', '32', '33', '24', '31', '33', '8', '33', '32', '32', '32', '5', '32', '32', '5', '12', '41', '8', '33', '32', '32', '17', '5', '32', '32', '49', '32', '32', '4', '32', '9', '32', '33', '31', '33', '33', '31', '5', '32', '32', '4', '32', '32', '27', '32', '32', '32', '33', '32', '12', '49', '13', '32', '32', '30', '32', '5', '11', '32', '32', '3', '4', '33', '32', '58', '33', '30', '33', '49', '32', '33', '32', '16', '4', '33', '16', '33', '32', '5', '15', '33', '33', '32', '32', '35', '32', '33', '32', '34', '32', '32', '33', '10', '32', '31', '34', '33', '12', '32', '33', '27', '5', '4', '32', '32', '32', '31', '32', '33', '33', '31', '32', '33', '33', '32', '32', '6', '32', '49', '32', '6', '5', '4', '33', '15', '32', '32', '32', '5', '32', '33', '49', '32', '32', '32', '32', '33', '17', '32', '32', '4', '32', '31', '32', '37', '35', '1', '32', '12', '30', '33', '5', '32', '20', '5', '5', '32', '32', '49', '31', '32', '32', '6', '4', '32', '26', '31', '5', '5', '32', '32', '32', '33', '32', '32', '33', '30', '33', '32', '31', '32', '5', '32', '32', '32', '4', '49', '31', '32', '32', '33', '31', '32', '32', '11', '32', '49', '31', '4', '36', '5', '3', '9', '31', '12', '32', '32', '30', '4', '4', '4', '33', '49', '32', '32', '30', '4', '49', '31', '31', '33', '33', '32', '34', '32', '49', '32', '32', '5', '4', '8', '32', '32', '33', '12', '5', '32', '32', '32', '32', '32', '32', '8', '32', '32', '32', '32', '33', '2', '33', '32', '30', '33', '31', '32', '23', '30', '25', '5', '66', '36', '5', '32', '33', '31', '32', '32', '10', '33', '33', '14', '33', '33', '32', '13', '9', '18', '32', '34', '2', '32', '32', '4', '49', '5', '19', '4', '32', '33', '33', '35', '31', '22', '32', '32', '5', '30', '28', '32', '32', '32', '34', '32', '4', '6', '31', '32', '4', '32', '4', '33', '32', '33', '31', '6', '4', '32', '29', '13', '34', '32', '11', '34', '32', '8', '32', '33', '32', '49', '4', '32', '36', '33', '33', '7', '32', '32', '85', '32', '32', '33', '32', '9', '5', '4', '32', '12', '32', '32', '4', '30', '16', '32', '32', '1', '32', '33', '5', '32', '49', '33', '72', '31', '11', '5', '33', '49', '4', '31', '6', '33', '17', '33', '32', '5', '32', '32', '32', '14', '5', '26', '5', '17', '31', '4', '33', '30', '4', '32', '27', '23', '12', '32', '32', '32', '32', '32', '25', '32', '30', '32', '31', '33', '32', '32', '4', '5', '4', '33', '32', '33', '32', '32', '32', '32', '49', '31', '25', '32', '6', '33', '32', '5', '65', '8', '7', '32', '32', '32', '49', '32', '32', '6', '32', '15', '32', '11', '32', '32', '31', '32', '34', '6', '33', '32', '33', '32', '31', '15', '33', '32', '33', '32', '34', '25', '32', '32', '32', '33', '32', '50', '33', '32', '32', '49', '32', '6', '32', '5', '32', '32', '49', '32', '32', '5', '32', '4', '49', '32', '32', '33', '9', '32', '16', '33', '32', '33', '31', '4', '8', '5', '35', '5', '49', '6', '49', '32', '32', '32', '34', '32', '1', '9', '49', '32', '33', '4', '30', '49', '30', '4', '33', '32', '5', '30', '33', '11', '32', '32', '49', '4', '5', '33', '31', '5', '5', '25', '58', '32', '32', '13', '5', '31', '30', '32', '40', '12', '32', '12', '34', '33', '5', '35', '22', '25', '33', '28', '30', '5', '32', '27', '33', '33', '32', '5', '33', '5', '33', '30', '32', '9', '5', '30', '33', '48', '32', '12', '32', '32', '25', '32', '4', '32', '32', '16', '4', '5', '32', '45', '32', '5', '33', '32', '54', '14', '7', '5', '32', '4', '47', '33', '49', '5', '30', '7', '30', '5', '6', '30', '32', '5', '7', '5', '33', '32', '33', '5', '49', '30', '30', '35', '4', '8', '33', '32', '30', '8', '32', '5', '5', '32', '15', '30', '5', '32', '5', '72', '13', '10', '31', '4', '28', '20', '71', '32', '5', '19', '33', '32', '32', '7', '10', '94', '32', '32', '33', '28', '8', '34', '15', '4', '32', '1', '32', '15', '8', '32', '8', '5', '33', '34', '6', '32', '32', '12', '11', '79', '32', '32', '32', '33', '33', '18', '5', '49', '5', '33', '32', '6', '32', '13', '4', '33', '32', '4', '33', '4', '5', '73', '33', '31', '12', '13', '33', '32', '32', '33', '23', '33', '33', '33', '32', '32', '32', '33', '57', '4', '35', '6', '31', '33', '5', '30', '30', '32', '33', '6', '32', '32', '5', '8', '82', '33', '32', '34', '11', '5', '15', '33', '32', '6', '32', '5', '33', '32', '32', '32', '33', '33', '11', '28', '28', '32', '5', '35', '33', '32', '33', '32', '33', '32', '5', '32', '32', '33', '19', '32', '49', '33', '33', '32', '3', '32', '32', '34', '32', '5', '32', '32', '33', '13', '29', '35', '32', '32', '5', '29', '33', '5', '33', '32', '33', '33', '7', '32', '33', '32', '7', '32', '14', '5', '32', '32', '32', '5', '5', '5', '4', '5', '5', '5', '14', '8', '32', '33', '32', '30', '32', '33', '24', '11', '32', '4', '32', '32', '27', '32', '32', '51', '31', '33', '49', '6', '33', '12', '33', '5', '33', '8', '5', '33', '32', '30', '9', '31', '33', '32', '14', '5', '32', '32', '32', '32', '32', '49', '32', '32', '32', '21', '33', '33', '32', '32', '32', '33', '32', '33', '32', '19', '23', '33', '33', '32', '32', '32', '33', '33', '30', '32', '33', '5', '32', '4', '32', '32', '7', '33', '5', '5', '5', '30', '5', '32', '30', '12', '7', '53', '6', '32', '6', '5', '5', '48', '33', '34', '4', '33', '32', '32', '33', '8', '32', '32', '33', '32', '32', '32', '12', '32', '5', '33', '32', '33', '15', '32', '16', '32', '33', '32', '32', '32', '32', '27', '33', '32', '32', '34', '33', '32', '34', '7', '32', '33', '32', '32', '33', '48', '12', '33', '32', '33', '33', '32', '33', '4', '5', '32', '33', '32', '32', '61', '13', '32', '32', '35', '32', '35', '32', '32', '33', '85', '32', '5', '30', '32', '33', '32', '5', '33', '4', '4', '32', '5', '4', '32', '25', '34', '32', '11', '32', '33', '32', '5', '4', '32', '32', '33', '47', '33', '12', '12', '32', '32', '33', '7', '32', '32', '32', '30', '32', '32', '32', '32', '4', '32', '33', '5', '31', '8', '11', '76', '32', '6', '32', '11', '49', '5', '25', '49', '32', '11', '4', '32', '32', '32', '33', '32', '32', '71', '32', '4', '32', '32', '33', '32', '12', '32', '29', '13', '12', '5', '31', '32', '32', '34', '33', '31', '8', '33', '32', '32', '33', '33', '32', '32', '9', '12', '32', '33', '32', '46', '32', '32', '34', '32', '33', '11', '5', '32', '32', '33', '30', '32', '21', '32', '33', '33', '33', '32', '33', '14', '33', '32', '32', '33', '33', '7', '33', '32', '45', '42', '32', '51', '1', '33', '8', '32', '33', '33', '5', '33', '32', '32', '10', '33', '32', '32', '32', '32', '32', '33', '31', '5', '6', '5', '10', '32', '30', '33', '5', '32', '27', '38', '12', '5', '32', '33', '32', '32', '12', '32', '67', '34', '33', '32', '32', '32', '33', '8', '33', '33', '60', '7', '33', '32', '8', '5', '61', '32', '32', '5', '7', '32', '19', '32', '6', '32', '33', '4', '49', '34', '33', '32', '32', '31', '49', '30', '10', '11', '33', '33', '33', '32', '30', '32', '32', '11', '33', '33', '32', '49', '15', '32', '64', '12', '33', '5', '6', '5', '30', '33', '32', '33', '11', '32', '26', '34', '31', '33', '33', '49', '13', '</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>['Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atend</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>['85974001107', '85981010387', '85981010504', '85981010801', '85981011300', '85981011982', '85981012709', '85981012859', '85981012916', '85981013105', '85981013139', '85981013252', '85981014486', '85981015083', '85981015199', '85981015345', '85981015408', '85981015858', '85981018191', '85981019737', '85981019859', '85981020615', '85981021220', '85981021847', '85981021858', '85981023473', '85981024243', '85981024932', '85981025159', '85981026077', '85981026188', '85981026342', '85981029941', '85981034608', '85981035347', '85981037998', '85981038369', '85981040609', '85981041303', '85981042289', '85981046232', '85981047325', '85981047447', '85981050094', '85981050305', '85981050670', '85981050778', '85981050921', '85981051007', '85981051157', '85981051236', '85981051357', '85981051407', '85981051960', '85981052023', '85981052147', '85981052388', '85981053361', '85981053645', '85981053870', '85981054245', '85981054310', '85981054721', '85981054784', '85981055402', '85981055606', '85981055887', '85981056204', '85981056432', '85981057133', '85981057473', '85981057594', '85981057657', '85981058510', '85981058575', '85981059167', '85981060358', '85981060840', '85981060881', '85981060903', '85981060912', '85981061514', '85981062036', '85981062783', '85981062811', '85981063144', '85981063180', '85981063445', '85981063577', '85981063706', '85981063708', '85981063769', '85981064311', '85981064501', '85981064633', '85981066228', '85981066596', '85981066800', '85981067063', '85981067120', '85981067303', '85981067738', '85981068259', '85981068383', '85981068838', '85981069073', '85981069268', '85981069285', '85981069288', '85981069331', '85981069531', '85981069805', '85981070139', '85981070716', '85981070933', '85981072516', '85981074292', '85981074824', '85981077799', '85981079793', '85981080110', '85981081102', '85981081645', '85981081717', '85981081963', '85981082567', '85981082798', '85981083944', '85981083955', '85981084430', '85981085176', '85981085425', '85981086055', '85981087566', '85981090951', '85981092003', '85981094270', '85981095658', '85981096027', '85981097092', '85981097525', '85981099771', '85981099834', '85981104139', '85981105541', '85981111379', '85981111687', '85981112198', '85981112368', '85981113354', '85981116111', '85981116475', '85981117229', '85981117240', '85981117970', '85981118916', '85981119356', '85981121743', '85981121756', '85981121918', '85981122659', '85981122830', '85981124417', '85981125198', '85981125364', '85981127000', '85981127863', '85981128332', '85981128640', '85981129033', '85981130954', '85981131390', '85981132338', '85981132657', '85981132861', '85981133001', '85981136515', '85981137269', '85981137935', '85981138484', '85981139818', '85981141110', '85981141235', '85981142047', '85981142397', '85981144074', '85981144194', '85981144290', '85981144476', '85981145210', '85981145431', '85981146150', '85981147761', '85981148652', '85981149605', '85981149798', '85981149833', '85981150270', '85981152513', '85981152668', '85981152923', '85981153276', '85981154070', '85981154704', '85981154767', '85981155516', '85981155609', '85981155832', '85981157497', '85981159783', '85981160701', '85981162279', '85981163532', '85981168773', '85981169336', '85981170375', '85981170419', '85981172174', '85981172237', '85981173080', '85981173491', '85981173596', '85981174595', '85981175102', '85981175961', '85981176245', '85981176511', '85981176843', '85981176855', '85981177377', '85981177436', '85981178111', '85981180220', '85981180748', '85981181223', '85981181460', '85981184568', '85981185113', '85981185397', '85981185432', '85981186162', '85981187777', '85981187790', '85981188522', '85981190449', '85981190603', '85981190941', '85981191324', '85981191501', '85981192668', '85981193462', '85981194504', '85981195274', '85981195777', '85981196765', '85981199009', '85981200624', '85981204580', '85981205000', '85981207224', '85981210397', '85981211722', '85981211785', '85981212297', '85981212335', '85981215121', '85981215323', '85981217007', '85981217070', '85981217271', '85981217334', '85981217865', '85981217880', '85981217928', '85981219726', '85981220015', '85981220097', '85981220132', '85981221107', '85981221148', '85981222412', '85981224119', '85981224486', '85981224995', '85981225097', '85981225167', '85981226403', '85981227172', '85981227283', '85981227812', '85981228111', '85981228405', '85981228468', '85981229862', '85981229918', '85981229981', '85981230013', '85981230104', '85981233010', '85981233031', '85981233110', '85981234275', '85981235443', '85981237281', '85981238571', '85981240151', '85981240906', '85981241794', '85981243937', '85981245200', '85981245595', '85981245660', '85981246453', '85981246810', '85981247191', '85981247682', '85981247801', '85981248056', '85981248614', '85981248938', '85981249006', '85981249077', '85981249520', '85981249804', '85981250065', '85981251340', '85981252190', '85981252202', '85981252814', '85981253454', '85981256347', '85981256415', '85981256918', '85981257594', '85981257644', '85981258954', '85981259116', '85981259996', '85981260093', '85981260293', '85981261976', '85981264023', '85981265628', '85981266155', '85981266554', '85981267575', '85981268163', '85981269254', '85981270887', '85981273817', '85981276088', '85981277050', '85981277171', '85981277778', '85981277862', '85981278172', '85981278481', '85981281110', '85981281122', '85981283976', '85981284254', '85981284771', '85981284904', '85981285694', '85981285757', '85981286755', '85981287954', '85981288208', '85981288338', '85981289201', '85981290315', '85981291170', '85981291852', '85981292335', '85981292898', '85981293237', '85981296943', '85981297006', '85981297774', '85981298411', '85981298474', '85981299369', '85981300207', '85981300265', '85981301018', '85981301029', '85981301090', '85981301430', '85981302820', '85981303653', '85981304383', '85981304684', '85981304736', '85981304842', '85981305581', '85981306366', '85981307620', '85981307802', '85981308045', '85981308259', '85981308292', '85981308328', '85981308337', '85981308391', '85981310114', '85981310742', '85981311091', '85981311398', '85981312075', '85981313089', '85981313134', '85981313616', '85981313627', '85981314051', '85981314422', '85981315654', '85981316754', '85981318080', '85981323921', '85981325550', '85981327070', '85981327436', '85981327760', '85981328852', '85981330136', '85981330758', '85981331850', '85981331913', '85981332190', '85981333065', '85981333339', '85981334650', '85981334713', '85981334761', '85981335534', '85981337373', '85981338263', '85981338307', '85981342092', '85981342565', '85981343138', '85981343533', '85981344833', '85981345060', '85981347012', '85981347371', '85981348351', '85981348558', '85981349404', '85981351875', '85981352588', '85981352826', '85981353374', '85981353997', '85981354648', '85981355846', '85981357814', '85981359310', '85981360852', '85981361507', '85981361779', '85981362003', '85981362066', '85981363777', '85981365886', '85981366880', '85981367170', '85981368633', '85981370043', '85981370894', '85981371153', '85981371868', '85981372645', '85981374219', '85981375527', '85981375801', '85981375825', '85981376079', '85981377391', '85981378159', '85981378792', '85981378905', '85981379505', '85981379662', '85981380597', '85981380924', '85981381707', '85981381999', '85981383237', '85981383353', '85981384426', '85981385151', '85981385624', '85981385673', '85981385841', '85981386704', '85981386821', '85981387227', '85981387362', '85981388619', '85981391330', '85981391423', '85981391880', '85981392100', '85981392565', '85981395635', '85981395687', '85981395818', '85981397246', '85981397372', '85981397409', '85981397411', '85981398764', '85981400369', '85981401399', '85981401626', '85981401752', '85981402041', '85981402081', '85981402748', '85981402997', '85981403093', '85981403964', '85981404116', '85981404174', '85981404374', '85981404793', '85981405917', '85981408267', '85981409242', '85981409843', '85981411024', '85981411624', '85981411687', '85981413039', '85981413532', '85981413653', '85981413838', '85981413892', '85981414546', '85981415469', '85981416386', '85981416409', '85981418850', '85981419344', '85981420019', '85981421525', '85981421738', '85981422245', '85981422308', '85981422576', '85981422856', '85981423490', '85981423505', '85981423933', '85981424271', '85981424607', '85981425703', '85981426537', '85981426942', '85981427253', '85981428860', '85981428912', '85981432332', '85981433880', '85981436330', '85981437233', '85981437797', '85981440921', '85981442203', '85981443375', '85981444452', '85981444515', '85981445843', '85981447674', '85981448037', '85981452309', '85981453385', '85981460147', '85981460175', '85981460392', '85981460457', '85981460646', '85981460699', '85981460861', '85981460924', '85981460996', '85981461065', '85981461106', '85981461610', '85981462406', '85981463746', '85981463860', '85981464262', '85981464411', '85981464530', '85981464545', '85981465735', '85981465772', '85981465798', '85981466545', '85981467570', '85981468790', '85981470659', '85981470831', '85981471492', '85981471759', '85981472233', '85981473750', '85981474263', '85981474389', '85981474696', '85981474697', '85981474756', '85981474760', '85981474778', '85981474912', '85981474923', '85981475220', '85981475230', '85981475761', '85981475972', '85981475980', '85981476043', '85981476212', '85981476638', '85981477326', '85981477413', '85981477799', '85981477812', '85981477813', '85981477916', '85981478494', '85981478784', '85981479493', '85981479515', '85981479752', '85981479774', '85981481053', '85981481331', '85981481726', '85981482109', '85981482140', '85981482476', '85981482990', '85981483810', '85981484967', '85981485284', '85981485480', '85981486380', '85981486397', '85981487878', '85981488161', '85981488741', '85981489506', '85981489546', '85981489609', '85981489986', '85981491380', '85981491428', '85981491439', '85981492666', '85981492729', '85981495205', '85981495268', '85981495465', '85981495615', '85981495911', '85981495935', '85981496025', '85981496943', '85981497099', '85981497122', '85981497496', '85981497614', '85981499186', '85981500414', '85981500847', '85981500940', '85981501090', '85981501968', '85981502098', '85981502241', '85981505500', '85981505522', '85981505531', '85981505586', '85981505887', '85981506224', '85981506332', '85981506467', '85981506955', '85981507053', '85981507770', '85981507930', '85981509140', '85981509349', '85981509981', '85981510677', '85981511295', '85981512929', '85981514081', '85981514747', '85981518467', '85981518484', '85981520304', '85981521334', '85981521816', '85981521879', '85981521962', '85981522121', '85981522321', '85981522480', '85981522523', '85981522914', '85981522917', '85981522933', '85981522980', '85981523042', '85981523247', '85981523548', '85981523703', '85981523830', '85981523864', '85981524209', '85981524336', '85981524345', '85981524388', '85981524433', '85981524474', '85981525329', '85981525392', '85981525946', '85981525956', '85981525970', '85981526066', '85981526142', '85981526377', '85981526414', '85981526660', '85981526890', '85981526953', '85981527026', '85981527241', '85981527738', '85981527876', '85981527926', '85981528100', '85981528344', '85981528523', '85981529250', '85981530016', '85981530202', '85981530228', '85981530264', '85981530358', '85981530695', '85981531466', '85981532323', '85981532367', '85981532706', '85981533140', '85981533536', '85981533817', '85981533861', '85981533924', '85981534836', '85981535019', '85981535381', '85981535444', '85981535702', '85981536001', '85981536037', '85981536784', '85981537054', '85981537071', '85981537451', '85981537531', '85981537646', '85981538008', '85981538403', '85981538473', '85981539100', '85981539364', '85981539374', '85981539613', '85981539674', '85981539710', '85981539904', '85981542565', '85981544220', '85981544377', '85981544415', '85981544420', '85981544535', '85981544744', '85981545730', '85981545967', '85981546135', '85981546201', '85981546486', '85981546524', '85981547100', '85981547151', '85981547181', '85981548573', '85981548663', '85981549807', '85981550607', '85981551701', '85981552786', '85981552815', '85981553207', '85981553257', '85981553774', '85981554041', '85981554682', '85981555448', '85981556360', '85981556386', '85981556391', '85981556708', '85981557599', '85981557763', '85981557766', '85981557996', '85981558443', '85981558444', '85981558593', '85981558734', '85981558921', '85981559352', '85981559880', '85981559990', '85981561122', '85981561397', '85981563114', '85981563918', '85981565385', '85981566296', '85981569388', '85981570332', '85981570553', '85981571936', '85981571948', '85981573149', '85981574029', '85981574749', '85981574828', '85981575288', '85981576121', '85981577685', '85981579715', '85981580747', '85981582223', '85981587265', '85981588881', '85981589028', '85981590283', '85981590581', '85981591212', '85981591394', '85981592814', '85981594445', '85981594455', '85981598314', '85981599091', '85981599720', '85981600032', '85981600288', '85981600746', '85981601467', '85981601515', '85981601621', '85981603545', '85981603701', '85981603764', '85981603922', '85981604044', '85981604097', '85981604901', '85981605888', '85981606241', '85981606453', '85981606516', '85981606875', '85981607061', '85981607171', '85981607847', '85981608039', '85981608131', '85981608656', '85981608885', '85981609224', '85981609765', '85981611504', '85981611687', '85981612354', '85981612497', '85981613707', '85981614805', '85981615721', '85981615726', '85981616672', '85981617048', '85981617443', '85981617809', '85981618157', '85981618463', '85981618696', '85981619089', '85981621012', '85981625207', '85981625719', '85981625789', '85981625797', '85981626292', '85981626455', '85981627178', '85981627515', '85981627750', '85981628353', '85981628962', '85981629450', '85981630101', '85981630164', '85981631945', '85981632116', '85981635515', '85981635650', '85981636098', '85981636649', '85981638200', '85981638739', '85981639201', '85981642110', '85981642480', '85981645543', '85981646909', '85981647853', '85981649485', '85981651235', '85981651813', '85981651856', '85981653359', '85981654096', '85981655420', '85981655504', '85981656015', '85981656761', '85981663973', '85981664051', '85981665088', '85981665658', '85981665867', '85981666220', '85981666585', '85981666685', '85981668986', '85981669316', '85981669696', '85981669892', '85981670050', '85981670209', '85981670557', '85981671233', '85981672007', '85981672198', '85981672687', '85981676600', '85981677013', '85981677923', '85981677986', '85981679022', '85981679393', '85981684827', '85981685253', '85981687262', '85981688088', '85981688530', '85981689614', '85981690885', '85981692225', '85981693076', '85981694698', '85981696440', '85981700371', '85981701616', '85981701789', '85981702211', '85981704587', '85981705823', '85981706117', '85981706812', '85981707565', '85981709424', '85981709639', '85981709959', '85981709997', '85981711415', '85981712700', '85981715589', '85981717124', '85981721330', '85981721470', '85981723162', '85981723682', '85981727178', '85981727333', '85981730276', '85981731368', '85981733009', '85981733173', '85981734225', '85981735351', '85981735457', '85981738337', '85981742689', '85981745007', '85981746191', '85981746231', '85981747230', '85981747684', '85981747880', '85981748018', '85981749098', '85981749311', '85981780097', '85981780698', '85981781860', '85981781956', '85981782615', '85981783993', '85981787014', '85981787375', '85981787694', '85981787878', '85981795562', '85981797415', '85981799011', '85981799243', '85981799393', '85981799969', '85981800644', '85981801187', '85981801628', '85981801718', '85981801761', '85981802537', '85981802631', '85981803848', '85981804731', '85981805074', '85981805578', '85981805682', '85981805712', '85981805995', '85981806062', '85981806192', '85981806838', '85981807096', '85981807746', '85981808109', '85981808226', '85981808940', '85981809310', '85981809579', '85981810401', '85981811681', '85981812231', '85981812420', '85981813215', '85981813326', '85981813696', '85981813745', '85981814222', '85981815518', '85981815719', '85981815951', '85981815995', '85981816185', '85981816597', '85981816953', '85981817644', '85981819191', '85981819878', '85981819898', '85981819971', '85981820302', '85981820909', '85981822288', '85981822627', '85981823737', '85981824050', '85981825667', '85981827171', '85981827298', '85981828133', '85981829674', '85981829888', '85981830615', '85981831333', '85981831807', '85981832616', '85981833911', '85981836027', '85981836192', '85981838197', '85981839905', '85981840699', '85981840997', '85981841498', '85981842018', '85981842026', '85981847568', '85981849140', '85981849448', '85981850329', '85981851336', '85981851657', '85981851806', '85981852483', '85981852871', '85981853361', '85981853473', '85981853498', '85981854188', '85981854400', '85981854701', '85981854966', '85981855387', '85981855943', '85981857602', '85981858378', '85981858585', '85981859714', '85981859843', '85981860190', '85981860939', '85981861386', '85981861390', '85981862200', '85981862732', '85981862812', '85981863520', '85981863917', '85981864665', '85981866872', '85981867198', '85981867874', '85981868706', '85981869078', '85981869877', '85981870279', '85981870625', '85981870769', '85981871433', '85981871482', '85981871725', '85981872527', '85981873853', '85981874873', '85981875089', '85981875839', '85981876038', '85981876387', '85981877277', '85981877340', '85981877666', '85981878608', '85981879558', '85981879727', '85981881447', '85981881564', '85981881903', '85981882019', '85981882233', '85981883888', '85981885848', '85981886408', '85981888076', '85981890073', '85981890692', '85981890804', '85981890897', '85981891321', '85981891476', '85981892737', '85981892922', '85981893512', '85981894559', '85981895421', '85981895778', '85981895877', '85981899243', '85981900080', '85981900730', '85981901391', '85981904698', '85981905011', '85981905074', '85981905075', '85981906452', '85981910262', '85981910771', '85981911604', '85981911984', '85981914747', '85981917082', '85981917653', '85981917936', '85981918090', '85981918203', '85981921936', '85981921999', '85981922555', '85981924869', '85981926087', '85981926161', '85981927362', '85981928269', '85981930502', '85981933090', '85981933446', '85981934488', '85981937771', '85981942675', '85981944086', '85981946447', '85981947455', '85981948504', '85981948560', '85981948709', '85981949370', '85981949405', '85981950680', '85981951197', '85981951207', '85981951277', '85981951294', '85981951433', '85981952223', '85981952606', '85981953266', '85981955156', '85981955666', '85981956683', '85981956798', '85981956914', '85981956977', '85981958219', '85981958833', '85981959454', '85981962203', '85981963748', '85981964770', '85981966391', '85981966744', '85981967093', '85981967347', '85981967672', '85981972215', '85981973787', '85981973850', '85981974619', '85981975003', '85981975335', '85981975643', '85981978964', '85981982384', '85981982415', '85981983536', '85981984160', '85981984196', '85981984205', '85981985320', '85981987749', '85981990206', '85981991814', '85981992200', '85981992221', '85981993841', '85981994171', '85981994544', '85981996677', '85981996968', '85981997233', '85981998183', '85981998880', '85981999101', '85981999393', '85982000080', '85982000103', '85982000124', '85982000407', '85982000597', '85982001158', '85982001480', '85982001603', '85982002244', '85982003360', '85982009691', '85982012352', '85982013350', '85982013725', '85982014410', '85982014728', '85982014859', '85982015963', '85982016650', '85982018181', '85982019178', '85982020684', '85982020732', '85982021675', '85982021901', '85982021970', '85982022116', '85982022707', '85982023008', '85982023198', '85982023449', '85982024092', '85982024412', '85982024556', '85982025193', '85982025465', '85982025505', '85982026115', '85982026559', '85982026582', '85982026618', '85982026681', '85982026958', '85982027257', '85982027456', '85982028016', '85982028614', '85982028717', '85982029544', '85982029630', '85982029656', '85982031994', '85982033246', '85982036215', '85982038136', '85982038199', '85982038964', '85982041982', '85982048028', '85982048400', '85982048768', '85982049005', '85982050430', '85982051850', '85982052170', '85982052833', '85982053074', '85982058486', '85982059867', '85982060243', '85982061188', '85982061715', '85982065404', '85982066323', '85982066720', '85982067095', '85982067924', '85982069921', '85982070325', '85982070442', '85982070505', '85982070537', '85982075392', '85982076079', '85982077220', '85982080055', '85982080963', '85982081863', '85982082408', '85982082685', '85982086204', '85982086988', '85982088181', '85982088401', '85982090444', '85982092229', '85982092410', '85982092535', '85982095933', '85982096408', '85982096638', '85982096702', '85982098898', '85982099596', '85982101224', '85982102764', '85982103459', '85982103837', '85982104191', '85982105219', '85982105253', '85982105588', '85982106049', '85982107612', '85982108435', '85982108824', '85982108871', '85982108995', '85982109939', '85982110388', '85982110918', '85982111162', '85982111405', '85982111461', '85982111682', '85982111714', '85982112134', '85982112150', '85982112252', '85982112330', '85982112561', '85982112835', '85982113153', '85982113424', '85982113947', '85982114041', '85982114590', '85982114798', '85982115352', '85982115530', '85982116277', '85982116934', '85982116997', '85982118281', '85982118296', '85982118359', '85982118717', '85982119038', '85982119077', '85982120196', '85982120770', '85982121018', '85982121624', '85982122300', '85982122468', '85982123793', '85982123880', '85982125254', '85982126275', '85982127512', '85982130408', '85982130446', '85982131720', '85982132411', '85982132443', '85982132450', '85982133520', '85982134594', '85982134658', '85982140032', '85982141654', '85982144572', '85982145647', '85982145648', '85982147385', '85982147517', '85982148150', '85982148935', '85982150345', '85982154109', '85982154431', '85982154497', '85982155595', '85982155633', '85982161243', '85982161749', '85982162384', '85982162735', '85982163153', '85982164038', '85982166162', '85982166295', '85982166369', '85982170184', '85982171502', '85982171541', '85982171985', '85982184521', '85982185872', '85982190343', '85982204545', '85982205828', '85982207580', '85982217764', '85982222262', '85982223649', '85982225298', '85982234415', '85982243000', '85982254767', '85982254833', '85984000187', '85984000206', '85984000276', '85984000283', '85984000366', '85984000374', '85984000408', '85984000419', '85984000570', '85984000752', '85984000901', '85984000924', '85984001030', '85984001034', '85984001146', '85984001200', '85984001263', '85984001399', '85984001670', '85984001714', '85984001904', '85984002329', '85984002699', '85984004021', '85984004143', '85984004381', '85984004513', '85984004885', '85984004934', '85984004937', '85984005030', '85984005089', '85984005191', '85984005207', '85984005486', '85984005676', '85984005684', '85984005854', '85984006088', '85984006430', '85984006519', '85984006807', '85984006822', '85984006945', '85984007418', '85984007839', '85984007934', '85984008090', '85984008165', '85984008494', '85984008541', '85984008711', '85984008837', '85984008876', '85984009118', '85984009152', '85984010102', '85984010119', '85984010346', '85984010352', '85984010376', '85984010523', '85984010651', '85984010721', '85984010796', '85984011030', '85984011127', '85984011205', '85984011272', '85984011345', '85984011423', '85984012202', '85984012591', '85984012893', '85984013559', '85984013847', '85984013900', '85984013932', '85984013963', '85984014210', '85984014231', '85984014288', '85984014376', '85984014432', '85984014547', '85984015074', '85984015099', '85984015349', '85984015384', '85984015385', '85984015469', '85984015572', '85984015631', '85984015661', '85984015695', '85984015758', '85984015793', '85984015918', '85984015943', '85984015948', '85984016599', '85984016848', '85984017946', '85984018354', '85984019606', '85984019846', '85984019986', '85984020049', '85984020051', '85984020177', '85984020235', '85984020417', '85984020826', '85984020911', '85984021324', '85984021461', '85984021871', '85984022102', '85984022241', '85984022389', '85984022437', '85984022645', '85984023016', '85984023231', '85984023332', '85984023361', '85984023534', '85984024023', '85984024057', '85984024750', '85984024773', '85984024790', '85984024966', '85984025156', '85984025366', '85984025761', '85984026229', '85984026355', '85984026707', '85984026882', '85984026909', '85984026937', '85984027014', '85984027778', '85984027803', '85984027980', '85984028311', '85984028478', '85984028528', '85984028635', '85984028807', '85984029384', '85984029403', '85984029645', '85984029647', '85984029806', '85984029997', '85984030002', '85984030015', '85984030126', '85984030128', '85984030255', '85984030534', '85984030799', '85984030914', '85984031018', '85984031134', '85984031235', '85984031240', '85984031369', '85984031377', '85984031387', '85984031438', '85984031757', '85984031799', '85984031859', '85984031951', '85984031983', '85984031996', '85984032024', '85984032030', '85984032046', '85984032152', '85984032209', '85984032278', '85984032838', '85984032911', '85984033253', '85984033308', '85984033709', '85984033733', '85984033741', '85984033796', '85984033825', '85984033893', '85984033983', '85984034114', '85984034385', '85984034577', '85984034588', '85984034633', '85984034782', '85984034964', '85984035081', '85984035134', '85984035188', '85984035416', '85984035423', '85984035459', '85984035494', '85984035559', '85984035765', '85984036032', '85984036315', '85984036485', '85984036570', '85984036614', '85984036676', '85984036734', '85984036808', '85984036872', '85984037291', '85984037296', '85984037302', '85984037313', '85984037354', '85984037682', '85984037921', '85984037935', '85984037947', '85984038033', '85984038229', '85984038524', '85984038538', '85984038620', '85984038850', '85984038856', '85984039320', '85984039429', '85984039451', '85984039728', '85984040449', '85984040502', '85984040554', '85984040731', '85984040757', '85984040783', '85984040792', '85984040899', '85984041029', '85984041044', '85984041297', '85984041417', '85984041458', '85984041670', '85984041713', '85984041805', '85984041914', '85984041986', '85984042380', '85984042425', '85984042497', '85984042509', '85984042623', '85984042895', '85984042963', '85984043070', '85984043137', '85984043296', '85984043323', '85984043326', '85984043413', '85984043751', '85984044012', '85984044067', '85984044191', '85984044248', '85984044283', '85984044300', '85984044346', '85984044633', '85984044683', '85984044763', '85984044963', '85984045050', '85984045056', '85984045115', '85984045640', '85984045722', '85984046240', '85984046424', '85984046625', '85984046753', '85984046806', '85984046807', '85984046867', '85984047111', '85984047230', '85984047233', '85984047367', '85984047472', '85984047476', '85984047517', '85984047596', '85984048175', '85984048182', '85984048183', '85984048283', '85984048339', '85984048508', '85984048524', '85984048559', '85984048759', '85984048849', '85984049026', '85984049029', '85984049263', '85984049442', '85984049451', '85984049504', '85984049679', '85984049735', '85984049763', '85984049858', '85984049949', '85984050227', '85984050228', '85984050250', '85984050371', '85984050677', '85984050801', '85984050882', '85984050887', '85984050928', '85984051292', '85984051333', '85984051412', '85984051489', '85984051523', '85984051742', '85984051769', '85984051840', '85984051889', '85984051935', '85984052109', '85984052112', '85984052208', '85984052217', '85984052263', '85984052298', '85984052611', '85984052730', '85984052764', '85984052843', '85984053038', '85984053174', '85984053179', '85984053330', '85984053556', '85984053869', '85984053880', '85984053887', '85984053943', '85984053956', '85984054025', '85984054056', '85984054133', '85984054160', '85984054172', '85984054228', '85984054266', '85984054556', '85984054674', '85984054734', '85984054739', '85984054879', '85984054912', '85984055156', '85984055310', '85984055345', '85984055442', '85984055473', '85984055502', '85984055688', '85984055714', '85984055899', '85984055933', '85984056265', '85984056517', '85984056826', '85984056911', '85984056971', '85984057268', '85984057361', '85984057589', '85984057713', '85984057802', '85984057880', '85984058809', '85984059297', '85984059565', '85984059708', '85984060013', '85984060654', '85984060832', '85984061103', '85984061137', '85984061447', '85984061486', '85984061543', '85984061639', '85984061962', '85984062029', '85984062279', '85984062320', '85984062358', '85984062494', '85984062505', '85984062530', '85984063166', '85984063203', '85984063719', '85984063744', '85984063839', '85984064263', '85984064393', '85984064541', '85984064961', '85984065160', '85984065816', '85984066050', '85984066966', '85984067046', '85984067756', '85984067873', '85984068456', '85984069092', '85984069667', '85984069722', '85984069938', '85984070019', '85984070211', '85984070265', '85984070421', '85984070652', '85984070895', '85984071052', '85984071611', '85984071870', '85984072029', '85984072045', '85984072051', '85984072058', '85984072071', '85984072145', '85984072225', '85984072316', '85984072445', '85984072480', '85984072653', '85984072933', '85984073162', '85984073973', '85984074264', '85984074313', '85984074778', '85984075096', '85984075666', '85984076005', '85984076212', '85984076393', '85984076578', '85984076839', '85984076847', '85984077031', '85984077361', '85984077370', '85984077740', '85984077801', '85984078005', '85984078034', '85984078218', '85984078233', '85984078314', '85984078445', '85984078614', '85984079116', '85984079245', '85984079370', '85984079725', '85984079880', '85984079915', '85984080469', '85984080471', '85984080593', '85984080601', '85984081278', '85984081475', '85984081680', '85984082025', '85984082125', '85984082555', '85984082670', '85984082940', '85984082979', '85984083419', '85984083846', '85984084306', '85984084464', '85984084549', '85984084550', '85984084823', '85984084857', '85984085018', '85984085176', '85984085262', '85984085880', '85984086976', '85984087409', '85984088006', '85984088529', '85984089052', '85984089070', '85984089220', '85984089798', '85984090380', '85984090552', '85984090594', '85984090882', '85984090929', '85984091124', '85984091289', '85984091406', '85984091518', '85984092054', '85984092195', '85984092230', '85984092539', '85984093168', '85984093610', '85984093759', '85984093855', '85984094073', '85984094849', '85984095284', '85984096033', '85984098963', '85984099235', '85984099245', '85984099377', '85984099885', '85984100300', '85984100698', '85984100822', '85984101624', '85984101697', '85984102042', '85984102155', '85984102262', '85984102480', '85984102514', '85984102560', '85984102571', '85984103927', '85984104957', '85984105301', '85984105524', '85984106425', '85984107192', '85984107381', '85984107762', '85984108029', '85984108520', '85984108531', '85984108645', '85984108950', '85984109045', '85984109435', '85984109534', '85984110121', '85984110186', '85984110449', '85984110493', '85984110570', '85984110730', '85984110811', '85984111215', '85984111369', '85984111609', '85984111626', '85984111796', '85984111877', '85984111930', '85984112126', '85984112139', '85984112386', '85984112657', '85984113012', '85984113687', '85984113734', '85984113870', '85984113916', '85984114001', '85984114121', '85984114826', '85984114827', '85984115475', '85984115569', '85984115651', '85984116121', '85984116540', '85984116596', '85984116734', '85984116933', '85984117008', '85984117204', '85984117429', '85984117798', '85984118037', '85984118042', '85984118203', '85984118581', '85984118664', '85984118708', '85984118774', '85984119107', '85984119481', '85984119572', '85984119808', '85984120393', '85984120682', '85984121272', '85984122145', '85984122414', '85984123034', '85984123448', '85984124093', '85984124208', '85984125015', '85984125036', '85984126078', '85984126186', '85984126390', '85984126584', '85984126778', '85984126955', '85984127219', '85984127242', '85984127734', '85984128627', '85984128634', '85984128869', '85984128924', '85984129311', '85984129612', '85984130038', '85984130659', '85984130724', '85984130979', '85984131046', '85984131139', '85984131313', '85984131574', '85984131761', '85984131881', '85984132127', '85984132128', '85984132149', '85984132782', '85984132844', '85984133084', '85984133130', '85984133206', '85984133331', '85984133448', '85984133534', '85984134089', '85984134736', '85984135015', '85984135302', '85984135420', '85984135573', '85984</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>['24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['10', '27', '27', '27', '46', '30', '27', '1', '5', '29', '1', '35', '16', '43', '27', '27', '27', '11', '5', '28', '1', '49', '27', '27', '1', '27', '0', '27', '11', '1', '28', '10', '3', '27', '3', '28', '27', '31', '1', '25', '1', '27', '27', '40', '27', '27', '28', '27', '27', '12', '28', '5', '7', '6', '28', '40', '49', '1', '2', '8', '78', '1', '1', '27', '5', '27', '1', '27', '27', '11', '1', '28', '12', '27', '27', '1', '5', '27', '27', '2', '27', '27', '27', '25', '7', '27', '28', '1', '11', '27', '1', '1', '27', '21', '13', '6', '27', '5', '1', '0', '28', '27', '28', '27', '27', '27', '27', '27', '27', '7', '28', '5', '5', '27', '27', '47', '28', '27', '34', '1', '35', '5', '8', '12', '28', '27', '12', '49', '28', '27', '6', '27', '1', '1', '17', '5', '27', '1', '1', '28', '31', '1', '27', '12', '5', '27', '39', '49', '19', '16', '28', '27', '5', '27', '8', '27', '4', '35', '8', '30', '35', '1', '27', '27', '10', '40', '1', '27', '27', '49', '27', '29', '27', '27', '1', '28', '43', '32', '45', '30', '27', '27', '6', '27', '5', '2', '27', '7', '49', '13', '28', '6', '27', '27', '27', '27', '26', '27', '27', '27', '28', '49', '1', '27', '11', '28', '27', '27', '27', '27', '1', '18', '28', '27', '27', '27', '1', '27', '1', '49', '10', '27', '5', '49', '1', '11', '27', '49', '27', '27', '5', '49', '27', '7', '5', '28', '1', '29', '27', '11', '31', '38', '27', '15', '27', '27', '49', '17', '41', '8', '27', '1', '28', '30', '28', '3', '27', '30', '30', '5', '27', '10', '1', '49', '27', '28', '1', '27', '4', '1', '28', '5', '27', '27', '12', '28', '10', '27', '27', '48', '1', '1', '1', '27', '30', '1', '27', '27', '27', '29', '27', '5', '27', '27', '6', '1', '30', '27', '28', '1', '12', '5', '29', '25', '27', '49', '27', '27', '6', '11', '27', '27', '27', '27', '11', '27', '1', '27', '27', '27', '27', '27', '30', '27', '49', '28', '28', '23', '40', '27', '28', '27', '27', '27', '5', '11', '27', '27', '1', '5', '11', '28', '27', '27', '27', '28', '9', '5', '27', '11', '27', '1', '35', '1', '27', '1', '27', '27', '1', '30', '27', '27', '28', '17', '27', '27', '1', '27', '35', '49', '27', '49', '27', '27', '11', '27', '12', '27', '27', '8', '4', '49', '11', '27', '35', '4', '28', '27', '27', '27', '5', '18', '1', '5', '27', '27', '1', '28', '27', '1', '1', '11', '1', '1', '28', '114', '9', '27', '27', '5', '28', '27', '27', '1', '23', '27', '27', '5', '1', '27', '1', '5', '27', '27', '27', '27', '87', '27', '28', '31', '39', '34', '27', '27', '27', '9', '13', '9', '1', '17', '27', '35', '27', '30', '12', '27', '27', '49', '6', '27', '27', '27', '1', '28', '1', '30', '27', '27', '27', '12', '27', '27', '27', '1', '28', '0', '27', '49', '27', '27', '1', '28', '27', '27', '49', '27', '27', '27', '49', '27', '27', '6', '49', '1', '27', '9', '1', '28', '42', '13', '31', '27', '15', '8', '49', '27', '5', '27', '8', '27', '29', '27', '27', '49', '27', '14', '27', '28', '27', '27', '49', '29', '11', '27', '27', '12', '27', '27', '27', '27', '27', '1', '27', '5', '22', '1', '27', '27', '49', '17', '29', '11', '27', '27', '5', '13', '1', '10', '27', '28', '27', '27', '27', '27', '27', '5', '24', '27', '1', '1', '27', '1', '30', '27', '27', '27', '1', '14', '19', '25', '27', '27', '27', '27', '49', '27', '30', '11', '30', '5', '27', '27', '1', '27', '28', '27', '1', '29', '27', '27', '1', '5', '1', '37', '49', '1', '5', '2', '82', '5', '27', '27', '30', '8', '27', '5', '27', '27', '27', '28', '49', '27', '27', '27', '27', '28', '5', '27', '27', '1', '27', '14', '5', '49', '31', '1', '27', '1', '27', '5', '27', '27', '27', '28', '1', '12', '40', '27', '43', '27', '27', '1', '27', '49', '49', '21', '27', '27', '22', '27', '7', '12', '27', '27', '0', '1', '27', '27', '27', '28', '1', '7', '28', '49', '27', '27', '27', '7', '28', '16', '1', '1', '27', '12', '10', '12', '27', '27', '4', '27', '27', '30', '5', '12', '29', '27', '27', '17', '27', '27', '13', '5', '27', '12', '16', '49', '27', '1', '27', '6', '49', '29', '27', '28', '18', '28', '49', '27', '27', '27', '30', '27', '7', '23', '49', '12', '16', '27', '1', '5', '1', '27', '27', '27', '27', '27', '27', '27', '49', '27', '28', '27', '1', '27', '27', '27', '27', '27', '49', '21', '27', '28', '27', '27', '28', '35', '27', '49', '1', '27', '27', '26', '27', '38', '27', '1', '6', '27', '27', '28', '7', '28', '27', '27', '27', '27', '12', '5', '6', '27', '18', '28', '17', '27', '27', '28', '23', '14', '27', '12', '29', '28', '28', '27', '27', '27', '27', '28', '28', '49', '5', '27', '12', '27', '27', '27', '49', '27', '27', '12', '8', '27', '28', '28', '1', '9', '28', '27', '27', '27', '1', '1', '10', '1', '28', '27', '12', '1', '7', '27', '27', '27', '27', '28', '27', '27', '27', '5', '27', '12', '46', '27', '27', '31', '35', '17', '28', '27', '20', '24', '23', '1', '41', '36', '49', '49', '7', '28', '49', '27', '27', '5', '5', '27', '1', '5', '17', '27', '28', '13', '7', '49', '28', '27', '27', '27', '1', '34', '42', '35', '27', '28', '28', '28', '35', '11', '27', '5', '5', '28', '28', '27', '28', '1', '28', '13', '27', '28', '27', '28', '30', '28', '28', '18', '27', '5', '1', '76', '28', '28', '1', '5', '1', '28', '26', '2', '28', '1', '7', '12', '28', '37', '11', '28', '27', '27', '27', '27', '28', '28', '27', '20', '8', '30', '14', '27', '4', '10', '4', '49', '28', '28', '1', '1', '22', '27', '1', '10', '28', '11', '28', '77', '28', '2', '27', '30', '27', '27', '31', '1', '28', '28', '12', '27', '28', '10', '30', '27', '9', '27', '18', '28', '0', '12', '28', '49', '27', '27', '27', '27', '30', '1', '28', '27', '50', '31', '1', '27', '1', '27', '28', '28', '28', '27', '7', '1', '28', '27', '1', '27', '31', '28', '27', '1', '28', '1', '49', '49', '27', '28', '27', '27', '1', '27', '28', '27', '5', '26', '12', '1', '28', '2', '8', '13', '1', '12', '1', '28', '27', '1', '30', '7', '7', '37', '27', '28', '8', '5', '27', '28', '27', '27', '13', '13', '27', '30', '13', '13', '27', '1', '28', '27', '28', '27', '31', '27', '13', '28', '27', '27', '28', '12', '27', '27', '7', '1', '29', '27', '27', '1', '5', '27', '13', '27', '28', '49', '27', '6', '28', '27', '1', '27', '27', '21', '28', '31', '46', '27', '28', '5', '5', '27', '27', '30', '7', '27', '28', '28', '28', '30', '9', '17', '1', '3', '30', '7', '27', '28', '27', '7', '37', '27', '14', '13', '28', '27', '27', '27', '1', '27', '27', '27', '27', '28', '6', '28', '27', '12', '27', '47', '49', '28', '28', '27', '27', '13', '14', '28', '12', '28', '7', '27', '28', '27', '27', '1', '1', '27', '14', '0', '1', '27', '1', '1', '31', '1', '5', '39', '35', '27', '28', '11', '30', '27', '1', '27', '49', '27', '28', '28', '27', '47', '27', '28', '28', '5', '28', '30', '11', '49', '27', '28', '1', '28', '28', '28', '27', '49', '30', '27', '28', '30', '27', '15', '49', '8', '28', '12', '27', '17', '28', '27', '30', '49', '1', '28', '28', '27', '27', '27', '49', '1', '26', '1', '27', '49', '1', '6', '27', '5', '28', '1', '27', '11', '16', '28', '114', '27', '27', '27', '34', '1', '6', '28', '49', '21', '27', '27', '27', '28', '10', '1', '27', '27', '27', '49', '1', '28', '28', '27', '31', '28', '28', '28', '49', '49', '27', '27', '27', '8', '28', '1', '11', '5', '1', '1', '27', '32', '49', '27', '9', '33', '27', '5', '28', '27', '31', '28', '27', '27', '27', '27', '27', '39', '30', '12', '13', '28', '34', '1', '27', '27', '28', '28', '15', '11', '27', '28', '1', '27', '1', '35', '27', '7', '17', '1', '35', '23', '27', '28', '1', '5', '28', '2', '21', '27', '28', '28', '28', '11', '49', '32', '28', '14', '14', '30', '27', '1', '28', '28', '28', '23', '1', '27', '27', '27', '28', '47', '27', '28', '1', '27', '27', '28', '42', '49', '27', '27', '5', '28', '27', '1', '28', '27', '26', '27', '27', '28', '28', '8', '5', '0', '49', '28', '28', '5', '28', '27', '28', '28', '41', '8', '27', '27', '27', '6', '27', '27', '27', '6', '1', '28', '30', '5', '27', '12', '2', '5', '28', '15', '5', '27', '28', '27', '12', '28', '28', '5', '27', '12', '28', '27', '27', '6', '1', '30', '28', '27', '28', '12', '27', '13', '1', '49', '31', '27', '12', '28', '27', '28', '27', '33', '27', '40', '27', '28', '28', '27', '0', '20', '27', '1', '43', '28', '28', '1', '49', '33', '27', '10', '28', '27', '28', '27', '27', '2', '27', '27', '49', '1', '28', '28', '43', '27', '27', '28', '49', '5', '28', '146', '10', '18', '28', '27', '27', '27', '28', '27', '28', '28', '28', '11', '1', '5', '6', '27', '8', '5', '9', '28', '1', '27', '28', '18', '27', '6', '6', '26', '27', '7', '27', '49', '8', '27', '75', '21', '58', '27', '27', '21', '27', '21', '6', '27', '29', '27', '27', '62', '69', '65', '17', '27', '49', '8', '27', '8', '5', '27', '1', '30', '1', '27', '32', '32', '49', '5', '5', '4', '13', '32', '33', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '32', '5', '4', '5', '32', '4', '3', '4', '4', '4', '5', '35', '33', '4', '5', '5', '5', '4', '30', '32', '5', '4', '5', '19', '5', '5', '4', '5', '5', '5', '5', '5', '4', '4', '5', '5', '5', '32', '32', '39', '4', '4', '4', '34', '5', '33', '34', '49', '4', '5', '4', '5', '3', '77', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '5', '6', '5', '5', '4', '4', '5', '4', '5', '4', '4', '32', '5', '51', '4', '32', '4', '33', '4', '4', '5', '12', '32', '4', '4', '32', '5', '5', '4', '5', '4', '3', '4', '5', '4', '5', '6', '4', '5', '32', '4', '4', '4', '5', '4', '5', '5', '5', '2', '5', '6', '4', '49', '5', '4', '32', '5', '32', '5', '5', '5', '39', '49', '33', '33', '4', '4', '5', '5', '5', '4', '5', '5', '4', '33', '32', '32', '32', '32', '33', '5', '32', '32', '32', '33', '44', '20', '14', '33', '6', '32', '12', '49', '32', '32', '49', '33', '34', '5', '32', '32', '32', '32', '4', '32', '32', '5', '6', '42', '33', '35', '32', '31', '31', '5', '32', '49', '32', '4', '27', '11', '32', '4', '69', '32', '6', '32', '34', '5', '32', '49', '32', '21', '32', '32', '5', '30', '33', '32', '16', '32', '33', '34', '32', '48', '49', '31', '32', '6', '32', '34', '34', '5', '33', '49', '39', '32', '33', '33', '4', '32', '11', '32', '6', '6', '33', '32', '33', '33', '31', '32', '32', '5', '32', '4', '32', '4', '32', '32', '33', '32', '32', '5', '34', '32', '33', '32', '49', '32', '27', '31', '4', '12', '33', '34', '49', '5', '31', '32', '6', '30', '5', '32', '27', '34', '32', '22', '32', '4', '32', '33', '32', '32', '4', '6', '33', '33', '72', '32', '32', '5', '30', '32', '5', '32', '32', '60', '32', '33', '15', '34', '32', '33', '33', '32', '32', '12', '33', '33', '33', '32', '32', '5', '32', '33', '7', '32', '46', '5', '33', '32', '41', '34', '32', '32', '32', '5', '32', '32', '33', '33', '33', '32', '32', '7', '33', '32', '32', '32', '12', '32', '5', '32', '49', '9', '30', '32', '33', '33', '33', '27', '5', '5', '31', '32', '6', '30', '79', '35', '49', '34', '32', '33', '33', '32', '32', '32', '49', '32', '70', '26', '32', '32', '6', '32', '31', '5', '28', '32', '5', '5', '10', '4', '49', '33', '5', '32', '32', '6', '5', '4', '4', '4', '5', '5', '32', '5', '4', '5', '5', '75', '4', '4', '4', '4', '34', '4', '5', '5', '49', '42', '4', '5', '32', '2', '4', '5', '33', '4', '5', '5', '5', '5', '5', '4', '11', '32', '49', '4', '30', '5', '27', '4', '31', '29', '2', '4', '5', '33', '5', '4', '5', '32', '4', '4', '5', '32', '5', '4', '32', '14', '37', '5', '4', '33', '4', '5', '5', '31', '4', '4', '5', '32', '33', '33', '5', '5', '5', '5', '4', '4', '4', '4', '5', '5', '30', '4', '0', '4', '16', '4', '5', '4', '4', '5', '5', '5', '5', '4', '5', '4', '30', '5', '5', '5', '15', '5', '4', '5', '5', '5', '5', '7', '4', '4', '4', '32', '32', '5', '32', '4', '4', '5', '4', '4', '4', '4', '4', '4', '4', '4', '30', '4', '5', '4', '4', '5', '34', '4', '5', '64', '4', '4', '4', '4', '4', '4', '4', '5', '4', '4', '5', '5', '5', '4', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '31', '4', '4', '5', '4', '5', '35', '4', '4', '4', '5', '4', '4', '5', '4', '5', '4', '5', '4', '5', '4', '4', '4', '4', '32', '4', '4', '31', '13', '4', '11', '4', '32', '5', '4', '33', '5', '32', '4', '30', '4', '5', '32', '33', '5', '5', '5', '4', '5', '3', '4', '4', '5', '32', '4', '4', '5', '31', '32', '5', '49', '12', '5', '4', '5', '4', '33', '2', '5', '5', '30', '80', '4', '33', '33', '3', '5', '34', '31', '34', '7', '59', '32', '33', '5', '32', '95', '5', '32', '32', '5', '5', '32', '30', '5', '32', '5', '4', '4', '32', '5', '4', '4', '5', '5', '33', '11', '4', '32', '4', '4', '33', '4', '63', '4', '4', '4', '34', '4', '18', '33', '32', '33', '32', '4', '32', '47', '5', '4', '32', '5', '5', '49', '35', '32', '33', '32', '5', '7', '32', '4', '32', '21', '12', '5', '32', '32', '4', '4', '4', '5', '5', '4', '32', '5', '4', '5', '32', '5', '4', '34', '4', '5', '4', '5', '5', '4', '5', '4', '4', '30', '32', '5', '33', '33', '32', '31', '33', '32', '32', '4', '6', '34', '1', '15', '30', '32', '5', '4', '32', '4', '5', '32', '2', '49', '8', '32', '11', '6', '5', '31', '33', '12', '34', '33', '31', '4', '33', '34', '34', '32', '32', '32', '32', '8', '32', '33', '4', '74', '4', '33', '32', '28', '4', '5', '33', '14', '32', '33', '31', '5', '32', '5', '33', '33', '32', '33', '32', '5', '32', '33', '23', '27', '31', '31', '34', '31', '5', '41', '32', '32', '33', '32', '11', '32', '7', '11', '32', '33', '32', '33', '34', '32', '32', '4', '32', '31', '32', '32', '32', '32', '33', '46', '32', '66', '32', '33', '30', '5', '32', '32', '32', '4', '32', '32', '32', '32', '33', '32', '49', '32', '32', '32', '33', '33', '32', '5', '33', '32', '12', '32', '33', '16', '32', '33', '5', '32', '32', '9', '34', '64', '4', '32', '32', '33', '32', '31', '32', '32', '10', '32', '6', '33', '13', '32', '5', '5', '4', '31', '3', '32', '25', '40', '34', '32', '32', '34', '5', '32', '44', '33', '8', '32', '33', '32', '33', '5', '33', '32', '32', '32', '18', '30', '32', '33', '32', '49', '32', '32', '32', '6', '17', '33', '33', '5', '49', '32', '19', '4', '5', '5', '4', '5', '7', '4', '11', '33', '32', '32', '4', '3', '32', '27', '4', '4', '33', '5', '4', '34', '31', '5', '30', '1', '4', '5', '32', '5', '4', '5', '4', '61', '9', '4', '11', '5', '32', '33', '33', '34', '4', '33', '34', '4', '32', '32', '5', '32', '4', '31', '32', '33', '5', '4', '33', '5', '4', '27', '5', '5', '4', '35', '5', '5', '4', '5', '4', '4', '4', '33', '5', '32', '5', '5', '5', '27', '4', '4', '4', '4', '4', '5', '5', '5', '5', '6', '5', '5', '5', '5', '4', '5', '5', '5', '4', '5', '4', '66', '4', '4', '4', '4', '5', '4', '4', '4', '32', '7', '33', '5', '7', '4', '5', '55', '32', '43', '21', '5', '4', '5', '3', '4', '5', '4', '4', '32', '32', '33', '34', '5', '69', '4', '32', '4', '32', '25', '30', '32', '30', '32', '63', '35', '33', '5', '32', '5', '32', '4', '5', '4', '5', '4', '5', '4', '4', '33', '33', '33', '4', '30', '5', '33', '32', '4', '32', '33', '27', '5', '4', '32', '5', '4', '32', '5', '5', '5', '33', '4', '5', '4', '4', '4', '5', '5', '7', '33', '5', '32', '5', '5', '49', '5', '4', '4', '5', '4', '4', '5', '4', '4', '5', '32', '4', '4', '4', '4', '4', '5', '32', '4', '5', '4', '4', '4', '5', '4', '5', '4', '4', '61', '4', '5', '4', '38', '33', '4', '5', '34', '13', '4', '4', '32', '32', '32', '4', '5', '5', '32', '5', '32', '4', '33', '33', '33', '5', '5', '33', '5', '5', '4', '12', '4', '28', '5', '5', '5', '5', '5', '4', '5', '5', '4', '32', '6', '4', '4', '5', '9', '13', '32', '34', '4', '33', '15', '32', '32', '4', '32', '5', '5', '27', '4', '5', '4', '4', '5', '4', '4', '4', '5', '4', '21', '5', '5', '33', '5', '4', '34', '5', '4', '4', '4', '5', '4', '4', '5', '5', '4', '5', '5', '13', '4', '5', '4', '5', '4', '4', '31', '5', '4', '5', '4', '4', '5', '30', '4', '4', '5', '4', '5', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '5', '5', '5', '46', '4', '4', '4', '4', '5', '4', '5', '22', '5', '5', '4', '49', '5', '5', '32', '5', '4', '5', '5', '5', '4', '4', '32', '4', '30', '32', '4', '4', '4', '4', '5', '5', '12', '5', '4', '5', '4', '33', '4', '4', '4', '32', '4', '4', '4', '4', '5', '4', '4', '32', '4', '35', '5', '4', '4', '5', '4', '5', '32', '0', '67', '4', '31', '4', '5', '30', '4', '17', '3', '5', '4', '4', '4', '5', '22', '5', '4', '4', '4', '4', '5', '5', '5', '5', '4', '5', '5', '2', '4', '4', '5', '32', '5', '5', '5', '4', '4', '4', '50', '4', '5', '4', '4', '5', '5', '5', '32', '5', '30', '32', '4', '5', '32', '4', '4', '4', '4', '4', '5', '5', '4', '5', '68', '5', '29', '4', '5', '5', '4', '5', '5', '6', '6', '6', '6', '6', '6', '5', '6', '6', '32', '35', '6', '33', '6', '24', '5', '34', '33', '32', '30', '31', '32', '33', '13', '32', '32', '93', '8', '33', '32', '32', '5', '33', '31', '32', '32', '33', '13', '32', '9', '32', '30', '3', '4', '9', '33', '3', '32', '33', '19', '32', '32', '33', '32', '33', '30', '30', '32', '5', '33', '32', '81', '7', '7', '32', '79', '33', '15', '32', '32', '32', '32', '5', '30', '32', '7', '32', '33', '5', '32', '33', '33', '35', '33', '32', '33', '33', '33', '31', '33', '32', '34', '32', '32', '32', '34', '33', '7', '33', '13', '32', '32', '32', '49', '32', '33', '33', '32', '32', '4', '32', '32', '33', '33', '4', '32', '33', '33', '12', '49', '33', '32', '80', '32', '33', '32', '25', '32', '34', '33', '4', '32', '32', '33', '32', '33', '33', '32', '33', '32', '4', '21', '32', '5', '32', '49', '71', '33', '33', '16', '13', '4', '32', '32', '5', '27', '18', '34', '33', '32', '65', '32', '32', '22', '27', '49', '34', '33', '33', '5', '4', '5', '5', '44', '32', '30', '12', '32', '32', '11', '33', '33', '33', '33', '32', '4', '11', '32', '32', '11', '8', '32', '4', '5', '5', '5', '33', '4', '4', '4', '70', '12', '27', '32', '32', '5', '17', '33', '32', '32', '8', '34', '32', '59', '32', '32', '33', '31', '31', '32', '49', '5', '15', '13', '33', '34', '32', '4', '33', '32', '4', '8', '32', '33', '22', '34', '49', '11', '33', '32', '32', '5', '28', '32', '31', '32', '32', '12', '32', '32', '32', '28', '49', '30', '33', '33', '32', '3', '18', '30', '33', '4', '32', '4', '31', '1', '12', '28', '5', '49', '33', '23', '32', '32', '33', '33', '33', '8', '33', '4', '29', '4', '32', '13', '32', '33', '33', '34', '32', '31', '33', '32', '4', '5', '32', '32', '5', '33', '15', '11', '33', '9', '50', '59', '13', '32', '32', '34', '33', '34', '33', '33', '33', '32', '20', '20', '33', '33', '34', '33', '32', '31', '12', '32', '33', '33', '5', '32', '32', '31', '33', '5', '32', '33', '7', '33', '32', '26', '13', '34', '12', '4', '5', '12', '49', '32', '33', '33', '32', '32', '32', '33', '33', '32', '17', '13', '32', '33', '10', '32', '32', '30', '32', '32', '32', '8', '5', '32', '32', '32', '32', '32', '12', '30', '12', '34', '33', '32', '45', '32', '34', '28', '32', '4', '4', '17', '32', '33', '49', '33', '26', '33', '49', '33', '31', '32', '32', '14', '5', '32', '32', '32', '32', '27', '32', '5', '33', '32', '32', '32', '32', '32', '32', '13', '15', '32', '30', '32', '32', '32', '32', '26', '32', '18', '33', '32', '32', '32', '49', '32', '33', '31', '32', '4', '5', '34', '32', '33', '33', '34', '32', '32', '6', '33', '5', '31', '32', '33', '32', '31', '29', '12', '32', '32', '5', '33', '30', '33', '32', '32', '31', '32', '39', '7', '61', '25', '34', '33', '32', '32', '7', '32', '31', '31', '33', '10', '34', '32', '31', '22', '32', '20', '9', '32', '32', '33', '30', '12', '33', '33', '33', '27', '5', '32', '5', '27', '24', '12', '32', '32', '62', '32', '22', '32', '5', '32', '33', '24', '49', '32', '32', '32', '4', '6', '33', '4', '33', '32', '32', '32', '32', '1', '11', '32', '26', '24', '5', '5', '32', '7', '5', '31', '33', '5', '54', '32', '33', '32', '32', '32', '32', '30', '32', '32', '12', '31', '32', '33', '33', '32', '33', '49', '33', '22', '32', '12', '32', '27', '55', '32', '34', '60', '32', '4', '5', '4', '4', '4', '4', '4', '4', '4', '5', '6', '4', '4', '34', '33', '4', '4', '33', '5', '35', '33', '33', '4', '5', '5', '33', '32', '32', '32', '5', '4', '4', '5', '5', '5', '32', '32', '4', '49', '5', '15', '33', '32', '32', '32', '34', '32', '60', '32', '32', '32', '27', '33', '30', '15', '5', '5', '72', '4', '4', '33', '33', '11', '32', '32', '32', '44', '63', '6', '7', '32', '32', '32', '5', '4', '19', '32', '14', '1', '33', '32', '71', '4', '48', '4', '31', '34', '5', '35', '5', '32', '32', '33', '32', '32', '26', '13', '32', '28', '32', '6', '21', '31', '64', '11', '33', '32', '32', '34', '5', '32', '26', '32', '5', '14', '32', '5', '5', '32', '4', '39', '13', '4', '35', '0', '32', '33', '33', '32', '32', '32', '49', '15', '33', '32', '32', '27', '32', '32', '5', '46', '11', '24', '33', '11', '4', '32', '12', '5', '5', '5', '32', '33', '32', '1', '32', '7', '13', '32', '32', '32', '13', '5', '30', '5', '4', '32', '30', '33', '33', '4', '7', '5', '33', '33', '33', '32', '14', '29', '6', '13', '32', '10', '33', '33', '5', '30', '12', '21', '33', '32', '33', '31', '30', '32', '18', '34', '32', '32', '34', '30', '12', '32', '32', '30', '32', '33', '34', '30', '32', '5', '33', '32', '12', '33', '33', '32', '32', '32', '11', '32', '32', '33', '32', '33', '32', '30', '32', '5', '32', '32', '25', '32', '33', '31', '32', '14', '33', '57', '30', '32', '49', '27', '5', '32', '12', '33', '33', '32', '32', '33', '21', '33', '33', '32', '10', '33', '33', '33', '32', '4', '4', '32', '32', '31', '33', '33', '33', '32', '24', '5', '35', '32', '32', '5', '3', '34', '32', '32', '5', '32', '33', '57', '33', '4', '34', '52', '33', '32', '33', '32', '33', '33', '1', '33', '33', '33', '22', '27', '33', '32', '32', '34', '33', '7', '12', '1', '4', '33', '32', '33', '33', '32', '32', '31', '32', '32', '29', '33', '31', '49', '5', '11', '34', '32', '32', '25', '35', '32', '25', '32', '33', '33', '5', '32', '27', '32', '31', '30', '30', '34', '32', '31', '5', '13', '30', '32', '4', '33', '32', '32', '32', '34', '4', '33', '30', '31', '32', '32', '33', '34', '49', '32', '5', '31', '33', '32', '32', '49', '8', '33', '32', '5', '32', '32', '33', '5', '32', '4', '36', '5', '32', '4', '32', '32', '18', '33', '33', '34', '34', '32', '8', '41', '32', '33', '49', '32', '32', '32', '5', '30', '49', '27', '32', '55', '49', '49', '26', '5', '33', '33', '33', '32', '32', '34', '32', '32', '12', '32', '11', '31', '33', '34', '32', '21', '28', '57', '32', '30', '4', '32', '4', '32', '17', '31', '33', '32', '32', '32', '32', '5', '30', '32', '32', '32', '32', '34', '32', '32', '32', '32', '32', '32', '33', '33', '13', '32', '34', '32', '32', '32', '32', '32', '5', '33', '32', '32', '33', '32', '5', '12', '33', '32', '5', '32', '32', '32', '5', '32', '5', '16', '34', '33', '33', '4', '30', '11', '34', '32', '35', '94', '10', '4', '14', '32', '28', '4', '32', '32', '17', '15', '4', '27', '4', '32', '32', '5', '34', '32', '32', '7', '33', '18', '31', '58', '20', '32', '11', '67', '36', '4', '27', '12', '32', '33', '26', '33', '5', '32', '32', '32', '32', '33', '77', '4', '33', '35', '32', '31', '31', '24', '32', '32', '33', '32', '24', '29', '33', '32', '32', '32', '24', '32', '5', '32', '16', '33', '33', '32', '32', '32', '11', '32', '5', '32', '32', '32', '32', '45', '32', '32', '31', '32', '32', '15', '32', '30', '31', '32', '5', '33', '5', '32', '32', '32', '32', '52', '26', '32', '32', '5', '33', '2', '34', '36', '33', '49', '33', '32', '5', '32', '6', '14', '32', '33', '32', '31', '31', '32', '33', '32', '33', '32', '32', '5', '32', '28', '32', '33', '32', '33', '8', '32', '5', '33', '12', '48', '32', '32', '32', '32', '32', '33', '4', '32', '13', '8', '32', '32', '33', '38', '33', '34', '33', '6', '33', '32', '32', '32', '13', '5', '4', '32', '16', '34', '7', '11', '12', '5', '11', '9', '33', '11', '33', '4', '34', '32', '32', '6', '49', '31', '32', '32', '5', '32', '4', '32', '32', '15', '6', '49', '32', '5', '32', '32', '32', '32', '6', '32', '32', '33', '32', '5', '11', '7', '5', '32', '31', '45', '33', '31', '32', '30', '6', '33', '33', '31', '34', '70', '1', '32', '31', '5', '32', '19', '5', '32', '32', '32', '32', '32', '31', '4', '32', '4', '32', '32', '11', '33', '32', '49', '33', '32', '33', '5', '32', '32', '33', '12', '49', '33', '32', '32', '11', '32', '32', '32', '33', '26', '33', '32', '32', '26', '0', '32', '31', '10', '32', '4', '31', '27', '5', '32', '33', '51', '12', '49', '6', '33', '33', '34', '32', '32', '32', '33', '32', '33', '5', '33', '32', '4', '49', '34', '32', '32', '5', '25', '31', '32', '33', '2', '5', '32', '14', '32', '32', '78', '32', '32', '32', '9', '20', '33', '33', '34', '32', '15', '33', '31', '32', '31', '32', '7', '11', '33', '32', '22', '49', '32', '32', '31', '33', '33', '32', '24', '32', '34', '33', '32', '34', '33', '14', '32', '33', '33', '19', '32', '32', '32', '14', '32', '8', '33', '33', '33', '32', '1', '33', '32', '32', '33', '27', '33', '11', '32', '33', '5', '32', '32', '12', '5', '11', '32', '33', '32', '32', '33', '32', '32', '45', '9', '32', '33', '32', '32', '32', '32', '32', '13', '32', '32', '5', '32', '32', '8', '7', '32', '33', '13', '49', '38', '6', '32', '33', '33', '19', '32', '32', '4', '4', '32', '32', '32', '33', '5', '33', '32', '12', '31', '32', '32', '33', '32', '38', '49', '33', '11', '32', '14', '6', '32', '33', '5', '5', '31', '32', '32', '32', '49', '32', '30', '70', '5', '33', '4', '16', '32', '32', '4', '32', '63', '6', '33', '49', '49', '5', '33', '32', '33', '33', '32', '5', '22', '5', '32', '11', '33', '32', '32', '11', '30', '33', '30', '34', '24', '21', '5', '32', '32', '32', '9', '13', '32', '48', '18', '5', '8', '7', '33', '32', '32', '32', '32', '19', '8', '32', '30', '33', '5', '32', '33', '32', '32', '32', '35', '11', '4', '32', '31', '32', '32', '32', '33', '33', '32', '10', '32', '32', '32', '1', '30', '7', '24', '33', '33', '32', '4', '33', '32', '5', '10', '27', '32', '33', '34', '32', '33', '33', '32', '32', '32', '32', '32', '32', '5', '33', '4', '32', '5', '32', '32', '7', '32', '33', '33', '32', '30', '16', '32', '5', '5', '5', '5', '5', '31', '33', '33', '4', '33', '32', '32', '5', '32', '33', '24', '31', '33', '8', '33', '32', '32', '32', '5', '32', '32', '5', '12', '41', '8', '33', '32', '32', '17', '5', '32', '32', '49', '32', '32', '4', '32', '9', '32', '33', '31', '33', '33', '31', '5', '32', '32', '4', '32', '32', '27', '32', '32', '32', '33', '32', '12', '49', '13', '32', '32', '30', '32', '5', '11', '32', '32', '3', '4', '33', '32', '58', '33', '30', '33', '49', '32', '33', '32', '16', '4', '33', '16', '33', '32', '5', '15', '33', '33', '32', '32', '35', '32', '33', '32', '34', '32', '32', '33', '10', '32', '31', '34', '33', '12', '32', '33', '27', '5', '4', '32', '32', '32', '31', '32', '33', '33', '31', '32', '33', '33', '32', '32', '6', '32', '49', '32', '6', '5', '4', '33', '15', '32', '32', '32', '5', '32', '33', '49', '32', '32', '32', '32', '33', '17', '32', '32', '4', '32', '31', '32', '37', '35', '1', '32', '12', '30', '33', '5', '32', '20', '5', '5', '32', '32', '49', '31', '32', '32', '6', '4', '32', '26', '31', '5', '5', '32', '32', '32', '33', '32', '32', '33', '30', '33', '32', '31', '32', '5', '32', '32', '32', '4', '49', '31', '32', '32', '33', '31', '32', '32', '11', '32', '49', '31', '4', '36', '5', '3', '9', '31', '12', '32', '32', '30', '4', '4', '4', '33', '49', '32', '32', '30', '4', '49', '31', '31', '33', '33', '32', '34', '32', '49', '32', '32', '5', '4', '8', '32', '32', '33', '12', '5', '32', '32', '32', '32', '32', '32', '8', '32', '32', '32', '32', '33', '2', '33', '32', '30', '33', '31', '32', '23', '30', '25', '5', '66', '36', '5', '32', '33', '31', '32', '32', '10', '33', '33', '14', '33', '33', '32', '13', '9', '18', '32', '34', '2', '32', '32', '4', '49', '5', '19', '4', '32', '33', '33', '35', '31', '22', '32', '32', '5', '30', '28', '32', '32', '32', '34', '32', '4', '6', '31', '32', '4', '32', '4', '33', '32', '33', '31', '6', '4', '32', '29', '13', '34', '32', '11', '34', '32', '8', '32', '33', '32', '49', '4', '32', '36', '33', '33', '7', '32', '32', '85', '32', '32', '33', '32', '9', '5', '4', '32', '12', '32', '32', '4', '30', '16', '32', '32', '1', '32', '33', '5', '32', '49', '33', '72', '31', '11', '5', '33', '49', '4', '31', '6', '33', '17', '33', '32', '5', '32', '32', '32', '14', '5', '26', '5', '17', '31', '4', '33', '30', '4', '32', '27', '23', '12', '32', '32', '32', '32', '32', '25', '32', '30', '32', '31', '33', '32', '32', '4', '5', '4', '33', '32', '33', '32', '32', '32', '32', '49', '31', '25', '32', '6', '33', '32', '5', '65', '8', '7', '32', '32', '32', '49', '32', '32', '6', '32', '15', '32', '11', '32', '32', '31', '32', '34', '6', '33', '32', '33', '32', '31', '15', '33', '32', '33', '32', '34', '25', '32', '32', '32', '33', '32', '50', '33', '32', '32', '49', '32', '6', '32', '5', '32', '32', '49', '32', '32', '5', '32', '4', '49', '32', '32', '33', '9', '32', '16', '33', '32', '33', '31', '4', '8', '5', '35', '5', '49', '6', '49', '32', '32', '32', '34', '32', '1', '9', '49', '32', '33', '4', '30', '49', '30', '4', '33', '32', '5', '30', '33', '11', '32', '32', '49', '4', '5', '33', '31', '5', '5', '25', '58', '32', '32', '13', '5', '31', '30', '32', '40', '12', '32', '12', '34', '33', '5', '35', '22', '25', '33', '28', '30', '5', '32', '27', '33', '33', '32', '5', '33', '5', '33', '30', '32', '9', '5', '30', '33', '48', '32', '12', '32', '32', '25', '32', '4', '32', '32', '16', '4', '5', '32', '45', '32', '5', '33', '32', '54', '14', '7', '5', '32', '4', '47', '33', '49', '5', '30', '7', '30', '5', '6', '30', '32', '5', '7', '5', '33', '32', '33', '5', '49', '30', '30', '35', '4', '8', '33', '32', '30', '8', '32', '5', '5', '32', '15', '30', '5', '32', '5', '72', '13', '10', '31', '4', '28', '20', '71', '32', '5', '19', '33', '32', '32', '7', '10', '94', '32', '32', '33', '28', '8', '34', '15', '4', '32', '1', '32', '15', '8', '32', '8', '5', '33', '34', '6', '32', '32', '12', '11', '79', '32', '32', '32', '33', '33', '18', '5', '49', '5', '33', '32', '6', '32', '13', '4', '33', '32', '4', '33', '4', '5', '73', '33', '31', '12', '13', '33', '32', '32', '33', '23', '33', '33', '33', '32', '32', '32', '33', '57', '4', '35', '6', '31', '33', '5', '30', '30', '32', '33', '6', '32', '32', '5', '8', '82', '33', '32', '34', '11', '5', '15', '33', '32', '6', '32', '5', '33', '32', '32', '32', '33', '33', '11', '28', '28', '32', '5', '35', '33', '32', '33', '32', '33', '32', '5', '32', '32', '33', '19', '32', '49', '33', '33', '32', '3', '32', '32', '34', '32', '5', '32', '32', '33', '13', '29', '35', '32', '32', '5', '29', '33', '5', '33', '32', '33', '33', '7', '32', '33', '32', '7', '32', '14', '5', '32', '32', '32', '5', '5', '5', '4', '5', '5', '5', '14', '8', '32', '33', '32', '30', '32', '33', '24', '11', '32', '4', '32', '32', '27', '32', '32', '51', '31', '33', '49', '6', '33', '12', '33', '5', '33', '8', '5', '33', '32', '30', '9', '31', '33', '32', '14', '5', '32', '32', '32', '32', '32', '49', '32', '32', '32', '21', '33', '33', '32', '32', '32', '33', '32', '33', '32', '19', '23', '33', '33', '32', '32', '32', '33', '33', '30', '32', '33', '5', '32', '4', '32', '32', '7', '33', '5', '5', '5', '30', '5', '32', '30', '12', '7', '53', '6', '32', '6', '5', '5', '48', '33', '34', '4', '33', '32', '32', '33', '8', '32', '32', '33', '32', '32', '32', '12', '32', '5', '33', '32', '33', '15', '32', '16', '32', '33', '32', '32', '32', '32', '27', '33', '32', '32', '34', '33', '32', '34', '7', '32', '33', '32', '32', '33', '48', '12', '33', '32', '33', '33', '32', '33', '4', '5', '32', '33', '32', '32', '61', '13', '32', '32', '35', '32', '35', '32', '32', '33', '85', '32', '5', '30', '32', '33', '32', '5', '33', '4', '4', '32', '5', '4', '32', '25', '34', '32', '11', '32', '33', '32', '5', '4', '32', '32', '33', '47', '33', '12', '12', '32', '32', '33', '7', '32', '32', '32', '30', '32', '32', '32', '32', '4', '32', '33', '5', '31', '8', '11', '76', '32', '6', '32', '11', '49', '5', '25', '49', '32', '11', '4', '32', '32', '32', '33', '32', '32', '71', '32', '4', '32', '32', '33', '32', '12', '32', '29', '13', '12', '5', '31', '32', '32', '34', '33', '31', '8', '33', '32', '32', '33', '33', '32', '32', '9', '12', '32', '33', '32', '46', '32', '32', '34', '32', '33', '11', '5', '32', '32', '33', '30', '32', '21', '32', '33', '33', '33', '32', '33', '14', '33', '32', '32', '33', '33', '7', '33', '32', '45', '42', '32', '51', '1', '33', '8', '32', '33', '33', '5', '33', '32', '32', '10', '33', '32', '32', '32', '32', '32', '33', '31', '5', '6', '5', '10', '32', '30', '33', '5', '32', '27', '38', '12', '5', '32', '33', '32', '32', '12', '32', '67', '34', '33', '32', '32', '32', '33', '8', '33', '33', '60', '7', '33', '32', '8', '5', '61', '32', '32', '5', '7', '32', '19', '32', '6', '32', '33', '4', '49', '34', '33', '32', '32', '31', '49', '30', '10', '11', '33', '33', '33', '32', '30', '32', '32', '11', '33', '33', '32', '49', '15', '32', '64', '12', '33', '5', '6', '5', '30', '33', '32', '33', '11', '32', '26', '34', '31', '33', '33', '49', '13', '</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>['Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atend</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>['85974001107', '85981010387', '85981010504', '85981010801', '85981011300', '85981011982', '85981012709', '85981012859', '85981012916', '85981013105', '85981013139', '85981013252', '85981014486', '85981015083', '85981015199', '85981015345', '85981015408', '85981015858', '85981018191', '85981019737', '85981019859', '85981020615', '85981021220', '85981021847', '85981021858', '85981023473', '85981024243', '85981024932', '85981025159', '85981026077', '85981026188', '85981026342', '85981029941', '85981034608', '85981035347', '85981037998', '85981038369', '85981040609', '85981041303', '85981042289', '85981046232', '85981047325', '85981047447', '85981050094', '85981050305', '85981050670', '85981050778', '85981050921', '85981051007', '85981051157', '85981051236', '85981051357', '85981051407', '85981051960', '85981052023', '85981052147', '85981052388', '85981053361', '85981053645', '85981053870', '85981054245', '85981054310', '85981054721', '85981054784', '85981055402', '85981055606', '85981055887', '85981056204', '85981056432', '85981057133', '85981057473', '85981057594', '85981057657', '85981058510', '85981058575', '85981059167', '85981060358', '85981060840', '85981060881', '85981060903', '85981060912', '85981061514', '85981062036', '85981062783', '85981062811', '85981063144', '85981063180', '85981063445', '85981063577', '85981063706', '85981063708', '85981063769', '85981064311', '85981064501', '85981064633', '85981066228', '85981066596', '85981066800', '85981067063', '85981067120', '85981067303', '85981067738', '85981068259', '85981068383', '85981068838', '85981069073', '85981069268', '85981069285', '85981069288', '85981069331', '85981069531', '85981069805', '85981070139', '85981070716', '85981070933', '85981072516', '85981074292', '85981074824', '85981077799', '85981079793', '85981080110', '85981081102', '85981081645', '85981081717', '85981081963', '85981082567', '85981082798', '85981083944', '85981083955', '85981084430', '85981085176', '85981085425', '85981086055', '85981087566', '85981090951', '85981092003', '85981094270', '85981095658', '85981096027', '85981097092', '85981097525', '85981099771', '85981099834', '85981104139', '85981105541', '85981111379', '85981111687', '85981112198', '85981112368', '85981113354', '85981116111', '85981116475', '85981117229', '85981117240', '85981117970', '85981118916', '85981119356', '85981121743', '85981121756', '85981121918', '85981122659', '85981122830', '85981124417', '85981125198', '85981125364', '85981127000', '85981127863', '85981128332', '85981128640', '85981129033', '85981130954', '85981131390', '85981132338', '85981132657', '85981132861', '85981133001', '85981136515', '85981137269', '85981137935', '85981138484', '85981139818', '85981141110', '85981141235', '85981142047', '85981142397', '85981144074', '85981144194', '85981144290', '85981144476', '85981145210', '85981145431', '85981146150', '85981147761', '85981148652', '85981149605', '85981149798', '85981149833', '85981150270', '85981152513', '85981152668', '85981152923', '85981153276', '85981154070', '85981154704', '85981154767', '85981155516', '85981155609', '85981155832', '85981157497', '85981159783', '85981160701', '85981162279', '85981163532', '85981168773', '85981169336', '85981170375', '85981170419', '85981172174', '85981172237', '85981173080', '85981173491', '85981173596', '85981174595', '85981175102', '85981175961', '85981176245', '85981176511', '85981176843', '85981176855', '85981177377', '85981177436', '85981178111', '85981180220', '85981180748', '85981181223', '85981181460', '85981184568', '85981185113', '85981185397', '85981185432', '85981186162', '85981187777', '85981187790', '85981188522', '85981190449', '85981190603', '85981190941', '85981191324', '85981191501', '85981192668', '85981193462', '85981194504', '85981195274', '85981195777', '85981196765', '85981199009', '85981200624', '85981204580', '85981205000', '85981207224', '85981210397', '85981211722', '85981211785', '85981212297', '85981212335', '85981215121', '85981215323', '85981217007', '85981217070', '85981217271', '85981217334', '85981217865', '85981217880', '85981217928', '85981219726', '85981220015', '85981220097', '85981220132', '85981221107', '85981221148', '85981222412', '85981224119', '85981224486', '85981224995', '85981225097', '85981225167', '85981226403', '85981227172', '85981227283', '85981227812', '85981228111', '85981228405', '85981228468', '85981229862', '85981229918', '85981229981', '85981230013', '85981230104', '85981233010', '85981233031', '85981233110', '85981234275', '85981235443', '85981237281', '85981238571', '85981240151', '85981240906', '85981241794', '85981243937', '85981245200', '85981245595', '85981245660', '85981246453', '85981246810', '85981247191', '85981247682', '85981247801', '85981248056', '85981248614', '85981248938', '85981249006', '85981249077', '85981249520', '85981249804', '85981250065', '85981251340', '85981252190', '85981252202', '85981252814', '85981253454', '85981256347', '85981256415', '85981256918', '85981257594', '85981257644', '85981258954', '85981259116', '85981259996', '85981260093', '85981260293', '85981261976', '85981264023', '85981265628', '85981266155', '85981266554', '85981267575', '85981268163', '85981269254', '85981270887', '85981273817', '85981276088', '85981277050', '85981277171', '85981277778', '85981277862', '85981278172', '85981278481', '85981281110', '85981281122', '85981283976', '85981284254', '85981284771', '85981284904', '85981285694', '85981285757', '85981286755', '85981287954', '85981288208', '85981288338', '85981289201', '85981290315', '85981291170', '85981291852', '85981292335', '85981292898', '85981293237', '85981296943', '85981297006', '85981297774', '85981298411', '85981298474', '85981299369', '85981300207', '85981300265', '85981301018', '85981301029', '85981301090', '85981301430', '85981302820', '85981303653', '85981304383', '85981304684', '85981304736', '85981304842', '85981305581', '85981306366', '85981307620', '85981307802', '85981308045', '85981308259', '85981308292', '85981308328', '85981308337', '85981308391', '85981310114', '85981310742', '85981311091', '85981311398', '85981312075', '85981313089', '85981313134', '85981313616', '85981313627', '85981314051', '85981314422', '85981315654', '85981316754', '85981318080', '85981323921', '85981325550', '85981327070', '85981327436', '85981327760', '85981328852', '85981330136', '85981330758', '85981331850', '85981331913', '85981332190', '85981333065', '85981333339', '85981334650', '85981334713', '85981334761', '85981335534', '85981337373', '85981338263', '85981338307', '85981342092', '85981342565', '85981343138', '85981343533', '85981344833', '85981345060', '85981347012', '85981347371', '85981348351', '85981348558', '85981349404', '85981351875', '85981352588', '85981352826', '85981353374', '85981353997', '85981354648', '85981355846', '85981357814', '85981359310', '85981360852', '85981361507', '85981361779', '85981362003', '85981362066', '85981363777', '85981365886', '85981366880', '85981367170', '85981368633', '85981370043', '85981370894', '85981371153', '85981371868', '85981372645', '85981374219', '85981375527', '85981375801', '85981375825', '85981376079', '85981377391', '85981378159', '85981378792', '85981378905', '85981379505', '85981379662', '85981380597', '85981380924', '85981381707', '85981381999', '85981383237', '85981383353', '85981384426', '85981385151', '85981385624', '85981385673', '85981385841', '85981386704', '85981386821', '85981387227', '85981387362', '85981388619', '85981391330', '85981391423', '85981391880', '85981392100', '85981392565', '85981395635', '85981395687', '85981395818', '85981397246', '85981397372', '85981397409', '85981397411', '85981398764', '85981400369', '85981401399', '85981401626', '85981401752', '85981402041', '85981402081', '85981402748', '85981402997', '85981403093', '85981403964', '85981404116', '85981404174', '85981404374', '85981404793', '85981405917', '85981408267', '85981409242', '85981409843', '85981411024', '85981411624', '85981411687', '85981413039', '85981413532', '85981413653', '85981413838', '85981413892', '85981414546', '85981415469', '85981416386', '85981416409', '85981418850', '85981419344', '85981420019', '85981421525', '85981421738', '85981422245', '85981422308', '85981422576', '85981422856', '85981423490', '85981423505', '85981423933', '85981424271', '85981424607', '85981425703', '85981426537', '85981426942', '85981427253', '85981428860', '85981428912', '85981432332', '85981433880', '85981436330', '85981437233', '85981437797', '85981440921', '85981442203', '85981443375', '85981444452', '85981444515', '85981445843', '85981447674', '85981448037', '85981452309', '85981453385', '85981460147', '85981460175', '85981460392', '85981460457', '85981460646', '85981460699', '85981460861', '85981460924', '85981460996', '85981461065', '85981461106', '85981461610', '85981462406', '85981463746', '85981463860', '85981464262', '85981464411', '85981464530', '85981464545', '85981465735', '85981465772', '85981465798', '85981466545', '85981467570', '85981468790', '85981470659', '85981470831', '85981471492', '85981471759', '85981472233', '85981473750', '85981474263', '85981474389', '85981474696', '85981474697', '85981474756', '85981474760', '85981474778', '85981474912', '85981474923', '85981475220', '85981475230', '85981475761', '85981475972', '85981475980', '85981476043', '85981476212', '85981476638', '85981477326', '85981477413', '85981477799', '85981477812', '85981477813', '85981477916', '85981478494', '85981478784', '85981479493', '85981479515', '85981479752', '85981479774', '85981481053', '85981481331', '85981481726', '85981482109', '85981482140', '85981482476', '85981482990', '85981483810', '85981484967', '85981485284', '85981485480', '85981486380', '85981486397', '85981487878', '85981488161', '85981488741', '85981489506', '85981489546', '85981489609', '85981489986', '85981491380', '85981491428', '85981491439', '85981492666', '85981492729', '85981495205', '85981495268', '85981495465', '85981495615', '85981495911', '85981495935', '85981496025', '85981496943', '85981497099', '85981497122', '85981497496', '85981497614', '85981499186', '85981500414', '85981500847', '85981500940', '85981501090', '85981501968', '85981502098', '85981502241', '85981505500', '85981505522', '85981505531', '85981505586', '85981505887', '85981506224', '85981506332', '85981506467', '85981506955', '85981507053', '85981507770', '85981507930', '85981509140', '85981509349', '85981509981', '85981510677', '85981511295', '85981512929', '85981514081', '85981514747', '85981518467', '85981518484', '85981520304', '85981521334', '85981521816', '85981521879', '85981521962', '85981522121', '85981522321', '85981522480', '85981522523', '85981522914', '85981522917', '85981522933', '85981522980', '85981523042', '85981523247', '85981523548', '85981523703', '85981523830', '85981523864', '85981524209', '85981524336', '85981524345', '85981524388', '85981524433', '85981524474', '85981525329', '85981525392', '85981525946', '85981525956', '85981525970', '85981526066', '85981526142', '85981526377', '85981526414', '85981526660', '85981526890', '85981526953', '85981527026', '85981527241', '85981527738', '85981527876', '85981527926', '85981528100', '85981528344', '85981528523', '85981529250', '85981530016', '85981530202', '85981530228', '85981530264', '85981530358', '85981530695', '85981531466', '85981532323', '85981532367', '85981532706', '85981533140', '85981533536', '85981533817', '85981533861', '85981533924', '85981534836', '85981535019', '85981535381', '85981535444', '85981535702', '85981536001', '85981536037', '85981536784', '85981537054', '85981537071', '85981537451', '85981537531', '85981537646', '85981538008', '85981538403', '85981538473', '85981539100', '85981539364', '85981539374', '85981539613', '85981539674', '85981539710', '85981539904', '85981542565', '85981544220', '85981544377', '85981544415', '85981544420', '85981544535', '85981544744', '85981545730', '85981545967', '85981546135', '85981546201', '85981546486', '85981546524', '85981547100', '85981547151', '85981547181', '85981548573', '85981548663', '85981549807', '85981550607', '85981551701', '85981552786', '85981552815', '85981553207', '85981553257', '85981553774', '85981554041', '85981554682', '85981555448', '85981556360', '85981556386', '85981556391', '85981556708', '85981557599', '85981557763', '85981557766', '85981557996', '85981558443', '85981558444', '85981558593', '85981558734', '85981558921', '85981559352', '85981559880', '85981559990', '85981561122', '85981561397', '85981563114', '85981563918', '85981565385', '85981566296', '85981569388', '85981570332', '85981570553', '85981571936', '85981571948', '85981573149', '85981574029', '85981574749', '85981574828', '85981575288', '85981576121', '85981577685', '85981579715', '85981580747', '85981582223', '85981587265', '85981588881', '85981589028', '85981590283', '85981590581', '85981591212', '85981591394', '85981592814', '85981594445', '85981594455', '85981598314', '85981599091', '85981599720', '85981600032', '85981600288', '85981600746', '85981601467', '85981601515', '85981601621', '85981603545', '85981603701', '85981603764', '85981603922', '85981604044', '85981604097', '85981604901', '85981605888', '85981606241', '85981606453', '85981606516', '85981606875', '85981607061', '85981607171', '85981607847', '85981608039', '85981608131', '85981608656', '85981608885', '85981609224', '85981609765', '85981611504', '85981611687', '85981612354', '85981612497', '85981613707', '85981614805', '85981615721', '85981615726', '85981616672', '85981617048', '85981617443', '85981617809', '85981618157', '85981618463', '85981618696', '85981619089', '85981621012', '85981625207', '85981625719', '85981625789', '85981625797', '85981626292', '85981626455', '85981627178', '85981627515', '85981627750', '85981628353', '85981628962', '85981629450', '85981630101', '85981630164', '85981631945', '85981632116', '85981635515', '85981635650', '85981636098', '85981636649', '85981638200', '85981638739', '85981639201', '85981642110', '85981642480', '85981645543', '85981646909', '85981647853', '85981649485', '85981651235', '85981651813', '85981651856', '85981653359', '85981654096', '85981655420', '85981655504', '85981656015', '85981656761', '85981663973', '85981664051', '85981665088', '85981665658', '85981665867', '85981666220', '85981666585', '85981666685', '85981668986', '85981669316', '85981669696', '85981669892', '85981670050', '85981670209', '85981670557', '85981671233', '85981672007', '85981672198', '85981672687', '85981676600', '85981677013', '85981677923', '85981677986', '85981679022', '85981679393', '85981684827', '85981685253', '85981687262', '85981688088', '85981688530', '85981689614', '85981690885', '85981692225', '85981693076', '85981694698', '85981696440', '85981700371', '85981701616', '85981701789', '85981702211', '85981704587', '85981705823', '85981706117', '85981706812', '85981707565', '85981709424', '85981709639', '85981709959', '85981709997', '85981711415', '85981712700', '85981715589', '85981717124', '85981721330', '85981721470', '85981723162', '85981723682', '85981727178', '85981727333', '85981730276', '85981731368', '85981733009', '85981733173', '85981734225', '85981735351', '85981735457', '85981738337', '85981742689', '85981745007', '85981746191', '85981746231', '85981747230', '85981747684', '85981747880', '85981748018', '85981749098', '85981749311', '85981780097', '85981780698', '85981781860', '85981781956', '85981782615', '85981783993', '85981787014', '85981787375', '85981787694', '85981787878', '85981795562', '85981797415', '85981799011', '85981799243', '85981799393', '85981799969', '85981800644', '85981801187', '85981801628', '85981801718', '85981801761', '85981802537', '85981802631', '85981803848', '85981804731', '85981805074', '85981805578', '85981805682', '85981805712', '85981805995', '85981806062', '85981806192', '85981806838', '85981807096', '85981807746', '85981808109', '85981808226', '85981808940', '85981809310', '85981809579', '85981810401', '85981811681', '85981812231', '85981812420', '85981813215', '85981813326', '85981813696', '85981813745', '85981814222', '85981815518', '85981815719', '85981815951', '85981815995', '85981816185', '85981816597', '85981816953', '85981817644', '85981819191', '85981819878', '85981819898', '85981819971', '85981820302', '85981820909', '85981822288', '85981822627', '85981823737', '85981824050', '85981825667', '85981827171', '85981827298', '85981828133', '85981829674', '85981829888', '85981830615', '85981831333', '85981831807', '85981832616', '85981833911', '85981836027', '85981836192', '85981838197', '85981839905', '85981840699', '85981840997', '85981841498', '85981842018', '85981842026', '85981847568', '85981849140', '85981849448', '85981850329', '85981851336', '85981851657', '85981851806', '85981852483', '85981852871', '85981853361', '85981853473', '85981853498', '85981854188', '85981854400', '85981854701', '85981854966', '85981855387', '85981855943', '85981857602', '85981858378', '85981858585', '85981859714', '85981859843', '85981860190', '85981860939', '85981861386', '85981861390', '85981862200', '85981862732', '85981862812', '85981863520', '85981863917', '85981864665', '85981866872', '85981867198', '85981867874', '85981868706', '85981869078', '85981869877', '85981870279', '85981870625', '85981870769', '85981871433', '85981871482', '85981871725', '85981872527', '85981873853', '85981874873', '85981875089', '85981875839', '85981876038', '85981876387', '85981877277', '85981877340', '85981877666', '85981878608', '85981879558', '85981879727', '85981881447', '85981881564', '85981881903', '85981882019', '85981882233', '85981883888', '85981885848', '85981886408', '85981888076', '85981890073', '85981890692', '85981890804', '85981890897', '85981891321', '85981891476', '85981892737', '85981892922', '85981893512', '85981894559', '85981895421', '85981895778', '85981895877', '85981899243', '85981900080', '85981900730', '85981901391', '85981904698', '85981905011', '85981905074', '85981905075', '85981906452', '85981910262', '85981910771', '85981911604', '85981911984', '85981914747', '85981917082', '85981917653', '85981917936', '85981918090', '85981918203', '85981921936', '85981921999', '85981922555', '85981924869', '85981926087', '85981926161', '85981927362', '85981928269', '85981930502', '85981933090', '85981933446', '85981934488', '85981937771', '85981942675', '85981944086', '85981946447', '85981947455', '85981948504', '85981948560', '85981948709', '85981949370', '85981949405', '85981950680', '85981951197', '85981951207', '85981951277', '85981951294', '85981951433', '85981952223', '85981952606', '85981953266', '85981955156', '85981955666', '85981956683', '85981956798', '85981956914', '85981956977', '85981958219', '85981958833', '85981959454', '85981962203', '85981963748', '85981964770', '85981966391', '85981966744', '85981967093', '85981967347', '85981967672', '85981972215', '85981973787', '85981973850', '85981974619', '85981975003', '85981975335', '85981975643', '85981978964', '85981982384', '85981982415', '85981983536', '85981984160', '85981984196', '85981984205', '85981985320', '85981987749', '85981990206', '85981991814', '85981992200', '85981992221', '85981993841', '85981994171', '85981994544', '85981996677', '85981996968', '85981997233', '85981998183', '85981998880', '85981999101', '85981999393', '85982000080', '85982000103', '85982000124', '85982000407', '85982000597', '85982001158', '85982001480', '85982001603', '85982002244', '85982003360', '85982009691', '85982012352', '85982013350', '85982013725', '85982014410', '85982014728', '85982014859', '85982015963', '85982016650', '85982018181', '85982019178', '85982020684', '85982020732', '85982021675', '85982021901', '85982021970', '85982022116', '85982022707', '85982023008', '85982023198', '85982023449', '85982024092', '85982024412', '85982024556', '85982025193', '85982025465', '85982025505', '85982026115', '85982026559', '85982026582', '85982026618', '85982026681', '85982026958', '85982027257', '85982027456', '85982028016', '85982028614', '85982028717', '85982029544', '85982029630', '85982029656', '85982031994', '85982033246', '85982036215', '85982038136', '85982038199', '85982038964', '85982041982', '85982048028', '85982048400', '85982048768', '85982049005', '85982050430', '85982051850', '85982052170', '85982052833', '85982053074', '85982058486', '85982059867', '85982060243', '85982061188', '85982061715', '85982065404', '85982066323', '85982066720', '85982067095', '85982067924', '85982069921', '85982070325', '85982070442', '85982070505', '85982070537', '85982075392', '85982076079', '85982077220', '85982080055', '85982080963', '85982081863', '85982082408', '85982082685', '85982086204', '85982086988', '85982088181', '85982088401', '85982090444', '85982092229', '85982092410', '85982092535', '85982095933', '85982096408', '85982096638', '85982096702', '85982098898', '85982099596', '85982101224', '85982102764', '85982103459', '85982103837', '85982104191', '85982105219', '85982105253', '85982105588', '85982106049', '85982107612', '85982108435', '85982108824', '85982108871', '85982108995', '85982109939', '85982110388', '85982110918', '85982111162', '85982111405', '85982111461', '85982111682', '85982111714', '85982112134', '85982112150', '85982112252', '85982112330', '85982112561', '85982112835', '85982113153', '85982113424', '85982113947', '85982114041', '85982114590', '85982114798', '85982115352', '85982115530', '85982116277', '85982116934', '85982116997', '85982118281', '85982118296', '85982118359', '85982118717', '85982119038', '85982119077', '85982120196', '85982120770', '85982121018', '85982121624', '85982122300', '85982122468', '85982123793', '85982123880', '85982125254', '85982126275', '85982127512', '85982130408', '85982130446', '85982131720', '85982132411', '85982132443', '85982132450', '85982133520', '85982134594', '85982134658', '85982140032', '85982141654', '85982144572', '85982145647', '85982145648', '85982147385', '85982147517', '85982148150', '85982148935', '85982150345', '85982154109', '85982154431', '85982154497', '85982155595', '85982155633', '85982161243', '85982161749', '85982162384', '85982162735', '85982163153', '85982164038', '85982166162', '85982166295', '85982166369', '85982170184', '85982171502', '85982171541', '85982171985', '85982184521', '85982185872', '85982190343', '85982204545', '85982205828', '85982207580', '85982217764', '85982222262', '85982223649', '85982225298', '85982234415', '85982243000', '85982254767', '85982254833', '85984000187', '85984000206', '85984000276', '85984000283', '85984000366', '85984000374', '85984000408', '85984000419', '85984000570', '85984000752', '85984000901', '85984000924', '85984001030', '85984001034', '85984001146', '85984001200', '85984001263', '85984001399', '85984001670', '85984001714', '85984001904', '85984002329', '85984002699', '85984004021', '85984004143', '85984004381', '85984004513', '85984004885', '85984004934', '85984004937', '85984005030', '85984005089', '85984005191', '85984005207', '85984005486', '85984005676', '85984005684', '85984005854', '85984006088', '85984006430', '85984006519', '85984006807', '85984006822', '85984006945', '85984007418', '85984007839', '85984007934', '85984008090', '85984008165', '85984008494', '85984008541', '85984008711', '85984008837', '85984008876', '85984009118', '85984009152', '85984010102', '85984010119', '85984010346', '85984010352', '85984010376', '85984010523', '85984010651', '85984010721', '85984010796', '85984011030', '85984011127', '85984011205', '85984011272', '85984011345', '85984011423', '85984012202', '85984012591', '85984012893', '85984013559', '85984013847', '85984013900', '85984013932', '85984013963', '85984014210', '85984014231', '85984014288', '85984014376', '85984014432', '85984014547', '85984015074', '85984015099', '85984015349', '85984015384', '85984015385', '85984015469', '85984015572', '85984015631', '85984015661', '85984015695', '85984015758', '85984015793', '85984015918', '85984015943', '85984015948', '85984016599', '85984016848', '85984017946', '85984018354', '85984019606', '85984019846', '85984019986', '85984020049', '85984020051', '85984020177', '85984020235', '85984020417', '85984020826', '85984020911', '85984021324', '85984021461', '85984021871', '85984022102', '85984022241', '85984022389', '85984022437', '85984022645', '85984023016', '85984023231', '85984023332', '85984023361', '85984023534', '85984024023', '85984024057', '85984024750', '85984024773', '85984024790', '85984024966', '85984025156', '85984025366', '85984025761', '85984026229', '85984026355', '85984026707', '85984026882', '85984026909', '85984026937', '85984027014', '85984027778', '85984027803', '85984027980', '85984028311', '85984028478', '85984028528', '85984028635', '85984028807', '85984029384', '85984029403', '85984029645', '85984029647', '85984029806', '85984029997', '85984030002', '85984030015', '85984030126', '85984030128', '85984030255', '85984030534', '85984030799', '85984030914', '85984031018', '85984031134', '85984031235', '85984031240', '85984031369', '85984031377', '85984031387', '85984031438', '85984031757', '85984031799', '85984031859', '85984031951', '85984031983', '85984031996', '85984032024', '85984032030', '85984032046', '85984032152', '85984032209', '85984032278', '85984032838', '85984032911', '85984033253', '85984033308', '85984033709', '85984033733', '85984033741', '85984033796', '85984033825', '85984033893', '85984033983', '85984034114', '85984034385', '85984034577', '85984034588', '85984034633', '85984034782', '85984034964', '85984035081', '85984035134', '85984035188', '85984035416', '85984035423', '85984035459', '85984035494', '85984035559', '85984035765', '85984036032', '85984036315', '85984036485', '85984036570', '85984036614', '85984036676', '85984036734', '85984036808', '85984036872', '85984037291', '85984037296', '85984037302', '85984037313', '85984037354', '85984037682', '85984037921', '85984037935', '85984037947', '85984038033', '85984038229', '85984038524', '85984038538', '85984038620', '85984038850', '85984038856', '85984039320', '85984039429', '85984039451', '85984039728', '85984040449', '85984040502', '85984040554', '85984040731', '85984040757', '85984040783', '85984040792', '85984040899', '85984041029', '85984041044', '85984041297', '85984041417', '85984041458', '85984041670', '85984041713', '85984041805', '85984041914', '85984041986', '85984042380', '85984042425', '85984042497', '85984042509', '85984042623', '85984042895', '85984042963', '85984043070', '85984043137', '85984043296', '85984043323', '85984043326', '85984043413', '85984043751', '85984044012', '85984044067', '85984044191', '85984044248', '85984044283', '85984044300', '85984044346', '85984044633', '85984044683', '85984044763', '85984044963', '85984045050', '85984045056', '85984045115', '85984045640', '85984045722', '85984046240', '85984046424', '85984046625', '85984046753', '85984046806', '85984046807', '85984046867', '85984047111', '85984047230', '85984047233', '85984047367', '85984047472', '85984047476', '85984047517', '85984047596', '85984048175', '85984048182', '85984048183', '85984048283', '85984048339', '85984048508', '85984048524', '85984048559', '85984048759', '85984048849', '85984049026', '85984049029', '85984049263', '85984049442', '85984049451', '85984049504', '85984049679', '85984049735', '85984049763', '85984049858', '85984049949', '85984050227', '85984050228', '85984050250', '85984050371', '85984050677', '85984050801', '85984050882', '85984050887', '85984050928', '85984051292', '85984051333', '85984051412', '85984051489', '85984051523', '85984051742', '85984051769', '85984051840', '85984051889', '85984051935', '85984052109', '85984052112', '85984052208', '85984052217', '85984052263', '85984052298', '85984052611', '85984052730', '85984052764', '85984052843', '85984053038', '85984053174', '85984053179', '85984053330', '85984053556', '85984053869', '85984053880', '85984053887', '85984053943', '85984053956', '85984054025', '85984054056', '85984054133', '85984054160', '85984054172', '85984054228', '85984054266', '85984054556', '85984054674', '85984054734', '85984054739', '85984054879', '85984054912', '85984055156', '85984055310', '85984055345', '85984055442', '85984055473', '85984055502', '85984055688', '85984055714', '85984055899', '85984055933', '85984056265', '85984056517', '85984056826', '85984056911', '85984056971', '85984057268', '85984057361', '85984057589', '85984057713', '85984057802', '85984057880', '85984058809', '85984059297', '85984059565', '85984059708', '85984060013', '85984060654', '85984060832', '85984061103', '85984061137', '85984061447', '85984061486', '85984061543', '85984061639', '85984061962', '85984062029', '85984062279', '85984062320', '85984062358', '85984062494', '85984062505', '85984062530', '85984063166', '85984063203', '85984063719', '85984063744', '85984063839', '85984064263', '85984064393', '85984064541', '85984064961', '85984065160', '85984065816', '85984066050', '85984066966', '85984067046', '85984067756', '85984067873', '85984068456', '85984069092', '85984069667', '85984069722', '85984069938', '85984070019', '85984070211', '85984070265', '85984070421', '85984070652', '85984070895', '85984071052', '85984071611', '85984071870', '85984072029', '85984072045', '85984072051', '85984072058', '85984072071', '85984072145', '85984072225', '85984072316', '85984072445', '85984072480', '85984072653', '85984072933', '85984073162', '85984073973', '85984074264', '85984074313', '85984074778', '85984075096', '85984075666', '85984076005', '85984076212', '85984076393', '85984076578', '85984076839', '85984076847', '85984077031', '85984077361', '85984077370', '85984077740', '85984077801', '85984078005', '85984078034', '85984078218', '85984078233', '85984078314', '85984078445', '85984078614', '85984079116', '85984079245', '85984079370', '85984079725', '85984079880', '85984079915', '85984080469', '85984080471', '85984080593', '85984080601', '85984081278', '85984081475', '85984081680', '85984082025', '85984082125', '85984082555', '85984082670', '85984082940', '85984082979', '85984083419', '85984083846', '85984084306', '85984084464', '85984084549', '85984084550', '85984084823', '85984084857', '85984085018', '85984085176', '85984085262', '85984085880', '85984086976', '85984087409', '85984088006', '85984088529', '85984089052', '85984089070', '85984089220', '85984089798', '85984090380', '85984090552', '85984090594', '85984090882', '85984090929', '85984091124', '85984091289', '85984091406', '85984091518', '85984092054', '85984092195', '85984092230', '85984092539', '85984093168', '85984093610', '85984093759', '85984093855', '85984094073', '85984094849', '85984095284', '85984096033', '85984098963', '85984099235', '85984099245', '85984099377', '85984099885', '85984100300', '85984100698', '85984100822', '85984101624', '85984101697', '85984102042', '85984102155', '85984102262', '85984102480', '85984102514', '85984102560', '85984102571', '85984103927', '85984104957', '85984105301', '85984105524', '85984106425', '85984107192', '85984107381', '85984107762', '85984108029', '85984108520', '85984108531', '85984108645', '85984108950', '85984109045', '85984109435', '85984109534', '85984110121', '85984110186', '85984110449', '85984110493', '85984110570', '85984110730', '85984110811', '85984111215', '85984111369', '85984111609', '85984111626', '85984111796', '85984111877', '85984111930', '85984112126', '85984112139', '85984112386', '85984112657', '85984113012', '85984113687', '85984113734', '85984113870', '85984113916', '85984114001', '85984114121', '85984114826', '85984114827', '85984115475', '85984115569', '85984115651', '85984116121', '85984116540', '85984116596', '85984116734', '85984116933', '85984117008', '85984117204', '85984117429', '85984117798', '85984118037', '85984118042', '85984118203', '85984118581', '85984118664', '85984118708', '85984118774', '85984119107', '85984119481', '85984119572', '85984119808', '85984120393', '85984120682', '85984121272', '85984122145', '85984122414', '85984123034', '85984123448', '85984124093', '85984124208', '85984125015', '85984125036', '85984126078', '85984126186', '85984126390', '85984126584', '85984126778', '85984126955', '85984127219', '85984127242', '85984127734', '85984128627', '85984128634', '85984128869', '85984128924', '85984129311', '85984129612', '85984130038', '85984130659', '85984130724', '85984130979', '85984131046', '85984131139', '85984131313', '85984131574', '85984131761', '85984131881', '85984132127', '85984132128', '85984132149', '85984132782', '85984132844', '85984133084', '85984133130', '85984133206', '85984133331', '85984133448', '85984133534', '85984134089', '85984134736', '85984135015', '85984135302', '85984135420', '85984135573', '85984</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08/2022', '24/08</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['10', '27', '27', '27', '46', '30', '27', '1', '5', '29', '1', '35', '16', '43', '27', '27', '27', '11', '5', '28', '1', '49', '27', '27', '1', '27', '0', '27', '11', '1', '28', '10', '3', '27', '3', '28', '27', '31', '1', '25', '1', '27', '27', '40', '27', '27', '28', '27', '27', '12', '28', '5', '7', '6', '28', '40', '49', '1', '2', '8', '78', '1', '1', '27', '5', '27', '1', '27', '27', '11', '1', '28', '12', '27', '27', '1', '5', '27', '27', '2', '27', '27', '27', '25', '7', '27', '28', '1', '11', '27', '1', '1', '27', '21', '13', '6', '27', '5', '1', '0', '28', '27', '28', '27', '27', '27', '27', '27', '27', '7', '28', '5', '5', '27', '27', '47', '28', '27', '34', '1', '35', '5', '8', '12', '28', '27', '12', '49', '28', '27', '6', '27', '1', '1', '17', '5', '27', '1', '1', '28', '31', '1', '27', '12', '5', '27', '39', '49', '19', '16', '28', '27', '5', '27', '8', '27', '4', '35', '8', '30', '35', '1', '27', '27', '10', '40', '1', '27', '27', '49', '27', '29', '27', '27', '1', '28', '43', '32', '45', '30', '27', '27', '6', '27', '5', '2', '27', '7', '49', '13', '28', '6', '27', '27', '27', '27', '26', '27', '27', '27', '28', '49', '1', '27', '11', '28', '27', '27', '27', '27', '1', '18', '28', '27', '27', '27', '1', '27', '1', '49', '10', '27', '5', '49', '1', '11', '27', '49', '27', '27', '5', '49', '27', '7', '5', '28', '1', '29', '27', '11', '31', '38', '27', '15', '27', '27', '49', '17', '41', '8', '27', '1', '28', '30', '28', '3', '27', '30', '30', '5', '27', '10', '1', '49', '27', '28', '1', '27', '4', '1', '28', '5', '27', '27', '12', '28', '10', '27', '27', '48', '1', '1', '1', '27', '30', '1', '27', '27', '27', '29', '27', '5', '27', '27', '6', '1', '30', '27', '28', '1', '12', '5', '29', '25', '27', '49', '27', '27', '6', '11', '27', '27', '27', '27', '11', '27', '1', '27', '27', '27', '27', '27', '30', '27', '49', '28', '28', '23', '40', '27', '28', '27', '27', '27', '5', '11', '27', '27', '1', '5', '11', '28', '27', '27', '27', '28', '9', '5', '27', '11', '27', '1', '35', '1', '27', '1', '27', '27', '1', '30', '27', '27', '28', '17', '27', '27', '1', '27', '35', '49', '27', '49', '27', '27', '11', '27', '12', '27', '27', '8', '4', '49', '11', '27', '35', '4', '28', '27', '27', '27', '5', '18', '1', '5', '27', '27', '1', '28', '27', '1', '1', '11', '1', '1', '28', '114', '9', '27', '27', '5', '28', '27', '27', '1', '23', '27', '27', '5', '1', '27', '1', '5', '27', '27', '27', '27', '87', '27', '28', '31', '39', '34', '27', '27', '27', '9', '13', '9', '1', '17', '27', '35', '27', '30', '12', '27', '27', '49', '6', '27', '27', '27', '1', '28', '1', '30', '27', '27', '27', '12', '27', '27', '27', '1', '28', '0', '27', '49', '27', '27', '1', '28', '27', '27', '49', '27', '27', '27', '49', '27', '27', '6', '49', '1', '27', '9', '1', '28', '42', '13', '31', '27', '15', '8', '49', '27', '5', '27', '8', '27', '29', '27', '27', '49', '27', '14', '27', '28', '27', '27', '49', '29', '11', '27', '27', '12', '27', '27', '27', '27', '27', '1', '27', '5', '22', '1', '27', '27', '49', '17', '29', '11', '27', '27', '5', '13', '1', '10', '27', '28', '27', '27', '27', '27', '27', '5', '24', '27', '1', '1', '27', '1', '30', '27', '27', '27', '1', '14', '19', '25', '27', '27', '27', '27', '49', '27', '30', '11', '30', '5', '27', '27', '1', '27', '28', '27', '1', '29', '27', '27', '1', '5', '1', '37', '49', '1', '5', '2', '82', '5', '27', '27', '30', '8', '27', '5', '27', '27', '27', '28', '49', '27', '27', '27', '27', '28', '5', '27', '27', '1', '27', '14', '5', '49', '31', '1', '27', '1', '27', '5', '27', '27', '27', '28', '1', '12', '40', '27', '43', '27', '27', '1', '27', '49', '49', '21', '27', '27', '22', '27', '7', '12', '27', '27', '0', '1', '27', '27', '27', '28', '1', '7', '28', '49', '27', '27', '27', '7', '28', '16', '1', '1', '27', '12', '10', '12', '27', '27', '4', '27', '27', '30', '5', '12', '29', '27', '27', '17', '27', '27', '13', '5', '27', '12', '16', '49', '27', '1', '27', '6', '49', '29', '27', '28', '18', '28', '49', '27', '27', '27', '30', '27', '7', '23', '49', '12', '16', '27', '1', '5', '1', '27', '27', '27', '27', '27', '27', '27', '49', '27', '28', '27', '1', '27', '27', '27', '27', '27', '49', '21', '27', '28', '27', '27', '28', '35', '27', '49', '1', '27', '27', '26', '27', '38', '27', '1', '6', '27', '27', '28', '7', '28', '27', '27', '27', '27', '12', '5', '6', '27', '18', '28', '17', '27', '27', '28', '23', '14', '27', '12', '29', '28', '28', '27', '27', '27', '27', '28', '28', '49', '5', '27', '12', '27', '27', '27', '49', '27', '27', '12', '8', '27', '28', '28', '1', '9', '28', '27', '27', '27', '1', '1', '10', '1', '28', '27', '12', '1', '7', '27', '27', '27', '27', '28', '27', '27', '27', '5', '27', '12', '46', '27', '27', '31', '35', '17', '28', '27', '20', '24', '23', '1', '41', '36', '49', '49', '7', '28', '49', '27', '27', '5', '5', '27', '1', '5', '17', '27', '28', '13', '7', '49', '28', '27', '27', '27', '1', '34', '42', '35', '27', '28', '28', '28', '35', '11', '27', '5', '5', '28', '28', '27', '28', '1', '28', '13', '27', '28', '27', '28', '30', '28', '28', '18', '27', '5', '1', '76', '28', '28', '1', '5', '1', '28', '26', '2', '28', '1', '7', '12', '28', '37', '11', '28', '27', '27', '27', '27', '28', '28', '27', '20', '8', '30', '14', '27', '4', '10', '4', '49', '28', '28', '1', '1', '22', '27', '1', '10', '28', '11', '28', '77', '28', '2', '27', '30', '27', '27', '31', '1', '28', '28', '12', '27', '28', '10', '30', '27', '9', '27', '18', '28', '0', '12', '28', '49', '27', '27', '27', '27', '30', '1', '28', '27', '50', '31', '1', '27', '1', '27', '28', '28', '28', '27', '7', '1', '28', '27', '1', '27', '31', '28', '27', '1', '28', '1', '49', '49', '27', '28', '27', '27', '1', '27', '28', '27', '5', '26', '12', '1', '28', '2', '8', '13', '1', '12', '1', '28', '27', '1', '30', '7', '7', '37', '27', '28', '8', '5', '27', '28', '27', '27', '13', '13', '27', '30', '13', '13', '27', '1', '28', '27', '28', '27', '31', '27', '13', '28', '27', '27', '28', '12', '27', '27', '7', '1', '29', '27', '27', '1', '5', '27', '13', '27', '28', '49', '27', '6', '28', '27', '1', '27', '27', '21', '28', '31', '46', '27', '28', '5', '5', '27', '27', '30', '7', '27', '28', '28', '28', '30', '9', '17', '1', '3', '30', '7', '27', '28', '27', '7', '37', '27', '14', '13', '28', '27', '27', '27', '1', '27', '27', '27', '27', '28', '6', '28', '27', '12', '27', '47', '49', '28', '28', '27', '27', '13', '14', '28', '12', '28', '7', '27', '28', '27', '27', '1', '1', '27', '14', '0', '1', '27', '1', '1', '31', '1', '5', '39', '35', '27', '28', '11', '30', '27', '1', '27', '49', '27', '28', '28', '27', '47', '27', '28', '28', '5', '28', '30', '11', '49', '27', '28', '1', '28', '28', '28', '27', '49', '30', '27', '28', '30', '27', '15', '49', '8', '28', '12', '27', '17', '28', '27', '30', '49', '1', '28', '28', '27', '27', '27', '49', '1', '26', '1', '27', '49', '1', '6', '27', '5', '28', '1', '27', '11', '16', '28', '114', '27', '27', '27', '34', '1', '6', '28', '49', '21', '27', '27', '27', '28', '10', '1', '27', '27', '27', '49', '1', '28', '28', '27', '31', '28', '28', '28', '49', '49', '27', '27', '27', '8', '28', '1', '11', '5', '1', '1', '27', '32', '49', '27', '9', '33', '27', '5', '28', '27', '31', '28', '27', '27', '27', '27', '27', '39', '30', '12', '13', '28', '34', '1', '27', '27', '28', '28', '15', '11', '27', '28', '1', '27', '1', '35', '27', '7', '17', '1', '35', '23', '27', '28', '1', '5', '28', '2', '21', '27', '28', '28', '28', '11', '49', '32', '28', '14', '14', '30', '27', '1', '28', '28', '28', '23', '1', '27', '27', '27', '28', '47', '27', '28', '1', '27', '27', '28', '42', '49', '27', '27', '5', '28', '27', '1', '28', '27', '26', '27', '27', '28', '28', '8', '5', '0', '49', '28', '28', '5', '28', '27', '28', '28', '41', '8', '27', '27', '27', '6', '27', '27', '27', '6', '1', '28', '30', '5', '27', '12', '2', '5', '28', '15', '5', '27', '28', '27', '12', '28', '28', '5', '27', '12', '28', '27', '27', '6', '1', '30', '28', '27', '28', '12', '27', '13', '1', '49', '31', '27', '12', '28', '27', '28', '27', '33', '27', '40', '27', '28', '28', '27', '0', '20', '27', '1', '43', '28', '28', '1', '49', '33', '27', '10', '28', '27', '28', '27', '27', '2', '27', '27', '49', '1', '28', '28', '43', '27', '27', '28', '49', '5', '28', '146', '10', '18', '28', '27', '27', '27', '28', '27', '28', '28', '28', '11', '1', '5', '6', '27', '8', '5', '9', '28', '1', '27', '28', '18', '27', '6', '6', '26', '27', '7', '27', '49', '8', '27', '75', '21', '58', '27', '27', '21', '27', '21', '6', '27', '29', '27', '27', '62', '69', '65', '17', '27', '49', '8', '27', '8', '5', '27', '1', '30', '1', '27', '32', '32', '49', '5', '5', '4', '13', '32', '33', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '32', '5', '4', '5', '32', '4', '3', '4', '4', '4', '5', '35', '33', '4', '5', '5', '5', '4', '30', '32', '5', '4', '5', '19', '5', '5', '4', '5', '5', '5', '5', '5', '4', '4', '5', '5', '5', '32', '32', '39', '4', '4', '4', '34', '5', '33', '34', '49', '4', '5', '4', '5', '3', '77', '4', '4', '5', '5', '4', '5', '5', '5', '5', '5', '5', '6', '5', '5', '4', '4', '5', '4', '5', '4', '4', '32', '5', '51', '4', '32', '4', '33', '4', '4', '5', '12', '32', '4', '4', '32', '5', '5', '4', '5', '4', '3', '4', '5', '4', '5', '6', '4', '5', '32', '4', '4', '4', '5', '4', '5', '5', '5', '2', '5', '6', '4', '49', '5', '4', '32', '5', '32', '5', '5', '5', '39', '49', '33', '33', '4', '4', '5', '5', '5', '4', '5', '5', '4', '33', '32', '32', '32', '32', '33', '5', '32', '32', '32', '33', '44', '20', '14', '33', '6', '32', '12', '49', '32', '32', '49', '33', '34', '5', '32', '32', '32', '32', '4', '32', '32', '5', '6', '42', '33', '35', '32', '31', '31', '5', '32', '49', '32', '4', '27', '11', '32', '4', '69', '32', '6', '32', '34', '5', '32', '49', '32', '21', '32', '32', '5', '30', '33', '32', '16', '32', '33', '34', '32', '48', '49', '31', '32', '6', '32', '34', '34', '5', '33', '49', '39', '32', '33', '33', '4', '32', '11', '32', '6', '6', '33', '32', '33', '33', '31', '32', '32', '5', '32', '4', '32', '4', '32', '32', '33', '32', '32', '5', '34', '32', '33', '32', '49', '32', '27', '31', '4', '12', '33', '34', '49', '5', '31', '32', '6', '30', '5', '32', '27', '34', '32', '22', '32', '4', '32', '33', '32', '32', '4', '6', '33', '33', '72', '32', '32', '5', '30', '32', '5', '32', '32', '60', '32', '33', '15', '34', '32', '33', '33', '32', '32', '12', '33', '33', '33', '32', '32', '5', '32', '33', '7', '32', '46', '5', '33', '32', '41', '34', '32', '32', '32', '5', '32', '32', '33', '33', '33', '32', '32', '7', '33', '32', '32', '32', '12', '32', '5', '32', '49', '9', '30', '32', '33', '33', '33', '27', '5', '5', '31', '32', '6', '30', '79', '35', '49', '34', '32', '33', '33', '32', '32', '32', '49', '32', '70', '26', '32', '32', '6', '32', '31', '5', '28', '32', '5', '5', '10', '4', '49', '33', '5', '32', '32', '6', '5', '4', '4', '4', '5', '5', '32', '5', '4', '5', '5', '75', '4', '4', '4', '4', '34', '4', '5', '5', '49', '42', '4', '5', '32', '2', '4', '5', '33', '4', '5', '5', '5', '5', '5', '4', '11', '32', '49', '4', '30', '5', '27', '4', '31', '29', '2', '4', '5', '33', '5', '4', '5', '32', '4', '4', '5', '32', '5', '4', '32', '14', '37', '5', '4', '33', '4', '5', '5', '31', '4', '4', '5', '32', '33', '33', '5', '5', '5', '5', '4', '4', '4', '4', '5', '5', '30', '4', '0', '4', '16', '4', '5', '4', '4', '5', '5', '5', '5', '4', '5', '4', '30', '5', '5', '5', '15', '5', '4', '5', '5', '5', '5', '7', '4', '4', '4', '32', '32', '5', '32', '4', '4', '5', '4', '4', '4', '4', '4', '4', '4', '4', '30', '4', '5', '4', '4', '5', '34', '4', '5', '64', '4', '4', '4', '4', '4', '4', '4', '5', '4', '4', '5', '5', '5', '4', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '31', '4', '4', '5', '4', '5', '35', '4', '4', '4', '5', '4', '4', '5', '4', '5', '4', '5', '4', '5', '4', '4', '4', '4', '32', '4', '4', '31', '13', '4', '11', '4', '32', '5', '4', '33', '5', '32', '4', '30', '4', '5', '32', '33', '5', '5', '5', '4', '5', '3', '4', '4', '5', '32', '4', '4', '5', '31', '32', '5', '49', '12', '5', '4', '5', '4', '33', '2', '5', '5', '30', '80', '4', '33', '33', '3', '5', '34', '31', '34', '7', '59', '32', '33', '5', '32', '95', '5', '32', '32', '5', '5', '32', '30', '5', '32', '5', '4', '4', '32', '5', '4', '4', '5', '5', '33', '11', '4', '32', '4', '4', '33', '4', '63', '4', '4', '4', '34', '4', '18', '33', '32', '33', '32', '4', '32', '47', '5', '4', '32', '5', '5', '49', '35', '32', '33', '32', '5', '7', '32', '4', '32', '21', '12', '5', '32', '32', '4', '4', '4', '5', '5', '4', '32', '5', '4', '5', '32', '5', '4', '34', '4', '5', '4', '5', '5', '4', '5', '4', '4', '30', '32', '5', '33', '33', '32', '31', '33', '32', '32', '4', '6', '34', '1', '15', '30', '32', '5', '4', '32', '4', '5', '32', '2', '49', '8', '32', '11', '6', '5', '31', '33', '12', '34', '33', '31', '4', '33', '34', '34', '32', '32', '32', '32', '8', '32', '33', '4', '74', '4', '33', '32', '28', '4', '5', '33', '14', '32', '33', '31', '5', '32', '5', '33', '33', '32', '33', '32', '5', '32', '33', '23', '27', '31', '31', '34', '31', '5', '41', '32', '32', '33', '32', '11', '32', '7', '11', '32', '33', '32', '33', '34', '32', '32', '4', '32', '31', '32', '32', '32', '32', '33', '46', '32', '66', '32', '33', '30', '5', '32', '32', '32', '4', '32', '32', '32', '32', '33', '32', '49', '32', '32', '32', '33', '33', '32', '5', '33', '32', '12', '32', '33', '16', '32', '33', '5', '32', '32', '9', '34', '64', '4', '32', '32', '33', '32', '31', '32', '32', '10', '32', '6', '33', '13', '32', '5', '5', '4', '31', '3', '32', '25', '40', '34', '32', '32', '34', '5', '32', '44', '33', '8', '32', '33', '32', '33', '5', '33', '32', '32', '32', '18', '30', '32', '33', '32', '49', '32', '32', '32', '6', '17', '33', '33', '5', '49', '32', '19', '4', '5', '5', '4', '5', '7', '4', '11', '33', '32', '32', '4', '3', '32', '27', '4', '4', '33', '5', '4', '34', '31', '5', '30', '1', '4', '5', '32', '5', '4', '5', '4', '61', '9', '4', '11', '5', '32', '33', '33', '34', '4', '33', '34', '4', '32', '32', '5', '32', '4', '31', '32', '33', '5', '4', '33', '5', '4', '27', '5', '5', '4', '35', '5', '5', '4', '5', '4', '4', '4', '33', '5', '32', '5', '5', '5', '27', '4', '4', '4', '4', '4', '5', '5', '5', '5', '6', '5', '5', '5', '5', '4', '5', '5', '5', '4', '5', '4', '66', '4', '4', '4', '4', '5', '4', '4', '4', '32', '7', '33', '5', '7', '4', '5', '55', '32', '43', '21', '5', '4', '5', '3', '4', '5', '4', '4', '32', '32', '33', '34', '5', '69', '4', '32', '4', '32', '25', '30', '32', '30', '32', '63', '35', '33', '5', '32', '5', '32', '4', '5', '4', '5', '4', '5', '4', '4', '33', '33', '33', '4', '30', '5', '33', '32', '4', '32', '33', '27', '5', '4', '32', '5', '4', '32', '5', '5', '5', '33', '4', '5', '4', '4', '4', '5', '5', '7', '33', '5', '32', '5', '5', '49', '5', '4', '4', '5', '4', '4', '5', '4', '4', '5', '32', '4', '4', '4', '4', '4', '5', '32', '4', '5', '4', '4', '4', '5', '4', '5', '4', '4', '61', '4', '5', '4', '38', '33', '4', '5', '34', '13', '4', '4', '32', '32', '32', '4', '5', '5', '32', '5', '32', '4', '33', '33', '33', '5', '5', '33', '5', '5', '4', '12', '4', '28', '5', '5', '5', '5', '5', '4', '5', '5', '4', '32', '6', '4', '4', '5', '9', '13', '32', '34', '4', '33', '15', '32', '32', '4', '32', '5', '5', '27', '4', '5', '4', '4', '5', '4', '4', '4', '5', '4', '21', '5', '5', '33', '5', '4', '34', '5', '4', '4', '4', '5', '4', '4', '5', '5', '4', '5', '5', '13', '4', '5', '4', '5', '4', '4', '31', '5', '4', '5', '4', '4', '5', '30', '4', '4', '5', '4', '5', '4', '4', '5', '4', '4', '4', '4', '4', '5', '4', '5', '5', '5', '46', '4', '4', '4', '4', '5', '4', '5', '22', '5', '5', '4', '49', '5', '5', '32', '5', '4', '5', '5', '5', '4', '4', '32', '4', '30', '32', '4', '4', '4', '4', '5', '5', '12', '5', '4', '5', '4', '33', '4', '4', '4', '32', '4', '4', '4', '4', '5', '4', '4', '32', '4', '35', '5', '4', '4', '5', '4', '5', '32', '0', '67', '4', '31', '4', '5', '30', '4', '17', '3', '5', '4', '4', '4', '5', '22', '5', '4', '4', '4', '4', '5', '5', '5', '5', '4', '5', '5', '2', '4', '4', '5', '32', '5', '5', '5', '4', '4', '4', '50', '4', '5', '4', '4', '5', '5', '5', '32', '5', '30', '32', '4', '5', '32', '4', '4', '4', '4', '4', '5', '5', '4', '5', '68', '5', '29', '4', '5', '5', '4', '5', '5', '6', '6', '6', '6', '6', '6', '5', '6', '6', '32', '35', '6', '33', '6', '24', '5', '34', '33', '32', '30', '31', '32', '33', '13', '32', '32', '93', '8', '33', '32', '32', '5', '33', '31', '32', '32', '33', '13', '32', '9', '32', '30', '3', '4', '9', '33', '3', '32', '33', '19', '32', '32', '33', '32', '33', '30', '30', '32', '5', '33', '32', '81', '7', '7', '32', '79', '33', '15', '32', '32', '32', '32', '5', '30', '32', '7', '32', '33', '5', '32', '33', '33', '35', '33', '32', '33', '33', '33', '31', '33', '32', '34', '32', '32', '32', '34', '33', '7', '33', '13', '32', '32', '32', '49', '32', '33', '33', '32', '32', '4', '32', '32', '33', '33', '4', '32', '33', '33', '12', '49', '33', '32', '80', '32', '33', '32', '25', '32', '34', '33', '4', '32', '32', '33', '32', '33', '33', '32', '33', '32', '4', '21', '32', '5', '32', '49', '71', '33', '33', '16', '13', '4', '32', '32', '5', '27', '18', '34', '33', '32', '65', '32', '32', '22', '27', '49', '34', '33', '33', '5', '4', '5', '5', '44', '32', '30', '12', '32', '32', '11', '33', '33', '33', '33', '32', '4', '11', '32', '32', '11', '8', '32', '4', '5', '5', '5', '33', '4', '4', '4', '70', '12', '27', '32', '32', '5', '17', '33', '32', '32', '8', '34', '32', '59', '32', '32', '33', '31', '31', '32', '49', '5', '15', '13', '33', '34', '32', '4', '33', '32', '4', '8', '32', '33', '22', '34', '49', '11', '33', '32', '32', '5', '28', '32', '31', '32', '32', '12', '32', '32', '32', '28', '49', '30', '33', '33', '32', '3', '18', '30', '33', '4', '32', '4', '31', '1', '12', '28', '5', '49', '33', '23', '32', '32', '33', '33', '33', '8', '33', '4', '29', '4', '32', '13', '32', '33', '33', '34', '32', '31', '33', '32', '4', '5', '32', '32', '5', '33', '15', '11', '33', '9', '50', '59', '13', '32', '32', '34', '33', '34', '33', '33', '33', '32', '20', '20', '33', '33', '34', '33', '32', '31', '12', '32', '33', '33', '5', '32', '32', '31', '33', '5', '32', '33', '7', '33', '32', '26', '13', '34', '12', '4', '5', '12', '49', '32', '33', '33', '32', '32', '32', '33', '33', '32', '17', '13', '32', '33', '10', '32', '32', '30', '32', '32', '32', '8', '5', '32', '32', '32', '32', '32', '12', '30', '12', '34', '33', '32', '45', '32', '34', '28', '32', '4', '4', '17', '32', '33', '49', '33', '26', '33', '49', '33', '31', '32', '32', '14', '5', '32', '32', '32', '32', '27', '32', '5', '33', '32', '32', '32', '32', '32', '32', '13', '15', '32', '30', '32', '32', '32', '32', '26', '32', '18', '33', '32', '32', '32', '49', '32', '33', '31', '32', '4', '5', '34', '32', '33', '33', '34', '32', '32', '6', '33', '5', '31', '32', '33', '32', '31', '29', '12', '32', '32', '5', '33', '30', '33', '32', '32', '31', '32', '39', '7', '61', '25', '34', '33', '32', '32', '7', '32', '31', '31', '33', '10', '34', '32', '31', '22', '32', '20', '9', '32', '32', '33', '30', '12', '33', '33', '33', '27', '5', '32', '5', '27', '24', '12', '32', '32', '62', '32', '22', '32', '5', '32', '33', '24', '49', '32', '32', '32', '4', '6', '33', '4', '33', '32', '32', '32', '32', '1', '11', '32', '26', '24', '5', '5', '32', '7', '5', '31', '33', '5', '54', '32', '33', '32', '32', '32', '32', '30', '32', '32', '12', '31', '32', '33', '33', '32', '33', '49', '33', '22', '32', '12', '32', '27', '55', '32', '34', '60', '32', '4', '5', '4', '4', '4', '4', '4', '4', '4', '5', '6', '4', '4', '34', '33', '4', '4', '33', '5', '35', '33', '33', '4', '5', '5', '33', '32', '32', '32', '5', '4', '4', '5', '5', '5', '32', '32', '4', '49', '5', '15', '33', '32', '32', '32', '34', '32', '60', '32', '32', '32', '27', '33', '30', '15', '5', '5', '72', '4', '4', '33', '33', '11', '32', '32', '32', '44', '63', '6', '7', '32', '32', '32', '5', '4', '19', '32', '14', '1', '33', '32', '71', '4', '48', '4', '31', '34', '5', '35', '5', '32', '32', '33', '32', '32', '26', '13', '32', '28', '32', '6', '21', '31', '64', '11', '33', '32', '32', '34', '5', '32', '26', '32', '5', '14', '32', '5', '5', '32', '4', '39', '13', '4', '35', '0', '32', '33', '33', '32', '32', '32', '49', '15', '33', '32', '32', '27', '32', '32', '5', '46', '11', '24', '33', '11', '4', '32', '12', '5', '5', '5', '32', '33', '32', '1', '32', '7', '13', '32', '32', '32', '13', '5', '30', '5', '4', '32', '30', '33', '33', '4', '7', '5', '33', '33', '33', '32', '14', '29', '6', '13', '32', '10', '33', '33', '5', '30', '12', '21', '33', '32', '33', '31', '30', '32', '18', '34', '32', '32', '34', '30', '12', '32', '32', '30', '32', '33', '34', '30', '32', '5', '33', '32', '12', '33', '33', '32', '32', '32', '11', '32', '32', '33', '32', '33', '32', '30', '32', '5', '32', '32', '25', '32', '33', '31', '32', '14', '33', '57', '30', '32', '49', '27', '5', '32', '12', '33', '33', '32', '32', '33', '21', '33', '33', '32', '10', '33', '33', '33', '32', '4', '4', '32', '32', '31', '33', '33', '33', '32', '24', '5', '35', '32', '32', '5', '3', '34', '32', '32', '5', '32', '33', '57', '33', '4', '34', '52', '33', '32', '33', '32', '33', '33', '1', '33', '33', '33', '22', '27', '33', '32', '32', '34', '33', '7', '12', '1', '4', '33', '32', '33', '33', '32', '32', '31', '32', '32', '29', '33', '31', '49', '5', '11', '34', '32', '32', '25', '35', '32', '25', '32', '33', '33', '5', '32', '27', '32', '31', '30', '30', '34', '32', '31', '5', '13', '30', '32', '4', '33', '32', '32', '32', '34', '4', '33', '30', '31', '32', '32', '33', '34', '49', '32', '5', '31', '33', '32', '32', '49', '8', '33', '32', '5', '32', '32', '33', '5', '32', '4', '36', '5', '32', '4', '32', '32', '18', '33', '33', '34', '34', '32', '8', '41', '32', '33', '49', '32', '32', '32', '5', '30', '49', '27', '32', '55', '49', '49', '26', '5', '33', '33', '33', '32', '32', '34', '32', '32', '12', '32', '11', '31', '33', '34', '32', '21', '28', '57', '32', '30', '4', '32', '4', '32', '17', '31', '33', '32', '32', '32', '32', '5', '30', '32', '32', '32', '32', '34', '32', '32', '32', '32', '32', '32', '33', '33', '13', '32', '34', '32', '32', '32', '32', '32', '5', '33', '32', '32', '33', '32', '5', '12', '33', '32', '5', '32', '32', '32', '5', '32', '5', '16', '34', '33', '33', '4', '30', '11', '34', '32', '35', '94', '10', '4', '14', '32', '28', '4', '32', '32', '17', '15', '4', '27', '4', '32', '32', '5', '34', '32', '32', '7', '33', '18', '31', '58', '20', '32', '11', '67', '36', '4', '27', '12', '32', '33', '26', '33', '5', '32', '32', '32', '32', '33', '77', '4', '33', '35', '32', '31', '31', '24', '32', '32', '33', '32', '24', '29', '33', '32', '32', '32', '24', '32', '5', '32', '16', '33', '33', '32', '32', '32', '11', '32', '5', '32', '32', '32', '32', '45', '32', '32', '31', '32', '32', '15', '32', '30', '31', '32', '5', '33', '5', '32', '32', '32', '32', '52', '26', '32', '32', '5', '33', '2', '34', '36', '33', '49', '33', '32', '5', '32', '6', '14', '32', '33', '32', '31', '31', '32', '33', '32', '33', '32', '32', '5', '32', '28', '32', '33', '32', '33', '8', '32', '5', '33', '12', '48', '32', '32', '32', '32', '32', '33', '4', '32', '13', '8', '32', '32', '33', '38', '33', '34', '33', '6', '33', '32', '32', '32', '13', '5', '4', '32', '16', '34', '7', '11', '12', '5', '11', '9', '33', '11', '33', '4', '34', '32', '32', '6', '49', '31', '32', '32', '5', '32', '4', '32', '32', '15', '6', '49', '32', '5', '32', '32', '32', '32', '6', '32', '32', '33', '32', '5', '11', '7', '5', '32', '31', '45', '33', '31', '32', '30', '6', '33', '33', '31', '34', '70', '1', '32', '31', '5', '32', '19', '5', '32', '32', '32', '32', '32', '31', '4', '32', '4', '32', '32', '11', '33', '32', '49', '33', '32', '33', '5', '32', '32', '33', '12', '49', '33', '32', '32', '11', '32', '32', '32', '33', '26', '33', '32', '32', '26', '0', '32', '31', '10', '32', '4', '31', '27', '5', '32', '33', '51', '12', '49', '6', '33', '33', '34', '32', '32', '32', '33', '32', '33', '5', '33', '32', '4', '49', '34', '32', '32', '5', '25', '31', '32', '33', '2', '5', '32', '14', '32', '32', '78', '32', '32', '32', '9', '20', '33', '33', '34', '32', '15', '33', '31', '32', '31', '32', '7', '11', '33', '32', '22', '49', '32', '32', '31', '33', '33', '32', '24', '32', '34', '33', '32', '34', '33', '14', '32', '33', '33', '19', '32', '32', '32', '14', '32', '8', '33', '33', '33', '32', '1', '33', '32', '32', '33', '27', '33', '11', '32', '33', '5', '32', '32', '12', '5', '11', '32', '33', '32', '32', '33', '32', '32', '45', '9', '32', '33', '32', '32', '32', '32', '32', '13', '32', '32', '5', '32', '32', '8', '7', '32', '33', '13', '49', '38', '6', '32', '33', '33', '19', '32', '32', '4', '4', '32', '32', '32', '33', '5', '33', '32', '12', '31', '32', '32', '33', '32', '38', '49', '33', '11', '32', '14', '6', '32', '33', '5', '5', '31', '32', '32', '32', '49', '32', '30', '70', '5', '33', '4', '16', '32', '32', '4', '32', '63', '6', '33', '49', '49', '5', '33', '32', '33', '33', '32', '5', '22', '5', '32', '11', '33', '32', '32', '11', '30', '33', '30', '34', '24', '21', '5', '32', '32', '32', '9', '13', '32', '48', '18', '5', '8', '7', '33', '32', '32', '32', '32', '19', '8', '32', '30', '33', '5', '32', '33', '32', '32', '32', '35', '11', '4', '32', '31', '32', '32', '32', '33', '33', '32', '10', '32', '32', '32', '1', '30', '7', '24', '33', '33', '32', '4', '33', '32', '5', '10', '27', '32', '33', '34', '32', '33', '33', '32', '32', '32', '32', '32', '32', '5', '33', '4', '32', '5', '32', '32', '7', '32', '33', '33', '32', '30', '16', '32', '5', '5', '5', '5', '5', '31', '33', '33', '4', '33', '32', '32', '5', '32', '33', '24', '31', '33', '8', '33', '32', '32', '32', '5', '32', '32', '5', '12', '41', '8', '33', '32', '32', '17', '5', '32', '32', '49', '32', '32', '4', '32', '9', '32', '33', '31', '33', '33', '31', '5', '32', '32', '4', '32', '32', '27', '32', '32', '32', '33', '32', '12', '49', '13', '32', '32', '30', '32', '5', '11', '32', '32', '3', '4', '33', '32', '58', '33', '30', '33', '49', '32', '33', '32', '16', '4', '33', '16', '33', '32', '5', '15', '33', '33', '32', '32', '35', '32', '33', '32', '34', '32', '32', '33', '10', '32', '31', '34', '33', '12', '32', '33', '27', '5', '4', '32', '32', '32', '31', '32', '33', '33', '31', '32', '33', '33', '32', '32', '6', '32', '49', '32', '6', '5', '4', '33', '15', '32', '32', '32', '5', '32', '33', '49', '32', '32', '32', '32', '33', '17', '32', '32', '4', '32', '31', '32', '37', '35', '1', '32', '12', '30', '33', '5', '32', '20', '5', '5', '32', '32', '49', '31', '32', '32', '6', '4', '32', '26', '31', '5', '5', '32', '32', '32', '33', '32', '32', '33', '30', '33', '32', '31', '32', '5', '32', '32', '32', '4', '49', '31', '32', '32', '33', '31', '32', '32', '11', '32', '49', '31', '4', '36', '5', '3', '9', '31', '12', '32', '32', '30', '4', '4', '4', '33', '49', '32', '32', '30', '4', '49', '31', '31', '33', '33', '32', '34', '32', '49', '32', '32', '5', '4', '8', '32', '32', '33', '12', '5', '32', '32', '32', '32', '32', '32', '8', '32', '32', '32', '32', '33', '2', '33', '32', '30', '33', '31', '32', '23', '30', '25', '5', '66', '36', '5', '32', '33', '31', '32', '32', '10', '33', '33', '14', '33', '33', '32', '13', '9', '18', '32', '34', '2', '32', '32', '4', '49', '5', '19', '4', '32', '33', '33', '35', '31', '22', '32', '32', '5', '30', '28', '32', '32', '32', '34', '32', '4', '6', '31', '32', '4', '32', '4', '33', '32', '33', '31', '6', '4', '32', '29', '13', '34', '32', '11', '34', '32', '8', '32', '33', '32', '49', '4', '32', '36', '33', '33', '7', '32', '32', '85', '32', '32', '33', '32', '9', '5', '4', '32', '12', '32', '32', '4', '30', '16', '32', '32', '1', '32', '33', '5', '32', '49', '33', '72', '31', '11', '5', '33', '49', '4', '31', '6', '33', '17', '33', '32', '5', '32', '32', '32', '14', '5', '26', '5', '17', '31', '4', '33', '30', '4', '32', '27', '23', '12', '32', '32', '32', '32', '32', '25', '32', '30', '32', '31', '33', '32', '32', '4', '5', '4', '33', '32', '33', '32', '32', '32', '32', '49', '31', '25', '32', '6', '33', '32', '5', '65', '8', '7', '32', '32', '32', '49', '32', '32', '6', '32', '15', '32', '11', '32', '32', '31', '32', '34', '6', '33', '32', '33', '32', '31', '15', '33', '32', '33', '32', '34', '25', '32', '32', '32', '33', '32', '50', '33', '32', '32', '49', '32', '6', '32', '5', '32', '32', '49', '32', '32', '5', '32', '4', '49', '32', '32', '33', '9', '32', '16', '33', '32', '33', '31', '4', '8', '5', '35', '5', '49', '6', '49', '32', '32', '32', '34', '32', '1', '9', '49', '32', '33', '4', '30', '49', '30', '4', '33', '32', '5', '30', '33', '11', '32', '32', '49', '4', '5', '33', '31', '5', '5', '25', '58', '32', '32', '13', '5', '31', '30', '32', '40', '12', '32', '12', '34', '33', '5', '35', '22', '25', '33', '28', '30', '5', '32', '27', '33', '33', '32', '5', '33', '5', '33', '30', '32', '9', '5', '30', '33', '48', '32', '12', '32', '32', '25', '32', '4', '32', '32', '16', '4', '5', '32', '45', '32', '5', '33', '32', '54', '14', '7', '5', '32', '4', '47', '33', '49', '5', '30', '7', '30', '5', '6', '30', '32', '5', '7', '5', '33', '32', '33', '5', '49', '30', '30', '35', '4', '8', '33', '32', '30', '8', '32', '5', '5', '32', '15', '30', '5', '32', '5', '72', '13', '10', '31', '4', '28', '20', '71', '32', '5', '19', '33', '32', '32', '7', '10', '94', '32', '32', '33', '28', '8', '34', '15', '4', '32', '1', '32', '15', '8', '32', '8', '5', '33', '34', '6', '32', '32', '12', '11', '79', '32', '32', '32', '33', '33', '18', '5', '49', '5', '33', '32', '6', '32', '13', '4', '33', '32', '4', '33', '4', '5', '73', '33', '31', '12', '13', '33', '32', '32', '33', '23', '33', '33', '33', '32', '32', '32', '33', '57', '4', '35', '6', '31', '33', '5', '30', '30', '32', '33', '6', '32', '32', '5', '8', '82', '33', '32', '34', '11', '5', '15', '33', '32', '6', '32', '5', '33', '32', '32', '32', '33', '33', '11', '28', '28', '32', '5', '35', '33', '32', '33', '32', '33', '32', '5', '32', '32', '33', '19', '32', '49', '33', '33', '32', '3', '32', '32', '34', '32', '5', '32', '32', '33', '13', '29', '35', '32', '32', '5', '29', '33', '5', '33', '32', '33', '33', '7', '32', '33', '32', '7', '32', '14', '5', '32', '32', '32', '5', '5', '5', '4', '5', '5', '5', '14', '8', '32', '33', '32', '30', '32', '33', '24', '11', '32', '4', '32', '32', '27', '32', '32', '51', '31', '33', '49', '6', '33', '12', '33', '5', '33', '8', '5', '33', '32', '30', '9', '31', '33', '32', '14', '5', '32', '32', '32', '32', '32', '49', '32', '32', '32', '21', '33', '33', '32', '32', '32', '33', '32', '33', '32', '19', '23', '33', '33', '32', '32', '32', '33', '33', '30', '32', '33', '5', '32', '4', '32', '32', '7', '33', '5', '5', '5', '30', '5', '32', '30', '12', '7', '53', '6', '32', '6', '5', '5', '48', '33', '34', '4', '33', '32', '32', '33', '8', '32', '32', '33', '32', '32', '32', '12', '32', '5', '33', '32', '33', '15', '32', '16', '32', '33', '32', '32', '32', '32', '27', '33', '32', '32', '34', '33', '32', '34', '7', '32', '33', '32', '32', '33', '48', '12', '33', '32', '33', '33', '32', '33', '4', '5', '32', '33', '32', '32', '61', '13', '32', '32', '35', '32', '35', '32', '32', '33', '85', '32', '5', '30', '32', '33', '32', '5', '33', '4', '4', '32', '5', '4', '32', '25', '34', '32', '11', '32', '33', '32', '5', '4', '32', '32', '33', '47', '33', '12', '12', '32', '32', '33', '7', '32', '32', '32', '30', '32', '32', '32', '32', '4', '32', '33', '5', '31', '8', '11', '76', '32', '6', '32', '11', '49', '5', '25', '49', '32', '11', '4', '32', '32', '32', '33', '32', '32', '71', '32', '4', '32', '32', '33', '32', '12', '32', '29', '13', '12', '5', '31', '32', '32', '34', '33', '31', '8', '33', '32', '32', '33', '33', '32', '32', '9', '12', '32', '33', '32', '46', '32', '32', '34', '32', '33', '11', '5', '32', '32', '33', '30', '32', '21', '32', '33', '33', '33', '32', '33', '14', '33', '32', '32', '33', '33', '7', '33', '32', '45', '42', '32', '51', '1', '33', '8', '32', '33', '33', '5', '33', '32', '32', '10', '33', '32', '32', '32', '32', '32', '33', '31', '5', '6', '5', '10', '32', '30', '33', '5', '32', '27', '38', '12', '5', '32', '33', '32', '32', '12', '32', '67', '34', '33', '32', '32', '32', '33', '8', '33', '33', '60', '7', '33', '32', '8', '5', '61', '32', '32', '5', '7', '32', '19', '32', '6', '32', '33', '4', '49', '34', '33', '32', '32', '31', '49', '30', '10', '11', '33', '33', '33', '32', '30', '32', '32', '11', '33', '33', '32', '49', '15', '32', '64', '12', '33', '5', '6', '5', '30', '33', '32', '33', '11', '32', '26', '34', '31', '33', '33', '49', '13', '</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atendido', 'Atend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>